<commit_message>
Added code to fix discovered memory leaks and to verify that the genomes were saved correctly to the database.  Also fixed bug which prevented mutations.
</commit_message>
<xml_diff>
--- a/Progress.xlsx
+++ b/Progress.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/c51537410c5afe56/Projects/Source/Repos/EdGarrity/SOS/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="3" documentId="8_{5E2EAEB4-78E5-45C6-8971-9CA846BBA1BA}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{72FFCFF5-A381-4D8F-B191-1A254FD82E65}"/>
+  <xr:revisionPtr revIDLastSave="84" documentId="114_{B2D123C0-10CD-4892-A2B1-0D4FB86B9D90}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{03E40BBD-7F1B-443B-BDB9-A8E176704BE9}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{D7613C25-2959-4D88-A8C3-21B00E74DE47}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{D7613C25-2959-4D88-A8C3-21B00E74DE47}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Run 1" sheetId="1" r:id="rId1"/>
+    <sheet name="Run 2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -33,12 +34,27 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="7">
   <si>
     <t>BestIndividual_Training_Error</t>
   </si>
   <si>
     <t>Average_Training_Error</t>
+  </si>
+  <si>
+    <t>% Change</t>
+  </si>
+  <si>
+    <t>M = 40%</t>
+  </si>
+  <si>
+    <t>M = 0%</t>
+  </si>
+  <si>
+    <t>M = 10%</t>
+  </si>
+  <si>
+    <t>R</t>
   </si>
 </sst>
 </file>
@@ -74,9 +90,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="4" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -149,7 +166,7 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$B$1</c:f>
+              <c:f>'Run 1'!$B$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -172,7 +189,7 @@
           </c:marker>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$B$2:$B$127</c:f>
+              <c:f>'Run 1'!$B$2:$B$127</c:f>
               <c:numCache>
                 <c:formatCode>#,##0.00</c:formatCode>
                 <c:ptCount val="126"/>
@@ -585,7 +602,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$A$1</c:f>
+              <c:f>'Run 1'!$A$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -608,7 +625,7 @@
           </c:marker>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$A$2:$A$127</c:f>
+              <c:f>'Run 1'!$A$2:$A$127</c:f>
               <c:numCache>
                 <c:formatCode>#,##0.00</c:formatCode>
                 <c:ptCount val="126"/>
@@ -1270,7 +1287,864 @@
 </c:chartSpace>
 </file>
 
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="2000" b="0" i="0" u="none" strike="noStrike" kern="1200" cap="none" spc="0" normalizeH="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mj-lt"/>
+              <a:ea typeface="+mj-ea"/>
+              <a:cs typeface="+mj-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Run 2'!$B$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Average_Training_Error</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="38100" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>'Run 2'!$B$2:$B$67</c:f>
+              <c:numCache>
+                <c:formatCode>#,##0.00</c:formatCode>
+                <c:ptCount val="66"/>
+                <c:pt idx="0">
+                  <c:v>136667774.57913801</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>274062515.59008598</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>210352008.09481099</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>169807469.161365</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>121838079.11397199</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>84377645.149830297</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>54192036.462487601</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>38435280.561887503</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>33030848.500149298</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>25610150.373538401</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>17288092.747179199</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>14042736.7002797</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>11390428.0866795</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>10208246.7685271</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>7704297.22659811</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>14546398.465387501</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>9754650.6662177294</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>8283439.0387913603</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>8361174.7327378001</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>43991225.192548402</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>61135667.578934602</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>79319545.024535805</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>100120450.547058</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>105806325.15772399</c:v>
+                </c:pt>
+                <c:pt idx="24" formatCode="General">
+                  <c:v>91951300.754062593</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>89041890.227582097</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>86295205.693590596</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>93446945.459736899</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>92077216.120756999</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>95874402.522303</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>86209857.688098401</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>90809600.017914802</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>84972293.675822303</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>79087201.253378496</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>83751474.098197594</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>93074767.790921107</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>103259261.885226</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>95185118.625503093</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>93100334.827988595</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>98921197.781541899</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>61720181.108913101</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>52576559.470010601</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>38685770.0761609</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>44115700.054772697</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>28201029.4247839</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>59146609.222422197</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>95361726.737619504</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>65260390.734304801</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>40832490.112844199</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>48384640.8640147</c:v>
+                </c:pt>
+                <c:pt idx="50">
+                  <c:v>41086223.4482444</c:v>
+                </c:pt>
+                <c:pt idx="51">
+                  <c:v>33752405.253435202</c:v>
+                </c:pt>
+                <c:pt idx="52">
+                  <c:v>36424633.449873596</c:v>
+                </c:pt>
+                <c:pt idx="53">
+                  <c:v>42957896.887764998</c:v>
+                </c:pt>
+                <c:pt idx="54">
+                  <c:v>77827984.499236196</c:v>
+                </c:pt>
+                <c:pt idx="55">
+                  <c:v>57981992.971203998</c:v>
+                </c:pt>
+                <c:pt idx="56">
+                  <c:v>73639792.256328002</c:v>
+                </c:pt>
+                <c:pt idx="57">
+                  <c:v>68837326.034295902</c:v>
+                </c:pt>
+                <c:pt idx="58">
+                  <c:v>84232326.485389099</c:v>
+                </c:pt>
+                <c:pt idx="59">
+                  <c:v>82741629.529615596</c:v>
+                </c:pt>
+                <c:pt idx="60">
+                  <c:v>78953070.296337202</c:v>
+                </c:pt>
+                <c:pt idx="61">
+                  <c:v>72031365.619615495</c:v>
+                </c:pt>
+                <c:pt idx="62">
+                  <c:v>53033679.468397498</c:v>
+                </c:pt>
+                <c:pt idx="63">
+                  <c:v>43423538.441263199</c:v>
+                </c:pt>
+                <c:pt idx="64">
+                  <c:v>47772331.350540496</c:v>
+                </c:pt>
+                <c:pt idx="65">
+                  <c:v>35553504.029974498</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-0D6D-4B3D-B50B-88FE47EF97BF}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:marker val="1"/>
+        <c:smooth val="0"/>
+        <c:axId val="715829080"/>
+        <c:axId val="715823504"/>
+      </c:lineChart>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Run 2'!$A$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>BestIndividual_Training_Error</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="38100" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>'Run 2'!$A$2:$A$67</c:f>
+              <c:numCache>
+                <c:formatCode>#,##0.00</c:formatCode>
+                <c:ptCount val="66"/>
+                <c:pt idx="0">
+                  <c:v>15.2970585407784</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>13.076696830622</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>13.076696830622</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>13.076696830622</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>13.076696830622</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>13.076696830622</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>13.076696830622</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>13.076696830622</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>13.076696830622</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>13.076696830622</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>13.076696830622</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>13.076696830622</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>13.076696830622</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>13.076696830622</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>13.076696830622</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>13.076696830622</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>13.076696830622</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>13.076696830622</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>13.076696830622</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>13.0384048104053</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>13.0384048104053</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>13.0384048104053</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>13.0384048104053</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>13.0384048104053</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>13.0384048104053</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>13.0384048104053</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>13.0384048104053</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>13.0384048104053</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>13.0384048104053</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>13.0384048104053</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>13.0384048104053</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>13.0384048104053</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>13.0384048104053</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>13.0384048104053</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>13.0384048104053</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>13.0384048104053</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>13.0384048104053</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>13.0384048104053</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>13.0384048104053</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>13.0384048104053</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>16.7928556237467</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>15.2970585407784</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>13.076696830622</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>13.076696830622</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>19.104973174542799</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>15.2970585407784</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>15.2970585407784</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>15.2970585407784</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>15.2970585407784</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>15.2970585407784</c:v>
+                </c:pt>
+                <c:pt idx="50">
+                  <c:v>15.2970585407784</c:v>
+                </c:pt>
+                <c:pt idx="51">
+                  <c:v>15.2970585407784</c:v>
+                </c:pt>
+                <c:pt idx="52">
+                  <c:v>15.2970585407784</c:v>
+                </c:pt>
+                <c:pt idx="53">
+                  <c:v>15.2970585407784</c:v>
+                </c:pt>
+                <c:pt idx="54">
+                  <c:v>15.2970585407784</c:v>
+                </c:pt>
+                <c:pt idx="55">
+                  <c:v>15.2970585407784</c:v>
+                </c:pt>
+                <c:pt idx="56">
+                  <c:v>15.2970585407784</c:v>
+                </c:pt>
+                <c:pt idx="57">
+                  <c:v>15.2970585407784</c:v>
+                </c:pt>
+                <c:pt idx="58">
+                  <c:v>15.2970585407784</c:v>
+                </c:pt>
+                <c:pt idx="59">
+                  <c:v>15.2970585407784</c:v>
+                </c:pt>
+                <c:pt idx="60">
+                  <c:v>15.2970585407784</c:v>
+                </c:pt>
+                <c:pt idx="61">
+                  <c:v>15.2970585407784</c:v>
+                </c:pt>
+                <c:pt idx="62">
+                  <c:v>15.2970585407784</c:v>
+                </c:pt>
+                <c:pt idx="63">
+                  <c:v>15.2970585407784</c:v>
+                </c:pt>
+                <c:pt idx="64">
+                  <c:v>15.2970585407784</c:v>
+                </c:pt>
+                <c:pt idx="65">
+                  <c:v>19.3907194296653</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-0D6D-4B3D-B50B-88FE47EF97BF}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:marker val="1"/>
+        <c:smooth val="0"/>
+        <c:axId val="840836808"/>
+        <c:axId val="840833856"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="715829080"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" cap="none" spc="0" normalizeH="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="715823504"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="715823504"/>
+        <c:scaling>
+          <c:logBase val="10"/>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:minorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="5000"/>
+                  <a:lumOff val="95000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:minorGridlines>
+        <c:numFmt formatCode="#,##0.00" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="715829080"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="840833856"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="r"/>
+        <c:numFmt formatCode="#,##0.00" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="840836808"/>
+        <c:crosses val="max"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:catAx>
+        <c:axId val="840836808"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="1"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="840833856"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="t"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
 <file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors2.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
   <a:schemeClr val="accent2"/>
@@ -1810,6 +2684,506 @@
 </cs:chartStyle>
 </file>
 
+<file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="235">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200" cap="all"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" b="0" kern="1200" cap="none" spc="0" normalizeH="0" baseline="0"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="38100" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="8"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:prstDash val="dash"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:prstDash val="dash"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="major">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="2000" b="0" kern="1200" cap="none" spc="0" normalizeH="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
@@ -1835,6 +3209,49 @@
           </a:extLst>
         </xdr:cNvPr>
         <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>561975</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>26</xdr:col>
+      <xdr:colOff>518160</xdr:colOff>
+      <xdr:row>37</xdr:row>
+      <xdr:rowOff>19050</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{87DD270B-4708-4B98-A301-85905BA2B53B}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
         <a:off x="0" y="0"/>
@@ -2150,15 +3567,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{98DDA464-7CD7-4D3D-AE21-4B05822D1057}">
   <dimension ref="A1:B127"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="27.7109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="22.140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="27.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="22.109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2166,7 +3583,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" s="1">
         <v>16.9705627484771</v>
       </c>
@@ -2174,7 +3591,7 @@
         <v>133309653.864713</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" s="1">
         <v>15.2970585407784</v>
       </c>
@@ -2182,7 +3599,7 @@
         <v>295757858.59359902</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" s="1">
         <v>15.2970585407784</v>
       </c>
@@ -2190,7 +3607,7 @@
         <v>237732284.50958899</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5" s="1">
         <v>12</v>
       </c>
@@ -2198,7 +3615,7 @@
         <v>158986595.06644401</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A6" s="1">
         <v>15.2970585407784</v>
       </c>
@@ -2206,7 +3623,7 @@
         <v>109085283.752441</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A7" s="1">
         <v>12.1655250605964</v>
       </c>
@@ -2214,7 +3631,7 @@
         <v>135784738.7274</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A8" s="1">
         <v>15.2970585407784</v>
       </c>
@@ -2222,7 +3639,7 @@
         <v>125146244.002275</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A9" s="1">
         <v>15.2970585407784</v>
       </c>
@@ -2230,7 +3647,7 @@
         <v>78062152.874164894</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A10" s="1">
         <v>13.076696830622</v>
       </c>
@@ -2238,7 +3655,7 @@
         <v>72532880.897681907</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A11" s="1">
         <v>15.2970585407784</v>
       </c>
@@ -2246,7 +3663,7 @@
         <v>106312943.231591</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A12" s="1">
         <v>18.083141320025099</v>
       </c>
@@ -2254,7 +3671,7 @@
         <v>117197857.637825</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A13" s="1">
         <v>18.083141320025099</v>
       </c>
@@ -2262,7 +3679,7 @@
         <v>146517422.96852201</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A14" s="1">
         <v>17.606816861658999</v>
       </c>
@@ -2270,7 +3687,7 @@
         <v>159276989.17551699</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A15" s="1">
         <v>19.798989873223299</v>
       </c>
@@ -2278,7 +3695,7 @@
         <v>165708691.59843701</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A16" s="1">
         <v>16.031219541881399</v>
       </c>
@@ -2286,7 +3703,7 @@
         <v>161634818.71100199</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A17" s="1">
         <v>16.340134638368198</v>
       </c>
@@ -2294,7 +3711,7 @@
         <v>213141440.36674699</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A18" s="1">
         <v>16.703293088490099</v>
       </c>
@@ -2302,7 +3719,7 @@
         <v>219590793.08662599</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A19" s="1">
         <v>13.076696830622</v>
       </c>
@@ -2310,7 +3727,7 @@
         <v>206822485.65399301</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A20" s="1">
         <v>15.2970585407784</v>
       </c>
@@ -2318,7 +3735,7 @@
         <v>313606715.04114002</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A21" s="1">
         <v>13.076696830622</v>
       </c>
@@ -2326,7 +3743,7 @@
         <v>283465461.93871301</v>
       </c>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A22" s="1">
         <v>15.2970585407784</v>
       </c>
@@ -2334,7 +3751,7 @@
         <v>249366128.73950601</v>
       </c>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A23" s="1">
         <v>15.2970585407784</v>
       </c>
@@ -2342,7 +3759,7 @@
         <v>190257797.28316799</v>
       </c>
     </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A24" s="1">
         <v>20.049937655763401</v>
       </c>
@@ -2350,7 +3767,7 @@
         <v>183821751.93959701</v>
       </c>
     </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A25" s="1">
         <v>15.2970585407784</v>
       </c>
@@ -2358,7 +3775,7 @@
         <v>168364365.740325</v>
       </c>
     </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A26" s="1">
         <v>15.2970585407784</v>
       </c>
@@ -2366,7 +3783,7 @@
         <v>189665778.70659801</v>
       </c>
     </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A27" s="1">
         <v>20.297783130184399</v>
       </c>
@@ -2374,7 +3791,7 @@
         <v>184479035.88859501</v>
       </c>
     </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A28" s="1">
         <v>16.7928556237467</v>
       </c>
@@ -2382,7 +3799,7 @@
         <v>183063352.253883</v>
       </c>
     </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A29" s="1">
         <v>18.466185312619402</v>
       </c>
@@ -2390,7 +3807,7 @@
         <v>173618366.69787201</v>
       </c>
     </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A30" s="1">
         <v>16.613247725836199</v>
       </c>
@@ -2398,7 +3815,7 @@
         <v>174265737.53803101</v>
       </c>
     </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A31" s="1">
         <v>15.3297097167559</v>
       </c>
@@ -2406,7 +3823,7 @@
         <v>157335982.41585499</v>
       </c>
     </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A32" s="1">
         <v>15.2970585407784</v>
       </c>
@@ -2414,7 +3831,7 @@
         <v>168388978.502368</v>
       </c>
     </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A33" s="1">
         <v>15.2970585407784</v>
       </c>
@@ -2422,7 +3839,7 @@
         <v>158590933.55726799</v>
       </c>
     </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A34" s="1">
         <v>15.2970585407784</v>
       </c>
@@ -2430,7 +3847,7 @@
         <v>158507648.19407001</v>
       </c>
     </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A35" s="1">
         <v>18.439088914585799</v>
       </c>
@@ -2438,7 +3855,7 @@
         <v>155533869.682794</v>
       </c>
     </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A36" s="1">
         <v>15.2970585407784</v>
       </c>
@@ -2446,7 +3863,7 @@
         <v>143126326.531555</v>
       </c>
     </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A37" s="1">
         <v>15.2970585407784</v>
       </c>
@@ -2454,7 +3871,7 @@
         <v>158444104.23501801</v>
       </c>
     </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A38" s="1">
         <v>17.0880074906351</v>
       </c>
@@ -2462,7 +3879,7 @@
         <v>150483022.80139399</v>
       </c>
     </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A39" s="1">
         <v>15.2970585407784</v>
       </c>
@@ -2470,7 +3887,7 @@
         <v>169726703.82701901</v>
       </c>
     </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A40" s="1">
         <v>15.2970585407784</v>
       </c>
@@ -2478,7 +3895,7 @@
         <v>190249221.96164</v>
       </c>
     </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A41" s="1">
         <v>14.456832294801</v>
       </c>
@@ -2486,7 +3903,7 @@
         <v>180039907.988796</v>
       </c>
     </row>
-    <row r="42" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A42" s="1">
         <v>15.937377450509199</v>
       </c>
@@ -2494,7 +3911,7 @@
         <v>176464122.88058999</v>
       </c>
     </row>
-    <row r="43" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A43" s="1">
         <v>15.2970585407784</v>
       </c>
@@ -2502,7 +3919,7 @@
         <v>161343688.722247</v>
       </c>
     </row>
-    <row r="44" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A44" s="1">
         <v>15.2970585407784</v>
       </c>
@@ -2510,7 +3927,7 @@
         <v>165191652.71832499</v>
       </c>
     </row>
-    <row r="45" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A45" s="1">
         <v>15.2970585407784</v>
       </c>
@@ -2518,7 +3935,7 @@
         <v>193988055.97467101</v>
       </c>
     </row>
-    <row r="46" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A46" s="1">
         <v>15.2970585407784</v>
       </c>
@@ -2526,7 +3943,7 @@
         <v>200436619.88411099</v>
       </c>
     </row>
-    <row r="47" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A47" s="1">
         <v>15</v>
       </c>
@@ -2534,7 +3951,7 @@
         <v>186958353.910992</v>
       </c>
     </row>
-    <row r="48" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A48" s="1">
         <v>14.832396974191299</v>
       </c>
@@ -2542,7 +3959,7 @@
         <v>169483554.895769</v>
       </c>
     </row>
-    <row r="49" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A49" s="1">
         <v>15</v>
       </c>
@@ -2550,7 +3967,7 @@
         <v>186713982.97504199</v>
       </c>
     </row>
-    <row r="50" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A50" s="1">
         <v>15</v>
       </c>
@@ -2558,7 +3975,7 @@
         <v>195151631.72571701</v>
       </c>
     </row>
-    <row r="51" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A51" s="1">
         <v>15</v>
       </c>
@@ -2566,7 +3983,7 @@
         <v>172708932.329956</v>
       </c>
     </row>
-    <row r="52" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A52" s="1">
         <v>15</v>
       </c>
@@ -2574,7 +3991,7 @@
         <v>140210706.88954401</v>
       </c>
     </row>
-    <row r="53" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A53" s="1">
         <v>14.5258390463339</v>
       </c>
@@ -2582,7 +3999,7 @@
         <v>169008189.40406999</v>
       </c>
     </row>
-    <row r="54" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A54" s="1">
         <v>15.2970585407784</v>
       </c>
@@ -2590,7 +4007,7 @@
         <v>173481799.53326601</v>
       </c>
     </row>
-    <row r="55" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A55" s="1">
         <v>15.6843871413581</v>
       </c>
@@ -2598,7 +4015,7 @@
         <v>190722447.56489199</v>
       </c>
     </row>
-    <row r="56" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A56" s="1">
         <v>15.2970585407784</v>
       </c>
@@ -2606,7 +4023,7 @@
         <v>183440239.813041</v>
       </c>
     </row>
-    <row r="57" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A57" s="1">
         <v>15.2970585407784</v>
       </c>
@@ -2614,7 +4031,7 @@
         <v>205283777.170423</v>
       </c>
     </row>
-    <row r="58" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A58" s="1">
         <v>15.2970585407784</v>
       </c>
@@ -2622,7 +4039,7 @@
         <v>202371516.67750499</v>
       </c>
     </row>
-    <row r="59" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A59" s="1">
         <v>15.6843871413581</v>
       </c>
@@ -2630,7 +4047,7 @@
         <v>210259529.58863899</v>
       </c>
     </row>
-    <row r="60" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A60" s="1">
         <v>15.6843871413581</v>
       </c>
@@ -2638,7 +4055,7 @@
         <v>226704922.84898999</v>
       </c>
     </row>
-    <row r="61" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A61" s="1">
         <v>15.3297097167559</v>
       </c>
@@ -2646,7 +4063,7 @@
         <v>221791156.57853401</v>
       </c>
     </row>
-    <row r="62" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A62" s="1">
         <v>15.2970585407784</v>
       </c>
@@ -2654,7 +4071,7 @@
         <v>211704154.76751599</v>
       </c>
     </row>
-    <row r="63" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A63" s="1">
         <v>15.6843871413581</v>
       </c>
@@ -2662,7 +4079,7 @@
         <v>212989524.79824099</v>
       </c>
     </row>
-    <row r="64" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A64" s="1">
         <v>15.6843871413581</v>
       </c>
@@ -2670,7 +4087,7 @@
         <v>175376275.08457699</v>
       </c>
     </row>
-    <row r="65" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A65" s="1">
         <v>15.6843871413581</v>
       </c>
@@ -2678,7 +4095,7 @@
         <v>181310827.06749499</v>
       </c>
     </row>
-    <row r="66" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A66" s="1">
         <v>15.6843871413581</v>
       </c>
@@ -2686,7 +4103,7 @@
         <v>211035911.99666899</v>
       </c>
     </row>
-    <row r="67" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A67" s="1">
         <v>15.2970585407784</v>
       </c>
@@ -2694,7 +4111,7 @@
         <v>221654934.579108</v>
       </c>
     </row>
-    <row r="68" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A68" s="1">
         <v>15.2970585407784</v>
       </c>
@@ -2702,7 +4119,7 @@
         <v>202837907.036448</v>
       </c>
     </row>
-    <row r="69" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A69" s="1">
         <v>15.2970585407784</v>
       </c>
@@ -2710,7 +4127,7 @@
         <v>195895085.82306299</v>
       </c>
     </row>
-    <row r="70" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A70" s="1">
         <v>15.2970585407784</v>
       </c>
@@ -2718,7 +4135,7 @@
         <v>218775769.160465</v>
       </c>
     </row>
-    <row r="71" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A71" s="1">
         <v>13.3790881602597</v>
       </c>
@@ -2726,7 +4143,7 @@
         <v>223315564.80693001</v>
       </c>
     </row>
-    <row r="72" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A72" s="1">
         <v>16.6433169770932</v>
       </c>
@@ -2734,7 +4151,7 @@
         <v>257808893.66757199</v>
       </c>
     </row>
-    <row r="73" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A73" s="1">
         <v>15.2970585407784</v>
       </c>
@@ -2742,7 +4159,7 @@
         <v>289484904.381387</v>
       </c>
     </row>
-    <row r="74" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A74" s="1">
         <v>16.6433169770932</v>
       </c>
@@ -2750,7 +4167,7 @@
         <v>310999508.21957099</v>
       </c>
     </row>
-    <row r="75" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A75" s="1">
         <v>17.7482393492988</v>
       </c>
@@ -2758,7 +4175,7 @@
         <v>287303146.81806803</v>
       </c>
     </row>
-    <row r="76" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A76" s="1">
         <v>18.493242008906901</v>
       </c>
@@ -2766,7 +4183,7 @@
         <v>293147059.69437498</v>
       </c>
     </row>
-    <row r="77" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A77" s="1">
         <v>17.7482393492988</v>
       </c>
@@ -2774,7 +4191,7 @@
         <v>277296417.03704298</v>
       </c>
     </row>
-    <row r="78" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A78" s="1">
         <v>16.7928556237467</v>
       </c>
@@ -2782,7 +4199,7 @@
         <v>254266072.182239</v>
       </c>
     </row>
-    <row r="79" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A79" s="1">
         <v>16.6433169770932</v>
       </c>
@@ -2790,7 +4207,7 @@
         <v>244803578.08134499</v>
       </c>
     </row>
-    <row r="80" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A80" s="1">
         <v>15.2970585407784</v>
       </c>
@@ -2798,7 +4215,7 @@
         <v>241979689.331981</v>
       </c>
     </row>
-    <row r="81" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A81" s="1">
         <v>13.0384048104053</v>
       </c>
@@ -2806,7 +4223,7 @@
         <v>235462257.22058499</v>
       </c>
     </row>
-    <row r="82" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A82" s="1">
         <v>18.0554700852678</v>
       </c>
@@ -2814,7 +4231,7 @@
         <v>237620887.86837</v>
       </c>
     </row>
-    <row r="83" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A83" s="1">
         <v>17.4928556845359</v>
       </c>
@@ -2822,7 +4239,7 @@
         <v>237065108.71807399</v>
       </c>
     </row>
-    <row r="84" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A84" s="1">
         <v>16.7928556237467</v>
       </c>
@@ -2830,7 +4247,7 @@
         <v>223565414.13950101</v>
       </c>
     </row>
-    <row r="85" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A85" s="1">
         <v>15.2970585407784</v>
       </c>
@@ -2838,7 +4255,7 @@
         <v>220920489.94237301</v>
       </c>
     </row>
-    <row r="86" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A86" s="1">
         <v>17.4928556845359</v>
       </c>
@@ -2846,7 +4263,7 @@
         <v>221461780.76565501</v>
       </c>
     </row>
-    <row r="87" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A87" s="1">
         <v>15.2970585407784</v>
       </c>
@@ -2854,7 +4271,7 @@
         <v>206948718.13720599</v>
       </c>
     </row>
-    <row r="88" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A88" s="1">
         <v>13.076696830622</v>
       </c>
@@ -2862,7 +4279,7 @@
         <v>209672261.19197699</v>
       </c>
     </row>
-    <row r="89" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A89" s="1">
         <v>17.058722109232001</v>
       </c>
@@ -2870,7 +4287,7 @@
         <v>201193401.78613299</v>
       </c>
     </row>
-    <row r="90" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A90" s="1">
         <v>15.2970585407784</v>
       </c>
@@ -2878,7 +4295,7 @@
         <v>186356196.35809201</v>
       </c>
     </row>
-    <row r="91" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A91" s="1">
         <v>15.2970585407784</v>
       </c>
@@ -2886,7 +4303,7 @@
         <v>153154245.987854</v>
       </c>
     </row>
-    <row r="92" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A92" s="1">
         <v>15.2970585407784</v>
       </c>
@@ -2894,7 +4311,7 @@
         <v>173305017.328269</v>
       </c>
     </row>
-    <row r="93" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A93" s="1">
         <v>15.2970585407784</v>
       </c>
@@ -2902,7 +4319,7 @@
         <v>154232221.534468</v>
       </c>
     </row>
-    <row r="94" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A94" s="1">
         <v>15.2970585407784</v>
       </c>
@@ -2910,7 +4327,7 @@
         <v>182384102.515457</v>
       </c>
     </row>
-    <row r="95" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A95" s="1">
         <v>15.2970585407784</v>
       </c>
@@ -2918,7 +4335,7 @@
         <v>154580064.32901701</v>
       </c>
     </row>
-    <row r="96" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A96" s="1">
         <v>15.2970585407784</v>
       </c>
@@ -2926,7 +4343,7 @@
         <v>212932250.76803401</v>
       </c>
     </row>
-    <row r="97" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A97" s="1">
         <v>15.2970585407784</v>
       </c>
@@ -2934,7 +4351,7 @@
         <v>214645263.92091</v>
       </c>
     </row>
-    <row r="98" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A98" s="1">
         <v>15.2970585407784</v>
       </c>
@@ -2942,7 +4359,7 @@
         <v>187307096.270044</v>
       </c>
     </row>
-    <row r="99" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A99" s="1">
         <v>15.2970585407784</v>
       </c>
@@ -2950,7 +4367,7 @@
         <v>159428813.456352</v>
       </c>
     </row>
-    <row r="100" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A100" s="1">
         <v>15.2970585407784</v>
       </c>
@@ -2958,7 +4375,7 @@
         <v>150968764.775859</v>
       </c>
     </row>
-    <row r="101" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A101" s="1">
         <v>16.7928556237467</v>
       </c>
@@ -2966,7 +4383,7 @@
         <v>121112125.23019999</v>
       </c>
     </row>
-    <row r="102" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A102" s="1">
         <v>15.5884572681199</v>
       </c>
@@ -2974,7 +4391,7 @@
         <v>134410349.58807901</v>
       </c>
     </row>
-    <row r="103" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A103" s="1">
         <v>15.2970585407784</v>
       </c>
@@ -2982,7 +4399,7 @@
         <v>151308865.98785201</v>
       </c>
     </row>
-    <row r="104" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A104" s="1">
         <v>18.248287590894702</v>
       </c>
@@ -2990,7 +4407,7 @@
         <v>182045915.95560601</v>
       </c>
     </row>
-    <row r="105" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A105" s="1">
         <v>15.2970585407784</v>
       </c>
@@ -2998,7 +4415,7 @@
         <v>231996357.272567</v>
       </c>
     </row>
-    <row r="106" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A106" s="1">
         <v>15.2970585407784</v>
       </c>
@@ -3006,7 +4423,7 @@
         <v>259723119.45256999</v>
       </c>
     </row>
-    <row r="107" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A107" s="1">
         <v>15.2970585407784</v>
       </c>
@@ -3014,7 +4431,7 @@
         <v>258746666.94246799</v>
       </c>
     </row>
-    <row r="108" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A108" s="1">
         <v>18.248287590894702</v>
       </c>
@@ -3022,7 +4439,7 @@
         <v>298474962.46452701</v>
       </c>
     </row>
-    <row r="109" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A109" s="1">
         <v>15.2970585407784</v>
       </c>
@@ -3030,7 +4447,7 @@
         <v>324083046.06996697</v>
       </c>
     </row>
-    <row r="110" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A110" s="1">
         <v>15.2970585407784</v>
       </c>
@@ -3038,7 +4455,7 @@
         <v>294273134.85311198</v>
       </c>
     </row>
-    <row r="111" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A111" s="1">
         <v>17.521415467935199</v>
       </c>
@@ -3046,7 +4463,7 @@
         <v>272843218.510023</v>
       </c>
     </row>
-    <row r="112" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A112" s="1">
         <v>15.2970585407784</v>
       </c>
@@ -3054,7 +4471,7 @@
         <v>235362474.49730399</v>
       </c>
     </row>
-    <row r="113" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A113" s="1">
         <v>18.439088914585799</v>
       </c>
@@ -3062,7 +4479,7 @@
         <v>207522393.71118</v>
       </c>
     </row>
-    <row r="114" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A114" s="1">
         <v>15.2970585407784</v>
       </c>
@@ -3070,7 +4487,7 @@
         <v>205405650.692128</v>
       </c>
     </row>
-    <row r="115" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A115" s="1">
         <v>15.2970585407784</v>
       </c>
@@ -3078,7 +4495,7 @@
         <v>201487732.521593</v>
       </c>
     </row>
-    <row r="116" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A116" s="1">
         <v>16.7928556237467</v>
       </c>
@@ -3086,7 +4503,7 @@
         <v>180643114.29775101</v>
       </c>
     </row>
-    <row r="117" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A117" s="1">
         <v>15.2970585407784</v>
       </c>
@@ -3094,7 +4511,7 @@
         <v>182916380.27036199</v>
       </c>
     </row>
-    <row r="118" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A118" s="1">
         <v>15.8429795177549</v>
       </c>
@@ -3102,7 +4519,7 @@
         <v>184774243.678478</v>
       </c>
     </row>
-    <row r="119" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A119" s="1">
         <v>16.7928556237467</v>
       </c>
@@ -3110,7 +4527,7 @@
         <v>178805013.650406</v>
       </c>
     </row>
-    <row r="120" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A120" s="1">
         <v>15.2970585407784</v>
       </c>
@@ -3118,7 +4535,7 @@
         <v>189674901.183274</v>
       </c>
     </row>
-    <row r="121" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A121" s="1">
         <v>15.2970585407784</v>
       </c>
@@ -3126,7 +4543,7 @@
         <v>178649498.310936</v>
       </c>
     </row>
-    <row r="122" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A122" s="1">
         <v>15.2970585407784</v>
       </c>
@@ -3134,7 +4551,7 @@
         <v>150655330.61517</v>
       </c>
     </row>
-    <row r="123" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A123" s="1">
         <v>15.2970585407784</v>
       </c>
@@ -3142,7 +4559,7 @@
         <v>170155431.841079</v>
       </c>
     </row>
-    <row r="124" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A124" s="1">
         <v>15.2970585407784</v>
       </c>
@@ -3150,7 +4567,7 @@
         <v>181922122.64351699</v>
       </c>
     </row>
-    <row r="125" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A125" s="1">
         <v>15.2970585407784</v>
       </c>
@@ -3158,7 +4575,7 @@
         <v>187711971.69815499</v>
       </c>
     </row>
-    <row r="126" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A126" s="1">
         <v>17.320508075688799</v>
       </c>
@@ -3166,13 +4583,1086 @@
         <v>212863208.303918</v>
       </c>
     </row>
-    <row r="127" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A127" s="1">
         <v>15.2970585407784</v>
       </c>
       <c r="B127" s="1">
         <v>211666625.626598</v>
       </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EFDF9A5F-6B77-43F5-8016-32B291B6E88B}">
+  <dimension ref="A1:D127"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
+      <selection activeCell="C8" sqref="C8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="27.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="22.109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.109375" style="2"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A2" s="1">
+        <v>15.2970585407784</v>
+      </c>
+      <c r="B2" s="1">
+        <v>136667774.57913801</v>
+      </c>
+      <c r="D2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A3" s="1">
+        <v>13.076696830622</v>
+      </c>
+      <c r="B3" s="1">
+        <v>274062515.59008598</v>
+      </c>
+      <c r="C3" s="2">
+        <f>(B3-B2)/B2</f>
+        <v>1.0053192234529948</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A4" s="1">
+        <v>13.076696830622</v>
+      </c>
+      <c r="B4" s="1">
+        <v>210352008.09481099</v>
+      </c>
+      <c r="C4" s="2">
+        <f t="shared" ref="C4:C67" si="0">(B4-B3)/B3</f>
+        <v>-0.23246706087514171</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A5" s="1">
+        <v>13.076696830622</v>
+      </c>
+      <c r="B5" s="1">
+        <v>169807469.161365</v>
+      </c>
+      <c r="C5" s="2">
+        <f t="shared" si="0"/>
+        <v>-0.19274614633187404</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A6" s="1">
+        <v>13.076696830622</v>
+      </c>
+      <c r="B6" s="1">
+        <v>121838079.11397199</v>
+      </c>
+      <c r="C6" s="2">
+        <f t="shared" si="0"/>
+        <v>-0.28249281544740856</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A7" s="1">
+        <v>13.076696830622</v>
+      </c>
+      <c r="B7" s="1">
+        <v>84377645.149830297</v>
+      </c>
+      <c r="C7" s="2">
+        <f t="shared" si="0"/>
+        <v>-0.30746080565748068</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A8" s="1">
+        <v>13.076696830622</v>
+      </c>
+      <c r="B8" s="1">
+        <v>54192036.462487601</v>
+      </c>
+      <c r="C8" s="2">
+        <f t="shared" si="0"/>
+        <v>-0.35774414696856949</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A9" s="1">
+        <v>13.076696830622</v>
+      </c>
+      <c r="B9" s="1">
+        <v>38435280.561887503</v>
+      </c>
+      <c r="C9" s="2">
+        <f t="shared" si="0"/>
+        <v>-0.29075777418896448</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A10" s="1">
+        <v>13.076696830622</v>
+      </c>
+      <c r="B10" s="1">
+        <v>33030848.500149298</v>
+      </c>
+      <c r="C10" s="2">
+        <f t="shared" si="0"/>
+        <v>-0.14061122964969974</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A11" s="1">
+        <v>13.076696830622</v>
+      </c>
+      <c r="B11" s="1">
+        <v>25610150.373538401</v>
+      </c>
+      <c r="C11" s="2">
+        <f t="shared" si="0"/>
+        <v>-0.22465962769855446</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A12" s="1">
+        <v>13.076696830622</v>
+      </c>
+      <c r="B12" s="1">
+        <v>17288092.747179199</v>
+      </c>
+      <c r="C12" s="2">
+        <f t="shared" si="0"/>
+        <v>-0.32495153308267721</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A13" s="1">
+        <v>13.076696830622</v>
+      </c>
+      <c r="B13" s="1">
+        <v>14042736.7002797</v>
+      </c>
+      <c r="C13" s="2">
+        <f t="shared" si="0"/>
+        <v>-0.18772204050264746</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A14" s="1">
+        <v>13.076696830622</v>
+      </c>
+      <c r="B14" s="1">
+        <v>11390428.0866795</v>
+      </c>
+      <c r="C14" s="2">
+        <f t="shared" si="0"/>
+        <v>-0.18887405426802398</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A15" s="1">
+        <v>13.076696830622</v>
+      </c>
+      <c r="B15" s="1">
+        <v>10208246.7685271</v>
+      </c>
+      <c r="C15" s="2">
+        <f t="shared" si="0"/>
+        <v>-0.10378725971984301</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A16" s="1">
+        <v>13.076696830622</v>
+      </c>
+      <c r="B16" s="1">
+        <v>7704297.22659811</v>
+      </c>
+      <c r="C16" s="2">
+        <f t="shared" si="0"/>
+        <v>-0.24528693307541125</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A17" s="1">
+        <v>13.076696830622</v>
+      </c>
+      <c r="B17" s="1">
+        <v>14546398.465387501</v>
+      </c>
+      <c r="C17" s="2">
+        <f t="shared" si="0"/>
+        <v>0.88808895056227877</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A18" s="1">
+        <v>13.076696830622</v>
+      </c>
+      <c r="B18" s="1">
+        <v>9754650.6662177294</v>
+      </c>
+      <c r="C18" s="2">
+        <f t="shared" si="0"/>
+        <v>-0.32941128421385674</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A19" s="1">
+        <v>13.076696830622</v>
+      </c>
+      <c r="B19" s="1">
+        <v>8283439.0387913603</v>
+      </c>
+      <c r="C19" s="2">
+        <f t="shared" si="0"/>
+        <v>-0.15082155966091781</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A20" s="1">
+        <v>13.076696830622</v>
+      </c>
+      <c r="B20" s="1">
+        <v>8361174.7327378001</v>
+      </c>
+      <c r="C20" s="2">
+        <f t="shared" si="0"/>
+        <v>9.3844710611623236E-3</v>
+      </c>
+      <c r="D20" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A21" s="1">
+        <v>13.0384048104053</v>
+      </c>
+      <c r="B21" s="1">
+        <v>43991225.192548402</v>
+      </c>
+      <c r="C21" s="2">
+        <f t="shared" si="0"/>
+        <v>4.261368958156412</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A22" s="1">
+        <v>13.0384048104053</v>
+      </c>
+      <c r="B22" s="1">
+        <v>61135667.578934602</v>
+      </c>
+      <c r="C22" s="2">
+        <f t="shared" si="0"/>
+        <v>0.38972413956068375</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A23" s="1">
+        <v>13.0384048104053</v>
+      </c>
+      <c r="B23" s="1">
+        <v>79319545.024535805</v>
+      </c>
+      <c r="C23" s="2">
+        <f t="shared" si="0"/>
+        <v>0.29743483903440332</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A24" s="1">
+        <v>13.0384048104053</v>
+      </c>
+      <c r="B24" s="1">
+        <v>100120450.547058</v>
+      </c>
+      <c r="C24" s="2">
+        <f t="shared" si="0"/>
+        <v>0.26224186631539403</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A25" s="1">
+        <v>13.0384048104053</v>
+      </c>
+      <c r="B25" s="1">
+        <v>105806325.15772399</v>
+      </c>
+      <c r="C25" s="2">
+        <f t="shared" si="0"/>
+        <v>5.6790341829250475E-2</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A26" s="1">
+        <v>13.0384048104053</v>
+      </c>
+      <c r="B26">
+        <v>91951300.754062593</v>
+      </c>
+      <c r="C26" s="2">
+        <f t="shared" si="0"/>
+        <v>-0.13094703348791209</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A27" s="1">
+        <v>13.0384048104053</v>
+      </c>
+      <c r="B27" s="1">
+        <v>89041890.227582097</v>
+      </c>
+      <c r="C27" s="2">
+        <f t="shared" si="0"/>
+        <v>-3.1640776178491987E-2</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A28" s="1">
+        <v>13.0384048104053</v>
+      </c>
+      <c r="B28" s="1">
+        <v>86295205.693590596</v>
+      </c>
+      <c r="C28" s="2">
+        <f t="shared" si="0"/>
+        <v>-3.0847104963419487E-2</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A29" s="1">
+        <v>13.0384048104053</v>
+      </c>
+      <c r="B29" s="1">
+        <v>93446945.459736899</v>
+      </c>
+      <c r="C29" s="2">
+        <f t="shared" si="0"/>
+        <v>8.2875285001811905E-2</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A30" s="1">
+        <v>13.0384048104053</v>
+      </c>
+      <c r="B30" s="1">
+        <v>92077216.120756999</v>
+      </c>
+      <c r="C30" s="2">
+        <f t="shared" si="0"/>
+        <v>-1.4657828912878373E-2</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A31" s="1">
+        <v>13.0384048104053</v>
+      </c>
+      <c r="B31" s="1">
+        <v>95874402.522303</v>
+      </c>
+      <c r="C31" s="2">
+        <f t="shared" si="0"/>
+        <v>4.1239152979669638E-2</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A32" s="1">
+        <v>13.0384048104053</v>
+      </c>
+      <c r="B32" s="1">
+        <v>86209857.688098401</v>
+      </c>
+      <c r="C32" s="2">
+        <f t="shared" si="0"/>
+        <v>-0.10080422490201556</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A33" s="1">
+        <v>13.0384048104053</v>
+      </c>
+      <c r="B33" s="1">
+        <v>90809600.017914802</v>
+      </c>
+      <c r="C33" s="2">
+        <f t="shared" si="0"/>
+        <v>5.3355178319142646E-2</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A34" s="1">
+        <v>13.0384048104053</v>
+      </c>
+      <c r="B34" s="1">
+        <v>84972293.675822303</v>
+      </c>
+      <c r="C34" s="2">
+        <f t="shared" si="0"/>
+        <v>-6.4280718568751796E-2</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A35" s="1">
+        <v>13.0384048104053</v>
+      </c>
+      <c r="B35" s="1">
+        <v>79087201.253378496</v>
+      </c>
+      <c r="C35" s="2">
+        <f t="shared" si="0"/>
+        <v>-6.9258956865352092E-2</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A36" s="1">
+        <v>13.0384048104053</v>
+      </c>
+      <c r="B36" s="1">
+        <v>83751474.098197594</v>
+      </c>
+      <c r="C36" s="2">
+        <f t="shared" si="0"/>
+        <v>5.897632955648241E-2</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A37" s="1">
+        <v>13.0384048104053</v>
+      </c>
+      <c r="B37" s="1">
+        <v>93074767.790921107</v>
+      </c>
+      <c r="C37" s="2">
+        <f t="shared" si="0"/>
+        <v>0.1113209503846113</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A38" s="1">
+        <v>13.0384048104053</v>
+      </c>
+      <c r="B38" s="1">
+        <v>103259261.885226</v>
+      </c>
+      <c r="C38" s="2">
+        <f t="shared" si="0"/>
+        <v>0.10942271827293591</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A39" s="1">
+        <v>13.0384048104053</v>
+      </c>
+      <c r="B39" s="1">
+        <v>95185118.625503093</v>
+      </c>
+      <c r="C39" s="2">
+        <f t="shared" si="0"/>
+        <v>-7.8192920541088298E-2</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A40" s="1">
+        <v>13.0384048104053</v>
+      </c>
+      <c r="B40" s="1">
+        <v>93100334.827988595</v>
+      </c>
+      <c r="C40" s="2">
+        <f t="shared" si="0"/>
+        <v>-2.1902413188314492E-2</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A41" s="1">
+        <v>13.0384048104053</v>
+      </c>
+      <c r="B41" s="1">
+        <v>98921197.781541899</v>
+      </c>
+      <c r="C41" s="2">
+        <f t="shared" si="0"/>
+        <v>6.2522470668960342E-2</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A42" s="1">
+        <v>16.7928556237467</v>
+      </c>
+      <c r="B42" s="1">
+        <v>61720181.108913101</v>
+      </c>
+      <c r="C42" s="2">
+        <f t="shared" si="0"/>
+        <v>-0.37606718789216159</v>
+      </c>
+      <c r="D42" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A43" s="1">
+        <v>15.2970585407784</v>
+      </c>
+      <c r="B43" s="1">
+        <v>52576559.470010601</v>
+      </c>
+      <c r="C43" s="2">
+        <f t="shared" si="0"/>
+        <v>-0.14814638380220269</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A44" s="1">
+        <v>13.076696830622</v>
+      </c>
+      <c r="B44" s="1">
+        <v>38685770.0761609</v>
+      </c>
+      <c r="C44" s="2">
+        <f t="shared" si="0"/>
+        <v>-0.2642011864959124</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A45" s="1">
+        <v>13.076696830622</v>
+      </c>
+      <c r="B45" s="1">
+        <v>44115700.054772697</v>
+      </c>
+      <c r="C45" s="2">
+        <f t="shared" si="0"/>
+        <v>0.14035987826846572</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A46" s="1">
+        <v>19.104973174542799</v>
+      </c>
+      <c r="B46" s="1">
+        <v>28201029.4247839</v>
+      </c>
+      <c r="C46" s="2">
+        <f t="shared" si="0"/>
+        <v>-0.36074845486367962</v>
+      </c>
+      <c r="D46" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="47" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A47" s="1">
+        <v>15.2970585407784</v>
+      </c>
+      <c r="B47" s="1">
+        <v>59146609.222422197</v>
+      </c>
+      <c r="C47" s="2">
+        <f t="shared" si="0"/>
+        <v>1.097320928662356</v>
+      </c>
+    </row>
+    <row r="48" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A48" s="1">
+        <v>15.2970585407784</v>
+      </c>
+      <c r="B48" s="1">
+        <v>95361726.737619504</v>
+      </c>
+      <c r="C48" s="2">
+        <f t="shared" si="0"/>
+        <v>0.61229406032405875</v>
+      </c>
+    </row>
+    <row r="49" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A49" s="1">
+        <v>15.2970585407784</v>
+      </c>
+      <c r="B49" s="1">
+        <v>65260390.734304801</v>
+      </c>
+      <c r="C49" s="2">
+        <f t="shared" si="0"/>
+        <v>-0.31565426752533776</v>
+      </c>
+    </row>
+    <row r="50" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A50" s="1">
+        <v>15.2970585407784</v>
+      </c>
+      <c r="B50" s="1">
+        <v>40832490.112844199</v>
+      </c>
+      <c r="C50" s="2">
+        <f t="shared" si="0"/>
+        <v>-0.37431434820723225</v>
+      </c>
+    </row>
+    <row r="51" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A51" s="1">
+        <v>15.2970585407784</v>
+      </c>
+      <c r="B51" s="1">
+        <v>48384640.8640147</v>
+      </c>
+      <c r="C51" s="2">
+        <f t="shared" si="0"/>
+        <v>0.18495445000536251</v>
+      </c>
+    </row>
+    <row r="52" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A52" s="1">
+        <v>15.2970585407784</v>
+      </c>
+      <c r="B52" s="1">
+        <v>41086223.4482444</v>
+      </c>
+      <c r="C52" s="2">
+        <f t="shared" si="0"/>
+        <v>-0.15084161596409368</v>
+      </c>
+    </row>
+    <row r="53" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A53" s="1">
+        <v>15.2970585407784</v>
+      </c>
+      <c r="B53" s="1">
+        <v>33752405.253435202</v>
+      </c>
+      <c r="C53" s="2">
+        <f t="shared" si="0"/>
+        <v>-0.17849823077673424</v>
+      </c>
+    </row>
+    <row r="54" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A54" s="1">
+        <v>15.2970585407784</v>
+      </c>
+      <c r="B54" s="1">
+        <v>36424633.449873596</v>
+      </c>
+      <c r="C54" s="2">
+        <f t="shared" si="0"/>
+        <v>7.9171489450116289E-2</v>
+      </c>
+    </row>
+    <row r="55" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A55" s="1">
+        <v>15.2970585407784</v>
+      </c>
+      <c r="B55" s="1">
+        <v>42957896.887764998</v>
+      </c>
+      <c r="C55" s="2">
+        <f t="shared" si="0"/>
+        <v>0.1793638760121572</v>
+      </c>
+    </row>
+    <row r="56" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A56" s="1">
+        <v>15.2970585407784</v>
+      </c>
+      <c r="B56" s="1">
+        <v>77827984.499236196</v>
+      </c>
+      <c r="C56" s="2">
+        <f t="shared" si="0"/>
+        <v>0.81172706621498225</v>
+      </c>
+    </row>
+    <row r="57" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A57" s="1">
+        <v>15.2970585407784</v>
+      </c>
+      <c r="B57" s="1">
+        <v>57981992.971203998</v>
+      </c>
+      <c r="C57" s="2">
+        <f t="shared" si="0"/>
+        <v>-0.25499814309372187</v>
+      </c>
+    </row>
+    <row r="58" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A58" s="1">
+        <v>15.2970585407784</v>
+      </c>
+      <c r="B58" s="1">
+        <v>73639792.256328002</v>
+      </c>
+      <c r="C58" s="2">
+        <f t="shared" si="0"/>
+        <v>0.27004589671314411</v>
+      </c>
+    </row>
+    <row r="59" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A59" s="1">
+        <v>15.2970585407784</v>
+      </c>
+      <c r="B59" s="1">
+        <v>68837326.034295902</v>
+      </c>
+      <c r="C59" s="2">
+        <f t="shared" si="0"/>
+        <v>-6.5215640550906298E-2</v>
+      </c>
+    </row>
+    <row r="60" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A60" s="1">
+        <v>15.2970585407784</v>
+      </c>
+      <c r="B60" s="1">
+        <v>84232326.485389099</v>
+      </c>
+      <c r="C60" s="2">
+        <f t="shared" si="0"/>
+        <v>0.22364320838701887</v>
+      </c>
+    </row>
+    <row r="61" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A61" s="1">
+        <v>15.2970585407784</v>
+      </c>
+      <c r="B61" s="1">
+        <v>82741629.529615596</v>
+      </c>
+      <c r="C61" s="2">
+        <f t="shared" si="0"/>
+        <v>-1.7697444888122357E-2</v>
+      </c>
+    </row>
+    <row r="62" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A62" s="1">
+        <v>15.2970585407784</v>
+      </c>
+      <c r="B62" s="1">
+        <v>78953070.296337202</v>
+      </c>
+      <c r="C62" s="2">
+        <f t="shared" si="0"/>
+        <v>-4.5787824760235837E-2</v>
+      </c>
+    </row>
+    <row r="63" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A63" s="1">
+        <v>15.2970585407784</v>
+      </c>
+      <c r="B63" s="1">
+        <v>72031365.619615495</v>
+      </c>
+      <c r="C63" s="2">
+        <f t="shared" si="0"/>
+        <v>-8.7668594150198856E-2</v>
+      </c>
+    </row>
+    <row r="64" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A64" s="1">
+        <v>15.2970585407784</v>
+      </c>
+      <c r="B64" s="1">
+        <v>53033679.468397498</v>
+      </c>
+      <c r="C64" s="2">
+        <f t="shared" si="0"/>
+        <v>-0.26374185728396865</v>
+      </c>
+    </row>
+    <row r="65" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A65" s="1">
+        <v>15.2970585407784</v>
+      </c>
+      <c r="B65" s="1">
+        <v>43423538.441263199</v>
+      </c>
+      <c r="C65" s="2">
+        <f t="shared" si="0"/>
+        <v>-0.181208264700188</v>
+      </c>
+    </row>
+    <row r="66" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A66" s="1">
+        <v>15.2970585407784</v>
+      </c>
+      <c r="B66" s="1">
+        <v>47772331.350540496</v>
+      </c>
+      <c r="C66" s="2">
+        <f t="shared" si="0"/>
+        <v>0.1001482851324907</v>
+      </c>
+    </row>
+    <row r="67" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A67" s="1">
+        <v>19.3907194296653</v>
+      </c>
+      <c r="B67" s="1">
+        <v>35553504.029974498</v>
+      </c>
+      <c r="C67" s="2">
+        <f t="shared" si="0"/>
+        <v>-0.25577205413961351</v>
+      </c>
+    </row>
+    <row r="68" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A68" s="1"/>
+      <c r="B68" s="1"/>
+    </row>
+    <row r="69" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A69" s="1"/>
+      <c r="B69" s="1"/>
+    </row>
+    <row r="70" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A70" s="1"/>
+      <c r="B70" s="1"/>
+    </row>
+    <row r="71" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A71" s="1"/>
+      <c r="B71" s="1"/>
+    </row>
+    <row r="72" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A72" s="1"/>
+      <c r="B72" s="1"/>
+    </row>
+    <row r="73" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A73" s="1"/>
+      <c r="B73" s="1"/>
+    </row>
+    <row r="74" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A74" s="1"/>
+      <c r="B74" s="1"/>
+    </row>
+    <row r="75" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A75" s="1"/>
+      <c r="B75" s="1"/>
+    </row>
+    <row r="76" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A76" s="1"/>
+      <c r="B76" s="1"/>
+    </row>
+    <row r="77" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A77" s="1"/>
+      <c r="B77" s="1"/>
+    </row>
+    <row r="78" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A78" s="1"/>
+      <c r="B78" s="1"/>
+    </row>
+    <row r="79" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A79" s="1"/>
+      <c r="B79" s="1"/>
+    </row>
+    <row r="80" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A80" s="1"/>
+      <c r="B80" s="1"/>
+    </row>
+    <row r="81" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A81" s="1"/>
+      <c r="B81" s="1"/>
+    </row>
+    <row r="82" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A82" s="1"/>
+      <c r="B82" s="1"/>
+    </row>
+    <row r="83" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A83" s="1"/>
+      <c r="B83" s="1"/>
+    </row>
+    <row r="84" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A84" s="1"/>
+      <c r="B84" s="1"/>
+    </row>
+    <row r="85" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A85" s="1"/>
+      <c r="B85" s="1"/>
+    </row>
+    <row r="86" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A86" s="1"/>
+      <c r="B86" s="1"/>
+    </row>
+    <row r="87" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A87" s="1"/>
+      <c r="B87" s="1"/>
+    </row>
+    <row r="88" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A88" s="1"/>
+      <c r="B88" s="1"/>
+    </row>
+    <row r="89" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A89" s="1"/>
+      <c r="B89" s="1"/>
+    </row>
+    <row r="90" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A90" s="1"/>
+      <c r="B90" s="1"/>
+    </row>
+    <row r="91" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A91" s="1"/>
+      <c r="B91" s="1"/>
+    </row>
+    <row r="92" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A92" s="1"/>
+      <c r="B92" s="1"/>
+    </row>
+    <row r="93" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A93" s="1"/>
+      <c r="B93" s="1"/>
+    </row>
+    <row r="94" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A94" s="1"/>
+      <c r="B94" s="1"/>
+    </row>
+    <row r="95" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A95" s="1"/>
+      <c r="B95" s="1"/>
+    </row>
+    <row r="96" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A96" s="1"/>
+      <c r="B96" s="1"/>
+    </row>
+    <row r="97" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A97" s="1"/>
+      <c r="B97" s="1"/>
+    </row>
+    <row r="98" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A98" s="1"/>
+      <c r="B98" s="1"/>
+    </row>
+    <row r="99" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A99" s="1"/>
+      <c r="B99" s="1"/>
+    </row>
+    <row r="100" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A100" s="1"/>
+      <c r="B100" s="1"/>
+    </row>
+    <row r="101" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A101" s="1"/>
+      <c r="B101" s="1"/>
+    </row>
+    <row r="102" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A102" s="1"/>
+      <c r="B102" s="1"/>
+    </row>
+    <row r="103" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A103" s="1"/>
+      <c r="B103" s="1"/>
+    </row>
+    <row r="104" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A104" s="1"/>
+      <c r="B104" s="1"/>
+    </row>
+    <row r="105" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A105" s="1"/>
+      <c r="B105" s="1"/>
+    </row>
+    <row r="106" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A106" s="1"/>
+      <c r="B106" s="1"/>
+    </row>
+    <row r="107" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A107" s="1"/>
+      <c r="B107" s="1"/>
+    </row>
+    <row r="108" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A108" s="1"/>
+      <c r="B108" s="1"/>
+    </row>
+    <row r="109" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A109" s="1"/>
+      <c r="B109" s="1"/>
+    </row>
+    <row r="110" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A110" s="1"/>
+      <c r="B110" s="1"/>
+    </row>
+    <row r="111" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A111" s="1"/>
+      <c r="B111" s="1"/>
+    </row>
+    <row r="112" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A112" s="1"/>
+      <c r="B112" s="1"/>
+    </row>
+    <row r="113" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A113" s="1"/>
+      <c r="B113" s="1"/>
+    </row>
+    <row r="114" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A114" s="1"/>
+      <c r="B114" s="1"/>
+    </row>
+    <row r="115" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A115" s="1"/>
+      <c r="B115" s="1"/>
+    </row>
+    <row r="116" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A116" s="1"/>
+      <c r="B116" s="1"/>
+    </row>
+    <row r="117" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A117" s="1"/>
+      <c r="B117" s="1"/>
+    </row>
+    <row r="118" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A118" s="1"/>
+      <c r="B118" s="1"/>
+    </row>
+    <row r="119" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A119" s="1"/>
+      <c r="B119" s="1"/>
+    </row>
+    <row r="120" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A120" s="1"/>
+      <c r="B120" s="1"/>
+    </row>
+    <row r="121" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A121" s="1"/>
+      <c r="B121" s="1"/>
+    </row>
+    <row r="122" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A122" s="1"/>
+      <c r="B122" s="1"/>
+    </row>
+    <row r="123" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A123" s="1"/>
+      <c r="B123" s="1"/>
+    </row>
+    <row r="124" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A124" s="1"/>
+      <c r="B124" s="1"/>
+    </row>
+    <row r="125" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A125" s="1"/>
+      <c r="B125" s="1"/>
+    </row>
+    <row r="126" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A126" s="1"/>
+      <c r="B126" s="1"/>
+    </row>
+    <row r="127" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A127" s="1"/>
+      <c r="B127" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
It seems like the program is converging on a solution.  However, after 127 generations, it is still struggling.  It seems that it was on a path to a solution early on.  However, it lost its way after I added mutation to the genetic algorithm.  Next time I will try with no mutation to see how far it can get. In preparation for updating the code for multi-threading, I am cleaning up and documenting the code.
</commit_message>
<xml_diff>
--- a/Progress.xlsx
+++ b/Progress.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/c51537410c5afe56/Projects/Source/Repos/EdGarrity/SOS/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="84" documentId="114_{B2D123C0-10CD-4892-A2B1-0D4FB86B9D90}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{03E40BBD-7F1B-443B-BDB9-A8E176704BE9}"/>
+  <xr:revisionPtr revIDLastSave="133" documentId="114_{B2D123C0-10CD-4892-A2B1-0D4FB86B9D90}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{C3E42DCE-092D-4567-A4A4-C12FF766C2C9}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{D7613C25-2959-4D88-A8C3-21B00E74DE47}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="7">
   <si>
     <t>BestIndividual_Training_Error</t>
   </si>
@@ -1365,10 +1365,10 @@
           </c:marker>
           <c:val>
             <c:numRef>
-              <c:f>'Run 2'!$B$2:$B$67</c:f>
+              <c:f>'Run 2'!$B$2:$B$129</c:f>
               <c:numCache>
                 <c:formatCode>#,##0.00</c:formatCode>
-                <c:ptCount val="66"/>
+                <c:ptCount val="128"/>
                 <c:pt idx="0">
                   <c:v>136667774.57913801</c:v>
                 </c:pt>
@@ -1566,6 +1566,192 @@
                 </c:pt>
                 <c:pt idx="65">
                   <c:v>35553504.029974498</c:v>
+                </c:pt>
+                <c:pt idx="66">
+                  <c:v>58708844.4126487</c:v>
+                </c:pt>
+                <c:pt idx="67">
+                  <c:v>55572910.721497402</c:v>
+                </c:pt>
+                <c:pt idx="68">
+                  <c:v>33592860.6885878</c:v>
+                </c:pt>
+                <c:pt idx="69">
+                  <c:v>45751946.818608798</c:v>
+                </c:pt>
+                <c:pt idx="70">
+                  <c:v>66055665.006507002</c:v>
+                </c:pt>
+                <c:pt idx="71">
+                  <c:v>142813395.46954501</c:v>
+                </c:pt>
+                <c:pt idx="72">
+                  <c:v>60743559.156494603</c:v>
+                </c:pt>
+                <c:pt idx="73">
+                  <c:v>29305608.906848799</c:v>
+                </c:pt>
+                <c:pt idx="74">
+                  <c:v>55736088.541952699</c:v>
+                </c:pt>
+                <c:pt idx="75">
+                  <c:v>48955277.498168901</c:v>
+                </c:pt>
+                <c:pt idx="76">
+                  <c:v>35047908.063196599</c:v>
+                </c:pt>
+                <c:pt idx="77">
+                  <c:v>34065479.905309997</c:v>
+                </c:pt>
+                <c:pt idx="78">
+                  <c:v>33790487.626270898</c:v>
+                </c:pt>
+                <c:pt idx="79">
+                  <c:v>39421980.606656201</c:v>
+                </c:pt>
+                <c:pt idx="80">
+                  <c:v>30610712.303584602</c:v>
+                </c:pt>
+                <c:pt idx="81">
+                  <c:v>28092971.959025599</c:v>
+                </c:pt>
+                <c:pt idx="82">
+                  <c:v>31924789.280047499</c:v>
+                </c:pt>
+                <c:pt idx="83">
+                  <c:v>24298632.110529099</c:v>
+                </c:pt>
+                <c:pt idx="84">
+                  <c:v>36278258.887203902</c:v>
+                </c:pt>
+                <c:pt idx="85">
+                  <c:v>46654658.806578703</c:v>
+                </c:pt>
+                <c:pt idx="86">
+                  <c:v>81508741.980708301</c:v>
+                </c:pt>
+                <c:pt idx="87">
+                  <c:v>90672979.018749401</c:v>
+                </c:pt>
+                <c:pt idx="88">
+                  <c:v>92114573.239602506</c:v>
+                </c:pt>
+                <c:pt idx="89">
+                  <c:v>69395303.0678657</c:v>
+                </c:pt>
+                <c:pt idx="90">
+                  <c:v>162852996.13370901</c:v>
+                </c:pt>
+                <c:pt idx="91">
+                  <c:v>247234766.27470201</c:v>
+                </c:pt>
+                <c:pt idx="92">
+                  <c:v>140173824.24173</c:v>
+                </c:pt>
+                <c:pt idx="93">
+                  <c:v>72334212.419697404</c:v>
+                </c:pt>
+                <c:pt idx="94">
+                  <c:v>43293175.784926899</c:v>
+                </c:pt>
+                <c:pt idx="95">
+                  <c:v>43833094.518789202</c:v>
+                </c:pt>
+                <c:pt idx="96">
+                  <c:v>35859214.7371585</c:v>
+                </c:pt>
+                <c:pt idx="97">
+                  <c:v>41733751.6653018</c:v>
+                </c:pt>
+                <c:pt idx="98">
+                  <c:v>43948012.389472798</c:v>
+                </c:pt>
+                <c:pt idx="99">
+                  <c:v>40841079.553213596</c:v>
+                </c:pt>
+                <c:pt idx="100">
+                  <c:v>32925311.835851599</c:v>
+                </c:pt>
+                <c:pt idx="101">
+                  <c:v>38174028.2093959</c:v>
+                </c:pt>
+                <c:pt idx="102">
+                  <c:v>40497139.543315001</c:v>
+                </c:pt>
+                <c:pt idx="103">
+                  <c:v>30154677.378249701</c:v>
+                </c:pt>
+                <c:pt idx="104">
+                  <c:v>84826389.965819195</c:v>
+                </c:pt>
+                <c:pt idx="105">
+                  <c:v>43965797.817585602</c:v>
+                </c:pt>
+                <c:pt idx="106">
+                  <c:v>29223680.200228699</c:v>
+                </c:pt>
+                <c:pt idx="107">
+                  <c:v>31320152.0018567</c:v>
+                </c:pt>
+                <c:pt idx="108">
+                  <c:v>29585062.469802901</c:v>
+                </c:pt>
+                <c:pt idx="109">
+                  <c:v>22155397.701639999</c:v>
+                </c:pt>
+                <c:pt idx="110">
+                  <c:v>24261891.964023799</c:v>
+                </c:pt>
+                <c:pt idx="111">
+                  <c:v>23751963.409465998</c:v>
+                </c:pt>
+                <c:pt idx="112">
+                  <c:v>28436972.471882399</c:v>
+                </c:pt>
+                <c:pt idx="113">
+                  <c:v>32790463.7812564</c:v>
+                </c:pt>
+                <c:pt idx="114">
+                  <c:v>41059798.974095501</c:v>
+                </c:pt>
+                <c:pt idx="115">
+                  <c:v>29250438.004896302</c:v>
+                </c:pt>
+                <c:pt idx="116">
+                  <c:v>28254023.175344002</c:v>
+                </c:pt>
+                <c:pt idx="117">
+                  <c:v>31712594.137946401</c:v>
+                </c:pt>
+                <c:pt idx="118">
+                  <c:v>32378638.330914501</c:v>
+                </c:pt>
+                <c:pt idx="119">
+                  <c:v>25558557.986409299</c:v>
+                </c:pt>
+                <c:pt idx="120">
+                  <c:v>22322436.468534399</c:v>
+                </c:pt>
+                <c:pt idx="121">
+                  <c:v>20479803.527571101</c:v>
+                </c:pt>
+                <c:pt idx="122">
+                  <c:v>24956415.896892902</c:v>
+                </c:pt>
+                <c:pt idx="123">
+                  <c:v>30931088.520068299</c:v>
+                </c:pt>
+                <c:pt idx="124">
+                  <c:v>30974356.154456601</c:v>
+                </c:pt>
+                <c:pt idx="125">
+                  <c:v>33063929.435010999</c:v>
+                </c:pt>
+                <c:pt idx="126">
+                  <c:v>27570603.826418102</c:v>
+                </c:pt>
+                <c:pt idx="127">
+                  <c:v>28204727.997801401</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1621,10 +1807,10 @@
           </c:marker>
           <c:val>
             <c:numRef>
-              <c:f>'Run 2'!$A$2:$A$67</c:f>
+              <c:f>'Run 2'!$A$2:$A$129</c:f>
               <c:numCache>
                 <c:formatCode>#,##0.00</c:formatCode>
-                <c:ptCount val="66"/>
+                <c:ptCount val="128"/>
                 <c:pt idx="0">
                   <c:v>15.2970585407784</c:v>
                 </c:pt>
@@ -1822,6 +2008,192 @@
                 </c:pt>
                 <c:pt idx="65">
                   <c:v>19.3907194296653</c:v>
+                </c:pt>
+                <c:pt idx="66">
+                  <c:v>18.466185312619402</c:v>
+                </c:pt>
+                <c:pt idx="67">
+                  <c:v>15.8429795177549</c:v>
+                </c:pt>
+                <c:pt idx="68">
+                  <c:v>18.681541692269398</c:v>
+                </c:pt>
+                <c:pt idx="69">
+                  <c:v>18.681541692269398</c:v>
+                </c:pt>
+                <c:pt idx="70">
+                  <c:v>18.681541692269398</c:v>
+                </c:pt>
+                <c:pt idx="71">
+                  <c:v>16.9705627484771</c:v>
+                </c:pt>
+                <c:pt idx="72">
+                  <c:v>16.9705627484771</c:v>
+                </c:pt>
+                <c:pt idx="73">
+                  <c:v>16.9705627484771</c:v>
+                </c:pt>
+                <c:pt idx="74">
+                  <c:v>16.9705627484771</c:v>
+                </c:pt>
+                <c:pt idx="75">
+                  <c:v>16.9705627484771</c:v>
+                </c:pt>
+                <c:pt idx="76">
+                  <c:v>16.9705627484771</c:v>
+                </c:pt>
+                <c:pt idx="77">
+                  <c:v>13.490737563232001</c:v>
+                </c:pt>
+                <c:pt idx="78">
+                  <c:v>13.3416640641263</c:v>
+                </c:pt>
+                <c:pt idx="79">
+                  <c:v>13.3416640641263</c:v>
+                </c:pt>
+                <c:pt idx="80">
+                  <c:v>13.3416640641263</c:v>
+                </c:pt>
+                <c:pt idx="81">
+                  <c:v>13.3416640641263</c:v>
+                </c:pt>
+                <c:pt idx="82">
+                  <c:v>13.3416640641263</c:v>
+                </c:pt>
+                <c:pt idx="83">
+                  <c:v>13.3416640641263</c:v>
+                </c:pt>
+                <c:pt idx="84">
+                  <c:v>13.3416640641263</c:v>
+                </c:pt>
+                <c:pt idx="85">
+                  <c:v>13.3416640641263</c:v>
+                </c:pt>
+                <c:pt idx="86">
+                  <c:v>13.3416640641263</c:v>
+                </c:pt>
+                <c:pt idx="87">
+                  <c:v>13.3416640641263</c:v>
+                </c:pt>
+                <c:pt idx="88">
+                  <c:v>13.3416640641263</c:v>
+                </c:pt>
+                <c:pt idx="89">
+                  <c:v>20.566963801203102</c:v>
+                </c:pt>
+                <c:pt idx="90">
+                  <c:v>13.7840487520902</c:v>
+                </c:pt>
+                <c:pt idx="91">
+                  <c:v>13.7840487520902</c:v>
+                </c:pt>
+                <c:pt idx="92">
+                  <c:v>13.490737563232001</c:v>
+                </c:pt>
+                <c:pt idx="93">
+                  <c:v>13.266499161421599</c:v>
+                </c:pt>
+                <c:pt idx="94">
+                  <c:v>13.266499161421599</c:v>
+                </c:pt>
+                <c:pt idx="95">
+                  <c:v>13.266499161421599</c:v>
+                </c:pt>
+                <c:pt idx="96">
+                  <c:v>13.114877048604001</c:v>
+                </c:pt>
+                <c:pt idx="97">
+                  <c:v>13.114877048604001</c:v>
+                </c:pt>
+                <c:pt idx="98">
+                  <c:v>13.114877048604001</c:v>
+                </c:pt>
+                <c:pt idx="99">
+                  <c:v>13.114877048604001</c:v>
+                </c:pt>
+                <c:pt idx="100">
+                  <c:v>13.114877048604001</c:v>
+                </c:pt>
+                <c:pt idx="101">
+                  <c:v>13.114877048604001</c:v>
+                </c:pt>
+                <c:pt idx="102">
+                  <c:v>13.114877048604001</c:v>
+                </c:pt>
+                <c:pt idx="103">
+                  <c:v>17.2626765016321</c:v>
+                </c:pt>
+                <c:pt idx="104">
+                  <c:v>15.2970585407784</c:v>
+                </c:pt>
+                <c:pt idx="105">
+                  <c:v>14.6287388383278</c:v>
+                </c:pt>
+                <c:pt idx="106">
+                  <c:v>14.6287388383278</c:v>
+                </c:pt>
+                <c:pt idx="107">
+                  <c:v>14.6287388383278</c:v>
+                </c:pt>
+                <c:pt idx="108">
+                  <c:v>13.3416640641263</c:v>
+                </c:pt>
+                <c:pt idx="109">
+                  <c:v>13.3416640641263</c:v>
+                </c:pt>
+                <c:pt idx="110">
+                  <c:v>13.3416640641263</c:v>
+                </c:pt>
+                <c:pt idx="111">
+                  <c:v>13.3416640641263</c:v>
+                </c:pt>
+                <c:pt idx="112">
+                  <c:v>13.3416640641263</c:v>
+                </c:pt>
+                <c:pt idx="113">
+                  <c:v>13.3416640641263</c:v>
+                </c:pt>
+                <c:pt idx="114">
+                  <c:v>13.3416640641263</c:v>
+                </c:pt>
+                <c:pt idx="115">
+                  <c:v>13.3416640641263</c:v>
+                </c:pt>
+                <c:pt idx="116">
+                  <c:v>13.3416640641263</c:v>
+                </c:pt>
+                <c:pt idx="117">
+                  <c:v>13.3416640641263</c:v>
+                </c:pt>
+                <c:pt idx="118">
+                  <c:v>13.3416640641263</c:v>
+                </c:pt>
+                <c:pt idx="119">
+                  <c:v>13.3416640641263</c:v>
+                </c:pt>
+                <c:pt idx="120">
+                  <c:v>12.328828005938</c:v>
+                </c:pt>
+                <c:pt idx="121">
+                  <c:v>12.328828005938</c:v>
+                </c:pt>
+                <c:pt idx="122">
+                  <c:v>12.328828005938</c:v>
+                </c:pt>
+                <c:pt idx="123">
+                  <c:v>12.328828005938</c:v>
+                </c:pt>
+                <c:pt idx="124">
+                  <c:v>12.328828005938</c:v>
+                </c:pt>
+                <c:pt idx="125">
+                  <c:v>12.328828005938</c:v>
+                </c:pt>
+                <c:pt idx="126">
+                  <c:v>12.328828005938</c:v>
+                </c:pt>
+                <c:pt idx="127">
+                  <c:v>12.328828005938</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3235,8 +3607,8 @@
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>26</xdr:col>
-      <xdr:colOff>518160</xdr:colOff>
+      <xdr:col>30</xdr:col>
+      <xdr:colOff>409575</xdr:colOff>
       <xdr:row>37</xdr:row>
       <xdr:rowOff>19050</xdr:rowOff>
     </xdr:to>
@@ -4600,10 +4972,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EFDF9A5F-6B77-43F5-8016-32B291B6E88B}">
-  <dimension ref="A1:D127"/>
+  <dimension ref="A1:D129"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+    <sheetView tabSelected="1" topLeftCell="E1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="J4" sqref="J4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4655,7 +5027,7 @@
         <v>210352008.09481099</v>
       </c>
       <c r="C4" s="2">
-        <f t="shared" ref="C4:C67" si="0">(B4-B3)/B3</f>
+        <f t="shared" ref="C4:C71" si="0">(B4-B3)/B3</f>
         <v>-0.23246706087514171</v>
       </c>
     </row>
@@ -5388,7 +5760,7 @@
         <v>-0.26374185728396865</v>
       </c>
     </row>
-    <row r="65" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A65" s="1">
         <v>15.2970585407784</v>
       </c>
@@ -5400,7 +5772,7 @@
         <v>-0.181208264700188</v>
       </c>
     </row>
-    <row r="66" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A66" s="1">
         <v>15.2970585407784</v>
       </c>
@@ -5412,7 +5784,7 @@
         <v>0.1001482851324907</v>
       </c>
     </row>
-    <row r="67" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A67" s="1">
         <v>19.3907194296653</v>
       </c>
@@ -5423,246 +5795,768 @@
         <f t="shared" si="0"/>
         <v>-0.25577205413961351</v>
       </c>
-    </row>
-    <row r="68" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A68" s="1"/>
-      <c r="B68" s="1"/>
-    </row>
-    <row r="69" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A69" s="1"/>
-      <c r="B69" s="1"/>
-    </row>
-    <row r="70" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A70" s="1"/>
-      <c r="B70" s="1"/>
-    </row>
-    <row r="71" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A71" s="1"/>
-      <c r="B71" s="1"/>
-    </row>
-    <row r="72" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A72" s="1"/>
-      <c r="B72" s="1"/>
-    </row>
-    <row r="73" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A73" s="1"/>
-      <c r="B73" s="1"/>
-    </row>
-    <row r="74" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A74" s="1"/>
-      <c r="B74" s="1"/>
-    </row>
-    <row r="75" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A75" s="1"/>
-      <c r="B75" s="1"/>
-    </row>
-    <row r="76" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A76" s="1"/>
-      <c r="B76" s="1"/>
-    </row>
-    <row r="77" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A77" s="1"/>
-      <c r="B77" s="1"/>
-    </row>
-    <row r="78" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A78" s="1"/>
-      <c r="B78" s="1"/>
-    </row>
-    <row r="79" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A79" s="1"/>
-      <c r="B79" s="1"/>
-    </row>
-    <row r="80" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A80" s="1"/>
-      <c r="B80" s="1"/>
-    </row>
-    <row r="81" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A81" s="1"/>
-      <c r="B81" s="1"/>
-    </row>
-    <row r="82" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A82" s="1"/>
-      <c r="B82" s="1"/>
-    </row>
-    <row r="83" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A83" s="1"/>
-      <c r="B83" s="1"/>
-    </row>
-    <row r="84" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A84" s="1"/>
-      <c r="B84" s="1"/>
-    </row>
-    <row r="85" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A85" s="1"/>
-      <c r="B85" s="1"/>
-    </row>
-    <row r="86" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A86" s="1"/>
-      <c r="B86" s="1"/>
-    </row>
-    <row r="87" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A87" s="1"/>
-      <c r="B87" s="1"/>
-    </row>
-    <row r="88" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A88" s="1"/>
-      <c r="B88" s="1"/>
-    </row>
-    <row r="89" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A89" s="1"/>
-      <c r="B89" s="1"/>
-    </row>
-    <row r="90" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A90" s="1"/>
-      <c r="B90" s="1"/>
-    </row>
-    <row r="91" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A91" s="1"/>
-      <c r="B91" s="1"/>
-    </row>
-    <row r="92" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A92" s="1"/>
-      <c r="B92" s="1"/>
-    </row>
-    <row r="93" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A93" s="1"/>
-      <c r="B93" s="1"/>
-    </row>
-    <row r="94" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A94" s="1"/>
-      <c r="B94" s="1"/>
-    </row>
-    <row r="95" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A95" s="1"/>
-      <c r="B95" s="1"/>
-    </row>
-    <row r="96" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A96" s="1"/>
-      <c r="B96" s="1"/>
-    </row>
-    <row r="97" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A97" s="1"/>
-      <c r="B97" s="1"/>
-    </row>
-    <row r="98" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A98" s="1"/>
-      <c r="B98" s="1"/>
-    </row>
-    <row r="99" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A99" s="1"/>
-      <c r="B99" s="1"/>
-    </row>
-    <row r="100" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A100" s="1"/>
-      <c r="B100" s="1"/>
-    </row>
-    <row r="101" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A101" s="1"/>
-      <c r="B101" s="1"/>
-    </row>
-    <row r="102" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A102" s="1"/>
-      <c r="B102" s="1"/>
-    </row>
-    <row r="103" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A103" s="1"/>
-      <c r="B103" s="1"/>
-    </row>
-    <row r="104" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A104" s="1"/>
-      <c r="B104" s="1"/>
-    </row>
-    <row r="105" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A105" s="1"/>
-      <c r="B105" s="1"/>
-    </row>
-    <row r="106" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A106" s="1"/>
-      <c r="B106" s="1"/>
-    </row>
-    <row r="107" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A107" s="1"/>
-      <c r="B107" s="1"/>
-    </row>
-    <row r="108" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A108" s="1"/>
-      <c r="B108" s="1"/>
-    </row>
-    <row r="109" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A109" s="1"/>
-      <c r="B109" s="1"/>
-    </row>
-    <row r="110" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A110" s="1"/>
-      <c r="B110" s="1"/>
-    </row>
-    <row r="111" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A111" s="1"/>
-      <c r="B111" s="1"/>
-    </row>
-    <row r="112" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A112" s="1"/>
-      <c r="B112" s="1"/>
-    </row>
-    <row r="113" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A113" s="1"/>
-      <c r="B113" s="1"/>
-    </row>
-    <row r="114" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A114" s="1"/>
-      <c r="B114" s="1"/>
-    </row>
-    <row r="115" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A115" s="1"/>
-      <c r="B115" s="1"/>
-    </row>
-    <row r="116" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A116" s="1"/>
-      <c r="B116" s="1"/>
-    </row>
-    <row r="117" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A117" s="1"/>
-      <c r="B117" s="1"/>
-    </row>
-    <row r="118" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A118" s="1"/>
-      <c r="B118" s="1"/>
-    </row>
-    <row r="119" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A119" s="1"/>
-      <c r="B119" s="1"/>
-    </row>
-    <row r="120" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A120" s="1"/>
-      <c r="B120" s="1"/>
-    </row>
-    <row r="121" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A121" s="1"/>
-      <c r="B121" s="1"/>
-    </row>
-    <row r="122" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A122" s="1"/>
-      <c r="B122" s="1"/>
-    </row>
-    <row r="123" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A123" s="1"/>
-      <c r="B123" s="1"/>
-    </row>
-    <row r="124" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A124" s="1"/>
-      <c r="B124" s="1"/>
-    </row>
-    <row r="125" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A125" s="1"/>
-      <c r="B125" s="1"/>
-    </row>
-    <row r="126" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A126" s="1"/>
-      <c r="B126" s="1"/>
-    </row>
-    <row r="127" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A127" s="1"/>
-      <c r="B127" s="1"/>
+      <c r="D67" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="68" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A68" s="1">
+        <v>18.466185312619402</v>
+      </c>
+      <c r="B68" s="1">
+        <v>58708844.4126487</v>
+      </c>
+      <c r="C68" s="2">
+        <f t="shared" si="0"/>
+        <v>0.65128152665774841</v>
+      </c>
+    </row>
+    <row r="69" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A69" s="1">
+        <v>15.8429795177549</v>
+      </c>
+      <c r="B69" s="1">
+        <v>55572910.721497402</v>
+      </c>
+      <c r="C69" s="2">
+        <f t="shared" si="0"/>
+        <v>-5.3415013061910446E-2</v>
+      </c>
+    </row>
+    <row r="70" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A70" s="1">
+        <v>18.681541692269398</v>
+      </c>
+      <c r="B70" s="1">
+        <v>33592860.6885878</v>
+      </c>
+      <c r="C70" s="2">
+        <f t="shared" si="0"/>
+        <v>-0.3955173437479676</v>
+      </c>
+      <c r="D70" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="71" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A71" s="1">
+        <v>18.681541692269398</v>
+      </c>
+      <c r="B71" s="1">
+        <v>45751946.818608798</v>
+      </c>
+      <c r="C71" s="2">
+        <f t="shared" si="0"/>
+        <v>0.36195447130085279</v>
+      </c>
+      <c r="D71" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="72" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A72" s="1">
+        <v>18.681541692269398</v>
+      </c>
+      <c r="B72" s="1">
+        <v>66055665.006507002</v>
+      </c>
+      <c r="C72" s="2">
+        <f t="shared" ref="C72:C129" si="1">(B72-B71)/B71</f>
+        <v>0.44377823458301502</v>
+      </c>
+      <c r="D72" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="73" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A73" s="1">
+        <v>16.9705627484771</v>
+      </c>
+      <c r="B73" s="1">
+        <v>142813395.46954501</v>
+      </c>
+      <c r="C73" s="2">
+        <f t="shared" si="1"/>
+        <v>1.1620158612509126</v>
+      </c>
+    </row>
+    <row r="74" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A74" s="1">
+        <v>16.9705627484771</v>
+      </c>
+      <c r="B74" s="1">
+        <v>60743559.156494603</v>
+      </c>
+      <c r="C74" s="2">
+        <f t="shared" si="1"/>
+        <v>-0.57466483478821717</v>
+      </c>
+    </row>
+    <row r="75" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A75" s="1">
+        <v>16.9705627484771</v>
+      </c>
+      <c r="B75" s="1">
+        <v>29305608.906848799</v>
+      </c>
+      <c r="C75" s="2">
+        <f t="shared" si="1"/>
+        <v>-0.51755199540829855</v>
+      </c>
+    </row>
+    <row r="76" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A76" s="1">
+        <v>16.9705627484771</v>
+      </c>
+      <c r="B76" s="1">
+        <v>55736088.541952699</v>
+      </c>
+      <c r="C76" s="2">
+        <f t="shared" si="1"/>
+        <v>0.90189150203690283</v>
+      </c>
+    </row>
+    <row r="77" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A77" s="1">
+        <v>16.9705627484771</v>
+      </c>
+      <c r="B77" s="1">
+        <v>48955277.498168901</v>
+      </c>
+      <c r="C77" s="2">
+        <f t="shared" si="1"/>
+        <v>-0.12165925563075465</v>
+      </c>
+    </row>
+    <row r="78" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A78" s="1">
+        <v>16.9705627484771</v>
+      </c>
+      <c r="B78" s="1">
+        <v>35047908.063196599</v>
+      </c>
+      <c r="C78" s="2">
+        <f t="shared" si="1"/>
+        <v>-0.28408314988087824</v>
+      </c>
+    </row>
+    <row r="79" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A79" s="1">
+        <v>13.490737563232001</v>
+      </c>
+      <c r="B79" s="1">
+        <v>34065479.905309997</v>
+      </c>
+      <c r="C79" s="2">
+        <f t="shared" si="1"/>
+        <v>-2.8031007046558604E-2</v>
+      </c>
+    </row>
+    <row r="80" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A80" s="1">
+        <v>13.3416640641263</v>
+      </c>
+      <c r="B80" s="1">
+        <v>33790487.626270898</v>
+      </c>
+      <c r="C80" s="2">
+        <f t="shared" si="1"/>
+        <v>-8.072461618138984E-3</v>
+      </c>
+    </row>
+    <row r="81" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A81" s="1">
+        <v>13.3416640641263</v>
+      </c>
+      <c r="B81" s="1">
+        <v>39421980.606656201</v>
+      </c>
+      <c r="C81" s="2">
+        <f t="shared" si="1"/>
+        <v>0.16665912142703199</v>
+      </c>
+    </row>
+    <row r="82" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A82" s="1">
+        <v>13.3416640641263</v>
+      </c>
+      <c r="B82" s="1">
+        <v>30610712.303584602</v>
+      </c>
+      <c r="C82" s="2">
+        <f t="shared" si="1"/>
+        <v>-0.22351155795515412</v>
+      </c>
+    </row>
+    <row r="83" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A83" s="1">
+        <v>13.3416640641263</v>
+      </c>
+      <c r="B83" s="1">
+        <v>28092971.959025599</v>
+      </c>
+      <c r="C83" s="2">
+        <f t="shared" si="1"/>
+        <v>-8.225030242972059E-2</v>
+      </c>
+    </row>
+    <row r="84" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A84" s="1">
+        <v>13.3416640641263</v>
+      </c>
+      <c r="B84" s="1">
+        <v>31924789.280047499</v>
+      </c>
+      <c r="C84" s="2">
+        <f t="shared" si="1"/>
+        <v>0.13639771992122138</v>
+      </c>
+    </row>
+    <row r="85" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A85" s="1">
+        <v>13.3416640641263</v>
+      </c>
+      <c r="B85" s="1">
+        <v>24298632.110529099</v>
+      </c>
+      <c r="C85" s="2">
+        <f t="shared" si="1"/>
+        <v>-0.23887885688519267</v>
+      </c>
+    </row>
+    <row r="86" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A86" s="1">
+        <v>13.3416640641263</v>
+      </c>
+      <c r="B86" s="1">
+        <v>36278258.887203902</v>
+      </c>
+      <c r="C86" s="2">
+        <f t="shared" si="1"/>
+        <v>0.49301650900273453</v>
+      </c>
+    </row>
+    <row r="87" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A87" s="1">
+        <v>13.3416640641263</v>
+      </c>
+      <c r="B87" s="1">
+        <v>46654658.806578703</v>
+      </c>
+      <c r="C87" s="2">
+        <f t="shared" si="1"/>
+        <v>0.28602254456689963</v>
+      </c>
+    </row>
+    <row r="88" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A88" s="1">
+        <v>13.3416640641263</v>
+      </c>
+      <c r="B88" s="1">
+        <v>81508741.980708301</v>
+      </c>
+      <c r="C88" s="2">
+        <f t="shared" si="1"/>
+        <v>0.74706543924429847</v>
+      </c>
+    </row>
+    <row r="89" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A89" s="1">
+        <v>13.3416640641263</v>
+      </c>
+      <c r="B89" s="1">
+        <v>90672979.018749401</v>
+      </c>
+      <c r="C89" s="2">
+        <f t="shared" si="1"/>
+        <v>0.1124325663155262</v>
+      </c>
+    </row>
+    <row r="90" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A90" s="1">
+        <v>13.3416640641263</v>
+      </c>
+      <c r="B90" s="1">
+        <v>92114573.239602506</v>
+      </c>
+      <c r="C90" s="2">
+        <f t="shared" si="1"/>
+        <v>1.5898829358578941E-2</v>
+      </c>
+    </row>
+    <row r="91" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A91" s="1">
+        <v>20.566963801203102</v>
+      </c>
+      <c r="B91" s="1">
+        <v>69395303.0678657</v>
+      </c>
+      <c r="C91" s="2">
+        <f t="shared" si="1"/>
+        <v>-0.24664143112991363</v>
+      </c>
+      <c r="D91" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="92" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A92" s="1">
+        <v>13.7840487520902</v>
+      </c>
+      <c r="B92" s="1">
+        <v>162852996.13370901</v>
+      </c>
+      <c r="C92" s="2">
+        <f t="shared" si="1"/>
+        <v>1.3467437842939545</v>
+      </c>
+    </row>
+    <row r="93" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A93" s="1">
+        <v>13.7840487520902</v>
+      </c>
+      <c r="B93" s="1">
+        <v>247234766.27470201</v>
+      </c>
+      <c r="C93" s="2">
+        <f t="shared" si="1"/>
+        <v>0.51814686953448552</v>
+      </c>
+    </row>
+    <row r="94" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A94" s="1">
+        <v>13.490737563232001</v>
+      </c>
+      <c r="B94" s="1">
+        <v>140173824.24173</v>
+      </c>
+      <c r="C94" s="2">
+        <f t="shared" si="1"/>
+        <v>-0.4330335237480995</v>
+      </c>
+    </row>
+    <row r="95" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A95" s="1">
+        <v>13.266499161421599</v>
+      </c>
+      <c r="B95" s="1">
+        <v>72334212.419697404</v>
+      </c>
+      <c r="C95" s="2">
+        <f t="shared" si="1"/>
+        <v>-0.48396776066438102</v>
+      </c>
+    </row>
+    <row r="96" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A96" s="1">
+        <v>13.266499161421599</v>
+      </c>
+      <c r="B96" s="1">
+        <v>43293175.784926899</v>
+      </c>
+      <c r="C96" s="2">
+        <f t="shared" si="1"/>
+        <v>-0.40148410639032978</v>
+      </c>
+    </row>
+    <row r="97" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A97" s="1">
+        <v>13.266499161421599</v>
+      </c>
+      <c r="B97" s="1">
+        <v>43833094.518789202</v>
+      </c>
+      <c r="C97" s="2">
+        <f t="shared" si="1"/>
+        <v>1.2471220326836896E-2</v>
+      </c>
+    </row>
+    <row r="98" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A98" s="1">
+        <v>13.114877048604001</v>
+      </c>
+      <c r="B98" s="1">
+        <v>35859214.7371585</v>
+      </c>
+      <c r="C98" s="2">
+        <f t="shared" si="1"/>
+        <v>-0.18191459829998249</v>
+      </c>
+    </row>
+    <row r="99" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A99" s="1">
+        <v>13.114877048604001</v>
+      </c>
+      <c r="B99" s="1">
+        <v>41733751.6653018</v>
+      </c>
+      <c r="C99" s="2">
+        <f t="shared" si="1"/>
+        <v>0.16382224126218556</v>
+      </c>
+    </row>
+    <row r="100" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A100" s="1">
+        <v>13.114877048604001</v>
+      </c>
+      <c r="B100" s="1">
+        <v>43948012.389472798</v>
+      </c>
+      <c r="C100" s="2">
+        <f t="shared" si="1"/>
+        <v>5.3056833757219445E-2</v>
+      </c>
+    </row>
+    <row r="101" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A101" s="1">
+        <v>13.114877048604001</v>
+      </c>
+      <c r="B101" s="1">
+        <v>40841079.553213596</v>
+      </c>
+      <c r="C101" s="2">
+        <f t="shared" si="1"/>
+        <v>-7.0695639400598434E-2</v>
+      </c>
+    </row>
+    <row r="102" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A102" s="1">
+        <v>13.114877048604001</v>
+      </c>
+      <c r="B102" s="1">
+        <v>32925311.835851599</v>
+      </c>
+      <c r="C102" s="2">
+        <f t="shared" si="1"/>
+        <v>-0.19381876786700028</v>
+      </c>
+    </row>
+    <row r="103" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A103" s="1">
+        <v>13.114877048604001</v>
+      </c>
+      <c r="B103" s="1">
+        <v>38174028.2093959</v>
+      </c>
+      <c r="C103" s="2">
+        <f t="shared" si="1"/>
+        <v>0.159412806770416</v>
+      </c>
+    </row>
+    <row r="104" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A104" s="1">
+        <v>13.114877048604001</v>
+      </c>
+      <c r="B104" s="1">
+        <v>40497139.543315001</v>
+      </c>
+      <c r="C104" s="2">
+        <f t="shared" si="1"/>
+        <v>6.0855808068672863E-2</v>
+      </c>
+    </row>
+    <row r="105" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A105" s="1">
+        <v>17.2626765016321</v>
+      </c>
+      <c r="B105" s="1">
+        <v>30154677.378249701</v>
+      </c>
+      <c r="C105" s="2">
+        <f t="shared" si="1"/>
+        <v>-0.25538747382400162</v>
+      </c>
+      <c r="D105" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="106" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A106" s="1">
+        <v>15.2970585407784</v>
+      </c>
+      <c r="B106" s="1">
+        <v>84826389.965819195</v>
+      </c>
+      <c r="C106" s="2">
+        <f t="shared" si="1"/>
+        <v>1.8130425307419706</v>
+      </c>
+    </row>
+    <row r="107" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A107" s="1">
+        <v>14.6287388383278</v>
+      </c>
+      <c r="B107" s="1">
+        <v>43965797.817585602</v>
+      </c>
+      <c r="C107" s="2">
+        <f t="shared" si="1"/>
+        <v>-0.48169670033934453</v>
+      </c>
+    </row>
+    <row r="108" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A108" s="1">
+        <v>14.6287388383278</v>
+      </c>
+      <c r="B108" s="1">
+        <v>29223680.200228699</v>
+      </c>
+      <c r="C108" s="2">
+        <f t="shared" si="1"/>
+        <v>-0.33530877066127746</v>
+      </c>
+    </row>
+    <row r="109" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A109" s="1">
+        <v>14.6287388383278</v>
+      </c>
+      <c r="B109" s="1">
+        <v>31320152.0018567</v>
+      </c>
+      <c r="C109" s="2">
+        <f t="shared" si="1"/>
+        <v>7.1738801795798279E-2</v>
+      </c>
+    </row>
+    <row r="110" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A110" s="1">
+        <v>13.3416640641263</v>
+      </c>
+      <c r="B110" s="1">
+        <v>29585062.469802901</v>
+      </c>
+      <c r="C110" s="2">
+        <f t="shared" si="1"/>
+        <v>-5.5398502917576517E-2</v>
+      </c>
+    </row>
+    <row r="111" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A111" s="1">
+        <v>13.3416640641263</v>
+      </c>
+      <c r="B111" s="1">
+        <v>22155397.701639999</v>
+      </c>
+      <c r="C111" s="2">
+        <f t="shared" si="1"/>
+        <v>-0.25112891939120519</v>
+      </c>
+    </row>
+    <row r="112" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A112" s="1">
+        <v>13.3416640641263</v>
+      </c>
+      <c r="B112" s="1">
+        <v>24261891.964023799</v>
+      </c>
+      <c r="C112" s="2">
+        <f t="shared" si="1"/>
+        <v>9.5078151642832925E-2</v>
+      </c>
+    </row>
+    <row r="113" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A113" s="1">
+        <v>13.3416640641263</v>
+      </c>
+      <c r="B113" s="1">
+        <v>23751963.409465998</v>
+      </c>
+      <c r="C113" s="2">
+        <f t="shared" si="1"/>
+        <v>-2.1017674768065753E-2</v>
+      </c>
+    </row>
+    <row r="114" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A114" s="1">
+        <v>13.3416640641263</v>
+      </c>
+      <c r="B114" s="1">
+        <v>28436972.471882399</v>
+      </c>
+      <c r="C114" s="2">
+        <f t="shared" si="1"/>
+        <v>0.19724723306660447</v>
+      </c>
+    </row>
+    <row r="115" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A115" s="1">
+        <v>13.3416640641263</v>
+      </c>
+      <c r="B115" s="1">
+        <v>32790463.7812564</v>
+      </c>
+      <c r="C115" s="2">
+        <f t="shared" si="1"/>
+        <v>0.15309264422148311</v>
+      </c>
+    </row>
+    <row r="116" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A116" s="1">
+        <v>13.3416640641263</v>
+      </c>
+      <c r="B116" s="1">
+        <v>41059798.974095501</v>
+      </c>
+      <c r="C116" s="2">
+        <f t="shared" si="1"/>
+        <v>0.25218719832703301</v>
+      </c>
+    </row>
+    <row r="117" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A117" s="1">
+        <v>13.3416640641263</v>
+      </c>
+      <c r="B117" s="1">
+        <v>29250438.004896302</v>
+      </c>
+      <c r="C117" s="2">
+        <f t="shared" si="1"/>
+        <v>-0.28761370645408391</v>
+      </c>
+    </row>
+    <row r="118" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A118" s="1">
+        <v>13.3416640641263</v>
+      </c>
+      <c r="B118" s="1">
+        <v>28254023.175344002</v>
+      </c>
+      <c r="C118" s="2">
+        <f t="shared" si="1"/>
+        <v>-3.4064954151644088E-2</v>
+      </c>
+    </row>
+    <row r="119" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A119" s="1">
+        <v>13.3416640641263</v>
+      </c>
+      <c r="B119" s="1">
+        <v>31712594.137946401</v>
+      </c>
+      <c r="C119" s="2">
+        <f t="shared" si="1"/>
+        <v>0.12240985792142113</v>
+      </c>
+    </row>
+    <row r="120" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A120" s="1">
+        <v>13.3416640641263</v>
+      </c>
+      <c r="B120" s="1">
+        <v>32378638.330914501</v>
+      </c>
+      <c r="C120" s="2">
+        <f t="shared" si="1"/>
+        <v>2.100251370388935E-2</v>
+      </c>
+    </row>
+    <row r="121" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A121" s="1">
+        <v>13.3416640641263</v>
+      </c>
+      <c r="B121" s="1">
+        <v>25558557.986409299</v>
+      </c>
+      <c r="C121" s="2">
+        <f t="shared" si="1"/>
+        <v>-0.21063518097342346</v>
+      </c>
+    </row>
+    <row r="122" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A122" s="1">
+        <v>12.328828005938</v>
+      </c>
+      <c r="B122" s="1">
+        <v>22322436.468534399</v>
+      </c>
+      <c r="C122" s="2">
+        <f t="shared" si="1"/>
+        <v>-0.12661596634660297</v>
+      </c>
+    </row>
+    <row r="123" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A123" s="1">
+        <v>12.328828005938</v>
+      </c>
+      <c r="B123" s="1">
+        <v>20479803.527571101</v>
+      </c>
+      <c r="C123" s="2">
+        <f t="shared" si="1"/>
+        <v>-8.2546228480061518E-2</v>
+      </c>
+    </row>
+    <row r="124" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A124" s="1">
+        <v>12.328828005938</v>
+      </c>
+      <c r="B124" s="1">
+        <v>24956415.896892902</v>
+      </c>
+      <c r="C124" s="2">
+        <f t="shared" si="1"/>
+        <v>0.21858668533099573</v>
+      </c>
+    </row>
+    <row r="125" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A125" s="1">
+        <v>12.328828005938</v>
+      </c>
+      <c r="B125" s="1">
+        <v>30931088.520068299</v>
+      </c>
+      <c r="C125" s="2">
+        <f t="shared" si="1"/>
+        <v>0.23940427374907028</v>
+      </c>
+    </row>
+    <row r="126" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A126" s="1">
+        <v>12.328828005938</v>
+      </c>
+      <c r="B126" s="1">
+        <v>30974356.154456601</v>
+      </c>
+      <c r="C126" s="2">
+        <f t="shared" si="1"/>
+        <v>1.3988396936056482E-3</v>
+      </c>
+    </row>
+    <row r="127" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A127" s="1">
+        <v>12.328828005938</v>
+      </c>
+      <c r="B127" s="1">
+        <v>33063929.435010999</v>
+      </c>
+      <c r="C127" s="2">
+        <f t="shared" si="1"/>
+        <v>6.746139516619945E-2</v>
+      </c>
+    </row>
+    <row r="128" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A128" s="1">
+        <v>12.328828005938</v>
+      </c>
+      <c r="B128" s="1">
+        <v>27570603.826418102</v>
+      </c>
+      <c r="C128" s="2">
+        <f t="shared" si="1"/>
+        <v>-0.16614255179168394</v>
+      </c>
+    </row>
+    <row r="129" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A129" s="1">
+        <v>12.328828005938</v>
+      </c>
+      <c r="B129" s="1">
+        <v>28204727.997801401</v>
+      </c>
+      <c r="C129" s="2">
+        <f t="shared" si="1"/>
+        <v>2.3000010278181951E-2</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Program is not converging.  Will rerun with no mutations.  Continuing to clean up and document code.
</commit_message>
<xml_diff>
--- a/Progress.xlsx
+++ b/Progress.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/c51537410c5afe56/Projects/Source/Repos/EdGarrity/SOS/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="133" documentId="114_{B2D123C0-10CD-4892-A2B1-0D4FB86B9D90}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{C3E42DCE-092D-4567-A4A4-C12FF766C2C9}"/>
+  <xr:revisionPtr revIDLastSave="141" documentId="114_{B2D123C0-10CD-4892-A2B1-0D4FB86B9D90}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{FF232C8A-CAC8-40B6-A4A5-7779A11AEF58}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{D7613C25-2959-4D88-A8C3-21B00E74DE47}"/>
   </bookViews>
@@ -1365,10 +1365,10 @@
           </c:marker>
           <c:val>
             <c:numRef>
-              <c:f>'Run 2'!$B$2:$B$129</c:f>
+              <c:f>'Run 2'!$B$2:$B$137</c:f>
               <c:numCache>
                 <c:formatCode>#,##0.00</c:formatCode>
-                <c:ptCount val="128"/>
+                <c:ptCount val="136"/>
                 <c:pt idx="0">
                   <c:v>136667774.57913801</c:v>
                 </c:pt>
@@ -1752,6 +1752,30 @@
                 </c:pt>
                 <c:pt idx="127">
                   <c:v>28204727.997801401</c:v>
+                </c:pt>
+                <c:pt idx="128">
+                  <c:v>30181015.068997201</c:v>
+                </c:pt>
+                <c:pt idx="129">
+                  <c:v>25263459.829275001</c:v>
+                </c:pt>
+                <c:pt idx="130">
+                  <c:v>25418286.691030201</c:v>
+                </c:pt>
+                <c:pt idx="131">
+                  <c:v>25564998.2441779</c:v>
+                </c:pt>
+                <c:pt idx="132">
+                  <c:v>27015850.369339801</c:v>
+                </c:pt>
+                <c:pt idx="133">
+                  <c:v>27399332.242027398</c:v>
+                </c:pt>
+                <c:pt idx="134">
+                  <c:v>32855212.3060726</c:v>
+                </c:pt>
+                <c:pt idx="135">
+                  <c:v>28522028.6611492</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1807,10 +1831,10 @@
           </c:marker>
           <c:val>
             <c:numRef>
-              <c:f>'Run 2'!$A$2:$A$129</c:f>
+              <c:f>'Run 2'!$A$2:$A$137</c:f>
               <c:numCache>
                 <c:formatCode>#,##0.00</c:formatCode>
-                <c:ptCount val="128"/>
+                <c:ptCount val="136"/>
                 <c:pt idx="0">
                   <c:v>15.2970585407784</c:v>
                 </c:pt>
@@ -2193,6 +2217,30 @@
                   <c:v>12.328828005938</c:v>
                 </c:pt>
                 <c:pt idx="127">
+                  <c:v>12.328828005938</c:v>
+                </c:pt>
+                <c:pt idx="128">
+                  <c:v>12.328828005938</c:v>
+                </c:pt>
+                <c:pt idx="129">
+                  <c:v>12.328828005938</c:v>
+                </c:pt>
+                <c:pt idx="130">
+                  <c:v>12.328828005938</c:v>
+                </c:pt>
+                <c:pt idx="131">
+                  <c:v>12.328828005938</c:v>
+                </c:pt>
+                <c:pt idx="132">
+                  <c:v>12.328828005938</c:v>
+                </c:pt>
+                <c:pt idx="133">
+                  <c:v>12.328828005938</c:v>
+                </c:pt>
+                <c:pt idx="134">
+                  <c:v>12.328828005938</c:v>
+                </c:pt>
+                <c:pt idx="135">
                   <c:v>12.328828005938</c:v>
                 </c:pt>
               </c:numCache>
@@ -4972,10 +5020,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EFDF9A5F-6B77-43F5-8016-32B291B6E88B}">
-  <dimension ref="A1:D129"/>
+  <dimension ref="A1:D137"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="J4" sqref="J4"/>
+    <sheetView tabSelected="1" topLeftCell="D1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="C25" sqref="C25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -5861,7 +5909,7 @@
         <v>66055665.006507002</v>
       </c>
       <c r="C72" s="2">
-        <f t="shared" ref="C72:C129" si="1">(B72-B71)/B71</f>
+        <f t="shared" ref="C72:C135" si="1">(B72-B71)/B71</f>
         <v>0.44377823458301502</v>
       </c>
       <c r="D72" t="s">
@@ -6556,6 +6604,102 @@
       <c r="C129" s="2">
         <f t="shared" si="1"/>
         <v>2.3000010278181951E-2</v>
+      </c>
+    </row>
+    <row r="130" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A130" s="1">
+        <v>12.328828005938</v>
+      </c>
+      <c r="B130" s="1">
+        <v>30181015.068997201</v>
+      </c>
+      <c r="C130" s="2">
+        <f t="shared" si="1"/>
+        <v>7.0069354022838093E-2</v>
+      </c>
+    </row>
+    <row r="131" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A131" s="1">
+        <v>12.328828005938</v>
+      </c>
+      <c r="B131" s="1">
+        <v>25263459.829275001</v>
+      </c>
+      <c r="C131" s="2">
+        <f t="shared" si="1"/>
+        <v>-0.16293538267285293</v>
+      </c>
+    </row>
+    <row r="132" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A132" s="1">
+        <v>12.328828005938</v>
+      </c>
+      <c r="B132" s="1">
+        <v>25418286.691030201</v>
+      </c>
+      <c r="C132" s="2">
+        <f t="shared" si="1"/>
+        <v>6.1284900326988535E-3</v>
+      </c>
+    </row>
+    <row r="133" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A133" s="1">
+        <v>12.328828005938</v>
+      </c>
+      <c r="B133" s="1">
+        <v>25564998.2441779</v>
+      </c>
+      <c r="C133" s="2">
+        <f t="shared" si="1"/>
+        <v>5.7718899362116478E-3</v>
+      </c>
+    </row>
+    <row r="134" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A134" s="1">
+        <v>12.328828005938</v>
+      </c>
+      <c r="B134" s="1">
+        <v>27015850.369339801</v>
+      </c>
+      <c r="C134" s="2">
+        <f t="shared" si="1"/>
+        <v>5.6751504979755438E-2</v>
+      </c>
+    </row>
+    <row r="135" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A135" s="1">
+        <v>12.328828005938</v>
+      </c>
+      <c r="B135" s="1">
+        <v>27399332.242027398</v>
+      </c>
+      <c r="C135" s="2">
+        <f t="shared" si="1"/>
+        <v>1.4194699313363429E-2</v>
+      </c>
+    </row>
+    <row r="136" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A136" s="1">
+        <v>12.328828005938</v>
+      </c>
+      <c r="B136" s="1">
+        <v>32855212.3060726</v>
+      </c>
+      <c r="C136" s="2">
+        <f t="shared" ref="C136:C137" si="2">(B136-B135)/B135</f>
+        <v>0.19912456317736513</v>
+      </c>
+    </row>
+    <row r="137" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A137" s="1">
+        <v>12.328828005938</v>
+      </c>
+      <c r="B137" s="1">
+        <v>28522028.6611492</v>
+      </c>
+      <c r="C137" s="2">
+        <f t="shared" si="2"/>
+        <v>-0.13188725139123517</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Made additional documentation and clean-up changes.
</commit_message>
<xml_diff>
--- a/Progress.xlsx
+++ b/Progress.xlsx
@@ -8,13 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/c51537410c5afe56/Projects/Source/Repos/EdGarrity/SOS/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="141" documentId="114_{B2D123C0-10CD-4892-A2B1-0D4FB86B9D90}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{FF232C8A-CAC8-40B6-A4A5-7779A11AEF58}"/>
+  <xr:revisionPtr revIDLastSave="149" documentId="114_{B2D123C0-10CD-4892-A2B1-0D4FB86B9D90}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{E375B0C1-8F9D-4DBE-A74B-7E1DB8C938F4}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{D7613C25-2959-4D88-A8C3-21B00E74DE47}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="2" xr2:uid="{D7613C25-2959-4D88-A8C3-21B00E74DE47}"/>
   </bookViews>
   <sheets>
     <sheet name="Run 1" sheetId="1" r:id="rId1"/>
     <sheet name="Run 2" sheetId="2" r:id="rId2"/>
+    <sheet name="Run 3" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -34,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="7">
   <si>
     <t>BestIndividual_Training_Error</t>
   </si>
@@ -2524,6 +2525,517 @@
 </c:chartSpace>
 </file>
 
+<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="2000" b="0" i="0" u="none" strike="noStrike" kern="1200" cap="none" spc="0" normalizeH="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mj-lt"/>
+              <a:ea typeface="+mj-ea"/>
+              <a:cs typeface="+mj-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Run 3'!$B$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Average_Training_Error</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="38100" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>'Run 3'!$B$2:$B$137</c:f>
+              <c:numCache>
+                <c:formatCode>#,##0.00</c:formatCode>
+                <c:ptCount val="136"/>
+                <c:pt idx="0">
+                  <c:v>427264626.113644</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>417822006.71020401</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>298281953.09392202</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>223203179.277098</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>179177464.95803601</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>210418407.923893</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>212876881.44677901</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>159790037.455652</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>99103290.209387407</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>67728389.194371104</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>44470283.622346498</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>25176138.681705698</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>17619567.055119999</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>3423991.20165007</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>10856379.476784499</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-905B-42CE-B919-4A78BDAA1C3D}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:marker val="1"/>
+        <c:smooth val="0"/>
+        <c:axId val="715829080"/>
+        <c:axId val="715823504"/>
+      </c:lineChart>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Run 3'!$A$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>BestIndividual_Training_Error</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="38100" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>'Run 3'!$A$2:$A$137</c:f>
+              <c:numCache>
+                <c:formatCode>#,##0.00</c:formatCode>
+                <c:ptCount val="136"/>
+                <c:pt idx="0">
+                  <c:v>15.2970585407784</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>15.2970585407784</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>15.2970585407784</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>15.2970585407784</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>15.2970585407784</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>15.2970585407784</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>15.2970585407784</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>13.6381816969859</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>13.6381816969859</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>13.6381816969859</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>13.6381816969859</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>13.6381816969859</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>13.6381816969859</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>13.6381816969859</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>13.6381816969859</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-905B-42CE-B919-4A78BDAA1C3D}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:marker val="1"/>
+        <c:smooth val="0"/>
+        <c:axId val="840836808"/>
+        <c:axId val="840833856"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="715829080"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" cap="none" spc="0" normalizeH="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="715823504"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="715823504"/>
+        <c:scaling>
+          <c:logBase val="10"/>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:minorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="5000"/>
+                  <a:lumOff val="95000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:minorGridlines>
+        <c:numFmt formatCode="#,##0.00" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="715829080"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="840833856"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="r"/>
+        <c:numFmt formatCode="#,##0.00" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="840836808"/>
+        <c:crosses val="max"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:catAx>
+        <c:axId val="840836808"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="1"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="840833856"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="t"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
 <file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
@@ -2565,6 +3077,46 @@
 </file>
 
 <file path=xl/charts/colors2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors3.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
   <a:schemeClr val="accent2"/>
@@ -3604,6 +4156,506 @@
 </cs:chartStyle>
 </file>
 
+<file path=xl/charts/style3.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="235">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200" cap="all"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" b="0" kern="1200" cap="none" spc="0" normalizeH="0" baseline="0"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="38100" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="8"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:prstDash val="dash"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:prstDash val="dash"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="major">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="2000" b="0" kern="1200" cap="none" spc="0" normalizeH="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
@@ -3666,6 +4718,49 @@
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
               <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{87DD270B-4708-4B98-A301-85905BA2B53B}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>561975</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>30</xdr:col>
+      <xdr:colOff>409575</xdr:colOff>
+      <xdr:row>37</xdr:row>
+      <xdr:rowOff>19050</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{9A251193-1AF6-4837-BCA5-854F267B1B1A}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3987,7 +5082,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{98DDA464-7CD7-4D3D-AE21-4B05822D1057}">
   <dimension ref="A1:B127"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView topLeftCell="A6" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -5022,7 +6117,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EFDF9A5F-6B77-43F5-8016-32B291B6E88B}">
   <dimension ref="A1:D137"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+    <sheetView topLeftCell="D1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
       <selection activeCell="C25" sqref="C25"/>
     </sheetView>
   </sheetViews>
@@ -6707,4 +7802,1181 @@
   <pageSetup orientation="portrait" r:id="rId1"/>
   <drawing r:id="rId2"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FD3AD4D7-7506-4E58-8F31-A8ACAD68134E}">
+  <dimension ref="A1:D137"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="C19" sqref="C19"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="27.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="22.109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="8.88671875" style="2"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A2" s="1">
+        <v>15.2970585407784</v>
+      </c>
+      <c r="B2" s="1">
+        <v>427264626.113644</v>
+      </c>
+      <c r="D2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A3" s="1">
+        <v>15.2970585407784</v>
+      </c>
+      <c r="B3" s="1">
+        <v>417822006.71020401</v>
+      </c>
+      <c r="C3" s="2">
+        <f>(B3-B2)/B2</f>
+        <v>-2.2100166562650209E-2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A4" s="1">
+        <v>15.2970585407784</v>
+      </c>
+      <c r="B4" s="1">
+        <v>298281953.09392202</v>
+      </c>
+      <c r="C4" s="2">
+        <f t="shared" ref="C4:C71" si="0">(B4-B3)/B3</f>
+        <v>-0.28610281817729488</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A5" s="1">
+        <v>15.2970585407784</v>
+      </c>
+      <c r="B5" s="1">
+        <v>223203179.277098</v>
+      </c>
+      <c r="C5" s="2">
+        <f t="shared" si="0"/>
+        <v>-0.25170404390232576</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A6" s="1">
+        <v>15.2970585407784</v>
+      </c>
+      <c r="B6" s="1">
+        <v>179177464.95803601</v>
+      </c>
+      <c r="C6" s="2">
+        <f t="shared" si="0"/>
+        <v>-0.19724501443774595</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A7" s="1">
+        <v>15.2970585407784</v>
+      </c>
+      <c r="B7" s="1">
+        <v>210418407.923893</v>
+      </c>
+      <c r="C7" s="2">
+        <f t="shared" si="0"/>
+        <v>0.17435754531505251</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A8" s="1">
+        <v>15.2970585407784</v>
+      </c>
+      <c r="B8" s="1">
+        <v>212876881.44677901</v>
+      </c>
+      <c r="C8" s="2">
+        <f t="shared" si="0"/>
+        <v>1.1683737877986522E-2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A9" s="1">
+        <v>13.6381816969859</v>
+      </c>
+      <c r="B9" s="1">
+        <v>159790037.455652</v>
+      </c>
+      <c r="C9" s="2">
+        <f t="shared" si="0"/>
+        <v>-0.24937815525261331</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A10" s="1">
+        <v>13.6381816969859</v>
+      </c>
+      <c r="B10" s="1">
+        <v>99103290.209387407</v>
+      </c>
+      <c r="C10" s="2">
+        <f t="shared" si="0"/>
+        <v>-0.37979055648639887</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A11" s="1">
+        <v>13.6381816969859</v>
+      </c>
+      <c r="B11" s="1">
+        <v>67728389.194371104</v>
+      </c>
+      <c r="C11" s="2">
+        <f t="shared" si="0"/>
+        <v>-0.31658788470823507</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A12" s="1">
+        <v>13.6381816969859</v>
+      </c>
+      <c r="B12" s="1">
+        <v>44470283.622346498</v>
+      </c>
+      <c r="C12" s="2">
+        <f t="shared" si="0"/>
+        <v>-0.34340260928511179</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A13" s="1">
+        <v>13.6381816969859</v>
+      </c>
+      <c r="B13" s="1">
+        <v>25176138.681705698</v>
+      </c>
+      <c r="C13" s="2">
+        <f t="shared" si="0"/>
+        <v>-0.43386601948599701</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A14" s="1">
+        <v>13.6381816969859</v>
+      </c>
+      <c r="B14" s="1">
+        <v>17619567.055119999</v>
+      </c>
+      <c r="C14" s="2">
+        <f t="shared" si="0"/>
+        <v>-0.30014815703556241</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A15" s="1">
+        <v>13.6381816969859</v>
+      </c>
+      <c r="B15" s="1">
+        <v>3423991.20165007</v>
+      </c>
+      <c r="C15" s="2">
+        <f t="shared" si="0"/>
+        <v>-0.80567109333965692</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A16" s="1">
+        <v>13.6381816969859</v>
+      </c>
+      <c r="B16" s="1">
+        <v>10856379.476784499</v>
+      </c>
+      <c r="C16" s="2">
+        <f t="shared" si="0"/>
+        <v>2.1706797235789201</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="C17" s="2">
+        <f t="shared" si="0"/>
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A18" s="1"/>
+      <c r="B18" s="1"/>
+      <c r="C18" s="2" t="e">
+        <f t="shared" si="0"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A19" s="1"/>
+      <c r="B19" s="1"/>
+      <c r="C19" s="2" t="e">
+        <f t="shared" si="0"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A20" s="1"/>
+      <c r="B20" s="1"/>
+      <c r="C20" s="2" t="e">
+        <f t="shared" si="0"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A21" s="1"/>
+      <c r="B21" s="1"/>
+      <c r="C21" s="2" t="e">
+        <f t="shared" si="0"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A22" s="1"/>
+      <c r="B22" s="1"/>
+      <c r="C22" s="2" t="e">
+        <f t="shared" si="0"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A23" s="1"/>
+      <c r="B23" s="1"/>
+      <c r="C23" s="2" t="e">
+        <f t="shared" si="0"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A24" s="1"/>
+      <c r="B24" s="1"/>
+      <c r="C24" s="2" t="e">
+        <f t="shared" si="0"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A25" s="1"/>
+      <c r="B25" s="1"/>
+      <c r="C25" s="2" t="e">
+        <f t="shared" si="0"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A26" s="1"/>
+      <c r="C26" s="2" t="e">
+        <f t="shared" si="0"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A27" s="1"/>
+      <c r="B27" s="1"/>
+      <c r="C27" s="2" t="e">
+        <f t="shared" si="0"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A28" s="1"/>
+      <c r="B28" s="1"/>
+      <c r="C28" s="2" t="e">
+        <f t="shared" si="0"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A29" s="1"/>
+      <c r="B29" s="1"/>
+      <c r="C29" s="2" t="e">
+        <f t="shared" si="0"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A30" s="1"/>
+      <c r="B30" s="1"/>
+      <c r="C30" s="2" t="e">
+        <f t="shared" si="0"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A31" s="1"/>
+      <c r="B31" s="1"/>
+      <c r="C31" s="2" t="e">
+        <f t="shared" si="0"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A32" s="1"/>
+      <c r="B32" s="1"/>
+      <c r="C32" s="2" t="e">
+        <f t="shared" si="0"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A33" s="1"/>
+      <c r="B33" s="1"/>
+      <c r="C33" s="2" t="e">
+        <f t="shared" si="0"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A34" s="1"/>
+      <c r="B34" s="1"/>
+      <c r="C34" s="2" t="e">
+        <f t="shared" si="0"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A35" s="1"/>
+      <c r="B35" s="1"/>
+      <c r="C35" s="2" t="e">
+        <f t="shared" si="0"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A36" s="1"/>
+      <c r="B36" s="1"/>
+      <c r="C36" s="2" t="e">
+        <f t="shared" si="0"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A37" s="1"/>
+      <c r="B37" s="1"/>
+      <c r="C37" s="2" t="e">
+        <f t="shared" si="0"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A38" s="1"/>
+      <c r="B38" s="1"/>
+      <c r="C38" s="2" t="e">
+        <f t="shared" si="0"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A39" s="1"/>
+      <c r="B39" s="1"/>
+      <c r="C39" s="2" t="e">
+        <f t="shared" si="0"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A40" s="1"/>
+      <c r="B40" s="1"/>
+      <c r="C40" s="2" t="e">
+        <f t="shared" si="0"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A41" s="1"/>
+      <c r="B41" s="1"/>
+      <c r="C41" s="2" t="e">
+        <f t="shared" si="0"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A42" s="1"/>
+      <c r="B42" s="1"/>
+      <c r="C42" s="2" t="e">
+        <f t="shared" si="0"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A43" s="1"/>
+      <c r="B43" s="1"/>
+      <c r="C43" s="2" t="e">
+        <f t="shared" si="0"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A44" s="1"/>
+      <c r="B44" s="1"/>
+      <c r="C44" s="2" t="e">
+        <f t="shared" si="0"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A45" s="1"/>
+      <c r="B45" s="1"/>
+      <c r="C45" s="2" t="e">
+        <f t="shared" si="0"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A46" s="1"/>
+      <c r="B46" s="1"/>
+      <c r="C46" s="2" t="e">
+        <f t="shared" si="0"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="47" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A47" s="1"/>
+      <c r="B47" s="1"/>
+      <c r="C47" s="2" t="e">
+        <f t="shared" si="0"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="48" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A48" s="1"/>
+      <c r="B48" s="1"/>
+      <c r="C48" s="2" t="e">
+        <f t="shared" si="0"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="49" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A49" s="1"/>
+      <c r="B49" s="1"/>
+      <c r="C49" s="2" t="e">
+        <f t="shared" si="0"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="50" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A50" s="1"/>
+      <c r="B50" s="1"/>
+      <c r="C50" s="2" t="e">
+        <f t="shared" si="0"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="51" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A51" s="1"/>
+      <c r="B51" s="1"/>
+      <c r="C51" s="2" t="e">
+        <f t="shared" si="0"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="52" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A52" s="1"/>
+      <c r="B52" s="1"/>
+      <c r="C52" s="2" t="e">
+        <f t="shared" si="0"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="53" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A53" s="1"/>
+      <c r="B53" s="1"/>
+      <c r="C53" s="2" t="e">
+        <f t="shared" si="0"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="54" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A54" s="1"/>
+      <c r="B54" s="1"/>
+      <c r="C54" s="2" t="e">
+        <f t="shared" si="0"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="55" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A55" s="1"/>
+      <c r="B55" s="1"/>
+      <c r="C55" s="2" t="e">
+        <f t="shared" si="0"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="56" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A56" s="1"/>
+      <c r="B56" s="1"/>
+      <c r="C56" s="2" t="e">
+        <f t="shared" si="0"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="57" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A57" s="1"/>
+      <c r="B57" s="1"/>
+      <c r="C57" s="2" t="e">
+        <f t="shared" si="0"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="58" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A58" s="1"/>
+      <c r="B58" s="1"/>
+      <c r="C58" s="2" t="e">
+        <f t="shared" si="0"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="59" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A59" s="1"/>
+      <c r="B59" s="1"/>
+      <c r="C59" s="2" t="e">
+        <f t="shared" si="0"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="60" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A60" s="1"/>
+      <c r="B60" s="1"/>
+      <c r="C60" s="2" t="e">
+        <f t="shared" si="0"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="61" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A61" s="1"/>
+      <c r="B61" s="1"/>
+      <c r="C61" s="2" t="e">
+        <f t="shared" si="0"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="62" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A62" s="1"/>
+      <c r="B62" s="1"/>
+      <c r="C62" s="2" t="e">
+        <f t="shared" si="0"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="63" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A63" s="1"/>
+      <c r="B63" s="1"/>
+      <c r="C63" s="2" t="e">
+        <f t="shared" si="0"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="64" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A64" s="1"/>
+      <c r="B64" s="1"/>
+      <c r="C64" s="2" t="e">
+        <f t="shared" si="0"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="65" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A65" s="1"/>
+      <c r="B65" s="1"/>
+      <c r="C65" s="2" t="e">
+        <f t="shared" si="0"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="66" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A66" s="1"/>
+      <c r="B66" s="1"/>
+      <c r="C66" s="2" t="e">
+        <f t="shared" si="0"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="67" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A67" s="1"/>
+      <c r="B67" s="1"/>
+      <c r="C67" s="2" t="e">
+        <f t="shared" si="0"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="68" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A68" s="1"/>
+      <c r="B68" s="1"/>
+      <c r="C68" s="2" t="e">
+        <f t="shared" si="0"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="69" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A69" s="1"/>
+      <c r="B69" s="1"/>
+      <c r="C69" s="2" t="e">
+        <f t="shared" si="0"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="70" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A70" s="1"/>
+      <c r="B70" s="1"/>
+      <c r="C70" s="2" t="e">
+        <f t="shared" si="0"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="71" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A71" s="1"/>
+      <c r="B71" s="1"/>
+      <c r="C71" s="2" t="e">
+        <f t="shared" si="0"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="72" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A72" s="1"/>
+      <c r="B72" s="1"/>
+      <c r="C72" s="2" t="e">
+        <f t="shared" ref="C72:C135" si="1">(B72-B71)/B71</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="73" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A73" s="1"/>
+      <c r="B73" s="1"/>
+      <c r="C73" s="2" t="e">
+        <f t="shared" si="1"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="74" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A74" s="1"/>
+      <c r="B74" s="1"/>
+      <c r="C74" s="2" t="e">
+        <f t="shared" si="1"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="75" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A75" s="1"/>
+      <c r="B75" s="1"/>
+      <c r="C75" s="2" t="e">
+        <f t="shared" si="1"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="76" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A76" s="1"/>
+      <c r="B76" s="1"/>
+      <c r="C76" s="2" t="e">
+        <f t="shared" si="1"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="77" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A77" s="1"/>
+      <c r="B77" s="1"/>
+      <c r="C77" s="2" t="e">
+        <f t="shared" si="1"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="78" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A78" s="1"/>
+      <c r="B78" s="1"/>
+      <c r="C78" s="2" t="e">
+        <f t="shared" si="1"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="79" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A79" s="1"/>
+      <c r="B79" s="1"/>
+      <c r="C79" s="2" t="e">
+        <f t="shared" si="1"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="80" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A80" s="1"/>
+      <c r="B80" s="1"/>
+      <c r="C80" s="2" t="e">
+        <f t="shared" si="1"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="81" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A81" s="1"/>
+      <c r="B81" s="1"/>
+      <c r="C81" s="2" t="e">
+        <f t="shared" si="1"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="82" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A82" s="1"/>
+      <c r="B82" s="1"/>
+      <c r="C82" s="2" t="e">
+        <f t="shared" si="1"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="83" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A83" s="1"/>
+      <c r="B83" s="1"/>
+      <c r="C83" s="2" t="e">
+        <f t="shared" si="1"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="84" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A84" s="1"/>
+      <c r="B84" s="1"/>
+      <c r="C84" s="2" t="e">
+        <f t="shared" si="1"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="85" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A85" s="1"/>
+      <c r="B85" s="1"/>
+      <c r="C85" s="2" t="e">
+        <f t="shared" si="1"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="86" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A86" s="1"/>
+      <c r="B86" s="1"/>
+      <c r="C86" s="2" t="e">
+        <f t="shared" si="1"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="87" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A87" s="1"/>
+      <c r="B87" s="1"/>
+      <c r="C87" s="2" t="e">
+        <f t="shared" si="1"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="88" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A88" s="1"/>
+      <c r="B88" s="1"/>
+      <c r="C88" s="2" t="e">
+        <f t="shared" si="1"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="89" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A89" s="1"/>
+      <c r="B89" s="1"/>
+      <c r="C89" s="2" t="e">
+        <f t="shared" si="1"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="90" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A90" s="1"/>
+      <c r="B90" s="1"/>
+      <c r="C90" s="2" t="e">
+        <f t="shared" si="1"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="91" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A91" s="1"/>
+      <c r="B91" s="1"/>
+      <c r="C91" s="2" t="e">
+        <f t="shared" si="1"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="92" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A92" s="1"/>
+      <c r="B92" s="1"/>
+      <c r="C92" s="2" t="e">
+        <f t="shared" si="1"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="93" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A93" s="1"/>
+      <c r="B93" s="1"/>
+      <c r="C93" s="2" t="e">
+        <f t="shared" si="1"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="94" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A94" s="1"/>
+      <c r="B94" s="1"/>
+      <c r="C94" s="2" t="e">
+        <f t="shared" si="1"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="95" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A95" s="1"/>
+      <c r="B95" s="1"/>
+      <c r="C95" s="2" t="e">
+        <f t="shared" si="1"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="96" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A96" s="1"/>
+      <c r="B96" s="1"/>
+      <c r="C96" s="2" t="e">
+        <f t="shared" si="1"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="97" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A97" s="1"/>
+      <c r="B97" s="1"/>
+      <c r="C97" s="2" t="e">
+        <f t="shared" si="1"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="98" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A98" s="1"/>
+      <c r="B98" s="1"/>
+      <c r="C98" s="2" t="e">
+        <f t="shared" si="1"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="99" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A99" s="1"/>
+      <c r="B99" s="1"/>
+      <c r="C99" s="2" t="e">
+        <f t="shared" si="1"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="100" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A100" s="1"/>
+      <c r="B100" s="1"/>
+      <c r="C100" s="2" t="e">
+        <f t="shared" si="1"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="101" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A101" s="1"/>
+      <c r="B101" s="1"/>
+      <c r="C101" s="2" t="e">
+        <f t="shared" si="1"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="102" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A102" s="1"/>
+      <c r="B102" s="1"/>
+      <c r="C102" s="2" t="e">
+        <f t="shared" si="1"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="103" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A103" s="1"/>
+      <c r="B103" s="1"/>
+      <c r="C103" s="2" t="e">
+        <f t="shared" si="1"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="104" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A104" s="1"/>
+      <c r="B104" s="1"/>
+      <c r="C104" s="2" t="e">
+        <f t="shared" si="1"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="105" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A105" s="1"/>
+      <c r="B105" s="1"/>
+      <c r="C105" s="2" t="e">
+        <f t="shared" si="1"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="106" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A106" s="1"/>
+      <c r="B106" s="1"/>
+      <c r="C106" s="2" t="e">
+        <f t="shared" si="1"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="107" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A107" s="1"/>
+      <c r="B107" s="1"/>
+      <c r="C107" s="2" t="e">
+        <f t="shared" si="1"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="108" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A108" s="1"/>
+      <c r="B108" s="1"/>
+      <c r="C108" s="2" t="e">
+        <f t="shared" si="1"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="109" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A109" s="1"/>
+      <c r="B109" s="1"/>
+      <c r="C109" s="2" t="e">
+        <f t="shared" si="1"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="110" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A110" s="1"/>
+      <c r="B110" s="1"/>
+      <c r="C110" s="2" t="e">
+        <f t="shared" si="1"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="111" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A111" s="1"/>
+      <c r="B111" s="1"/>
+      <c r="C111" s="2" t="e">
+        <f t="shared" si="1"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="112" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A112" s="1"/>
+      <c r="B112" s="1"/>
+      <c r="C112" s="2" t="e">
+        <f t="shared" si="1"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="113" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A113" s="1"/>
+      <c r="B113" s="1"/>
+      <c r="C113" s="2" t="e">
+        <f t="shared" si="1"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="114" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A114" s="1"/>
+      <c r="B114" s="1"/>
+      <c r="C114" s="2" t="e">
+        <f t="shared" si="1"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="115" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A115" s="1"/>
+      <c r="B115" s="1"/>
+      <c r="C115" s="2" t="e">
+        <f t="shared" si="1"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="116" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A116" s="1"/>
+      <c r="B116" s="1"/>
+      <c r="C116" s="2" t="e">
+        <f t="shared" si="1"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="117" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A117" s="1"/>
+      <c r="B117" s="1"/>
+      <c r="C117" s="2" t="e">
+        <f t="shared" si="1"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="118" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A118" s="1"/>
+      <c r="B118" s="1"/>
+      <c r="C118" s="2" t="e">
+        <f t="shared" si="1"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="119" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A119" s="1"/>
+      <c r="B119" s="1"/>
+      <c r="C119" s="2" t="e">
+        <f t="shared" si="1"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="120" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A120" s="1"/>
+      <c r="B120" s="1"/>
+      <c r="C120" s="2" t="e">
+        <f t="shared" si="1"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="121" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A121" s="1"/>
+      <c r="B121" s="1"/>
+      <c r="C121" s="2" t="e">
+        <f t="shared" si="1"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="122" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A122" s="1"/>
+      <c r="B122" s="1"/>
+      <c r="C122" s="2" t="e">
+        <f t="shared" si="1"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="123" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A123" s="1"/>
+      <c r="B123" s="1"/>
+      <c r="C123" s="2" t="e">
+        <f t="shared" si="1"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="124" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A124" s="1"/>
+      <c r="B124" s="1"/>
+      <c r="C124" s="2" t="e">
+        <f t="shared" si="1"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="125" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A125" s="1"/>
+      <c r="B125" s="1"/>
+      <c r="C125" s="2" t="e">
+        <f t="shared" si="1"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="126" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A126" s="1"/>
+      <c r="B126" s="1"/>
+      <c r="C126" s="2" t="e">
+        <f t="shared" si="1"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="127" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A127" s="1"/>
+      <c r="B127" s="1"/>
+      <c r="C127" s="2" t="e">
+        <f t="shared" si="1"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="128" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A128" s="1"/>
+      <c r="B128" s="1"/>
+      <c r="C128" s="2" t="e">
+        <f t="shared" si="1"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="129" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A129" s="1"/>
+      <c r="B129" s="1"/>
+      <c r="C129" s="2" t="e">
+        <f t="shared" si="1"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="130" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A130" s="1"/>
+      <c r="B130" s="1"/>
+      <c r="C130" s="2" t="e">
+        <f t="shared" si="1"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="131" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A131" s="1"/>
+      <c r="B131" s="1"/>
+      <c r="C131" s="2" t="e">
+        <f t="shared" si="1"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="132" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A132" s="1"/>
+      <c r="B132" s="1"/>
+      <c r="C132" s="2" t="e">
+        <f t="shared" si="1"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="133" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A133" s="1"/>
+      <c r="B133" s="1"/>
+      <c r="C133" s="2" t="e">
+        <f t="shared" si="1"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="134" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A134" s="1"/>
+      <c r="B134" s="1"/>
+      <c r="C134" s="2" t="e">
+        <f t="shared" si="1"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="135" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A135" s="1"/>
+      <c r="B135" s="1"/>
+      <c r="C135" s="2" t="e">
+        <f t="shared" si="1"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="136" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A136" s="1"/>
+      <c r="B136" s="1"/>
+      <c r="C136" s="2" t="e">
+        <f t="shared" ref="C136:C137" si="2">(B136-B135)/B135</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="137" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A137" s="1"/>
+      <c r="B137" s="1"/>
+      <c r="C137" s="2" t="e">
+        <f t="shared" si="2"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
It was making good progress for the first 25 generations.  However, it soon lost its gains and almost returned back to where it started.  Altered code to carry the best individual for each training case into the next generation.  Maybe this will help to hold on to early gains.
</commit_message>
<xml_diff>
--- a/Progress.xlsx
+++ b/Progress.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/c51537410c5afe56/Projects/Source/Repos/EdGarrity/SOS/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="149" documentId="114_{B2D123C0-10CD-4892-A2B1-0D4FB86B9D90}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{E375B0C1-8F9D-4DBE-A74B-7E1DB8C938F4}"/>
+  <xr:revisionPtr revIDLastSave="205" documentId="114_{B2D123C0-10CD-4892-A2B1-0D4FB86B9D90}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{B9B71E14-A50C-4D4D-9B1B-AA60A78DE739}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="2" xr2:uid="{D7613C25-2959-4D88-A8C3-21B00E74DE47}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="7">
   <si>
     <t>BestIndividual_Training_Error</t>
   </si>
@@ -2652,6 +2652,282 @@
                 <c:pt idx="14">
                   <c:v>10856379.476784499</c:v>
                 </c:pt>
+                <c:pt idx="15">
+                  <c:v>8105674.0381009895</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>1123511.5748859299</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>261992.21465051701</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>6040114.0010285396</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>819845.90682159597</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>186902.06076376201</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>1394395.7965162799</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>2258310.50596262</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>202306.75449899599</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>638925.16115978896</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>305204.48053149303</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>331018.63046860503</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>1160117.6145586399</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>326509.35434628098</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>407006.80523418199</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>279963.91868223302</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>644613.22197947802</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>814575.05639625702</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>2988484.8971202499</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>1288245.4587081</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>1992704.94724622</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>3279717.7496882598</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>4256054.38508958</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>3023483.4571230598</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>5066829.3221982298</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>5455599.0593245998</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>7429293.4540252797</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>3286600.4212237601</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>1541152.3623524499</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>3007127.4317932399</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>1308935.86300328</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>1461870.3058835301</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>1566350.6686763801</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>1540769.8480360601</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>1695855.25269494</c:v>
+                </c:pt>
+                <c:pt idx="50">
+                  <c:v>1674898.1140330201</c:v>
+                </c:pt>
+                <c:pt idx="51">
+                  <c:v>1051823.8203044001</c:v>
+                </c:pt>
+                <c:pt idx="52">
+                  <c:v>2536059.1656517899</c:v>
+                </c:pt>
+                <c:pt idx="53">
+                  <c:v>1797538.7378630701</c:v>
+                </c:pt>
+                <c:pt idx="54">
+                  <c:v>3513512.9916709298</c:v>
+                </c:pt>
+                <c:pt idx="55">
+                  <c:v>3643186.5226409398</c:v>
+                </c:pt>
+                <c:pt idx="56">
+                  <c:v>3665185.0668154499</c:v>
+                </c:pt>
+                <c:pt idx="57">
+                  <c:v>5998546.4360465501</c:v>
+                </c:pt>
+                <c:pt idx="58">
+                  <c:v>7560711.6513523301</c:v>
+                </c:pt>
+                <c:pt idx="59">
+                  <c:v>11551749.027298599</c:v>
+                </c:pt>
+                <c:pt idx="60">
+                  <c:v>27069930.117070898</c:v>
+                </c:pt>
+                <c:pt idx="61">
+                  <c:v>24448307.477344502</c:v>
+                </c:pt>
+                <c:pt idx="62">
+                  <c:v>34886004.961014703</c:v>
+                </c:pt>
+                <c:pt idx="63">
+                  <c:v>37273677.161567204</c:v>
+                </c:pt>
+                <c:pt idx="64">
+                  <c:v>37531095.067592703</c:v>
+                </c:pt>
+                <c:pt idx="65">
+                  <c:v>46896205.156459898</c:v>
+                </c:pt>
+                <c:pt idx="66">
+                  <c:v>43411193.076619796</c:v>
+                </c:pt>
+                <c:pt idx="67">
+                  <c:v>51359869.408075899</c:v>
+                </c:pt>
+                <c:pt idx="68">
+                  <c:v>49929962.202287801</c:v>
+                </c:pt>
+                <c:pt idx="69">
+                  <c:v>51333190.986514799</c:v>
+                </c:pt>
+                <c:pt idx="70">
+                  <c:v>52431370.403641596</c:v>
+                </c:pt>
+                <c:pt idx="71">
+                  <c:v>49495341.544683397</c:v>
+                </c:pt>
+                <c:pt idx="72">
+                  <c:v>57965005.974634498</c:v>
+                </c:pt>
+                <c:pt idx="73">
+                  <c:v>50153369.720200703</c:v>
+                </c:pt>
+                <c:pt idx="74">
+                  <c:v>50643338.515983202</c:v>
+                </c:pt>
+                <c:pt idx="75">
+                  <c:v>48363541.535302401</c:v>
+                </c:pt>
+                <c:pt idx="76">
+                  <c:v>56054166.219020799</c:v>
+                </c:pt>
+                <c:pt idx="77">
+                  <c:v>57953360.765222199</c:v>
+                </c:pt>
+                <c:pt idx="78">
+                  <c:v>56824063.3459801</c:v>
+                </c:pt>
+                <c:pt idx="79">
+                  <c:v>64079969.805582799</c:v>
+                </c:pt>
+                <c:pt idx="80">
+                  <c:v>57928890.345495597</c:v>
+                </c:pt>
+                <c:pt idx="81">
+                  <c:v>59282858.365850598</c:v>
+                </c:pt>
+                <c:pt idx="82">
+                  <c:v>53447047.8484127</c:v>
+                </c:pt>
+                <c:pt idx="83">
+                  <c:v>49071956.736541003</c:v>
+                </c:pt>
+                <c:pt idx="84">
+                  <c:v>51477999.774655603</c:v>
+                </c:pt>
+                <c:pt idx="85">
+                  <c:v>48853031.125621997</c:v>
+                </c:pt>
+                <c:pt idx="86">
+                  <c:v>49803137.921989501</c:v>
+                </c:pt>
+                <c:pt idx="87">
+                  <c:v>51538596.2054037</c:v>
+                </c:pt>
+                <c:pt idx="88">
+                  <c:v>50475261.2370639</c:v>
+                </c:pt>
+                <c:pt idx="89">
+                  <c:v>50195905.231444903</c:v>
+                </c:pt>
+                <c:pt idx="90">
+                  <c:v>50173379.660085402</c:v>
+                </c:pt>
+                <c:pt idx="91">
+                  <c:v>52896853.126407102</c:v>
+                </c:pt>
+                <c:pt idx="92">
+                  <c:v>50494729.686708599</c:v>
+                </c:pt>
+                <c:pt idx="93">
+                  <c:v>51410454.4501056</c:v>
+                </c:pt>
+                <c:pt idx="94">
+                  <c:v>50715103.540616103</c:v>
+                </c:pt>
+                <c:pt idx="95">
+                  <c:v>51035691.569823302</c:v>
+                </c:pt>
+                <c:pt idx="96">
+                  <c:v>47015286.477187</c:v>
+                </c:pt>
+                <c:pt idx="97">
+                  <c:v>47239138.569902197</c:v>
+                </c:pt>
+                <c:pt idx="98">
+                  <c:v>45951219.182515599</c:v>
+                </c:pt>
+                <c:pt idx="99">
+                  <c:v>46309992.449489698</c:v>
+                </c:pt>
+                <c:pt idx="100">
+                  <c:v>49371583.3037339</c:v>
+                </c:pt>
+                <c:pt idx="101">
+                  <c:v>46120420.895776697</c:v>
+                </c:pt>
+                <c:pt idx="102">
+                  <c:v>50195516.712118603</c:v>
+                </c:pt>
+                <c:pt idx="103">
+                  <c:v>48763308.9870397</c:v>
+                </c:pt>
+                <c:pt idx="104">
+                  <c:v>50501580.518040501</c:v>
+                </c:pt>
+                <c:pt idx="105">
+                  <c:v>47345508.514681697</c:v>
+                </c:pt>
+                <c:pt idx="106">
+                  <c:v>48712309.489059702</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -2754,6 +3030,282 @@
                 </c:pt>
                 <c:pt idx="14">
                   <c:v>13.6381816969859</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>13.6381816969859</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>13.6381816969859</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>13.6381816969859</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>13.6381816969859</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>13.6381816969859</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>13.6381816969859</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>13.6381816969859</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>13.1909059582729</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>13.1909059582729</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>13.1909059582729</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>13.1909059582729</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>13.1909059582729</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>13.1909059582729</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>13.1909059582729</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>13.1909059582729</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>13.1909059582729</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>13.1909059582729</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>13.1909059582729</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>13.1909059582729</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>13.1909059582729</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>13.1909059582729</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>13.1909059582729</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>13.1909059582729</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>13.1909059582729</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>13.1909059582729</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>13.1909059582729</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>13.1909059582729</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>13.1909059582729</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>13.1909059582729</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>13.1909059582729</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>13.1909059582729</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>13.1909059582729</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>13.1909059582729</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>13.1909059582729</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>13.1909059582729</c:v>
+                </c:pt>
+                <c:pt idx="50">
+                  <c:v>13.1909059582729</c:v>
+                </c:pt>
+                <c:pt idx="51">
+                  <c:v>13.1909059582729</c:v>
+                </c:pt>
+                <c:pt idx="52">
+                  <c:v>13.1909059582729</c:v>
+                </c:pt>
+                <c:pt idx="53">
+                  <c:v>13.1909059582729</c:v>
+                </c:pt>
+                <c:pt idx="54">
+                  <c:v>13.1909059582729</c:v>
+                </c:pt>
+                <c:pt idx="55">
+                  <c:v>13.1909059582729</c:v>
+                </c:pt>
+                <c:pt idx="56">
+                  <c:v>13.1909059582729</c:v>
+                </c:pt>
+                <c:pt idx="57">
+                  <c:v>13.1909059582729</c:v>
+                </c:pt>
+                <c:pt idx="58">
+                  <c:v>13.1909059582729</c:v>
+                </c:pt>
+                <c:pt idx="59">
+                  <c:v>13.1909059582729</c:v>
+                </c:pt>
+                <c:pt idx="60">
+                  <c:v>13.1909059582729</c:v>
+                </c:pt>
+                <c:pt idx="61">
+                  <c:v>13.1909059582729</c:v>
+                </c:pt>
+                <c:pt idx="62">
+                  <c:v>13.1909059582729</c:v>
+                </c:pt>
+                <c:pt idx="63">
+                  <c:v>13.1909059582729</c:v>
+                </c:pt>
+                <c:pt idx="64">
+                  <c:v>13.1909059582729</c:v>
+                </c:pt>
+                <c:pt idx="65">
+                  <c:v>13.1909059582729</c:v>
+                </c:pt>
+                <c:pt idx="66">
+                  <c:v>13.1909059582729</c:v>
+                </c:pt>
+                <c:pt idx="67">
+                  <c:v>13.1909059582729</c:v>
+                </c:pt>
+                <c:pt idx="68">
+                  <c:v>13.1909059582729</c:v>
+                </c:pt>
+                <c:pt idx="69">
+                  <c:v>13.1909059582729</c:v>
+                </c:pt>
+                <c:pt idx="70">
+                  <c:v>13.1909059582729</c:v>
+                </c:pt>
+                <c:pt idx="71">
+                  <c:v>13.1909059582729</c:v>
+                </c:pt>
+                <c:pt idx="72">
+                  <c:v>13.1909059582729</c:v>
+                </c:pt>
+                <c:pt idx="73">
+                  <c:v>13.1909059582729</c:v>
+                </c:pt>
+                <c:pt idx="74">
+                  <c:v>13.1909059582729</c:v>
+                </c:pt>
+                <c:pt idx="75">
+                  <c:v>13.1909059582729</c:v>
+                </c:pt>
+                <c:pt idx="76">
+                  <c:v>13.1909059582729</c:v>
+                </c:pt>
+                <c:pt idx="77">
+                  <c:v>13.1909059582729</c:v>
+                </c:pt>
+                <c:pt idx="78">
+                  <c:v>13.1909059582729</c:v>
+                </c:pt>
+                <c:pt idx="79">
+                  <c:v>13.1909059582729</c:v>
+                </c:pt>
+                <c:pt idx="80">
+                  <c:v>13.1909059582729</c:v>
+                </c:pt>
+                <c:pt idx="81">
+                  <c:v>13.1909059582729</c:v>
+                </c:pt>
+                <c:pt idx="82">
+                  <c:v>13.1909059582729</c:v>
+                </c:pt>
+                <c:pt idx="83">
+                  <c:v>13.1909059582729</c:v>
+                </c:pt>
+                <c:pt idx="84">
+                  <c:v>13.1909059582729</c:v>
+                </c:pt>
+                <c:pt idx="85">
+                  <c:v>13.1909059582729</c:v>
+                </c:pt>
+                <c:pt idx="86">
+                  <c:v>13.1909059582729</c:v>
+                </c:pt>
+                <c:pt idx="87">
+                  <c:v>13.1909059582729</c:v>
+                </c:pt>
+                <c:pt idx="88">
+                  <c:v>13.1909059582729</c:v>
+                </c:pt>
+                <c:pt idx="89">
+                  <c:v>13.1909059582729</c:v>
+                </c:pt>
+                <c:pt idx="90">
+                  <c:v>13.1909059582729</c:v>
+                </c:pt>
+                <c:pt idx="91">
+                  <c:v>13.1909059582729</c:v>
+                </c:pt>
+                <c:pt idx="92">
+                  <c:v>13.1909059582729</c:v>
+                </c:pt>
+                <c:pt idx="93">
+                  <c:v>13.1909059582729</c:v>
+                </c:pt>
+                <c:pt idx="94">
+                  <c:v>13.1909059582729</c:v>
+                </c:pt>
+                <c:pt idx="95">
+                  <c:v>13.1909059582729</c:v>
+                </c:pt>
+                <c:pt idx="96">
+                  <c:v>13.1909059582729</c:v>
+                </c:pt>
+                <c:pt idx="97">
+                  <c:v>13.1909059582729</c:v>
+                </c:pt>
+                <c:pt idx="98">
+                  <c:v>13.1909059582729</c:v>
+                </c:pt>
+                <c:pt idx="99">
+                  <c:v>13.1909059582729</c:v>
+                </c:pt>
+                <c:pt idx="100">
+                  <c:v>13.1909059582729</c:v>
+                </c:pt>
+                <c:pt idx="101">
+                  <c:v>13.1909059582729</c:v>
+                </c:pt>
+                <c:pt idx="102">
+                  <c:v>13.1909059582729</c:v>
+                </c:pt>
+                <c:pt idx="103">
+                  <c:v>13.1909059582729</c:v>
+                </c:pt>
+                <c:pt idx="104">
+                  <c:v>13.1909059582729</c:v>
+                </c:pt>
+                <c:pt idx="105">
+                  <c:v>13.1909059582729</c:v>
+                </c:pt>
+                <c:pt idx="106">
+                  <c:v>13.1909059582729</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -5082,7 +5634,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{98DDA464-7CD7-4D3D-AE21-4B05822D1057}">
   <dimension ref="A1:B127"/>
   <sheetViews>
-    <sheetView topLeftCell="A6" workbookViewId="0"/>
+    <sheetView topLeftCell="A10" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -7809,7 +8361,7 @@
   <dimension ref="A1:D137"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="C19" sqref="C19"/>
+      <selection activeCell="A16" sqref="A16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -8009,752 +8561,1132 @@
         <v>2.1706797235789201</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A17" s="1">
+        <v>13.6381816969859</v>
+      </c>
+      <c r="B17" s="1">
+        <v>8105674.0381009895</v>
+      </c>
       <c r="C17" s="2">
         <f t="shared" si="0"/>
-        <v>-1</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A18" s="1"/>
-      <c r="B18" s="1"/>
-      <c r="C18" s="2" t="e">
-        <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A19" s="1"/>
-      <c r="B19" s="1"/>
-      <c r="C19" s="2" t="e">
-        <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A20" s="1"/>
-      <c r="B20" s="1"/>
-      <c r="C20" s="2" t="e">
-        <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A21" s="1"/>
-      <c r="B21" s="1"/>
-      <c r="C21" s="2" t="e">
-        <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A22" s="1"/>
-      <c r="B22" s="1"/>
-      <c r="C22" s="2" t="e">
-        <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A23" s="1"/>
-      <c r="B23" s="1"/>
-      <c r="C23" s="2" t="e">
-        <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A24" s="1"/>
-      <c r="B24" s="1"/>
-      <c r="C24" s="2" t="e">
-        <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A25" s="1"/>
-      <c r="B25" s="1"/>
-      <c r="C25" s="2" t="e">
-        <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A26" s="1"/>
-      <c r="C26" s="2" t="e">
-        <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A27" s="1"/>
-      <c r="B27" s="1"/>
-      <c r="C27" s="2" t="e">
-        <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A28" s="1"/>
-      <c r="B28" s="1"/>
-      <c r="C28" s="2" t="e">
-        <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A29" s="1"/>
-      <c r="B29" s="1"/>
-      <c r="C29" s="2" t="e">
-        <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A30" s="1"/>
-      <c r="B30" s="1"/>
-      <c r="C30" s="2" t="e">
-        <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A31" s="1"/>
-      <c r="B31" s="1"/>
-      <c r="C31" s="2" t="e">
-        <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A32" s="1"/>
-      <c r="B32" s="1"/>
-      <c r="C32" s="2" t="e">
-        <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
+        <v>-0.25337226324537326</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A18" s="1">
+        <v>13.6381816969859</v>
+      </c>
+      <c r="B18" s="1">
+        <v>1123511.5748859299</v>
+      </c>
+      <c r="C18" s="2">
+        <f t="shared" si="0"/>
+        <v>-0.86139196202501767</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A19" s="1">
+        <v>13.6381816969859</v>
+      </c>
+      <c r="B19" s="1">
+        <v>261992.21465051701</v>
+      </c>
+      <c r="C19" s="2">
+        <f t="shared" si="0"/>
+        <v>-0.76680951001584741</v>
+      </c>
+      <c r="D19" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A20" s="1">
+        <v>13.6381816969859</v>
+      </c>
+      <c r="B20" s="1">
+        <v>6040114.0010285396</v>
+      </c>
+      <c r="C20" s="2">
+        <f t="shared" si="0"/>
+        <v>22.054555300758516</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A21" s="1">
+        <v>13.6381816969859</v>
+      </c>
+      <c r="B21" s="1">
+        <v>819845.90682159597</v>
+      </c>
+      <c r="C21" s="2">
+        <f t="shared" si="0"/>
+        <v>-0.86426648459251132</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A22" s="1">
+        <v>13.6381816969859</v>
+      </c>
+      <c r="B22" s="1">
+        <v>186902.06076376201</v>
+      </c>
+      <c r="C22" s="2">
+        <f t="shared" si="0"/>
+        <v>-0.77202781741223825</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A23" s="1">
+        <v>13.6381816969859</v>
+      </c>
+      <c r="B23" s="1">
+        <v>1394395.7965162799</v>
+      </c>
+      <c r="C23" s="2">
+        <f t="shared" si="0"/>
+        <v>6.4605694063413761</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A24" s="1">
+        <v>13.1909059582729</v>
+      </c>
+      <c r="B24" s="1">
+        <v>2258310.50596262</v>
+      </c>
+      <c r="C24" s="2">
+        <f t="shared" si="0"/>
+        <v>0.61956204372153212</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A25" s="1">
+        <v>13.1909059582729</v>
+      </c>
+      <c r="B25" s="1">
+        <v>202306.75449899599</v>
+      </c>
+      <c r="C25" s="2">
+        <f t="shared" si="0"/>
+        <v>-0.91041676777181646</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A26" s="1">
+        <v>13.1909059582729</v>
+      </c>
+      <c r="B26" s="1">
+        <v>638925.16115978896</v>
+      </c>
+      <c r="C26" s="2">
+        <f t="shared" si="0"/>
+        <v>2.1581998472668884</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A27" s="1">
+        <v>13.1909059582729</v>
+      </c>
+      <c r="B27" s="1">
+        <v>305204.48053149303</v>
+      </c>
+      <c r="C27" s="2">
+        <f t="shared" si="0"/>
+        <v>-0.5223157592080423</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A28" s="1">
+        <v>13.1909059582729</v>
+      </c>
+      <c r="B28" s="1">
+        <v>331018.63046860503</v>
+      </c>
+      <c r="C28" s="2">
+        <f t="shared" si="0"/>
+        <v>8.457985247188507E-2</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A29" s="1">
+        <v>13.1909059582729</v>
+      </c>
+      <c r="B29" s="1">
+        <v>1160117.6145586399</v>
+      </c>
+      <c r="C29" s="2">
+        <f t="shared" si="0"/>
+        <v>2.5046897901677756</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A30" s="1">
+        <v>13.1909059582729</v>
+      </c>
+      <c r="B30" s="1">
+        <v>326509.35434628098</v>
+      </c>
+      <c r="C30" s="2">
+        <f t="shared" si="0"/>
+        <v>-0.71855495490386156</v>
+      </c>
+      <c r="D30" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A31" s="1">
+        <v>13.1909059582729</v>
+      </c>
+      <c r="B31" s="1">
+        <v>407006.80523418199</v>
+      </c>
+      <c r="C31" s="2">
+        <f t="shared" si="0"/>
+        <v>0.24653949363585179</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A32" s="1">
+        <v>13.1909059582729</v>
+      </c>
+      <c r="B32" s="1">
+        <v>279963.91868223302</v>
+      </c>
+      <c r="C32" s="2">
+        <f>(B32-B30)/B30</f>
+        <v>-0.14255467736058791</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A33" s="1"/>
-      <c r="B33" s="1"/>
-      <c r="C33" s="2" t="e">
-        <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
+      <c r="A33" s="1">
+        <v>13.1909059582729</v>
+      </c>
+      <c r="B33" s="1">
+        <v>644613.22197947802</v>
+      </c>
+      <c r="C33" s="2">
+        <f t="shared" si="0"/>
+        <v>1.3024867812024459</v>
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A34" s="1"/>
-      <c r="B34" s="1"/>
-      <c r="C34" s="2" t="e">
-        <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
+      <c r="A34" s="1">
+        <v>13.1909059582729</v>
+      </c>
+      <c r="B34" s="1">
+        <v>814575.05639625702</v>
+      </c>
+      <c r="C34" s="2">
+        <f t="shared" si="0"/>
+        <v>0.26366482818155706</v>
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A35" s="1"/>
-      <c r="B35" s="1"/>
-      <c r="C35" s="2" t="e">
-        <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
+      <c r="A35" s="1">
+        <v>13.1909059582729</v>
+      </c>
+      <c r="B35" s="1">
+        <v>2988484.8971202499</v>
+      </c>
+      <c r="C35" s="2">
+        <f t="shared" si="0"/>
+        <v>2.6687655405771173</v>
       </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A36" s="1"/>
-      <c r="B36" s="1"/>
-      <c r="C36" s="2" t="e">
-        <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
+      <c r="A36" s="1">
+        <v>13.1909059582729</v>
+      </c>
+      <c r="B36" s="1">
+        <v>1288245.4587081</v>
+      </c>
+      <c r="C36" s="2">
+        <f t="shared" si="0"/>
+        <v>-0.56893024289683602</v>
       </c>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A37" s="1"/>
-      <c r="B37" s="1"/>
-      <c r="C37" s="2" t="e">
-        <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
+      <c r="A37" s="1">
+        <v>13.1909059582729</v>
+      </c>
+      <c r="B37" s="1">
+        <v>1992704.94724622</v>
+      </c>
+      <c r="C37" s="2">
+        <f t="shared" si="0"/>
+        <v>0.54683638415040703</v>
       </c>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A38" s="1"/>
-      <c r="B38" s="1"/>
-      <c r="C38" s="2" t="e">
-        <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
+      <c r="A38" s="1">
+        <v>13.1909059582729</v>
+      </c>
+      <c r="B38" s="1">
+        <v>3279717.7496882598</v>
+      </c>
+      <c r="C38" s="2">
+        <f t="shared" si="0"/>
+        <v>0.6458622006336675</v>
       </c>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A39" s="1"/>
-      <c r="B39" s="1"/>
-      <c r="C39" s="2" t="e">
-        <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
+      <c r="A39" s="1">
+        <v>13.1909059582729</v>
+      </c>
+      <c r="B39" s="1">
+        <v>4256054.38508958</v>
+      </c>
+      <c r="C39" s="2">
+        <f t="shared" si="0"/>
+        <v>0.29768922508472623</v>
       </c>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A40" s="1"/>
-      <c r="B40" s="1"/>
-      <c r="C40" s="2" t="e">
-        <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
+      <c r="A40" s="1">
+        <v>13.1909059582729</v>
+      </c>
+      <c r="B40" s="1">
+        <v>3023483.4571230598</v>
+      </c>
+      <c r="C40" s="2">
+        <f t="shared" si="0"/>
+        <v>-0.28960413012687042</v>
       </c>
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A41" s="1"/>
-      <c r="B41" s="1"/>
-      <c r="C41" s="2" t="e">
-        <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
+      <c r="A41" s="1">
+        <v>13.1909059582729</v>
+      </c>
+      <c r="B41" s="1">
+        <v>5066829.3221982298</v>
+      </c>
+      <c r="C41" s="2">
+        <f t="shared" si="0"/>
+        <v>0.675825052146797</v>
       </c>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A42" s="1"/>
-      <c r="B42" s="1"/>
-      <c r="C42" s="2" t="e">
-        <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
+      <c r="A42" s="1">
+        <v>13.1909059582729</v>
+      </c>
+      <c r="B42" s="1">
+        <v>5455599.0593245998</v>
+      </c>
+      <c r="C42" s="2">
+        <f t="shared" si="0"/>
+        <v>7.6728405952640868E-2</v>
       </c>
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A43" s="1"/>
-      <c r="B43" s="1"/>
-      <c r="C43" s="2" t="e">
-        <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
+      <c r="A43" s="1">
+        <v>13.1909059582729</v>
+      </c>
+      <c r="B43" s="1">
+        <v>7429293.4540252797</v>
+      </c>
+      <c r="C43" s="2">
+        <f t="shared" si="0"/>
+        <v>0.3617740917612487</v>
       </c>
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A44" s="1"/>
-      <c r="B44" s="1"/>
-      <c r="C44" s="2" t="e">
-        <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
+      <c r="A44" s="1">
+        <v>13.1909059582729</v>
+      </c>
+      <c r="B44" s="1">
+        <v>3286600.4212237601</v>
+      </c>
+      <c r="C44" s="2">
+        <f t="shared" si="0"/>
+        <v>-0.55761601805578953</v>
       </c>
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A45" s="1"/>
-      <c r="B45" s="1"/>
-      <c r="C45" s="2" t="e">
-        <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
+      <c r="A45" s="1">
+        <v>13.1909059582729</v>
+      </c>
+      <c r="B45" s="1">
+        <v>1541152.3623524499</v>
+      </c>
+      <c r="C45" s="2">
+        <f t="shared" si="0"/>
+        <v>-0.53108009346064511</v>
       </c>
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A46" s="1"/>
-      <c r="B46" s="1"/>
-      <c r="C46" s="2" t="e">
-        <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
+      <c r="A46" s="1">
+        <v>13.1909059582729</v>
+      </c>
+      <c r="B46" s="1">
+        <v>3007127.4317932399</v>
+      </c>
+      <c r="C46" s="2">
+        <f t="shared" si="0"/>
+        <v>0.95122007742511094</v>
       </c>
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A47" s="1"/>
-      <c r="B47" s="1"/>
-      <c r="C47" s="2" t="e">
-        <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
+      <c r="A47" s="1">
+        <v>13.1909059582729</v>
+      </c>
+      <c r="B47" s="1">
+        <v>1308935.86300328</v>
+      </c>
+      <c r="C47" s="2">
+        <f t="shared" si="0"/>
+        <v>-0.56472218331541657</v>
       </c>
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A48" s="1"/>
-      <c r="B48" s="1"/>
-      <c r="C48" s="2" t="e">
-        <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
+      <c r="A48" s="1">
+        <v>13.1909059582729</v>
+      </c>
+      <c r="B48" s="1">
+        <v>1461870.3058835301</v>
+      </c>
+      <c r="C48" s="2">
+        <f t="shared" si="0"/>
+        <v>0.11683875979175216</v>
       </c>
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A49" s="1"/>
-      <c r="B49" s="1"/>
-      <c r="C49" s="2" t="e">
-        <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
+      <c r="A49" s="1">
+        <v>13.1909059582729</v>
+      </c>
+      <c r="B49" s="1">
+        <v>1566350.6686763801</v>
+      </c>
+      <c r="C49" s="2">
+        <f t="shared" si="0"/>
+        <v>7.1470336576611573E-2</v>
       </c>
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A50" s="1"/>
-      <c r="B50" s="1"/>
-      <c r="C50" s="2" t="e">
-        <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
+      <c r="A50" s="1">
+        <v>13.1909059582729</v>
+      </c>
+      <c r="B50" s="1">
+        <v>1540769.8480360601</v>
+      </c>
+      <c r="C50" s="2">
+        <f t="shared" si="0"/>
+        <v>-1.6331477460239874E-2</v>
       </c>
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A51" s="1"/>
-      <c r="B51" s="1"/>
-      <c r="C51" s="2" t="e">
-        <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
+      <c r="A51" s="1">
+        <v>13.1909059582729</v>
+      </c>
+      <c r="B51" s="1">
+        <v>1695855.25269494</v>
+      </c>
+      <c r="C51" s="2">
+        <f t="shared" si="0"/>
+        <v>0.10065449090697044</v>
       </c>
     </row>
     <row r="52" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A52" s="1"/>
-      <c r="B52" s="1"/>
-      <c r="C52" s="2" t="e">
-        <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
+      <c r="A52" s="1">
+        <v>13.1909059582729</v>
+      </c>
+      <c r="B52" s="1">
+        <v>1674898.1140330201</v>
+      </c>
+      <c r="C52" s="2">
+        <f t="shared" si="0"/>
+        <v>-1.2357858153646177E-2</v>
       </c>
     </row>
     <row r="53" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A53" s="1"/>
-      <c r="B53" s="1"/>
-      <c r="C53" s="2" t="e">
-        <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
+      <c r="A53" s="1">
+        <v>13.1909059582729</v>
+      </c>
+      <c r="B53" s="1">
+        <v>1051823.8203044001</v>
+      </c>
+      <c r="C53" s="2">
+        <f t="shared" si="0"/>
+        <v>-0.37200728122399468</v>
       </c>
     </row>
     <row r="54" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A54" s="1"/>
-      <c r="B54" s="1"/>
-      <c r="C54" s="2" t="e">
-        <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
+      <c r="A54" s="1">
+        <v>13.1909059582729</v>
+      </c>
+      <c r="B54" s="1">
+        <v>2536059.1656517899</v>
+      </c>
+      <c r="C54" s="2">
+        <f t="shared" si="0"/>
+        <v>1.4111064198164374</v>
       </c>
     </row>
     <row r="55" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A55" s="1"/>
-      <c r="B55" s="1"/>
-      <c r="C55" s="2" t="e">
-        <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
+      <c r="A55" s="1">
+        <v>13.1909059582729</v>
+      </c>
+      <c r="B55" s="1">
+        <v>1797538.7378630701</v>
+      </c>
+      <c r="C55" s="2">
+        <f t="shared" ref="C55" si="1">(B55-B54)/B54</f>
+        <v>-0.29120788575881407</v>
       </c>
     </row>
     <row r="56" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A56" s="1"/>
-      <c r="B56" s="1"/>
-      <c r="C56" s="2" t="e">
-        <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
+      <c r="A56" s="1">
+        <v>13.1909059582729</v>
+      </c>
+      <c r="B56" s="1">
+        <v>3513512.9916709298</v>
+      </c>
+      <c r="C56" s="2">
+        <f t="shared" si="0"/>
+        <v>0.95462435254542832</v>
       </c>
     </row>
     <row r="57" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A57" s="1"/>
-      <c r="B57" s="1"/>
-      <c r="C57" s="2" t="e">
-        <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
+      <c r="A57" s="1">
+        <v>13.1909059582729</v>
+      </c>
+      <c r="B57" s="1">
+        <v>3643186.5226409398</v>
+      </c>
+      <c r="C57" s="2">
+        <f t="shared" si="0"/>
+        <v>3.6907087373068408E-2</v>
       </c>
     </row>
     <row r="58" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A58" s="1"/>
-      <c r="B58" s="1"/>
-      <c r="C58" s="2" t="e">
-        <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
+      <c r="A58" s="1">
+        <v>13.1909059582729</v>
+      </c>
+      <c r="B58" s="1">
+        <v>3665185.0668154499</v>
+      </c>
+      <c r="C58" s="2">
+        <f t="shared" si="0"/>
+        <v>6.038270079722228E-3</v>
       </c>
     </row>
     <row r="59" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A59" s="1"/>
-      <c r="B59" s="1"/>
-      <c r="C59" s="2" t="e">
-        <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
+      <c r="A59" s="1">
+        <v>13.1909059582729</v>
+      </c>
+      <c r="B59" s="1">
+        <v>5998546.4360465501</v>
+      </c>
+      <c r="C59" s="2">
+        <f t="shared" si="0"/>
+        <v>0.63662852671679027</v>
       </c>
     </row>
     <row r="60" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A60" s="1"/>
-      <c r="B60" s="1"/>
-      <c r="C60" s="2" t="e">
-        <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
+      <c r="A60" s="1">
+        <v>13.1909059582729</v>
+      </c>
+      <c r="B60" s="1">
+        <v>7560711.6513523301</v>
+      </c>
+      <c r="C60" s="2">
+        <f t="shared" si="0"/>
+        <v>0.26042395969770188</v>
       </c>
     </row>
     <row r="61" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A61" s="1"/>
-      <c r="B61" s="1"/>
-      <c r="C61" s="2" t="e">
-        <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
+      <c r="A61" s="1">
+        <v>13.1909059582729</v>
+      </c>
+      <c r="B61" s="1">
+        <v>11551749.027298599</v>
+      </c>
+      <c r="C61" s="2">
+        <f t="shared" si="0"/>
+        <v>0.52786530686333222</v>
       </c>
     </row>
     <row r="62" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A62" s="1"/>
-      <c r="B62" s="1"/>
-      <c r="C62" s="2" t="e">
-        <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
+      <c r="A62" s="1">
+        <v>13.1909059582729</v>
+      </c>
+      <c r="B62" s="1">
+        <v>27069930.117070898</v>
+      </c>
+      <c r="C62" s="2">
+        <f t="shared" si="0"/>
+        <v>1.3433620357489067</v>
       </c>
     </row>
     <row r="63" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A63" s="1"/>
-      <c r="B63" s="1"/>
-      <c r="C63" s="2" t="e">
-        <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
+      <c r="A63" s="1">
+        <v>13.1909059582729</v>
+      </c>
+      <c r="B63" s="1">
+        <v>24448307.477344502</v>
+      </c>
+      <c r="C63" s="2">
+        <f t="shared" si="0"/>
+        <v>-9.6846302461384759E-2</v>
       </c>
     </row>
     <row r="64" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A64" s="1"/>
-      <c r="B64" s="1"/>
-      <c r="C64" s="2" t="e">
-        <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
+      <c r="A64" s="1">
+        <v>13.1909059582729</v>
+      </c>
+      <c r="B64" s="1">
+        <v>34886004.961014703</v>
+      </c>
+      <c r="C64" s="2">
+        <f t="shared" si="0"/>
+        <v>0.42692924626142303</v>
       </c>
     </row>
     <row r="65" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A65" s="1"/>
-      <c r="B65" s="1"/>
-      <c r="C65" s="2" t="e">
-        <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
+      <c r="A65" s="1">
+        <v>13.1909059582729</v>
+      </c>
+      <c r="B65" s="1">
+        <v>37273677.161567204</v>
+      </c>
+      <c r="C65" s="2">
+        <f t="shared" si="0"/>
+        <v>6.84421217969996E-2</v>
       </c>
     </row>
     <row r="66" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A66" s="1"/>
-      <c r="B66" s="1"/>
-      <c r="C66" s="2" t="e">
-        <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
+      <c r="A66" s="1">
+        <v>13.1909059582729</v>
+      </c>
+      <c r="B66" s="1">
+        <v>37531095.067592703</v>
+      </c>
+      <c r="C66" s="2">
+        <f t="shared" si="0"/>
+        <v>6.9061580618861524E-3</v>
       </c>
     </row>
     <row r="67" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A67" s="1"/>
-      <c r="B67" s="1"/>
-      <c r="C67" s="2" t="e">
-        <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
+      <c r="A67" s="1">
+        <v>13.1909059582729</v>
+      </c>
+      <c r="B67" s="1">
+        <v>46896205.156459898</v>
+      </c>
+      <c r="C67" s="2">
+        <f t="shared" si="0"/>
+        <v>0.24952935884233676</v>
       </c>
     </row>
     <row r="68" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A68" s="1"/>
-      <c r="B68" s="1"/>
-      <c r="C68" s="2" t="e">
-        <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
+      <c r="A68" s="1">
+        <v>13.1909059582729</v>
+      </c>
+      <c r="B68" s="1">
+        <v>43411193.076619796</v>
+      </c>
+      <c r="C68" s="2">
+        <f t="shared" si="0"/>
+        <v>-7.4313306763586717E-2</v>
       </c>
     </row>
     <row r="69" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A69" s="1"/>
-      <c r="B69" s="1"/>
-      <c r="C69" s="2" t="e">
-        <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
+      <c r="A69" s="1">
+        <v>13.1909059582729</v>
+      </c>
+      <c r="B69" s="1">
+        <v>51359869.408075899</v>
+      </c>
+      <c r="C69" s="2">
+        <f t="shared" si="0"/>
+        <v>0.18310200130705609</v>
       </c>
     </row>
     <row r="70" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A70" s="1"/>
-      <c r="B70" s="1"/>
-      <c r="C70" s="2" t="e">
-        <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
+      <c r="A70" s="1">
+        <v>13.1909059582729</v>
+      </c>
+      <c r="B70" s="1">
+        <v>49929962.202287801</v>
+      </c>
+      <c r="C70" s="2">
+        <f t="shared" si="0"/>
+        <v>-2.7840943177383889E-2</v>
       </c>
     </row>
     <row r="71" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A71" s="1"/>
-      <c r="B71" s="1"/>
-      <c r="C71" s="2" t="e">
-        <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
+      <c r="A71" s="1">
+        <v>13.1909059582729</v>
+      </c>
+      <c r="B71" s="1">
+        <v>51333190.986514799</v>
+      </c>
+      <c r="C71" s="2">
+        <f t="shared" si="0"/>
+        <v>2.8103942449263512E-2</v>
       </c>
     </row>
     <row r="72" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A72" s="1"/>
-      <c r="B72" s="1"/>
-      <c r="C72" s="2" t="e">
-        <f t="shared" ref="C72:C135" si="1">(B72-B71)/B71</f>
-        <v>#DIV/0!</v>
+      <c r="A72" s="1">
+        <v>13.1909059582729</v>
+      </c>
+      <c r="B72" s="1">
+        <v>52431370.403641596</v>
+      </c>
+      <c r="C72" s="2">
+        <f t="shared" ref="C72:C135" si="2">(B72-B71)/B71</f>
+        <v>2.1393164851475691E-2</v>
       </c>
     </row>
     <row r="73" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A73" s="1"/>
-      <c r="B73" s="1"/>
-      <c r="C73" s="2" t="e">
-        <f t="shared" si="1"/>
-        <v>#DIV/0!</v>
+      <c r="A73" s="1">
+        <v>13.1909059582729</v>
+      </c>
+      <c r="B73" s="1">
+        <v>49495341.544683397</v>
+      </c>
+      <c r="C73" s="2">
+        <f t="shared" si="2"/>
+        <v>-5.5997560932610664E-2</v>
       </c>
     </row>
     <row r="74" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A74" s="1"/>
-      <c r="B74" s="1"/>
-      <c r="C74" s="2" t="e">
-        <f t="shared" si="1"/>
-        <v>#DIV/0!</v>
+      <c r="A74" s="1">
+        <v>13.1909059582729</v>
+      </c>
+      <c r="B74" s="1">
+        <v>57965005.974634498</v>
+      </c>
+      <c r="C74" s="2">
+        <f t="shared" si="2"/>
+        <v>0.17112043609810954</v>
       </c>
     </row>
     <row r="75" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A75" s="1"/>
-      <c r="B75" s="1"/>
-      <c r="C75" s="2" t="e">
-        <f t="shared" si="1"/>
-        <v>#DIV/0!</v>
+      <c r="A75" s="1">
+        <v>13.1909059582729</v>
+      </c>
+      <c r="B75" s="1">
+        <v>50153369.720200703</v>
+      </c>
+      <c r="C75" s="2">
+        <f t="shared" si="2"/>
+        <v>-0.13476469333673785</v>
       </c>
     </row>
     <row r="76" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A76" s="1"/>
-      <c r="B76" s="1"/>
-      <c r="C76" s="2" t="e">
-        <f t="shared" si="1"/>
-        <v>#DIV/0!</v>
+      <c r="A76" s="1">
+        <v>13.1909059582729</v>
+      </c>
+      <c r="B76" s="1">
+        <v>50643338.515983202</v>
+      </c>
+      <c r="C76" s="2">
+        <f t="shared" si="2"/>
+        <v>9.7694092842808538E-3</v>
       </c>
     </row>
     <row r="77" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A77" s="1"/>
-      <c r="B77" s="1"/>
-      <c r="C77" s="2" t="e">
-        <f t="shared" si="1"/>
-        <v>#DIV/0!</v>
+      <c r="A77" s="1">
+        <v>13.1909059582729</v>
+      </c>
+      <c r="B77" s="1">
+        <v>48363541.535302401</v>
+      </c>
+      <c r="C77" s="2">
+        <f t="shared" si="2"/>
+        <v>-4.5016719819158245E-2</v>
       </c>
     </row>
     <row r="78" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A78" s="1"/>
-      <c r="B78" s="1"/>
-      <c r="C78" s="2" t="e">
-        <f t="shared" si="1"/>
-        <v>#DIV/0!</v>
+      <c r="A78" s="1">
+        <v>13.1909059582729</v>
+      </c>
+      <c r="B78" s="1">
+        <v>56054166.219020799</v>
+      </c>
+      <c r="C78" s="2">
+        <f t="shared" si="2"/>
+        <v>0.1590169875815384</v>
       </c>
     </row>
     <row r="79" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A79" s="1"/>
-      <c r="B79" s="1"/>
-      <c r="C79" s="2" t="e">
-        <f t="shared" si="1"/>
-        <v>#DIV/0!</v>
+      <c r="A79" s="1">
+        <v>13.1909059582729</v>
+      </c>
+      <c r="B79" s="1">
+        <v>57953360.765222199</v>
+      </c>
+      <c r="C79" s="2">
+        <f t="shared" si="2"/>
+        <v>3.3881416392506233E-2</v>
       </c>
     </row>
     <row r="80" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A80" s="1"/>
-      <c r="B80" s="1"/>
-      <c r="C80" s="2" t="e">
-        <f t="shared" si="1"/>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="81" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A81" s="1"/>
-      <c r="B81" s="1"/>
-      <c r="C81" s="2" t="e">
-        <f t="shared" si="1"/>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="82" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A82" s="1"/>
-      <c r="B82" s="1"/>
-      <c r="C82" s="2" t="e">
-        <f t="shared" si="1"/>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="83" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A83" s="1"/>
-      <c r="B83" s="1"/>
-      <c r="C83" s="2" t="e">
-        <f t="shared" si="1"/>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="84" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A84" s="1"/>
-      <c r="B84" s="1"/>
-      <c r="C84" s="2" t="e">
-        <f t="shared" si="1"/>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="85" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A85" s="1"/>
-      <c r="B85" s="1"/>
-      <c r="C85" s="2" t="e">
-        <f t="shared" si="1"/>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="86" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A86" s="1"/>
-      <c r="B86" s="1"/>
-      <c r="C86" s="2" t="e">
-        <f t="shared" si="1"/>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="87" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A87" s="1"/>
-      <c r="B87" s="1"/>
-      <c r="C87" s="2" t="e">
-        <f t="shared" si="1"/>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="88" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A88" s="1"/>
-      <c r="B88" s="1"/>
-      <c r="C88" s="2" t="e">
-        <f t="shared" si="1"/>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="89" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A89" s="1"/>
-      <c r="B89" s="1"/>
-      <c r="C89" s="2" t="e">
-        <f t="shared" si="1"/>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="90" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A90" s="1"/>
-      <c r="B90" s="1"/>
-      <c r="C90" s="2" t="e">
-        <f t="shared" si="1"/>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="91" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A91" s="1"/>
-      <c r="B91" s="1"/>
-      <c r="C91" s="2" t="e">
-        <f t="shared" si="1"/>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="92" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A92" s="1"/>
-      <c r="B92" s="1"/>
-      <c r="C92" s="2" t="e">
-        <f t="shared" si="1"/>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="93" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A93" s="1"/>
-      <c r="B93" s="1"/>
-      <c r="C93" s="2" t="e">
-        <f t="shared" si="1"/>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="94" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A94" s="1"/>
-      <c r="B94" s="1"/>
-      <c r="C94" s="2" t="e">
-        <f t="shared" si="1"/>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="95" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A95" s="1"/>
-      <c r="B95" s="1"/>
-      <c r="C95" s="2" t="e">
-        <f t="shared" si="1"/>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="96" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A96" s="1"/>
-      <c r="B96" s="1"/>
-      <c r="C96" s="2" t="e">
-        <f t="shared" si="1"/>
-        <v>#DIV/0!</v>
+      <c r="A80" s="1">
+        <v>13.1909059582729</v>
+      </c>
+      <c r="B80" s="1">
+        <v>56824063.3459801</v>
+      </c>
+      <c r="C80" s="2">
+        <f t="shared" si="2"/>
+        <v>-1.9486314586949549E-2</v>
+      </c>
+    </row>
+    <row r="81" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A81" s="1">
+        <v>13.1909059582729</v>
+      </c>
+      <c r="B81" s="1">
+        <v>64079969.805582799</v>
+      </c>
+      <c r="C81" s="2">
+        <f t="shared" si="2"/>
+        <v>0.12769073579663329</v>
+      </c>
+    </row>
+    <row r="82" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A82" s="1">
+        <v>13.1909059582729</v>
+      </c>
+      <c r="B82" s="1">
+        <v>57928890.345495597</v>
+      </c>
+      <c r="C82" s="2">
+        <f t="shared" si="2"/>
+        <v>-9.5990673509201707E-2</v>
+      </c>
+    </row>
+    <row r="83" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A83" s="1">
+        <v>13.1909059582729</v>
+      </c>
+      <c r="B83" s="1">
+        <v>59282858.365850598</v>
+      </c>
+      <c r="C83" s="2">
+        <f t="shared" si="2"/>
+        <v>2.3372932094499928E-2</v>
+      </c>
+      <c r="D83" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="84" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A84" s="1">
+        <v>13.1909059582729</v>
+      </c>
+      <c r="B84" s="1">
+        <v>53447047.8484127</v>
+      </c>
+      <c r="C84" s="2">
+        <f t="shared" si="2"/>
+        <v>-9.8440100195971117E-2</v>
+      </c>
+    </row>
+    <row r="85" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A85" s="1">
+        <v>13.1909059582729</v>
+      </c>
+      <c r="B85" s="1">
+        <v>49071956.736541003</v>
+      </c>
+      <c r="C85" s="2">
+        <f t="shared" si="2"/>
+        <v>-8.1858424141224684E-2</v>
+      </c>
+    </row>
+    <row r="86" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A86" s="1">
+        <v>13.1909059582729</v>
+      </c>
+      <c r="B86" s="1">
+        <v>51477999.774655603</v>
+      </c>
+      <c r="C86" s="2">
+        <f t="shared" si="2"/>
+        <v>4.9030917006881058E-2</v>
+      </c>
+    </row>
+    <row r="87" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A87" s="1">
+        <v>13.1909059582729</v>
+      </c>
+      <c r="B87" s="1">
+        <v>48853031.125621997</v>
+      </c>
+      <c r="C87" s="2">
+        <f t="shared" si="2"/>
+        <v>-5.0992048263809361E-2</v>
+      </c>
+    </row>
+    <row r="88" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A88" s="1">
+        <v>13.1909059582729</v>
+      </c>
+      <c r="B88" s="1">
+        <v>49803137.921989501</v>
+      </c>
+      <c r="C88" s="2">
+        <f t="shared" si="2"/>
+        <v>1.9448267067080721E-2</v>
+      </c>
+    </row>
+    <row r="89" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A89" s="1">
+        <v>13.1909059582729</v>
+      </c>
+      <c r="B89" s="1">
+        <v>51538596.2054037</v>
+      </c>
+      <c r="C89" s="2">
+        <f t="shared" si="2"/>
+        <v>3.4846364221719967E-2</v>
+      </c>
+    </row>
+    <row r="90" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A90" s="1">
+        <v>13.1909059582729</v>
+      </c>
+      <c r="B90" s="1">
+        <v>50475261.2370639</v>
+      </c>
+      <c r="C90" s="2">
+        <f t="shared" si="2"/>
+        <v>-2.0631818610308068E-2</v>
+      </c>
+    </row>
+    <row r="91" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A91" s="1">
+        <v>13.1909059582729</v>
+      </c>
+      <c r="B91" s="1">
+        <v>50195905.231444903</v>
+      </c>
+      <c r="C91" s="2">
+        <f t="shared" si="2"/>
+        <v>-5.5345133194450169E-3</v>
+      </c>
+    </row>
+    <row r="92" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A92" s="1">
+        <v>13.1909059582729</v>
+      </c>
+      <c r="B92" s="1">
+        <v>50173379.660085402</v>
+      </c>
+      <c r="C92" s="2">
+        <f t="shared" si="2"/>
+        <v>-4.4875316533567145E-4</v>
+      </c>
+    </row>
+    <row r="93" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A93" s="1">
+        <v>13.1909059582729</v>
+      </c>
+      <c r="B93" s="1">
+        <v>52896853.126407102</v>
+      </c>
+      <c r="C93" s="2">
+        <f t="shared" si="2"/>
+        <v>5.4281244053573562E-2</v>
+      </c>
+    </row>
+    <row r="94" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A94" s="1">
+        <v>13.1909059582729</v>
+      </c>
+      <c r="B94" s="1">
+        <v>50494729.686708599</v>
+      </c>
+      <c r="C94" s="2">
+        <f t="shared" si="2"/>
+        <v>-4.541146207616871E-2</v>
+      </c>
+    </row>
+    <row r="95" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A95" s="1">
+        <v>13.1909059582729</v>
+      </c>
+      <c r="B95" s="1">
+        <v>51410454.4501056</v>
+      </c>
+      <c r="C95" s="2">
+        <f t="shared" si="2"/>
+        <v>1.8135056253960717E-2</v>
+      </c>
+    </row>
+    <row r="96" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A96" s="1">
+        <v>13.1909059582729</v>
+      </c>
+      <c r="B96" s="1">
+        <v>50715103.540616103</v>
+      </c>
+      <c r="C96" s="2">
+        <f t="shared" si="2"/>
+        <v>-1.3525476810642534E-2</v>
       </c>
     </row>
     <row r="97" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A97" s="1"/>
-      <c r="B97" s="1"/>
-      <c r="C97" s="2" t="e">
-        <f t="shared" si="1"/>
-        <v>#DIV/0!</v>
+      <c r="A97" s="1">
+        <v>13.1909059582729</v>
+      </c>
+      <c r="B97" s="1">
+        <v>51035691.569823302</v>
+      </c>
+      <c r="C97" s="2">
+        <f t="shared" si="2"/>
+        <v>6.3213521579513514E-3</v>
       </c>
     </row>
     <row r="98" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A98" s="1"/>
-      <c r="B98" s="1"/>
-      <c r="C98" s="2" t="e">
-        <f t="shared" si="1"/>
-        <v>#DIV/0!</v>
+      <c r="A98" s="1">
+        <v>13.1909059582729</v>
+      </c>
+      <c r="B98" s="1">
+        <v>47015286.477187</v>
+      </c>
+      <c r="C98" s="2">
+        <f t="shared" si="2"/>
+        <v>-7.8776341986781503E-2</v>
       </c>
     </row>
     <row r="99" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A99" s="1"/>
-      <c r="B99" s="1"/>
-      <c r="C99" s="2" t="e">
-        <f t="shared" si="1"/>
-        <v>#DIV/0!</v>
+      <c r="A99" s="1">
+        <v>13.1909059582729</v>
+      </c>
+      <c r="B99" s="1">
+        <v>47239138.569902197</v>
+      </c>
+      <c r="C99" s="2">
+        <f t="shared" si="2"/>
+        <v>4.7612619105025546E-3</v>
       </c>
     </row>
     <row r="100" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A100" s="1"/>
-      <c r="B100" s="1"/>
-      <c r="C100" s="2" t="e">
-        <f t="shared" si="1"/>
-        <v>#DIV/0!</v>
+      <c r="A100" s="1">
+        <v>13.1909059582729</v>
+      </c>
+      <c r="B100" s="1">
+        <v>45951219.182515599</v>
+      </c>
+      <c r="C100" s="2">
+        <f t="shared" si="2"/>
+        <v>-2.726382034847644E-2</v>
       </c>
     </row>
     <row r="101" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A101" s="1"/>
-      <c r="B101" s="1"/>
-      <c r="C101" s="2" t="e">
-        <f t="shared" si="1"/>
-        <v>#DIV/0!</v>
+      <c r="A101" s="1">
+        <v>13.1909059582729</v>
+      </c>
+      <c r="B101" s="1">
+        <v>46309992.449489698</v>
+      </c>
+      <c r="C101" s="2">
+        <f t="shared" si="2"/>
+        <v>7.8076985411218843E-3</v>
       </c>
     </row>
     <row r="102" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A102" s="1"/>
-      <c r="B102" s="1"/>
-      <c r="C102" s="2" t="e">
-        <f t="shared" si="1"/>
-        <v>#DIV/0!</v>
+      <c r="A102" s="1">
+        <v>13.1909059582729</v>
+      </c>
+      <c r="B102" s="1">
+        <v>49371583.3037339</v>
+      </c>
+      <c r="C102" s="2">
+        <f t="shared" si="2"/>
+        <v>6.6110804435640519E-2</v>
       </c>
     </row>
     <row r="103" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A103" s="1"/>
-      <c r="B103" s="1"/>
-      <c r="C103" s="2" t="e">
-        <f t="shared" si="1"/>
-        <v>#DIV/0!</v>
+      <c r="A103" s="1">
+        <v>13.1909059582729</v>
+      </c>
+      <c r="B103" s="1">
+        <v>46120420.895776697</v>
+      </c>
+      <c r="C103" s="2">
+        <f t="shared" si="2"/>
+        <v>-6.5850884059278747E-2</v>
       </c>
     </row>
     <row r="104" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A104" s="1"/>
-      <c r="B104" s="1"/>
-      <c r="C104" s="2" t="e">
-        <f t="shared" si="1"/>
-        <v>#DIV/0!</v>
+      <c r="A104" s="1">
+        <v>13.1909059582729</v>
+      </c>
+      <c r="B104" s="1">
+        <v>50195516.712118603</v>
+      </c>
+      <c r="C104" s="2">
+        <f t="shared" si="2"/>
+        <v>8.8357732587715135E-2</v>
       </c>
     </row>
     <row r="105" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A105" s="1"/>
-      <c r="B105" s="1"/>
-      <c r="C105" s="2" t="e">
-        <f t="shared" si="1"/>
-        <v>#DIV/0!</v>
+      <c r="A105" s="1">
+        <v>13.1909059582729</v>
+      </c>
+      <c r="B105" s="1">
+        <v>48763308.9870397</v>
+      </c>
+      <c r="C105" s="2">
+        <f t="shared" si="2"/>
+        <v>-2.8532582566943236E-2</v>
       </c>
     </row>
     <row r="106" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A106" s="1"/>
-      <c r="B106" s="1"/>
-      <c r="C106" s="2" t="e">
-        <f t="shared" si="1"/>
-        <v>#DIV/0!</v>
+      <c r="A106" s="1">
+        <v>13.1909059582729</v>
+      </c>
+      <c r="B106" s="1">
+        <v>50501580.518040501</v>
+      </c>
+      <c r="C106" s="2">
+        <f t="shared" si="2"/>
+        <v>3.5647120080854189E-2</v>
       </c>
     </row>
     <row r="107" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A107" s="1"/>
-      <c r="B107" s="1"/>
-      <c r="C107" s="2" t="e">
-        <f t="shared" si="1"/>
-        <v>#DIV/0!</v>
+      <c r="A107" s="1">
+        <v>13.1909059582729</v>
+      </c>
+      <c r="B107" s="1">
+        <v>47345508.514681697</v>
+      </c>
+      <c r="C107" s="2">
+        <f t="shared" si="2"/>
+        <v>-6.249451939888042E-2</v>
       </c>
     </row>
     <row r="108" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A108" s="1"/>
-      <c r="B108" s="1"/>
-      <c r="C108" s="2" t="e">
-        <f t="shared" si="1"/>
-        <v>#DIV/0!</v>
+      <c r="A108" s="1">
+        <v>13.1909059582729</v>
+      </c>
+      <c r="B108" s="1">
+        <v>48712309.489059702</v>
+      </c>
+      <c r="C108" s="2">
+        <f t="shared" si="2"/>
+        <v>2.8868651267187549E-2</v>
       </c>
     </row>
     <row r="109" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A109" s="1"/>
       <c r="B109" s="1"/>
-      <c r="C109" s="2" t="e">
-        <f t="shared" si="1"/>
-        <v>#DIV/0!</v>
+      <c r="C109" s="2">
+        <f t="shared" si="2"/>
+        <v>-1</v>
       </c>
     </row>
     <row r="110" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A110" s="1"/>
       <c r="B110" s="1"/>
       <c r="C110" s="2" t="e">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>#DIV/0!</v>
       </c>
     </row>
@@ -8762,7 +9694,7 @@
       <c r="A111" s="1"/>
       <c r="B111" s="1"/>
       <c r="C111" s="2" t="e">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>#DIV/0!</v>
       </c>
     </row>
@@ -8770,7 +9702,7 @@
       <c r="A112" s="1"/>
       <c r="B112" s="1"/>
       <c r="C112" s="2" t="e">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>#DIV/0!</v>
       </c>
     </row>
@@ -8778,7 +9710,7 @@
       <c r="A113" s="1"/>
       <c r="B113" s="1"/>
       <c r="C113" s="2" t="e">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>#DIV/0!</v>
       </c>
     </row>
@@ -8786,7 +9718,7 @@
       <c r="A114" s="1"/>
       <c r="B114" s="1"/>
       <c r="C114" s="2" t="e">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>#DIV/0!</v>
       </c>
     </row>
@@ -8794,7 +9726,7 @@
       <c r="A115" s="1"/>
       <c r="B115" s="1"/>
       <c r="C115" s="2" t="e">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>#DIV/0!</v>
       </c>
     </row>
@@ -8802,7 +9734,7 @@
       <c r="A116" s="1"/>
       <c r="B116" s="1"/>
       <c r="C116" s="2" t="e">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>#DIV/0!</v>
       </c>
     </row>
@@ -8810,7 +9742,7 @@
       <c r="A117" s="1"/>
       <c r="B117" s="1"/>
       <c r="C117" s="2" t="e">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>#DIV/0!</v>
       </c>
     </row>
@@ -8818,7 +9750,7 @@
       <c r="A118" s="1"/>
       <c r="B118" s="1"/>
       <c r="C118" s="2" t="e">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>#DIV/0!</v>
       </c>
     </row>
@@ -8826,7 +9758,7 @@
       <c r="A119" s="1"/>
       <c r="B119" s="1"/>
       <c r="C119" s="2" t="e">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>#DIV/0!</v>
       </c>
     </row>
@@ -8834,7 +9766,7 @@
       <c r="A120" s="1"/>
       <c r="B120" s="1"/>
       <c r="C120" s="2" t="e">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>#DIV/0!</v>
       </c>
     </row>
@@ -8842,7 +9774,7 @@
       <c r="A121" s="1"/>
       <c r="B121" s="1"/>
       <c r="C121" s="2" t="e">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>#DIV/0!</v>
       </c>
     </row>
@@ -8850,7 +9782,7 @@
       <c r="A122" s="1"/>
       <c r="B122" s="1"/>
       <c r="C122" s="2" t="e">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>#DIV/0!</v>
       </c>
     </row>
@@ -8858,7 +9790,7 @@
       <c r="A123" s="1"/>
       <c r="B123" s="1"/>
       <c r="C123" s="2" t="e">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>#DIV/0!</v>
       </c>
     </row>
@@ -8866,7 +9798,7 @@
       <c r="A124" s="1"/>
       <c r="B124" s="1"/>
       <c r="C124" s="2" t="e">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>#DIV/0!</v>
       </c>
     </row>
@@ -8874,7 +9806,7 @@
       <c r="A125" s="1"/>
       <c r="B125" s="1"/>
       <c r="C125" s="2" t="e">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>#DIV/0!</v>
       </c>
     </row>
@@ -8882,7 +9814,7 @@
       <c r="A126" s="1"/>
       <c r="B126" s="1"/>
       <c r="C126" s="2" t="e">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>#DIV/0!</v>
       </c>
     </row>
@@ -8890,7 +9822,7 @@
       <c r="A127" s="1"/>
       <c r="B127" s="1"/>
       <c r="C127" s="2" t="e">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>#DIV/0!</v>
       </c>
     </row>
@@ -8898,7 +9830,7 @@
       <c r="A128" s="1"/>
       <c r="B128" s="1"/>
       <c r="C128" s="2" t="e">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>#DIV/0!</v>
       </c>
     </row>
@@ -8906,7 +9838,7 @@
       <c r="A129" s="1"/>
       <c r="B129" s="1"/>
       <c r="C129" s="2" t="e">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>#DIV/0!</v>
       </c>
     </row>
@@ -8914,7 +9846,7 @@
       <c r="A130" s="1"/>
       <c r="B130" s="1"/>
       <c r="C130" s="2" t="e">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>#DIV/0!</v>
       </c>
     </row>
@@ -8922,7 +9854,7 @@
       <c r="A131" s="1"/>
       <c r="B131" s="1"/>
       <c r="C131" s="2" t="e">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>#DIV/0!</v>
       </c>
     </row>
@@ -8930,7 +9862,7 @@
       <c r="A132" s="1"/>
       <c r="B132" s="1"/>
       <c r="C132" s="2" t="e">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>#DIV/0!</v>
       </c>
     </row>
@@ -8938,7 +9870,7 @@
       <c r="A133" s="1"/>
       <c r="B133" s="1"/>
       <c r="C133" s="2" t="e">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>#DIV/0!</v>
       </c>
     </row>
@@ -8946,7 +9878,7 @@
       <c r="A134" s="1"/>
       <c r="B134" s="1"/>
       <c r="C134" s="2" t="e">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>#DIV/0!</v>
       </c>
     </row>
@@ -8954,7 +9886,7 @@
       <c r="A135" s="1"/>
       <c r="B135" s="1"/>
       <c r="C135" s="2" t="e">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>#DIV/0!</v>
       </c>
     </row>
@@ -8962,7 +9894,7 @@
       <c r="A136" s="1"/>
       <c r="B136" s="1"/>
       <c r="C136" s="2" t="e">
-        <f t="shared" ref="C136:C137" si="2">(B136-B135)/B135</f>
+        <f t="shared" ref="C136:C137" si="3">(B136-B135)/B135</f>
         <v>#DIV/0!</v>
       </c>
     </row>
@@ -8970,7 +9902,7 @@
       <c r="A137" s="1"/>
       <c r="B137" s="1"/>
       <c r="C137" s="2" t="e">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>#DIV/0!</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Fixed bug with Async::bread() Results were not good.  After over 100 generations the solution is not diverging. Will try running Single-Threaded next to see if this may be a bug in the Multi-threaded section of the code.
</commit_message>
<xml_diff>
--- a/Progress.xlsx
+++ b/Progress.xlsx
@@ -1,21 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21929"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22026"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/c51537410c5afe56/Projects/Source/Repos/EdGarrity/SOS/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="205" documentId="114_{B2D123C0-10CD-4892-A2B1-0D4FB86B9D90}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{B9B71E14-A50C-4D4D-9B1B-AA60A78DE739}"/>
+  <xr:revisionPtr revIDLastSave="232" documentId="114_{B2D123C0-10CD-4892-A2B1-0D4FB86B9D90}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{30F6BED2-5AD4-4FD5-9CDE-CC5A5EB51F82}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="2" xr2:uid="{D7613C25-2959-4D88-A8C3-21B00E74DE47}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="16896" activeTab="3" xr2:uid="{D7613C25-2959-4D88-A8C3-21B00E74DE47}"/>
   </bookViews>
   <sheets>
     <sheet name="Run 1" sheetId="1" r:id="rId1"/>
     <sheet name="Run 2" sheetId="2" r:id="rId2"/>
     <sheet name="Run 3" sheetId="3" r:id="rId3"/>
+    <sheet name="Run 4" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -35,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="8">
   <si>
     <t>BestIndividual_Training_Error</t>
   </si>
@@ -56,6 +57,9 @@
   </si>
   <si>
     <t>R</t>
+  </si>
+  <si>
+    <t>BestIndividual_Training_Score</t>
   </si>
 </sst>
 </file>
@@ -3314,6 +3318,1081 @@
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000001-905B-42CE-B919-4A78BDAA1C3D}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:marker val="1"/>
+        <c:smooth val="0"/>
+        <c:axId val="840836808"/>
+        <c:axId val="840833856"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="715829080"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" cap="none" spc="0" normalizeH="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="715823504"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="715823504"/>
+        <c:scaling>
+          <c:logBase val="10"/>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:minorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="5000"/>
+                  <a:lumOff val="95000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:minorGridlines>
+        <c:numFmt formatCode="#,##0.00" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="715829080"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="840833856"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="r"/>
+        <c:numFmt formatCode="#,##0.00" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="840836808"/>
+        <c:crosses val="max"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:catAx>
+        <c:axId val="840836808"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="1"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="840833856"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="t"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="2000" b="0" i="0" u="none" strike="noStrike" kern="1200" cap="none" spc="0" normalizeH="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mj-lt"/>
+              <a:ea typeface="+mj-ea"/>
+              <a:cs typeface="+mj-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Run 4'!$B$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Average_Training_Error</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="38100" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>'Run 4'!$B$2:$B$137</c:f>
+              <c:numCache>
+                <c:formatCode>#,##0.00</c:formatCode>
+                <c:ptCount val="136"/>
+                <c:pt idx="0">
+                  <c:v>458264118.64827001</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>468580641.17486602</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>456323714.85712302</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>464406247.24860299</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>463442372.98281401</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>464600087.98785597</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>463742437.87246901</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>457555535.338238</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>461931684.70276302</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>448837132.67494398</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>470962425.26152903</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>454560462.827317</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>457398473.99491</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>471972912.66856098</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>464064130.29326397</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>462437791.54583198</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>460870888.976578</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>455320583.34386998</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>452622769.843171</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>459267789.01272202</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>464396344.47628897</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>457685093.91835499</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>462313975.29768401</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>459041509.411479</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>471434073.24250102</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>466303189.19594198</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>459670402.36795503</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>462356542.44878399</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>470772983.09584498</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>460450980.10194701</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>461260348.81571102</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>467736902.25147098</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>469959560.12909901</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>465309424.38307899</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>459274311.25669098</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>369213601.82731497</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>282045369.70910102</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>460810927.73641902</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>273830368.73894</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>464180580.27104902</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>470791047.23541898</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>451043875.211752</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>395461478.798724</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>455476483.68107402</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>394657646.57950401</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>454076630.949265</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>490399995.67273003</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>456182479.90430999</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>314024876.822227</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>460587525.91592199</c:v>
+                </c:pt>
+                <c:pt idx="50">
+                  <c:v>344839513.59429401</c:v>
+                </c:pt>
+                <c:pt idx="51">
+                  <c:v>459003700.75477999</c:v>
+                </c:pt>
+                <c:pt idx="52">
+                  <c:v>336789347.886352</c:v>
+                </c:pt>
+                <c:pt idx="53">
+                  <c:v>471506749.81214303</c:v>
+                </c:pt>
+                <c:pt idx="54">
+                  <c:v>372803704.890212</c:v>
+                </c:pt>
+                <c:pt idx="55">
+                  <c:v>459875754.48590398</c:v>
+                </c:pt>
+                <c:pt idx="56">
+                  <c:v>391491515.76593399</c:v>
+                </c:pt>
+                <c:pt idx="57">
+                  <c:v>463997687.08984101</c:v>
+                </c:pt>
+                <c:pt idx="58">
+                  <c:v>565512396.99179697</c:v>
+                </c:pt>
+                <c:pt idx="59">
+                  <c:v>450422884.00208902</c:v>
+                </c:pt>
+                <c:pt idx="60">
+                  <c:v>303164850.88721901</c:v>
+                </c:pt>
+                <c:pt idx="61">
+                  <c:v>453405538.00455701</c:v>
+                </c:pt>
+                <c:pt idx="62">
+                  <c:v>440214396.84135097</c:v>
+                </c:pt>
+                <c:pt idx="63">
+                  <c:v>460009397.09041899</c:v>
+                </c:pt>
+                <c:pt idx="64">
+                  <c:v>449654781.93667901</c:v>
+                </c:pt>
+                <c:pt idx="65">
+                  <c:v>468860564.89174098</c:v>
+                </c:pt>
+                <c:pt idx="66">
+                  <c:v>360547624.572236</c:v>
+                </c:pt>
+                <c:pt idx="67">
+                  <c:v>456657488.79168302</c:v>
+                </c:pt>
+                <c:pt idx="68">
+                  <c:v>394247504.42309397</c:v>
+                </c:pt>
+                <c:pt idx="69">
+                  <c:v>461257679.44627899</c:v>
+                </c:pt>
+                <c:pt idx="70">
+                  <c:v>649270885.81862795</c:v>
+                </c:pt>
+                <c:pt idx="71">
+                  <c:v>475932652.15538901</c:v>
+                </c:pt>
+                <c:pt idx="72">
+                  <c:v>379195512.090536</c:v>
+                </c:pt>
+                <c:pt idx="73">
+                  <c:v>466105743.98999602</c:v>
+                </c:pt>
+                <c:pt idx="74">
+                  <c:v>327314452.83603698</c:v>
+                </c:pt>
+                <c:pt idx="75">
+                  <c:v>470887650.431934</c:v>
+                </c:pt>
+                <c:pt idx="76">
+                  <c:v>338176782.41906101</c:v>
+                </c:pt>
+                <c:pt idx="77">
+                  <c:v>462520119.50717402</c:v>
+                </c:pt>
+                <c:pt idx="78">
+                  <c:v>442127742.83230501</c:v>
+                </c:pt>
+                <c:pt idx="79">
+                  <c:v>465619690.62842399</c:v>
+                </c:pt>
+                <c:pt idx="80">
+                  <c:v>355219026.69835401</c:v>
+                </c:pt>
+                <c:pt idx="81">
+                  <c:v>453947127.69318998</c:v>
+                </c:pt>
+                <c:pt idx="82">
+                  <c:v>403757564.49089301</c:v>
+                </c:pt>
+                <c:pt idx="83">
+                  <c:v>466919005.73879099</c:v>
+                </c:pt>
+                <c:pt idx="84">
+                  <c:v>370240113.23619199</c:v>
+                </c:pt>
+                <c:pt idx="85">
+                  <c:v>463936015.50753498</c:v>
+                </c:pt>
+                <c:pt idx="86">
+                  <c:v>410966659.01073098</c:v>
+                </c:pt>
+                <c:pt idx="87">
+                  <c:v>462538415.77899599</c:v>
+                </c:pt>
+                <c:pt idx="88">
+                  <c:v>410989219.61114299</c:v>
+                </c:pt>
+                <c:pt idx="89">
+                  <c:v>472829360.12418401</c:v>
+                </c:pt>
+                <c:pt idx="90">
+                  <c:v>382521658.53837699</c:v>
+                </c:pt>
+                <c:pt idx="91">
+                  <c:v>465080372.56080002</c:v>
+                </c:pt>
+                <c:pt idx="92">
+                  <c:v>402680713.03811902</c:v>
+                </c:pt>
+                <c:pt idx="93">
+                  <c:v>467611083.37385899</c:v>
+                </c:pt>
+                <c:pt idx="94">
+                  <c:v>594101022.57497001</c:v>
+                </c:pt>
+                <c:pt idx="95">
+                  <c:v>461128200.135019</c:v>
+                </c:pt>
+                <c:pt idx="96">
+                  <c:v>334958300.02285302</c:v>
+                </c:pt>
+                <c:pt idx="97">
+                  <c:v>450782974.39281303</c:v>
+                </c:pt>
+                <c:pt idx="98">
+                  <c:v>561048022.84938097</c:v>
+                </c:pt>
+                <c:pt idx="99">
+                  <c:v>466743717.44507301</c:v>
+                </c:pt>
+                <c:pt idx="100">
+                  <c:v>402492900.77467102</c:v>
+                </c:pt>
+                <c:pt idx="101">
+                  <c:v>464672887.65058398</c:v>
+                </c:pt>
+                <c:pt idx="102">
+                  <c:v>614131227.63888395</c:v>
+                </c:pt>
+                <c:pt idx="103">
+                  <c:v>467870838.564138</c:v>
+                </c:pt>
+                <c:pt idx="104">
+                  <c:v>476778088.87384099</c:v>
+                </c:pt>
+                <c:pt idx="105">
+                  <c:v>459821252.49602401</c:v>
+                </c:pt>
+                <c:pt idx="106">
+                  <c:v>286785776.35218298</c:v>
+                </c:pt>
+                <c:pt idx="107">
+                  <c:v>463648613.67455602</c:v>
+                </c:pt>
+                <c:pt idx="108">
+                  <c:v>468214436.74031198</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-7CE4-49D1-9475-DF23D8AD236E}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:marker val="1"/>
+        <c:smooth val="0"/>
+        <c:axId val="715829080"/>
+        <c:axId val="715823504"/>
+      </c:lineChart>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Run 4'!$A$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>BestIndividual_Training_Score</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="38100" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>'Run 4'!$A$2:$A$137</c:f>
+              <c:numCache>
+                <c:formatCode>#,##0.00</c:formatCode>
+                <c:ptCount val="136"/>
+                <c:pt idx="0">
+                  <c:v>0.9</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.9</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.9</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.9</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.9</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.9</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.9</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.9</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.9</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.9</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0.9</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0.9</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>0.9</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>0.9</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>0.9</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>0.9</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>0.9</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>0.9</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>0.9</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>0.9</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>0.9</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>0.9</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>0.9</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>0.9</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>0.9</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>0.9</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>0.9</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>0.9</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>0.9</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>0.9</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>0.9</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>0.9</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>0.9</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>0.9</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>0.9</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>0.9</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>0.9</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>0.9</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>0.9</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>0.9</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>0.9</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>0.9</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>0.9</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>0.9</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>0.9</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>0.9</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>0.9</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>0.9</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>0.9</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>0.9</c:v>
+                </c:pt>
+                <c:pt idx="50">
+                  <c:v>0.9</c:v>
+                </c:pt>
+                <c:pt idx="51">
+                  <c:v>0.9</c:v>
+                </c:pt>
+                <c:pt idx="52">
+                  <c:v>0.9</c:v>
+                </c:pt>
+                <c:pt idx="53">
+                  <c:v>0.9</c:v>
+                </c:pt>
+                <c:pt idx="54">
+                  <c:v>0.9</c:v>
+                </c:pt>
+                <c:pt idx="55">
+                  <c:v>0.9</c:v>
+                </c:pt>
+                <c:pt idx="56">
+                  <c:v>0.9</c:v>
+                </c:pt>
+                <c:pt idx="57">
+                  <c:v>0.9</c:v>
+                </c:pt>
+                <c:pt idx="58">
+                  <c:v>0.9</c:v>
+                </c:pt>
+                <c:pt idx="59">
+                  <c:v>0.9</c:v>
+                </c:pt>
+                <c:pt idx="60">
+                  <c:v>0.9</c:v>
+                </c:pt>
+                <c:pt idx="61">
+                  <c:v>0.9</c:v>
+                </c:pt>
+                <c:pt idx="62">
+                  <c:v>0.9</c:v>
+                </c:pt>
+                <c:pt idx="63">
+                  <c:v>0.9</c:v>
+                </c:pt>
+                <c:pt idx="64">
+                  <c:v>0.9</c:v>
+                </c:pt>
+                <c:pt idx="65">
+                  <c:v>0.9</c:v>
+                </c:pt>
+                <c:pt idx="66">
+                  <c:v>0.9</c:v>
+                </c:pt>
+                <c:pt idx="67">
+                  <c:v>0.9</c:v>
+                </c:pt>
+                <c:pt idx="68">
+                  <c:v>0.9</c:v>
+                </c:pt>
+                <c:pt idx="69">
+                  <c:v>0.9</c:v>
+                </c:pt>
+                <c:pt idx="70">
+                  <c:v>0.9</c:v>
+                </c:pt>
+                <c:pt idx="71">
+                  <c:v>0.9</c:v>
+                </c:pt>
+                <c:pt idx="72">
+                  <c:v>0.9</c:v>
+                </c:pt>
+                <c:pt idx="73">
+                  <c:v>0.9</c:v>
+                </c:pt>
+                <c:pt idx="74">
+                  <c:v>0.9</c:v>
+                </c:pt>
+                <c:pt idx="75">
+                  <c:v>0.9</c:v>
+                </c:pt>
+                <c:pt idx="76">
+                  <c:v>0.9</c:v>
+                </c:pt>
+                <c:pt idx="77">
+                  <c:v>0.9</c:v>
+                </c:pt>
+                <c:pt idx="78">
+                  <c:v>0.9</c:v>
+                </c:pt>
+                <c:pt idx="79">
+                  <c:v>0.9</c:v>
+                </c:pt>
+                <c:pt idx="80">
+                  <c:v>0.9</c:v>
+                </c:pt>
+                <c:pt idx="81">
+                  <c:v>0.9</c:v>
+                </c:pt>
+                <c:pt idx="82">
+                  <c:v>0.9</c:v>
+                </c:pt>
+                <c:pt idx="83">
+                  <c:v>0.9</c:v>
+                </c:pt>
+                <c:pt idx="84">
+                  <c:v>0.9</c:v>
+                </c:pt>
+                <c:pt idx="85">
+                  <c:v>0.9</c:v>
+                </c:pt>
+                <c:pt idx="86">
+                  <c:v>0.9</c:v>
+                </c:pt>
+                <c:pt idx="87">
+                  <c:v>0.9</c:v>
+                </c:pt>
+                <c:pt idx="88">
+                  <c:v>0.9</c:v>
+                </c:pt>
+                <c:pt idx="89">
+                  <c:v>0.9</c:v>
+                </c:pt>
+                <c:pt idx="90">
+                  <c:v>0.9</c:v>
+                </c:pt>
+                <c:pt idx="91">
+                  <c:v>0.9</c:v>
+                </c:pt>
+                <c:pt idx="92">
+                  <c:v>0.9</c:v>
+                </c:pt>
+                <c:pt idx="93">
+                  <c:v>0.9</c:v>
+                </c:pt>
+                <c:pt idx="94">
+                  <c:v>0.9</c:v>
+                </c:pt>
+                <c:pt idx="95">
+                  <c:v>0.9</c:v>
+                </c:pt>
+                <c:pt idx="96">
+                  <c:v>0.9</c:v>
+                </c:pt>
+                <c:pt idx="97">
+                  <c:v>0.9</c:v>
+                </c:pt>
+                <c:pt idx="98">
+                  <c:v>0.9</c:v>
+                </c:pt>
+                <c:pt idx="99">
+                  <c:v>0.9</c:v>
+                </c:pt>
+                <c:pt idx="100">
+                  <c:v>0.9</c:v>
+                </c:pt>
+                <c:pt idx="101">
+                  <c:v>0.9</c:v>
+                </c:pt>
+                <c:pt idx="102">
+                  <c:v>0.9</c:v>
+                </c:pt>
+                <c:pt idx="103">
+                  <c:v>0.9</c:v>
+                </c:pt>
+                <c:pt idx="104">
+                  <c:v>0.9</c:v>
+                </c:pt>
+                <c:pt idx="105">
+                  <c:v>0.9</c:v>
+                </c:pt>
+                <c:pt idx="106">
+                  <c:v>0.9</c:v>
+                </c:pt>
+                <c:pt idx="107">
+                  <c:v>0.9</c:v>
+                </c:pt>
+                <c:pt idx="108">
+                  <c:v>0.9</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-7CE4-49D1-9475-DF23D8AD236E}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -3669,6 +4748,46 @@
 </file>
 
 <file path=xl/charts/colors3.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors4.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
   <a:schemeClr val="accent2"/>
@@ -5208,6 +6327,506 @@
 </cs:chartStyle>
 </file>
 
+<file path=xl/charts/style4.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="235">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200" cap="all"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" b="0" kern="1200" cap="none" spc="0" normalizeH="0" baseline="0"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="38100" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="8"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:prstDash val="dash"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:prstDash val="dash"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="major">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="2000" b="0" kern="1200" cap="none" spc="0" normalizeH="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
@@ -5313,6 +6932,49 @@
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
               <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{9A251193-1AF6-4837-BCA5-854F267B1B1A}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing4.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>561975</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>30</xdr:col>
+      <xdr:colOff>409575</xdr:colOff>
+      <xdr:row>37</xdr:row>
+      <xdr:rowOff>19050</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{6677EAB1-3090-4CC8-A23D-EB7582065BD0}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -8360,7 +10022,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FD3AD4D7-7506-4E58-8F31-A8ACAD68134E}">
   <dimension ref="A1:D137"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
       <selection activeCell="A16" sqref="A16"/>
     </sheetView>
   </sheetViews>
@@ -9911,4 +11573,1560 @@
   <pageSetup orientation="portrait" r:id="rId1"/>
   <drawing r:id="rId2"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{46279A08-E6DD-4519-895C-48ADC6AEC5C3}">
+  <dimension ref="A1:D137"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="B1" sqref="B1:B110"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="27.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="22.109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="8.88671875" style="2"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A2" s="1">
+        <v>0.9</v>
+      </c>
+      <c r="B2" s="1">
+        <v>458264118.64827001</v>
+      </c>
+      <c r="D2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A3" s="1">
+        <v>0.9</v>
+      </c>
+      <c r="B3" s="1">
+        <v>468580641.17486602</v>
+      </c>
+      <c r="C3" s="2">
+        <f>(B3-B2)/B2</f>
+        <v>2.2512176072231868E-2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A4" s="1">
+        <v>0.9</v>
+      </c>
+      <c r="B4" s="1">
+        <v>456323714.85712302</v>
+      </c>
+      <c r="C4" s="2">
+        <f t="shared" ref="C4:C71" si="0">(B4-B3)/B3</f>
+        <v>-2.6157560173658421E-2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A5" s="1">
+        <v>0.9</v>
+      </c>
+      <c r="B5" s="1">
+        <v>464406247.24860299</v>
+      </c>
+      <c r="C5" s="2">
+        <f t="shared" si="0"/>
+        <v>1.7712277771955477E-2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A6" s="1">
+        <v>0.9</v>
+      </c>
+      <c r="B6" s="1">
+        <v>463442372.98281401</v>
+      </c>
+      <c r="C6" s="2">
+        <f t="shared" si="0"/>
+        <v>-2.0754980612330077E-3</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A7" s="1">
+        <v>0.9</v>
+      </c>
+      <c r="B7" s="1">
+        <v>464600087.98785597</v>
+      </c>
+      <c r="C7" s="2">
+        <f t="shared" si="0"/>
+        <v>2.4980775874908806E-3</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A8" s="1">
+        <v>0.9</v>
+      </c>
+      <c r="B8" s="1">
+        <v>463742437.87246901</v>
+      </c>
+      <c r="C8" s="2">
+        <f t="shared" si="0"/>
+        <v>-1.8459964549326145E-3</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A9" s="1">
+        <v>0.9</v>
+      </c>
+      <c r="B9" s="1">
+        <v>457555535.338238</v>
+      </c>
+      <c r="C9" s="2">
+        <f t="shared" si="0"/>
+        <v>-1.3341247272117092E-2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A10" s="1">
+        <v>0.9</v>
+      </c>
+      <c r="B10" s="1">
+        <v>461931684.70276302</v>
+      </c>
+      <c r="C10" s="2">
+        <f t="shared" si="0"/>
+        <v>9.564192817140868E-3</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A11" s="1">
+        <v>0.9</v>
+      </c>
+      <c r="B11" s="1">
+        <v>448837132.67494398</v>
+      </c>
+      <c r="C11" s="2">
+        <f t="shared" si="0"/>
+        <v>-2.8347377894731178E-2</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A12" s="1">
+        <v>0.9</v>
+      </c>
+      <c r="B12" s="1">
+        <v>470962425.26152903</v>
+      </c>
+      <c r="C12" s="2">
+        <f t="shared" si="0"/>
+        <v>4.9294701743424124E-2</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A13" s="1">
+        <v>0.9</v>
+      </c>
+      <c r="B13" s="1">
+        <v>454560462.827317</v>
+      </c>
+      <c r="C13" s="2">
+        <f t="shared" si="0"/>
+        <v>-3.4826477770713647E-2</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A14" s="1">
+        <v>0.9</v>
+      </c>
+      <c r="B14" s="1">
+        <v>457398473.99491</v>
+      </c>
+      <c r="C14" s="2">
+        <f t="shared" si="0"/>
+        <v>6.2434184221409825E-3</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A15" s="1">
+        <v>0.9</v>
+      </c>
+      <c r="B15" s="1">
+        <v>471972912.66856098</v>
+      </c>
+      <c r="C15" s="2">
+        <f t="shared" si="0"/>
+        <v>3.1863767594933354E-2</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A16" s="1">
+        <v>0.9</v>
+      </c>
+      <c r="B16" s="1">
+        <v>464064130.29326397</v>
+      </c>
+      <c r="C16" s="2">
+        <f t="shared" si="0"/>
+        <v>-1.6756856512337364E-2</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A17" s="1">
+        <v>0.9</v>
+      </c>
+      <c r="B17" s="1">
+        <v>462437791.54583198</v>
+      </c>
+      <c r="C17" s="2">
+        <f t="shared" si="0"/>
+        <v>-3.5045560328143301E-3</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A18" s="1">
+        <v>0.9</v>
+      </c>
+      <c r="B18" s="1">
+        <v>460870888.976578</v>
+      </c>
+      <c r="C18" s="2">
+        <f t="shared" si="0"/>
+        <v>-3.3883531966886972E-3</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A19" s="1">
+        <v>0.9</v>
+      </c>
+      <c r="B19" s="1">
+        <v>455320583.34386998</v>
+      </c>
+      <c r="C19" s="2">
+        <f t="shared" si="0"/>
+        <v>-1.2043081404063441E-2</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A20" s="1">
+        <v>0.9</v>
+      </c>
+      <c r="B20" s="1">
+        <v>452622769.843171</v>
+      </c>
+      <c r="C20" s="2">
+        <f t="shared" si="0"/>
+        <v>-5.9250857514199498E-3</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A21" s="1">
+        <v>0.9</v>
+      </c>
+      <c r="B21" s="1">
+        <v>459267789.01272202</v>
+      </c>
+      <c r="C21" s="2">
+        <f t="shared" si="0"/>
+        <v>1.4681142028832186E-2</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A22" s="1">
+        <v>0.9</v>
+      </c>
+      <c r="B22" s="1">
+        <v>464396344.47628897</v>
+      </c>
+      <c r="C22" s="2">
+        <f t="shared" si="0"/>
+        <v>1.1166808529271568E-2</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A23" s="1">
+        <v>0.9</v>
+      </c>
+      <c r="B23" s="1">
+        <v>457685093.91835499</v>
+      </c>
+      <c r="C23" s="2">
+        <f t="shared" si="0"/>
+        <v>-1.4451557678608401E-2</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A24" s="1">
+        <v>0.9</v>
+      </c>
+      <c r="B24" s="1">
+        <v>462313975.29768401</v>
+      </c>
+      <c r="C24" s="2">
+        <f t="shared" si="0"/>
+        <v>1.0113681745018241E-2</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A25" s="1">
+        <v>0.9</v>
+      </c>
+      <c r="B25" s="1">
+        <v>459041509.411479</v>
+      </c>
+      <c r="C25" s="2">
+        <f t="shared" si="0"/>
+        <v>-7.0784489785277989E-3</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A26" s="1">
+        <v>0.9</v>
+      </c>
+      <c r="B26" s="1">
+        <v>471434073.24250102</v>
+      </c>
+      <c r="C26" s="2">
+        <f t="shared" si="0"/>
+        <v>2.6996608317426663E-2</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A27" s="1">
+        <v>0.9</v>
+      </c>
+      <c r="B27" s="1">
+        <v>466303189.19594198</v>
+      </c>
+      <c r="C27" s="2">
+        <f t="shared" si="0"/>
+        <v>-1.0883566415276394E-2</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A28" s="1">
+        <v>0.9</v>
+      </c>
+      <c r="B28" s="1">
+        <v>459670402.36795503</v>
+      </c>
+      <c r="C28" s="2">
+        <f t="shared" si="0"/>
+        <v>-1.4224193575480435E-2</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A29" s="1">
+        <v>0.9</v>
+      </c>
+      <c r="B29" s="1">
+        <v>462356542.44878399</v>
+      </c>
+      <c r="C29" s="2">
+        <f t="shared" si="0"/>
+        <v>5.8436220104482054E-3</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A30" s="1">
+        <v>0.9</v>
+      </c>
+      <c r="B30" s="1">
+        <v>470772983.09584498</v>
+      </c>
+      <c r="C30" s="2">
+        <f t="shared" si="0"/>
+        <v>1.820335579655671E-2</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A31" s="1">
+        <v>0.9</v>
+      </c>
+      <c r="B31" s="1">
+        <v>460450980.10194701</v>
+      </c>
+      <c r="C31" s="2">
+        <f t="shared" si="0"/>
+        <v>-2.1925648591853263E-2</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A32" s="1">
+        <v>0.9</v>
+      </c>
+      <c r="B32" s="1">
+        <v>461260348.81571102</v>
+      </c>
+      <c r="C32" s="2">
+        <f>(B32-B30)/B30</f>
+        <v>-2.0206415027425817E-2</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A33" s="1">
+        <v>0.9</v>
+      </c>
+      <c r="B33" s="1">
+        <v>467736902.25147098</v>
+      </c>
+      <c r="C33" s="2">
+        <f t="shared" si="0"/>
+        <v>1.4040993231671777E-2</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A34" s="1">
+        <v>0.9</v>
+      </c>
+      <c r="B34" s="1">
+        <v>469959560.12909901</v>
+      </c>
+      <c r="C34" s="2">
+        <f t="shared" si="0"/>
+        <v>4.7519403898413247E-3</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A35" s="1">
+        <v>0.9</v>
+      </c>
+      <c r="B35" s="1">
+        <v>465309424.38307899</v>
+      </c>
+      <c r="C35" s="2">
+        <f t="shared" si="0"/>
+        <v>-9.8947572100514681E-3</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A36" s="1">
+        <v>0.9</v>
+      </c>
+      <c r="B36" s="1">
+        <v>459274311.25669098</v>
+      </c>
+      <c r="C36" s="2">
+        <f t="shared" si="0"/>
+        <v>-1.2970107223573958E-2</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A37" s="1">
+        <v>0.9</v>
+      </c>
+      <c r="B37" s="1">
+        <v>369213601.82731497</v>
+      </c>
+      <c r="C37" s="2">
+        <f t="shared" si="0"/>
+        <v>-0.1960935049533841</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A38" s="1">
+        <v>0.9</v>
+      </c>
+      <c r="B38" s="1">
+        <v>282045369.70910102</v>
+      </c>
+      <c r="C38" s="2">
+        <f t="shared" si="0"/>
+        <v>-0.23609160574475108</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A39" s="1">
+        <v>0.9</v>
+      </c>
+      <c r="B39" s="1">
+        <v>460810927.73641902</v>
+      </c>
+      <c r="C39" s="2">
+        <f t="shared" si="0"/>
+        <v>0.63381844634320761</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A40" s="1">
+        <v>0.9</v>
+      </c>
+      <c r="B40" s="1">
+        <v>273830368.73894</v>
+      </c>
+      <c r="C40" s="2">
+        <f t="shared" si="0"/>
+        <v>-0.4057641599689466</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A41" s="1">
+        <v>0.9</v>
+      </c>
+      <c r="B41" s="1">
+        <v>464180580.27104902</v>
+      </c>
+      <c r="C41" s="2">
+        <f t="shared" si="0"/>
+        <v>0.69513915643732727</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A42" s="1">
+        <v>0.9</v>
+      </c>
+      <c r="B42" s="1">
+        <v>470791047.23541898</v>
+      </c>
+      <c r="C42" s="2">
+        <f t="shared" si="0"/>
+        <v>1.4241153648672468E-2</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A43" s="1">
+        <v>0.9</v>
+      </c>
+      <c r="B43" s="1">
+        <v>451043875.211752</v>
+      </c>
+      <c r="C43" s="2">
+        <f t="shared" si="0"/>
+        <v>-4.1944663433228814E-2</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A44" s="1">
+        <v>0.9</v>
+      </c>
+      <c r="B44" s="1">
+        <v>395461478.798724</v>
+      </c>
+      <c r="C44" s="2">
+        <f t="shared" si="0"/>
+        <v>-0.12323057571047535</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A45" s="1">
+        <v>0.9</v>
+      </c>
+      <c r="B45" s="1">
+        <v>455476483.68107402</v>
+      </c>
+      <c r="C45" s="2">
+        <f t="shared" si="0"/>
+        <v>0.15175942057531111</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A46" s="1">
+        <v>0.9</v>
+      </c>
+      <c r="B46" s="1">
+        <v>394657646.57950401</v>
+      </c>
+      <c r="C46" s="2">
+        <f t="shared" si="0"/>
+        <v>-0.13352794113549787</v>
+      </c>
+    </row>
+    <row r="47" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A47" s="1">
+        <v>0.9</v>
+      </c>
+      <c r="B47" s="1">
+        <v>454076630.949265</v>
+      </c>
+      <c r="C47" s="2">
+        <f t="shared" si="0"/>
+        <v>0.15055830004750967</v>
+      </c>
+    </row>
+    <row r="48" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A48" s="1">
+        <v>0.9</v>
+      </c>
+      <c r="B48" s="1">
+        <v>490399995.67273003</v>
+      </c>
+      <c r="C48" s="2">
+        <f t="shared" si="0"/>
+        <v>7.9993909062286706E-2</v>
+      </c>
+    </row>
+    <row r="49" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A49" s="1">
+        <v>0.9</v>
+      </c>
+      <c r="B49" s="1">
+        <v>456182479.90430999</v>
+      </c>
+      <c r="C49" s="2">
+        <f t="shared" si="0"/>
+        <v>-6.9774706505615888E-2</v>
+      </c>
+    </row>
+    <row r="50" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A50" s="1">
+        <v>0.9</v>
+      </c>
+      <c r="B50" s="1">
+        <v>314024876.822227</v>
+      </c>
+      <c r="C50" s="2">
+        <f t="shared" si="0"/>
+        <v>-0.31162442519033684</v>
+      </c>
+    </row>
+    <row r="51" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A51" s="1">
+        <v>0.9</v>
+      </c>
+      <c r="B51" s="1">
+        <v>460587525.91592199</v>
+      </c>
+      <c r="C51" s="2">
+        <f t="shared" si="0"/>
+        <v>0.46672305257097751</v>
+      </c>
+    </row>
+    <row r="52" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A52" s="1">
+        <v>0.9</v>
+      </c>
+      <c r="B52" s="1">
+        <v>344839513.59429401</v>
+      </c>
+      <c r="C52" s="2">
+        <f t="shared" si="0"/>
+        <v>-0.2513051392163782</v>
+      </c>
+    </row>
+    <row r="53" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A53" s="1">
+        <v>0.9</v>
+      </c>
+      <c r="B53" s="1">
+        <v>459003700.75477999</v>
+      </c>
+      <c r="C53" s="2">
+        <f t="shared" si="0"/>
+        <v>0.33106469142860734</v>
+      </c>
+    </row>
+    <row r="54" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A54" s="1">
+        <v>0.9</v>
+      </c>
+      <c r="B54" s="1">
+        <v>336789347.886352</v>
+      </c>
+      <c r="C54" s="2">
+        <f t="shared" si="0"/>
+        <v>-0.26626005992426688</v>
+      </c>
+    </row>
+    <row r="55" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A55" s="1">
+        <v>0.9</v>
+      </c>
+      <c r="B55" s="1">
+        <v>471506749.81214303</v>
+      </c>
+      <c r="C55" s="2">
+        <f t="shared" si="0"/>
+        <v>0.40000493712541879</v>
+      </c>
+    </row>
+    <row r="56" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A56" s="1">
+        <v>0.9</v>
+      </c>
+      <c r="B56" s="1">
+        <v>372803704.890212</v>
+      </c>
+      <c r="C56" s="2">
+        <f t="shared" si="0"/>
+        <v>-0.20933538058841392</v>
+      </c>
+    </row>
+    <row r="57" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A57" s="1">
+        <v>0.9</v>
+      </c>
+      <c r="B57" s="1">
+        <v>459875754.48590398</v>
+      </c>
+      <c r="C57" s="2">
+        <f t="shared" si="0"/>
+        <v>0.23356004367320884</v>
+      </c>
+    </row>
+    <row r="58" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A58" s="1">
+        <v>0.9</v>
+      </c>
+      <c r="B58" s="1">
+        <v>391491515.76593399</v>
+      </c>
+      <c r="C58" s="2">
+        <f t="shared" si="0"/>
+        <v>-0.14870155265397034</v>
+      </c>
+    </row>
+    <row r="59" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A59" s="1">
+        <v>0.9</v>
+      </c>
+      <c r="B59" s="1">
+        <v>463997687.08984101</v>
+      </c>
+      <c r="C59" s="2">
+        <f t="shared" si="0"/>
+        <v>0.18520496205914511</v>
+      </c>
+    </row>
+    <row r="60" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A60" s="1">
+        <v>0.9</v>
+      </c>
+      <c r="B60" s="1">
+        <v>565512396.99179697</v>
+      </c>
+      <c r="C60" s="2">
+        <f t="shared" si="0"/>
+        <v>0.218782792945906</v>
+      </c>
+    </row>
+    <row r="61" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A61" s="1">
+        <v>0.9</v>
+      </c>
+      <c r="B61" s="1">
+        <v>450422884.00208902</v>
+      </c>
+      <c r="C61" s="2">
+        <f t="shared" si="0"/>
+        <v>-0.20351368705959133</v>
+      </c>
+    </row>
+    <row r="62" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A62" s="1">
+        <v>0.9</v>
+      </c>
+      <c r="B62" s="1">
+        <v>303164850.88721901</v>
+      </c>
+      <c r="C62" s="2">
+        <f t="shared" si="0"/>
+        <v>-0.32693284099257053</v>
+      </c>
+    </row>
+    <row r="63" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A63" s="1">
+        <v>0.9</v>
+      </c>
+      <c r="B63" s="1">
+        <v>453405538.00455701</v>
+      </c>
+      <c r="C63" s="2">
+        <f t="shared" si="0"/>
+        <v>0.49557422860089195</v>
+      </c>
+    </row>
+    <row r="64" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A64" s="1">
+        <v>0.9</v>
+      </c>
+      <c r="B64" s="1">
+        <v>440214396.84135097</v>
+      </c>
+      <c r="C64" s="2">
+        <f t="shared" si="0"/>
+        <v>-2.9093471644083584E-2</v>
+      </c>
+    </row>
+    <row r="65" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A65" s="1">
+        <v>0.9</v>
+      </c>
+      <c r="B65" s="1">
+        <v>460009397.09041899</v>
+      </c>
+      <c r="C65" s="2">
+        <f t="shared" si="0"/>
+        <v>4.4966726193196152E-2</v>
+      </c>
+    </row>
+    <row r="66" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A66" s="1">
+        <v>0.9</v>
+      </c>
+      <c r="B66" s="1">
+        <v>449654781.93667901</v>
+      </c>
+      <c r="C66" s="2">
+        <f t="shared" si="0"/>
+        <v>-2.2509573107056976E-2</v>
+      </c>
+    </row>
+    <row r="67" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A67" s="1">
+        <v>0.9</v>
+      </c>
+      <c r="B67" s="1">
+        <v>468860564.89174098</v>
+      </c>
+      <c r="C67" s="2">
+        <f t="shared" si="0"/>
+        <v>4.2712284460407576E-2</v>
+      </c>
+    </row>
+    <row r="68" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A68" s="1">
+        <v>0.9</v>
+      </c>
+      <c r="B68" s="1">
+        <v>360547624.572236</v>
+      </c>
+      <c r="C68" s="2">
+        <f t="shared" si="0"/>
+        <v>-0.23101311654247192</v>
+      </c>
+    </row>
+    <row r="69" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A69" s="1">
+        <v>0.9</v>
+      </c>
+      <c r="B69" s="1">
+        <v>456657488.79168302</v>
+      </c>
+      <c r="C69" s="2">
+        <f t="shared" si="0"/>
+        <v>0.26656634982264688</v>
+      </c>
+    </row>
+    <row r="70" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A70" s="1">
+        <v>0.9</v>
+      </c>
+      <c r="B70" s="1">
+        <v>394247504.42309397</v>
+      </c>
+      <c r="C70" s="2">
+        <f t="shared" si="0"/>
+        <v>-0.1366669460162058</v>
+      </c>
+    </row>
+    <row r="71" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A71" s="1">
+        <v>0.9</v>
+      </c>
+      <c r="B71" s="1">
+        <v>461257679.44627899</v>
+      </c>
+      <c r="C71" s="2">
+        <f t="shared" si="0"/>
+        <v>0.1699698140670329</v>
+      </c>
+    </row>
+    <row r="72" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A72" s="1">
+        <v>0.9</v>
+      </c>
+      <c r="B72" s="1">
+        <v>649270885.81862795</v>
+      </c>
+      <c r="C72" s="2">
+        <f t="shared" ref="C72:C135" si="1">(B72-B71)/B71</f>
+        <v>0.4076099212007725</v>
+      </c>
+    </row>
+    <row r="73" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A73" s="1">
+        <v>0.9</v>
+      </c>
+      <c r="B73" s="1">
+        <v>475932652.15538901</v>
+      </c>
+      <c r="C73" s="2">
+        <f t="shared" si="1"/>
+        <v>-0.2669736737766808</v>
+      </c>
+    </row>
+    <row r="74" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A74" s="1">
+        <v>0.9</v>
+      </c>
+      <c r="B74" s="1">
+        <v>379195512.090536</v>
+      </c>
+      <c r="C74" s="2">
+        <f t="shared" si="1"/>
+        <v>-0.20325804423536156</v>
+      </c>
+    </row>
+    <row r="75" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A75" s="1">
+        <v>0.9</v>
+      </c>
+      <c r="B75" s="1">
+        <v>466105743.98999602</v>
+      </c>
+      <c r="C75" s="2">
+        <f t="shared" si="1"/>
+        <v>0.22919636210965888</v>
+      </c>
+    </row>
+    <row r="76" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A76" s="1">
+        <v>0.9</v>
+      </c>
+      <c r="B76" s="1">
+        <v>327314452.83603698</v>
+      </c>
+      <c r="C76" s="2">
+        <f t="shared" si="1"/>
+        <v>-0.29776781973520994</v>
+      </c>
+    </row>
+    <row r="77" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A77" s="1">
+        <v>0.9</v>
+      </c>
+      <c r="B77" s="1">
+        <v>470887650.431934</v>
+      </c>
+      <c r="C77" s="2">
+        <f t="shared" si="1"/>
+        <v>0.43863995723958377</v>
+      </c>
+    </row>
+    <row r="78" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A78" s="1">
+        <v>0.9</v>
+      </c>
+      <c r="B78" s="1">
+        <v>338176782.41906101</v>
+      </c>
+      <c r="C78" s="2">
+        <f t="shared" si="1"/>
+        <v>-0.28183127735700964</v>
+      </c>
+    </row>
+    <row r="79" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A79" s="1">
+        <v>0.9</v>
+      </c>
+      <c r="B79" s="1">
+        <v>462520119.50717402</v>
+      </c>
+      <c r="C79" s="2">
+        <f t="shared" si="1"/>
+        <v>0.36768738586562566</v>
+      </c>
+    </row>
+    <row r="80" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A80" s="1">
+        <v>0.9</v>
+      </c>
+      <c r="B80" s="1">
+        <v>442127742.83230501</v>
+      </c>
+      <c r="C80" s="2">
+        <f t="shared" si="1"/>
+        <v>-4.4089707268513106E-2</v>
+      </c>
+    </row>
+    <row r="81" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A81" s="1">
+        <v>0.9</v>
+      </c>
+      <c r="B81" s="1">
+        <v>465619690.62842399</v>
+      </c>
+      <c r="C81" s="2">
+        <f t="shared" si="1"/>
+        <v>5.313384689598466E-2</v>
+      </c>
+    </row>
+    <row r="82" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A82" s="1">
+        <v>0.9</v>
+      </c>
+      <c r="B82" s="1">
+        <v>355219026.69835401</v>
+      </c>
+      <c r="C82" s="2">
+        <f t="shared" si="1"/>
+        <v>-0.23710480066052972</v>
+      </c>
+    </row>
+    <row r="83" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A83" s="1">
+        <v>0.9</v>
+      </c>
+      <c r="B83" s="1">
+        <v>453947127.69318998</v>
+      </c>
+      <c r="C83" s="2">
+        <f t="shared" si="1"/>
+        <v>0.27793584682803102</v>
+      </c>
+    </row>
+    <row r="84" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A84" s="1">
+        <v>0.9</v>
+      </c>
+      <c r="B84" s="1">
+        <v>403757564.49089301</v>
+      </c>
+      <c r="C84" s="2">
+        <f t="shared" si="1"/>
+        <v>-0.110562574671072</v>
+      </c>
+    </row>
+    <row r="85" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A85" s="1">
+        <v>0.9</v>
+      </c>
+      <c r="B85" s="1">
+        <v>466919005.73879099</v>
+      </c>
+      <c r="C85" s="2">
+        <f t="shared" si="1"/>
+        <v>0.15643407530343031</v>
+      </c>
+    </row>
+    <row r="86" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A86" s="1">
+        <v>0.9</v>
+      </c>
+      <c r="B86" s="1">
+        <v>370240113.23619199</v>
+      </c>
+      <c r="C86" s="2">
+        <f t="shared" si="1"/>
+        <v>-0.20705709408771461</v>
+      </c>
+    </row>
+    <row r="87" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A87" s="1">
+        <v>0.9</v>
+      </c>
+      <c r="B87" s="1">
+        <v>463936015.50753498</v>
+      </c>
+      <c r="C87" s="2">
+        <f t="shared" si="1"/>
+        <v>0.2530679386746254</v>
+      </c>
+    </row>
+    <row r="88" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A88" s="1">
+        <v>0.9</v>
+      </c>
+      <c r="B88" s="1">
+        <v>410966659.01073098</v>
+      </c>
+      <c r="C88" s="2">
+        <f t="shared" si="1"/>
+        <v>-0.114173840198323</v>
+      </c>
+    </row>
+    <row r="89" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A89" s="1">
+        <v>0.9</v>
+      </c>
+      <c r="B89" s="1">
+        <v>462538415.77899599</v>
+      </c>
+      <c r="C89" s="2">
+        <f t="shared" si="1"/>
+        <v>0.12548890679454947</v>
+      </c>
+    </row>
+    <row r="90" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A90" s="1">
+        <v>0.9</v>
+      </c>
+      <c r="B90" s="1">
+        <v>410989219.61114299</v>
+      </c>
+      <c r="C90" s="2">
+        <f t="shared" si="1"/>
+        <v>-0.11144846440708085</v>
+      </c>
+    </row>
+    <row r="91" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A91" s="1">
+        <v>0.9</v>
+      </c>
+      <c r="B91" s="1">
+        <v>472829360.12418401</v>
+      </c>
+      <c r="C91" s="2">
+        <f t="shared" si="1"/>
+        <v>0.15046657567210886</v>
+      </c>
+    </row>
+    <row r="92" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A92" s="1">
+        <v>0.9</v>
+      </c>
+      <c r="B92" s="1">
+        <v>382521658.53837699</v>
+      </c>
+      <c r="C92" s="2">
+        <f t="shared" si="1"/>
+        <v>-0.19099427658656515</v>
+      </c>
+    </row>
+    <row r="93" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A93" s="1">
+        <v>0.9</v>
+      </c>
+      <c r="B93" s="1">
+        <v>465080372.56080002</v>
+      </c>
+      <c r="C93" s="2">
+        <f t="shared" si="1"/>
+        <v>0.21582755428249881</v>
+      </c>
+    </row>
+    <row r="94" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A94" s="1">
+        <v>0.9</v>
+      </c>
+      <c r="B94" s="1">
+        <v>402680713.03811902</v>
+      </c>
+      <c r="C94" s="2">
+        <f t="shared" si="1"/>
+        <v>-0.13416962573393373</v>
+      </c>
+    </row>
+    <row r="95" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A95" s="1">
+        <v>0.9</v>
+      </c>
+      <c r="B95" s="1">
+        <v>467611083.37385899</v>
+      </c>
+      <c r="C95" s="2">
+        <f t="shared" si="1"/>
+        <v>0.16124529492822631</v>
+      </c>
+    </row>
+    <row r="96" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A96" s="1">
+        <v>0.9</v>
+      </c>
+      <c r="B96" s="1">
+        <v>594101022.57497001</v>
+      </c>
+      <c r="C96" s="2">
+        <f t="shared" si="1"/>
+        <v>0.27050244037945792</v>
+      </c>
+    </row>
+    <row r="97" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A97" s="1">
+        <v>0.9</v>
+      </c>
+      <c r="B97" s="1">
+        <v>461128200.135019</v>
+      </c>
+      <c r="C97" s="2">
+        <f t="shared" si="1"/>
+        <v>-0.22382190467139126</v>
+      </c>
+    </row>
+    <row r="98" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A98" s="1">
+        <v>0.9</v>
+      </c>
+      <c r="B98" s="1">
+        <v>334958300.02285302</v>
+      </c>
+      <c r="C98" s="2">
+        <f t="shared" si="1"/>
+        <v>-0.27361132994083481</v>
+      </c>
+    </row>
+    <row r="99" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A99" s="1">
+        <v>0.9</v>
+      </c>
+      <c r="B99" s="1">
+        <v>450782974.39281303</v>
+      </c>
+      <c r="C99" s="2">
+        <f t="shared" si="1"/>
+        <v>0.34578833950989629</v>
+      </c>
+    </row>
+    <row r="100" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A100" s="1">
+        <v>0.9</v>
+      </c>
+      <c r="B100" s="1">
+        <v>561048022.84938097</v>
+      </c>
+      <c r="C100" s="2">
+        <f t="shared" si="1"/>
+        <v>0.24460783729707325</v>
+      </c>
+    </row>
+    <row r="101" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A101" s="1">
+        <v>0.9</v>
+      </c>
+      <c r="B101" s="1">
+        <v>466743717.44507301</v>
+      </c>
+      <c r="C101" s="2">
+        <f t="shared" si="1"/>
+        <v>-0.16808597760556571</v>
+      </c>
+    </row>
+    <row r="102" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A102" s="1">
+        <v>0.9</v>
+      </c>
+      <c r="B102" s="1">
+        <v>402492900.77467102</v>
+      </c>
+      <c r="C102" s="2">
+        <f t="shared" si="1"/>
+        <v>-0.13765759295509555</v>
+      </c>
+    </row>
+    <row r="103" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A103" s="1">
+        <v>0.9</v>
+      </c>
+      <c r="B103" s="1">
+        <v>464672887.65058398</v>
+      </c>
+      <c r="C103" s="2">
+        <f t="shared" si="1"/>
+        <v>0.15448716426112419</v>
+      </c>
+    </row>
+    <row r="104" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A104" s="1">
+        <v>0.9</v>
+      </c>
+      <c r="B104" s="1">
+        <v>614131227.63888395</v>
+      </c>
+      <c r="C104" s="2">
+        <f t="shared" si="1"/>
+        <v>0.32164204962327575</v>
+      </c>
+    </row>
+    <row r="105" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A105" s="1">
+        <v>0.9</v>
+      </c>
+      <c r="B105" s="1">
+        <v>467870838.564138</v>
+      </c>
+      <c r="C105" s="2">
+        <f t="shared" si="1"/>
+        <v>-0.23815820217621095</v>
+      </c>
+    </row>
+    <row r="106" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A106" s="1">
+        <v>0.9</v>
+      </c>
+      <c r="B106" s="1">
+        <v>476778088.87384099</v>
+      </c>
+      <c r="C106" s="2">
+        <f t="shared" si="1"/>
+        <v>1.9037840308745686E-2</v>
+      </c>
+    </row>
+    <row r="107" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A107" s="1">
+        <v>0.9</v>
+      </c>
+      <c r="B107" s="1">
+        <v>459821252.49602401</v>
+      </c>
+      <c r="C107" s="2">
+        <f t="shared" si="1"/>
+        <v>-3.5565469079901192E-2</v>
+      </c>
+    </row>
+    <row r="108" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A108" s="1">
+        <v>0.9</v>
+      </c>
+      <c r="B108" s="1">
+        <v>286785776.35218298</v>
+      </c>
+      <c r="C108" s="2">
+        <f t="shared" si="1"/>
+        <v>-0.3763103058080971</v>
+      </c>
+    </row>
+    <row r="109" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A109" s="1">
+        <v>0.9</v>
+      </c>
+      <c r="B109" s="1">
+        <v>463648613.67455602</v>
+      </c>
+      <c r="C109" s="2">
+        <f t="shared" si="1"/>
+        <v>0.61670714486613609</v>
+      </c>
+    </row>
+    <row r="110" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A110" s="1">
+        <v>0.9</v>
+      </c>
+      <c r="B110" s="1">
+        <v>468214436.74031198</v>
+      </c>
+      <c r="C110" s="2">
+        <f t="shared" si="1"/>
+        <v>9.8475934815601615E-3</v>
+      </c>
+    </row>
+    <row r="111" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A111" s="1"/>
+      <c r="B111" s="1"/>
+      <c r="C111" s="2">
+        <f t="shared" si="1"/>
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="112" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A112" s="1"/>
+      <c r="B112" s="1"/>
+      <c r="C112" s="2" t="e">
+        <f t="shared" si="1"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="113" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A113" s="1"/>
+      <c r="B113" s="1"/>
+      <c r="C113" s="2" t="e">
+        <f t="shared" si="1"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="114" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A114" s="1"/>
+      <c r="B114" s="1"/>
+      <c r="C114" s="2" t="e">
+        <f t="shared" si="1"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="115" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A115" s="1"/>
+      <c r="B115" s="1"/>
+      <c r="C115" s="2" t="e">
+        <f t="shared" si="1"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="116" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A116" s="1"/>
+      <c r="B116" s="1"/>
+      <c r="C116" s="2" t="e">
+        <f t="shared" si="1"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="117" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A117" s="1"/>
+      <c r="B117" s="1"/>
+      <c r="C117" s="2" t="e">
+        <f t="shared" si="1"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="118" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A118" s="1"/>
+      <c r="B118" s="1"/>
+      <c r="C118" s="2" t="e">
+        <f t="shared" si="1"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="119" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A119" s="1"/>
+      <c r="B119" s="1"/>
+      <c r="C119" s="2" t="e">
+        <f t="shared" si="1"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="120" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A120" s="1"/>
+      <c r="B120" s="1"/>
+      <c r="C120" s="2" t="e">
+        <f t="shared" si="1"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="121" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A121" s="1"/>
+      <c r="B121" s="1"/>
+      <c r="C121" s="2" t="e">
+        <f t="shared" si="1"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="122" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A122" s="1"/>
+      <c r="B122" s="1"/>
+      <c r="C122" s="2" t="e">
+        <f t="shared" si="1"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="123" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A123" s="1"/>
+      <c r="B123" s="1"/>
+      <c r="C123" s="2" t="e">
+        <f t="shared" si="1"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="124" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A124" s="1"/>
+      <c r="B124" s="1"/>
+      <c r="C124" s="2" t="e">
+        <f t="shared" si="1"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="125" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A125" s="1"/>
+      <c r="B125" s="1"/>
+      <c r="C125" s="2" t="e">
+        <f t="shared" si="1"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="126" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A126" s="1"/>
+      <c r="B126" s="1"/>
+      <c r="C126" s="2" t="e">
+        <f t="shared" si="1"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="127" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A127" s="1"/>
+      <c r="B127" s="1"/>
+      <c r="C127" s="2" t="e">
+        <f t="shared" si="1"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="128" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A128" s="1"/>
+      <c r="B128" s="1"/>
+      <c r="C128" s="2" t="e">
+        <f t="shared" si="1"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="129" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A129" s="1"/>
+      <c r="B129" s="1"/>
+      <c r="C129" s="2" t="e">
+        <f t="shared" si="1"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="130" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A130" s="1"/>
+      <c r="B130" s="1"/>
+      <c r="C130" s="2" t="e">
+        <f t="shared" si="1"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="131" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A131" s="1"/>
+      <c r="B131" s="1"/>
+      <c r="C131" s="2" t="e">
+        <f t="shared" si="1"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="132" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A132" s="1"/>
+      <c r="B132" s="1"/>
+      <c r="C132" s="2" t="e">
+        <f t="shared" si="1"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="133" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A133" s="1"/>
+      <c r="B133" s="1"/>
+      <c r="C133" s="2" t="e">
+        <f t="shared" si="1"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="134" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A134" s="1"/>
+      <c r="B134" s="1"/>
+      <c r="C134" s="2" t="e">
+        <f t="shared" si="1"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="135" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A135" s="1"/>
+      <c r="B135" s="1"/>
+      <c r="C135" s="2" t="e">
+        <f t="shared" si="1"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="136" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A136" s="1"/>
+      <c r="B136" s="1"/>
+      <c r="C136" s="2" t="e">
+        <f t="shared" ref="C136:C137" si="2">(B136-B135)/B135</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="137" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A137" s="1"/>
+      <c r="B137" s="1"/>
+      <c r="C137" s="2" t="e">
+        <f t="shared" si="2"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Fixed.  Ready to merge.
</commit_message>
<xml_diff>
--- a/Progress.xlsx
+++ b/Progress.xlsx
@@ -8,15 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/c51537410c5afe56/Projects/Source/Repos/EdGarrity/SOS/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="232" documentId="114_{B2D123C0-10CD-4892-A2B1-0D4FB86B9D90}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{30F6BED2-5AD4-4FD5-9CDE-CC5A5EB51F82}"/>
+  <xr:revisionPtr revIDLastSave="237" documentId="114_{B2D123C0-10CD-4892-A2B1-0D4FB86B9D90}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{93029869-0C45-4CEC-94D3-406A34B69937}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="16896" activeTab="3" xr2:uid="{D7613C25-2959-4D88-A8C3-21B00E74DE47}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="16896" activeTab="4" xr2:uid="{D7613C25-2959-4D88-A8C3-21B00E74DE47}"/>
   </bookViews>
   <sheets>
     <sheet name="Run 1" sheetId="1" r:id="rId1"/>
     <sheet name="Run 2" sheetId="2" r:id="rId2"/>
     <sheet name="Run 3" sheetId="3" r:id="rId3"/>
     <sheet name="Run 4" sheetId="4" r:id="rId4"/>
+    <sheet name="Run 5" sheetId="5" r:id="rId5"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="8">
   <si>
     <t>BestIndividual_Training_Error</t>
   </si>
@@ -4393,6 +4394,685 @@
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000001-7CE4-49D1-9475-DF23D8AD236E}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:marker val="1"/>
+        <c:smooth val="0"/>
+        <c:axId val="840836808"/>
+        <c:axId val="840833856"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="715829080"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" cap="none" spc="0" normalizeH="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="715823504"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="715823504"/>
+        <c:scaling>
+          <c:logBase val="10"/>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:minorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="5000"/>
+                  <a:lumOff val="95000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:minorGridlines>
+        <c:numFmt formatCode="#,##0.00" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="715829080"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="840833856"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="r"/>
+        <c:numFmt formatCode="#,##0.00" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="840836808"/>
+        <c:crosses val="max"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:catAx>
+        <c:axId val="840836808"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="1"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="840833856"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="t"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart5.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="2000" b="0" i="0" u="none" strike="noStrike" kern="1200" cap="none" spc="0" normalizeH="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mj-lt"/>
+              <a:ea typeface="+mj-ea"/>
+              <a:cs typeface="+mj-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Run 5'!$B$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Average_Training_Error</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="38100" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>'Run 5'!$B$2:$B$137</c:f>
+              <c:numCache>
+                <c:formatCode>#,##0.00</c:formatCode>
+                <c:ptCount val="136"/>
+                <c:pt idx="0">
+                  <c:v>466828517.77193397</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>530838032.318699</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>370939279.01228499</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>287802144.25176901</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>248506795.35284099</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>219063937.33587301</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>138580850.40472999</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>143843237.58303201</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>84740447.071308702</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>50829498.939668</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>45881076.786539502</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>36884020.090438202</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>51961728.485883802</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>23300455.492954198</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>18673919.715530898</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>22387443.221550301</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>21727289.674221501</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>25023973.804324102</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>28457230.8928365</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>20707684.776952799</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>14613419.506552</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>14221412.3280422</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>13799211.4196239</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>10991181.9397649</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>7827470.0282455198</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>11158393.262985799</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>11228451.7032403</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>6580154.4599233698</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>5694237.1644831495</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>7602025.9353936203</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>7774374.1914764</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>8887725.9137989692</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>8256218.8607965596</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>9346117.9973511808</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>8787415.66559745</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>6106326.5948853297</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>10212688.134928999</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>12426570.6614541</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>7555045.1385022402</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>5974048.4311196003</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>5586637.8612419497</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>6283506.2962794499</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>7465580.1919447798</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-212E-400E-9313-37DCD10EEC5E}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:marker val="1"/>
+        <c:smooth val="0"/>
+        <c:axId val="715829080"/>
+        <c:axId val="715823504"/>
+      </c:lineChart>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Run 5'!$A$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>BestIndividual_Training_Score</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="38100" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>'Run 5'!$A$2:$A$137</c:f>
+              <c:numCache>
+                <c:formatCode>#,##0.00</c:formatCode>
+                <c:ptCount val="136"/>
+                <c:pt idx="0">
+                  <c:v>0.9</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.9</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.9</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.9</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.9</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.9</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.9</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.9</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.9</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.9</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0.9</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0.9</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>0.9</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>0.9</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>0.9</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>0.9</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>0.9</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>0.9</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>0.9</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>0.9</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>0.9</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>0.9</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>0.9</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>0.9</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>0.9</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>0.9</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>0.9</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>0.9</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>0.9</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>0.9</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>0.9</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>0.9</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>0.9</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>0.9</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>0.9</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>0.9</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>0.9</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>0.9</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>0.9</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>0.9</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>0.9</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>0.9</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>0.9</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-212E-400E-9313-37DCD10EEC5E}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -4788,6 +5468,46 @@
 </file>
 
 <file path=xl/charts/colors4.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors5.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
   <a:schemeClr val="accent2"/>
@@ -6827,6 +7547,506 @@
 </cs:chartStyle>
 </file>
 
+<file path=xl/charts/style5.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="235">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200" cap="all"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" b="0" kern="1200" cap="none" spc="0" normalizeH="0" baseline="0"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="38100" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="8"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:prstDash val="dash"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:prstDash val="dash"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="major">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="2000" b="0" kern="1200" cap="none" spc="0" normalizeH="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
@@ -6975,6 +8195,49 @@
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
               <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{6677EAB1-3090-4CC8-A23D-EB7582065BD0}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing5.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>561975</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>30</xdr:col>
+      <xdr:colOff>409575</xdr:colOff>
+      <xdr:row>37</xdr:row>
+      <xdr:rowOff>19050</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{7DFC844A-CA4D-4416-AB8A-185B200BC67E}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -11579,7 +12842,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{46279A08-E6DD-4519-895C-48ADC6AEC5C3}">
   <dimension ref="A1:D137"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
       <selection activeCell="B1" sqref="B1:B110"/>
     </sheetView>
   </sheetViews>
@@ -13129,4 +14392,1296 @@
   <pageSetup orientation="portrait" r:id="rId1"/>
   <drawing r:id="rId2"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0FE1FBB3-2F2A-4BF3-AA47-B20CE8C7B019}">
+  <dimension ref="A1:D137"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="B1" sqref="B1:B44"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="27.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="22.109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="8.88671875" style="2"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A2" s="1">
+        <v>0.9</v>
+      </c>
+      <c r="B2" s="1">
+        <v>466828517.77193397</v>
+      </c>
+      <c r="D2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A3" s="1">
+        <v>0.9</v>
+      </c>
+      <c r="B3" s="1">
+        <v>530838032.318699</v>
+      </c>
+      <c r="C3" s="2">
+        <f>(B3-B2)/B2</f>
+        <v>0.13711569047295533</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A4" s="1">
+        <v>0.9</v>
+      </c>
+      <c r="B4" s="1">
+        <v>370939279.01228499</v>
+      </c>
+      <c r="C4" s="2">
+        <f t="shared" ref="C4:C71" si="0">(B4-B3)/B3</f>
+        <v>-0.30121947481414757</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A5" s="1">
+        <v>0.9</v>
+      </c>
+      <c r="B5" s="1">
+        <v>287802144.25176901</v>
+      </c>
+      <c r="C5" s="2">
+        <f t="shared" si="0"/>
+        <v>-0.22412599437268707</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A6" s="1">
+        <v>0.9</v>
+      </c>
+      <c r="B6" s="1">
+        <v>248506795.35284099</v>
+      </c>
+      <c r="C6" s="2">
+        <f t="shared" si="0"/>
+        <v>-0.13653598377832962</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A7" s="1">
+        <v>0.9</v>
+      </c>
+      <c r="B7" s="1">
+        <v>219063937.33587301</v>
+      </c>
+      <c r="C7" s="2">
+        <f t="shared" si="0"/>
+        <v>-0.11847908615602927</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A8" s="1">
+        <v>0.9</v>
+      </c>
+      <c r="B8" s="1">
+        <v>138580850.40472999</v>
+      </c>
+      <c r="C8" s="2">
+        <f t="shared" si="0"/>
+        <v>-0.36739541847887458</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A9" s="1">
+        <v>0.9</v>
+      </c>
+      <c r="B9" s="1">
+        <v>143843237.58303201</v>
+      </c>
+      <c r="C9" s="2">
+        <f t="shared" si="0"/>
+        <v>3.7973408035331307E-2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A10" s="1">
+        <v>0.9</v>
+      </c>
+      <c r="B10" s="1">
+        <v>84740447.071308702</v>
+      </c>
+      <c r="C10" s="2">
+        <f t="shared" si="0"/>
+        <v>-0.41088334429073758</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A11" s="1">
+        <v>0.9</v>
+      </c>
+      <c r="B11" s="1">
+        <v>50829498.939668</v>
+      </c>
+      <c r="C11" s="2">
+        <f t="shared" si="0"/>
+        <v>-0.40017428870896554</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A12" s="1">
+        <v>0.9</v>
+      </c>
+      <c r="B12" s="1">
+        <v>45881076.786539502</v>
+      </c>
+      <c r="C12" s="2">
+        <f t="shared" si="0"/>
+        <v>-9.7353353000823789E-2</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A13" s="1">
+        <v>0.9</v>
+      </c>
+      <c r="B13" s="1">
+        <v>36884020.090438202</v>
+      </c>
+      <c r="C13" s="2">
+        <f t="shared" si="0"/>
+        <v>-0.19609515134005831</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A14" s="1">
+        <v>0.9</v>
+      </c>
+      <c r="B14" s="1">
+        <v>51961728.485883802</v>
+      </c>
+      <c r="C14" s="2">
+        <f t="shared" si="0"/>
+        <v>0.40878701287103841</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A15" s="1">
+        <v>0.9</v>
+      </c>
+      <c r="B15" s="1">
+        <v>23300455.492954198</v>
+      </c>
+      <c r="C15" s="2">
+        <f t="shared" si="0"/>
+        <v>-0.55158428766887302</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A16" s="1">
+        <v>0.9</v>
+      </c>
+      <c r="B16" s="1">
+        <v>18673919.715530898</v>
+      </c>
+      <c r="C16" s="2">
+        <f t="shared" si="0"/>
+        <v>-0.19855988561349427</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A17" s="1">
+        <v>0.9</v>
+      </c>
+      <c r="B17" s="1">
+        <v>22387443.221550301</v>
+      </c>
+      <c r="C17" s="2">
+        <f t="shared" si="0"/>
+        <v>0.19886149038816445</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A18" s="1">
+        <v>0.9</v>
+      </c>
+      <c r="B18" s="1">
+        <v>21727289.674221501</v>
+      </c>
+      <c r="C18" s="2">
+        <f t="shared" si="0"/>
+        <v>-2.9487670422915099E-2</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A19" s="1">
+        <v>0.9</v>
+      </c>
+      <c r="B19" s="1">
+        <v>25023973.804324102</v>
+      </c>
+      <c r="C19" s="2">
+        <f t="shared" si="0"/>
+        <v>0.15173011358218211</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A20" s="1">
+        <v>0.9</v>
+      </c>
+      <c r="B20" s="1">
+        <v>28457230.8928365</v>
+      </c>
+      <c r="C20" s="2">
+        <f t="shared" si="0"/>
+        <v>0.13719871653314858</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A21" s="1">
+        <v>0.9</v>
+      </c>
+      <c r="B21" s="1">
+        <v>20707684.776952799</v>
+      </c>
+      <c r="C21" s="2">
+        <f t="shared" si="0"/>
+        <v>-0.27232256522311465</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A22" s="1">
+        <v>0.9</v>
+      </c>
+      <c r="B22" s="1">
+        <v>14613419.506552</v>
+      </c>
+      <c r="C22" s="2">
+        <f t="shared" si="0"/>
+        <v>-0.29429969289389529</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A23" s="1">
+        <v>0.9</v>
+      </c>
+      <c r="B23" s="1">
+        <v>14221412.3280422</v>
+      </c>
+      <c r="C23" s="2">
+        <f t="shared" si="0"/>
+        <v>-2.6825150563428456E-2</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A24" s="1">
+        <v>0.9</v>
+      </c>
+      <c r="B24" s="1">
+        <v>13799211.4196239</v>
+      </c>
+      <c r="C24" s="2">
+        <f t="shared" si="0"/>
+        <v>-2.9687691959102504E-2</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A25" s="1">
+        <v>0.9</v>
+      </c>
+      <c r="B25" s="1">
+        <v>10991181.9397649</v>
+      </c>
+      <c r="C25" s="2">
+        <f t="shared" si="0"/>
+        <v>-0.20349202533890401</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A26" s="1">
+        <v>0.9</v>
+      </c>
+      <c r="B26" s="1">
+        <v>7827470.0282455198</v>
+      </c>
+      <c r="C26" s="2">
+        <f t="shared" si="0"/>
+        <v>-0.28784091909837423</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A27" s="1">
+        <v>0.9</v>
+      </c>
+      <c r="B27" s="1">
+        <v>11158393.262985799</v>
+      </c>
+      <c r="C27" s="2">
+        <f t="shared" si="0"/>
+        <v>0.42554276448464229</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A28" s="1">
+        <v>0.9</v>
+      </c>
+      <c r="B28" s="1">
+        <v>11228451.7032403</v>
+      </c>
+      <c r="C28" s="2">
+        <f t="shared" si="0"/>
+        <v>6.2785419552199642E-3</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A29" s="1">
+        <v>0.9</v>
+      </c>
+      <c r="B29" s="1">
+        <v>6580154.4599233698</v>
+      </c>
+      <c r="C29" s="2">
+        <f t="shared" si="0"/>
+        <v>-0.41397490644017526</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A30" s="1">
+        <v>0.9</v>
+      </c>
+      <c r="B30" s="1">
+        <v>5694237.1644831495</v>
+      </c>
+      <c r="C30" s="2">
+        <f t="shared" si="0"/>
+        <v>-0.13463472640892041</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A31" s="1">
+        <v>0.9</v>
+      </c>
+      <c r="B31" s="1">
+        <v>7602025.9353936203</v>
+      </c>
+      <c r="C31" s="2">
+        <f t="shared" si="0"/>
+        <v>0.33503851627571529</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A32" s="1">
+        <v>0.9</v>
+      </c>
+      <c r="B32" s="1">
+        <v>7774374.1914764</v>
+      </c>
+      <c r="C32" s="2">
+        <f>(B32-B30)/B30</f>
+        <v>0.36530565322564307</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A33" s="1">
+        <v>0.9</v>
+      </c>
+      <c r="B33" s="1">
+        <v>8887725.9137989692</v>
+      </c>
+      <c r="C33" s="2">
+        <f t="shared" si="0"/>
+        <v>0.14320788978014667</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A34" s="1">
+        <v>0.9</v>
+      </c>
+      <c r="B34" s="1">
+        <v>8256218.8607965596</v>
+      </c>
+      <c r="C34" s="2">
+        <f t="shared" si="0"/>
+        <v>-7.1053839770411895E-2</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A35" s="1">
+        <v>0.9</v>
+      </c>
+      <c r="B35" s="1">
+        <v>9346117.9973511808</v>
+      </c>
+      <c r="C35" s="2">
+        <f t="shared" si="0"/>
+        <v>0.13200947733227456</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A36" s="1">
+        <v>0.9</v>
+      </c>
+      <c r="B36" s="1">
+        <v>8787415.66559745</v>
+      </c>
+      <c r="C36" s="2">
+        <f t="shared" si="0"/>
+        <v>-5.9779079604181627E-2</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A37" s="1">
+        <v>0.9</v>
+      </c>
+      <c r="B37" s="1">
+        <v>6106326.5948853297</v>
+      </c>
+      <c r="C37" s="2">
+        <f t="shared" si="0"/>
+        <v>-0.30510552507587962</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A38" s="1">
+        <v>0.9</v>
+      </c>
+      <c r="B38" s="1">
+        <v>10212688.134928999</v>
+      </c>
+      <c r="C38" s="2">
+        <f t="shared" si="0"/>
+        <v>0.67247656610492557</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A39" s="1">
+        <v>0.9</v>
+      </c>
+      <c r="B39" s="1">
+        <v>12426570.6614541</v>
+      </c>
+      <c r="C39" s="2">
+        <f t="shared" si="0"/>
+        <v>0.21677764926094964</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A40" s="1">
+        <v>0.9</v>
+      </c>
+      <c r="B40" s="1">
+        <v>7555045.1385022402</v>
+      </c>
+      <c r="C40" s="2">
+        <f t="shared" si="0"/>
+        <v>-0.39202493235425068</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A41" s="1">
+        <v>0.9</v>
+      </c>
+      <c r="B41" s="1">
+        <v>5974048.4311196003</v>
+      </c>
+      <c r="C41" s="2">
+        <f t="shared" si="0"/>
+        <v>-0.20926370106321648</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A42" s="1">
+        <v>0.9</v>
+      </c>
+      <c r="B42" s="1">
+        <v>5586637.8612419497</v>
+      </c>
+      <c r="C42" s="2">
+        <f t="shared" si="0"/>
+        <v>-6.4848916834952031E-2</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A43" s="1">
+        <v>0.9</v>
+      </c>
+      <c r="B43" s="1">
+        <v>6283506.2962794499</v>
+      </c>
+      <c r="C43" s="2">
+        <f t="shared" si="0"/>
+        <v>0.12473842986532536</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A44" s="1">
+        <v>0.9</v>
+      </c>
+      <c r="B44" s="1">
+        <v>7465580.1919447798</v>
+      </c>
+      <c r="C44" s="2">
+        <f t="shared" si="0"/>
+        <v>0.18812329294000263</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A45" s="1"/>
+      <c r="B45" s="1"/>
+      <c r="C45" s="2">
+        <f t="shared" si="0"/>
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A46" s="1"/>
+      <c r="B46" s="1"/>
+      <c r="C46" s="2" t="e">
+        <f t="shared" si="0"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="47" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A47" s="1"/>
+      <c r="B47" s="1"/>
+      <c r="C47" s="2" t="e">
+        <f t="shared" si="0"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="48" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A48" s="1"/>
+      <c r="B48" s="1"/>
+      <c r="C48" s="2" t="e">
+        <f t="shared" si="0"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="49" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A49" s="1"/>
+      <c r="B49" s="1"/>
+      <c r="C49" s="2" t="e">
+        <f t="shared" si="0"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="50" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A50" s="1"/>
+      <c r="B50" s="1"/>
+      <c r="C50" s="2" t="e">
+        <f t="shared" si="0"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="51" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A51" s="1"/>
+      <c r="B51" s="1"/>
+      <c r="C51" s="2" t="e">
+        <f t="shared" si="0"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="52" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A52" s="1"/>
+      <c r="B52" s="1"/>
+      <c r="C52" s="2" t="e">
+        <f t="shared" si="0"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="53" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A53" s="1"/>
+      <c r="B53" s="1"/>
+      <c r="C53" s="2" t="e">
+        <f t="shared" si="0"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="54" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A54" s="1"/>
+      <c r="B54" s="1"/>
+      <c r="C54" s="2" t="e">
+        <f t="shared" si="0"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="55" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A55" s="1"/>
+      <c r="B55" s="1"/>
+      <c r="C55" s="2" t="e">
+        <f t="shared" si="0"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="56" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A56" s="1"/>
+      <c r="B56" s="1"/>
+      <c r="C56" s="2" t="e">
+        <f t="shared" si="0"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="57" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A57" s="1"/>
+      <c r="B57" s="1"/>
+      <c r="C57" s="2" t="e">
+        <f t="shared" si="0"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="58" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A58" s="1"/>
+      <c r="B58" s="1"/>
+      <c r="C58" s="2" t="e">
+        <f t="shared" si="0"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="59" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A59" s="1"/>
+      <c r="B59" s="1"/>
+      <c r="C59" s="2" t="e">
+        <f t="shared" si="0"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="60" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A60" s="1"/>
+      <c r="B60" s="1"/>
+      <c r="C60" s="2" t="e">
+        <f t="shared" si="0"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="61" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A61" s="1"/>
+      <c r="B61" s="1"/>
+      <c r="C61" s="2" t="e">
+        <f t="shared" si="0"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="62" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A62" s="1"/>
+      <c r="B62" s="1"/>
+      <c r="C62" s="2" t="e">
+        <f t="shared" si="0"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="63" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A63" s="1"/>
+      <c r="B63" s="1"/>
+      <c r="C63" s="2" t="e">
+        <f t="shared" si="0"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="64" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A64" s="1"/>
+      <c r="B64" s="1"/>
+      <c r="C64" s="2" t="e">
+        <f t="shared" si="0"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="65" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A65" s="1"/>
+      <c r="B65" s="1"/>
+      <c r="C65" s="2" t="e">
+        <f t="shared" si="0"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="66" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A66" s="1"/>
+      <c r="B66" s="1"/>
+      <c r="C66" s="2" t="e">
+        <f t="shared" si="0"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="67" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A67" s="1"/>
+      <c r="B67" s="1"/>
+      <c r="C67" s="2" t="e">
+        <f t="shared" si="0"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="68" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A68" s="1"/>
+      <c r="B68" s="1"/>
+      <c r="C68" s="2" t="e">
+        <f t="shared" si="0"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="69" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A69" s="1"/>
+      <c r="B69" s="1"/>
+      <c r="C69" s="2" t="e">
+        <f t="shared" si="0"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="70" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A70" s="1"/>
+      <c r="B70" s="1"/>
+      <c r="C70" s="2" t="e">
+        <f t="shared" si="0"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="71" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A71" s="1"/>
+      <c r="B71" s="1"/>
+      <c r="C71" s="2" t="e">
+        <f t="shared" si="0"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="72" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A72" s="1"/>
+      <c r="B72" s="1"/>
+      <c r="C72" s="2" t="e">
+        <f t="shared" ref="C72:C135" si="1">(B72-B71)/B71</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="73" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A73" s="1"/>
+      <c r="B73" s="1"/>
+      <c r="C73" s="2" t="e">
+        <f t="shared" si="1"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="74" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A74" s="1"/>
+      <c r="B74" s="1"/>
+      <c r="C74" s="2" t="e">
+        <f t="shared" si="1"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="75" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A75" s="1"/>
+      <c r="B75" s="1"/>
+      <c r="C75" s="2" t="e">
+        <f t="shared" si="1"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="76" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A76" s="1"/>
+      <c r="B76" s="1"/>
+      <c r="C76" s="2" t="e">
+        <f t="shared" si="1"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="77" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A77" s="1"/>
+      <c r="B77" s="1"/>
+      <c r="C77" s="2" t="e">
+        <f t="shared" si="1"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="78" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A78" s="1"/>
+      <c r="B78" s="1"/>
+      <c r="C78" s="2" t="e">
+        <f t="shared" si="1"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="79" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A79" s="1"/>
+      <c r="B79" s="1"/>
+      <c r="C79" s="2" t="e">
+        <f t="shared" si="1"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="80" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A80" s="1"/>
+      <c r="B80" s="1"/>
+      <c r="C80" s="2" t="e">
+        <f t="shared" si="1"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="81" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A81" s="1"/>
+      <c r="B81" s="1"/>
+      <c r="C81" s="2" t="e">
+        <f t="shared" si="1"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="82" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A82" s="1"/>
+      <c r="B82" s="1"/>
+      <c r="C82" s="2" t="e">
+        <f t="shared" si="1"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="83" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A83" s="1"/>
+      <c r="B83" s="1"/>
+      <c r="C83" s="2" t="e">
+        <f t="shared" si="1"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="84" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A84" s="1"/>
+      <c r="B84" s="1"/>
+      <c r="C84" s="2" t="e">
+        <f t="shared" si="1"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="85" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A85" s="1"/>
+      <c r="B85" s="1"/>
+      <c r="C85" s="2" t="e">
+        <f t="shared" si="1"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="86" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A86" s="1"/>
+      <c r="B86" s="1"/>
+      <c r="C86" s="2" t="e">
+        <f t="shared" si="1"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="87" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A87" s="1"/>
+      <c r="B87" s="1"/>
+      <c r="C87" s="2" t="e">
+        <f t="shared" si="1"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="88" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A88" s="1"/>
+      <c r="B88" s="1"/>
+      <c r="C88" s="2" t="e">
+        <f t="shared" si="1"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="89" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A89" s="1"/>
+      <c r="B89" s="1"/>
+      <c r="C89" s="2" t="e">
+        <f t="shared" si="1"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="90" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A90" s="1"/>
+      <c r="B90" s="1"/>
+      <c r="C90" s="2" t="e">
+        <f t="shared" si="1"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="91" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A91" s="1"/>
+      <c r="B91" s="1"/>
+      <c r="C91" s="2" t="e">
+        <f t="shared" si="1"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="92" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A92" s="1"/>
+      <c r="B92" s="1"/>
+      <c r="C92" s="2" t="e">
+        <f t="shared" si="1"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="93" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A93" s="1"/>
+      <c r="B93" s="1"/>
+      <c r="C93" s="2" t="e">
+        <f t="shared" si="1"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="94" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A94" s="1"/>
+      <c r="B94" s="1"/>
+      <c r="C94" s="2" t="e">
+        <f t="shared" si="1"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="95" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A95" s="1"/>
+      <c r="B95" s="1"/>
+      <c r="C95" s="2" t="e">
+        <f t="shared" si="1"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="96" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A96" s="1"/>
+      <c r="B96" s="1"/>
+      <c r="C96" s="2" t="e">
+        <f t="shared" si="1"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="97" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A97" s="1"/>
+      <c r="B97" s="1"/>
+      <c r="C97" s="2" t="e">
+        <f t="shared" si="1"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="98" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A98" s="1"/>
+      <c r="B98" s="1"/>
+      <c r="C98" s="2" t="e">
+        <f t="shared" si="1"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="99" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A99" s="1"/>
+      <c r="B99" s="1"/>
+      <c r="C99" s="2" t="e">
+        <f t="shared" si="1"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="100" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A100" s="1"/>
+      <c r="B100" s="1"/>
+      <c r="C100" s="2" t="e">
+        <f t="shared" si="1"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="101" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A101" s="1"/>
+      <c r="B101" s="1"/>
+      <c r="C101" s="2" t="e">
+        <f t="shared" si="1"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="102" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A102" s="1"/>
+      <c r="B102" s="1"/>
+      <c r="C102" s="2" t="e">
+        <f t="shared" si="1"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="103" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A103" s="1"/>
+      <c r="B103" s="1"/>
+      <c r="C103" s="2" t="e">
+        <f t="shared" si="1"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="104" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A104" s="1"/>
+      <c r="B104" s="1"/>
+      <c r="C104" s="2" t="e">
+        <f t="shared" si="1"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="105" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A105" s="1"/>
+      <c r="B105" s="1"/>
+      <c r="C105" s="2" t="e">
+        <f t="shared" si="1"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="106" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A106" s="1"/>
+      <c r="B106" s="1"/>
+      <c r="C106" s="2" t="e">
+        <f t="shared" si="1"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="107" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A107" s="1"/>
+      <c r="B107" s="1"/>
+      <c r="C107" s="2" t="e">
+        <f t="shared" si="1"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="108" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A108" s="1"/>
+      <c r="B108" s="1"/>
+      <c r="C108" s="2" t="e">
+        <f t="shared" si="1"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="109" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A109" s="1"/>
+      <c r="B109" s="1"/>
+      <c r="C109" s="2" t="e">
+        <f t="shared" si="1"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="110" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A110" s="1"/>
+      <c r="B110" s="1"/>
+      <c r="C110" s="2" t="e">
+        <f t="shared" si="1"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="111" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A111" s="1"/>
+      <c r="B111" s="1"/>
+      <c r="C111" s="2" t="e">
+        <f t="shared" si="1"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="112" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A112" s="1"/>
+      <c r="B112" s="1"/>
+      <c r="C112" s="2" t="e">
+        <f t="shared" si="1"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="113" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A113" s="1"/>
+      <c r="B113" s="1"/>
+      <c r="C113" s="2" t="e">
+        <f t="shared" si="1"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="114" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A114" s="1"/>
+      <c r="B114" s="1"/>
+      <c r="C114" s="2" t="e">
+        <f t="shared" si="1"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="115" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A115" s="1"/>
+      <c r="B115" s="1"/>
+      <c r="C115" s="2" t="e">
+        <f t="shared" si="1"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="116" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A116" s="1"/>
+      <c r="B116" s="1"/>
+      <c r="C116" s="2" t="e">
+        <f t="shared" si="1"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="117" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A117" s="1"/>
+      <c r="B117" s="1"/>
+      <c r="C117" s="2" t="e">
+        <f t="shared" si="1"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="118" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A118" s="1"/>
+      <c r="B118" s="1"/>
+      <c r="C118" s="2" t="e">
+        <f t="shared" si="1"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="119" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A119" s="1"/>
+      <c r="B119" s="1"/>
+      <c r="C119" s="2" t="e">
+        <f t="shared" si="1"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="120" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A120" s="1"/>
+      <c r="B120" s="1"/>
+      <c r="C120" s="2" t="e">
+        <f t="shared" si="1"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="121" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A121" s="1"/>
+      <c r="B121" s="1"/>
+      <c r="C121" s="2" t="e">
+        <f t="shared" si="1"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="122" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A122" s="1"/>
+      <c r="B122" s="1"/>
+      <c r="C122" s="2" t="e">
+        <f t="shared" si="1"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="123" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A123" s="1"/>
+      <c r="B123" s="1"/>
+      <c r="C123" s="2" t="e">
+        <f t="shared" si="1"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="124" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A124" s="1"/>
+      <c r="B124" s="1"/>
+      <c r="C124" s="2" t="e">
+        <f t="shared" si="1"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="125" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A125" s="1"/>
+      <c r="B125" s="1"/>
+      <c r="C125" s="2" t="e">
+        <f t="shared" si="1"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="126" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A126" s="1"/>
+      <c r="B126" s="1"/>
+      <c r="C126" s="2" t="e">
+        <f t="shared" si="1"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="127" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A127" s="1"/>
+      <c r="B127" s="1"/>
+      <c r="C127" s="2" t="e">
+        <f t="shared" si="1"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="128" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A128" s="1"/>
+      <c r="B128" s="1"/>
+      <c r="C128" s="2" t="e">
+        <f t="shared" si="1"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="129" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A129" s="1"/>
+      <c r="B129" s="1"/>
+      <c r="C129" s="2" t="e">
+        <f t="shared" si="1"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="130" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A130" s="1"/>
+      <c r="B130" s="1"/>
+      <c r="C130" s="2" t="e">
+        <f t="shared" si="1"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="131" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A131" s="1"/>
+      <c r="B131" s="1"/>
+      <c r="C131" s="2" t="e">
+        <f t="shared" si="1"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="132" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A132" s="1"/>
+      <c r="B132" s="1"/>
+      <c r="C132" s="2" t="e">
+        <f t="shared" si="1"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="133" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A133" s="1"/>
+      <c r="B133" s="1"/>
+      <c r="C133" s="2" t="e">
+        <f t="shared" si="1"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="134" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A134" s="1"/>
+      <c r="B134" s="1"/>
+      <c r="C134" s="2" t="e">
+        <f t="shared" si="1"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="135" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A135" s="1"/>
+      <c r="B135" s="1"/>
+      <c r="C135" s="2" t="e">
+        <f t="shared" si="1"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="136" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A136" s="1"/>
+      <c r="B136" s="1"/>
+      <c r="C136" s="2" t="e">
+        <f t="shared" ref="C136:C137" si="2">(B136-B135)/B135</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="137" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A137" s="1"/>
+      <c r="B137" s="1"/>
+      <c r="C137" s="2" t="e">
+        <f t="shared" si="2"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Simgle-Thread performed much better than Multi-Thread.  MT started with a 450M error and did not vary much for 110 generations.  ST started at 450M but quickly dropped to about 10M.  Need to investigate further and resolve this issue.
</commit_message>
<xml_diff>
--- a/Progress.xlsx
+++ b/Progress.xlsx
@@ -8,15 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/c51537410c5afe56/Projects/Source/Repos/EdGarrity/SOS/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="232" documentId="114_{B2D123C0-10CD-4892-A2B1-0D4FB86B9D90}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{30F6BED2-5AD4-4FD5-9CDE-CC5A5EB51F82}"/>
+  <xr:revisionPtr revIDLastSave="5" documentId="114_{3C4423BE-71A8-46AF-868D-FDDDC2B78D61}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{7726B95E-048A-4E02-B9D0-ED28C801C9D5}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="16896" activeTab="3" xr2:uid="{D7613C25-2959-4D88-A8C3-21B00E74DE47}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="16896" activeTab="4" xr2:uid="{D7613C25-2959-4D88-A8C3-21B00E74DE47}"/>
   </bookViews>
   <sheets>
     <sheet name="Run 1" sheetId="1" r:id="rId1"/>
     <sheet name="Run 2" sheetId="2" r:id="rId2"/>
     <sheet name="Run 3" sheetId="3" r:id="rId3"/>
     <sheet name="Run 4" sheetId="4" r:id="rId4"/>
+    <sheet name="Run 5" sheetId="5" r:id="rId5"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="8">
   <si>
     <t>BestIndividual_Training_Error</t>
   </si>
@@ -4393,6 +4394,1243 @@
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000001-7CE4-49D1-9475-DF23D8AD236E}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:marker val="1"/>
+        <c:smooth val="0"/>
+        <c:axId val="840836808"/>
+        <c:axId val="840833856"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="715829080"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" cap="none" spc="0" normalizeH="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="715823504"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="715823504"/>
+        <c:scaling>
+          <c:logBase val="10"/>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:minorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="5000"/>
+                  <a:lumOff val="95000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:minorGridlines>
+        <c:numFmt formatCode="#,##0.00" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="715829080"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="840833856"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="r"/>
+        <c:numFmt formatCode="#,##0.00" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="840836808"/>
+        <c:crosses val="max"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:catAx>
+        <c:axId val="840836808"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="1"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="840833856"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="t"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart5.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="2000" b="0" i="0" u="none" strike="noStrike" kern="1200" cap="none" spc="0" normalizeH="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mj-lt"/>
+              <a:ea typeface="+mj-ea"/>
+              <a:cs typeface="+mj-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Run 5'!$B$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Average_Training_Error</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="38100" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>'Run 5'!$B$2:$B$137</c:f>
+              <c:numCache>
+                <c:formatCode>#,##0.00</c:formatCode>
+                <c:ptCount val="136"/>
+                <c:pt idx="0">
+                  <c:v>466828517.77193397</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>530838032.318699</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>370939279.01228499</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>287802144.25176901</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>248506795.35284099</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>219063937.33587301</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>138580850.40472999</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>143843237.58303201</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>84740447.071308702</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>50829498.939668</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>45881076.786539502</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>36884020.090438202</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>51961728.485883802</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>23300455.492954198</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>18673919.715530898</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>22387443.221550301</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>21727289.674221501</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>25023973.804324102</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>28457230.8928365</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>20707684.776952799</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>14613419.506552</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>14221412.3280422</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>13799211.4196239</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>10991181.9397649</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>7827470.0282455198</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>11158393.262985799</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>11228451.7032403</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>6580154.4599233698</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>5694237.1644831495</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>7602025.9353936203</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>7774374.1914764</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>8887725.9137989692</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>8256218.8607965596</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>9346117.9973511808</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>8787415.66559745</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>6106326.5948853297</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>10212688.134928999</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>12426570.6614541</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>7555045.1385022402</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>5974048.4311196003</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>5586637.8612419497</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>6283506.2962794499</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>7465580.1919447798</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>6318532.6921694595</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>7805773.7823088001</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>8864587.4604190998</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>6943692.4762246301</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>5018393.19882455</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>5936583.2975150002</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>8225772.5154284202</c:v>
+                </c:pt>
+                <c:pt idx="50">
+                  <c:v>6907093.6067347797</c:v>
+                </c:pt>
+                <c:pt idx="51">
+                  <c:v>7761654.1245476799</c:v>
+                </c:pt>
+                <c:pt idx="52">
+                  <c:v>8243263.69838861</c:v>
+                </c:pt>
+                <c:pt idx="53">
+                  <c:v>8773894.6373157408</c:v>
+                </c:pt>
+                <c:pt idx="54">
+                  <c:v>8716087.0516568795</c:v>
+                </c:pt>
+                <c:pt idx="55">
+                  <c:v>9526198.3536674306</c:v>
+                </c:pt>
+                <c:pt idx="56">
+                  <c:v>11499360.383852899</c:v>
+                </c:pt>
+                <c:pt idx="57">
+                  <c:v>11166373.0106229</c:v>
+                </c:pt>
+                <c:pt idx="58">
+                  <c:v>9769672.7323780097</c:v>
+                </c:pt>
+                <c:pt idx="59">
+                  <c:v>9113302.0081548896</c:v>
+                </c:pt>
+                <c:pt idx="60">
+                  <c:v>8908424.5873359703</c:v>
+                </c:pt>
+                <c:pt idx="61">
+                  <c:v>6980347.5328304498</c:v>
+                </c:pt>
+                <c:pt idx="62">
+                  <c:v>10547658.4918481</c:v>
+                </c:pt>
+                <c:pt idx="63">
+                  <c:v>7893663.9331381703</c:v>
+                </c:pt>
+                <c:pt idx="64">
+                  <c:v>7872032.7382409796</c:v>
+                </c:pt>
+                <c:pt idx="65">
+                  <c:v>9625715.7394120805</c:v>
+                </c:pt>
+                <c:pt idx="66">
+                  <c:v>9473516.8728934303</c:v>
+                </c:pt>
+                <c:pt idx="67">
+                  <c:v>6771778.9840001902</c:v>
+                </c:pt>
+                <c:pt idx="68">
+                  <c:v>9345339.9283929896</c:v>
+                </c:pt>
+                <c:pt idx="69">
+                  <c:v>8749845.9247072209</c:v>
+                </c:pt>
+                <c:pt idx="70">
+                  <c:v>9261091.2615985703</c:v>
+                </c:pt>
+                <c:pt idx="71">
+                  <c:v>7223886.9166597603</c:v>
+                </c:pt>
+                <c:pt idx="72">
+                  <c:v>9094109.5142613109</c:v>
+                </c:pt>
+                <c:pt idx="73">
+                  <c:v>8086894.8526188498</c:v>
+                </c:pt>
+                <c:pt idx="74">
+                  <c:v>9608504.8194003105</c:v>
+                </c:pt>
+                <c:pt idx="75">
+                  <c:v>8167561.5776757495</c:v>
+                </c:pt>
+                <c:pt idx="76">
+                  <c:v>9162142.1501978301</c:v>
+                </c:pt>
+                <c:pt idx="77">
+                  <c:v>10179691.575688399</c:v>
+                </c:pt>
+                <c:pt idx="78">
+                  <c:v>10752796.858561199</c:v>
+                </c:pt>
+                <c:pt idx="79">
+                  <c:v>9900381.7571215592</c:v>
+                </c:pt>
+                <c:pt idx="80">
+                  <c:v>8339031.87166679</c:v>
+                </c:pt>
+                <c:pt idx="81">
+                  <c:v>7073649.2107376698</c:v>
+                </c:pt>
+                <c:pt idx="82">
+                  <c:v>7834860.1909906296</c:v>
+                </c:pt>
+                <c:pt idx="83">
+                  <c:v>7875096.2232888797</c:v>
+                </c:pt>
+                <c:pt idx="84">
+                  <c:v>6798184.0071253702</c:v>
+                </c:pt>
+                <c:pt idx="85">
+                  <c:v>5947294.9817488296</c:v>
+                </c:pt>
+                <c:pt idx="86">
+                  <c:v>9243918.2330143806</c:v>
+                </c:pt>
+                <c:pt idx="87">
+                  <c:v>10158971.5577267</c:v>
+                </c:pt>
+                <c:pt idx="88">
+                  <c:v>9430798.9976223409</c:v>
+                </c:pt>
+                <c:pt idx="89">
+                  <c:v>7920212.32179425</c:v>
+                </c:pt>
+                <c:pt idx="90">
+                  <c:v>7781097.7558316998</c:v>
+                </c:pt>
+                <c:pt idx="91">
+                  <c:v>8909239.7825026009</c:v>
+                </c:pt>
+                <c:pt idx="92">
+                  <c:v>8402575.5211147591</c:v>
+                </c:pt>
+                <c:pt idx="93">
+                  <c:v>9763055.8355248403</c:v>
+                </c:pt>
+                <c:pt idx="94">
+                  <c:v>8955216.1531386003</c:v>
+                </c:pt>
+                <c:pt idx="95">
+                  <c:v>9327090.2172295991</c:v>
+                </c:pt>
+                <c:pt idx="96">
+                  <c:v>11922100.641083799</c:v>
+                </c:pt>
+                <c:pt idx="97">
+                  <c:v>10177384.092680801</c:v>
+                </c:pt>
+                <c:pt idx="98">
+                  <c:v>10493422.551833799</c:v>
+                </c:pt>
+                <c:pt idx="99">
+                  <c:v>10571888.3616184</c:v>
+                </c:pt>
+                <c:pt idx="100">
+                  <c:v>11825761.163128899</c:v>
+                </c:pt>
+                <c:pt idx="101">
+                  <c:v>11766830.277974</c:v>
+                </c:pt>
+                <c:pt idx="102">
+                  <c:v>11358980.4696874</c:v>
+                </c:pt>
+                <c:pt idx="103">
+                  <c:v>10595959.5308841</c:v>
+                </c:pt>
+                <c:pt idx="104">
+                  <c:v>10612407.833329</c:v>
+                </c:pt>
+                <c:pt idx="105">
+                  <c:v>11111308.095895801</c:v>
+                </c:pt>
+                <c:pt idx="106">
+                  <c:v>11482697.728402199</c:v>
+                </c:pt>
+                <c:pt idx="107">
+                  <c:v>12108463.663791399</c:v>
+                </c:pt>
+                <c:pt idx="108">
+                  <c:v>12703801.894834301</c:v>
+                </c:pt>
+                <c:pt idx="109">
+                  <c:v>13554301.475640699</c:v>
+                </c:pt>
+                <c:pt idx="110">
+                  <c:v>10685609.0402385</c:v>
+                </c:pt>
+                <c:pt idx="111">
+                  <c:v>10060266.226524999</c:v>
+                </c:pt>
+                <c:pt idx="112">
+                  <c:v>13613881.8641649</c:v>
+                </c:pt>
+                <c:pt idx="113">
+                  <c:v>9865531.9064659998</c:v>
+                </c:pt>
+                <c:pt idx="114">
+                  <c:v>10216602.912662201</c:v>
+                </c:pt>
+                <c:pt idx="115">
+                  <c:v>10655126.5385125</c:v>
+                </c:pt>
+                <c:pt idx="116">
+                  <c:v>12130281.546378801</c:v>
+                </c:pt>
+                <c:pt idx="117">
+                  <c:v>13932043.1403326</c:v>
+                </c:pt>
+                <c:pt idx="118">
+                  <c:v>9715604.4035289604</c:v>
+                </c:pt>
+                <c:pt idx="119">
+                  <c:v>14176028.9669978</c:v>
+                </c:pt>
+                <c:pt idx="120">
+                  <c:v>11671773.8648635</c:v>
+                </c:pt>
+                <c:pt idx="121">
+                  <c:v>11033182.027128199</c:v>
+                </c:pt>
+                <c:pt idx="122">
+                  <c:v>11529359.8826105</c:v>
+                </c:pt>
+                <c:pt idx="123">
+                  <c:v>13431505.780205701</c:v>
+                </c:pt>
+                <c:pt idx="124">
+                  <c:v>9501113.5666300207</c:v>
+                </c:pt>
+                <c:pt idx="125">
+                  <c:v>10408189.666232301</c:v>
+                </c:pt>
+                <c:pt idx="126">
+                  <c:v>9508783.8172435593</c:v>
+                </c:pt>
+                <c:pt idx="127">
+                  <c:v>10907746.960920099</c:v>
+                </c:pt>
+                <c:pt idx="128">
+                  <c:v>10917398.9459047</c:v>
+                </c:pt>
+                <c:pt idx="129">
+                  <c:v>14160304.8346682</c:v>
+                </c:pt>
+                <c:pt idx="130">
+                  <c:v>13629440.0271507</c:v>
+                </c:pt>
+                <c:pt idx="131">
+                  <c:v>11985011.9607371</c:v>
+                </c:pt>
+                <c:pt idx="132">
+                  <c:v>12182880.250477999</c:v>
+                </c:pt>
+                <c:pt idx="133">
+                  <c:v>14521517.5582019</c:v>
+                </c:pt>
+                <c:pt idx="134">
+                  <c:v>13216335.4916855</c:v>
+                </c:pt>
+                <c:pt idx="135">
+                  <c:v>11703223.0840302</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-2915-4B42-8543-ED26A42B7887}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:marker val="1"/>
+        <c:smooth val="0"/>
+        <c:axId val="715829080"/>
+        <c:axId val="715823504"/>
+      </c:lineChart>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Run 5'!$A$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>BestIndividual_Training_Score</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="38100" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>'Run 5'!$A$2:$A$137</c:f>
+              <c:numCache>
+                <c:formatCode>#,##0.00</c:formatCode>
+                <c:ptCount val="136"/>
+                <c:pt idx="0">
+                  <c:v>0.9</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.9</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.9</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.9</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.9</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.9</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.9</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.9</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.9</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.9</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0.9</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0.9</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>0.9</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>0.9</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>0.9</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>0.9</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>0.9</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>0.9</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>0.9</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>0.9</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>0.9</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>0.9</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>0.9</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>0.9</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>0.9</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>0.9</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>0.9</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>0.9</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>0.9</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>0.9</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>0.9</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>0.9</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>0.9</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>0.9</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>0.9</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>0.9</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>0.9</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>0.9</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>0.9</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>0.9</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>0.9</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>0.9</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>0.9</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>0.9</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>0.9</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>0.9</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>0.9</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>0.9</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>0.9</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>0.9</c:v>
+                </c:pt>
+                <c:pt idx="50">
+                  <c:v>0.9</c:v>
+                </c:pt>
+                <c:pt idx="51">
+                  <c:v>0.9</c:v>
+                </c:pt>
+                <c:pt idx="52">
+                  <c:v>0.9</c:v>
+                </c:pt>
+                <c:pt idx="53">
+                  <c:v>0.9</c:v>
+                </c:pt>
+                <c:pt idx="54">
+                  <c:v>0.9</c:v>
+                </c:pt>
+                <c:pt idx="55">
+                  <c:v>0.9</c:v>
+                </c:pt>
+                <c:pt idx="56">
+                  <c:v>0.9</c:v>
+                </c:pt>
+                <c:pt idx="57">
+                  <c:v>0.9</c:v>
+                </c:pt>
+                <c:pt idx="58">
+                  <c:v>0.9</c:v>
+                </c:pt>
+                <c:pt idx="59">
+                  <c:v>0.9</c:v>
+                </c:pt>
+                <c:pt idx="60">
+                  <c:v>0.9</c:v>
+                </c:pt>
+                <c:pt idx="61">
+                  <c:v>0.9</c:v>
+                </c:pt>
+                <c:pt idx="62">
+                  <c:v>0.9</c:v>
+                </c:pt>
+                <c:pt idx="63">
+                  <c:v>0.9</c:v>
+                </c:pt>
+                <c:pt idx="64">
+                  <c:v>0.9</c:v>
+                </c:pt>
+                <c:pt idx="65">
+                  <c:v>0.9</c:v>
+                </c:pt>
+                <c:pt idx="66">
+                  <c:v>0.9</c:v>
+                </c:pt>
+                <c:pt idx="67">
+                  <c:v>0.9</c:v>
+                </c:pt>
+                <c:pt idx="68">
+                  <c:v>0.9</c:v>
+                </c:pt>
+                <c:pt idx="69">
+                  <c:v>0.9</c:v>
+                </c:pt>
+                <c:pt idx="70">
+                  <c:v>0.9</c:v>
+                </c:pt>
+                <c:pt idx="71">
+                  <c:v>0.9</c:v>
+                </c:pt>
+                <c:pt idx="72">
+                  <c:v>0.9</c:v>
+                </c:pt>
+                <c:pt idx="73">
+                  <c:v>0.9</c:v>
+                </c:pt>
+                <c:pt idx="74">
+                  <c:v>0.9</c:v>
+                </c:pt>
+                <c:pt idx="75">
+                  <c:v>0.9</c:v>
+                </c:pt>
+                <c:pt idx="76">
+                  <c:v>0.9</c:v>
+                </c:pt>
+                <c:pt idx="77">
+                  <c:v>0.9</c:v>
+                </c:pt>
+                <c:pt idx="78">
+                  <c:v>0.9</c:v>
+                </c:pt>
+                <c:pt idx="79">
+                  <c:v>0.9</c:v>
+                </c:pt>
+                <c:pt idx="80">
+                  <c:v>0.9</c:v>
+                </c:pt>
+                <c:pt idx="81">
+                  <c:v>0.9</c:v>
+                </c:pt>
+                <c:pt idx="82">
+                  <c:v>0.9</c:v>
+                </c:pt>
+                <c:pt idx="83">
+                  <c:v>0.9</c:v>
+                </c:pt>
+                <c:pt idx="84">
+                  <c:v>0.9</c:v>
+                </c:pt>
+                <c:pt idx="85">
+                  <c:v>0.9</c:v>
+                </c:pt>
+                <c:pt idx="86">
+                  <c:v>0.9</c:v>
+                </c:pt>
+                <c:pt idx="87">
+                  <c:v>0.9</c:v>
+                </c:pt>
+                <c:pt idx="88">
+                  <c:v>0.9</c:v>
+                </c:pt>
+                <c:pt idx="89">
+                  <c:v>0.9</c:v>
+                </c:pt>
+                <c:pt idx="90">
+                  <c:v>0.9</c:v>
+                </c:pt>
+                <c:pt idx="91">
+                  <c:v>0.9</c:v>
+                </c:pt>
+                <c:pt idx="92">
+                  <c:v>0.9</c:v>
+                </c:pt>
+                <c:pt idx="93">
+                  <c:v>0.9</c:v>
+                </c:pt>
+                <c:pt idx="94">
+                  <c:v>0.9</c:v>
+                </c:pt>
+                <c:pt idx="95">
+                  <c:v>0.9</c:v>
+                </c:pt>
+                <c:pt idx="96">
+                  <c:v>0.9</c:v>
+                </c:pt>
+                <c:pt idx="97">
+                  <c:v>0.9</c:v>
+                </c:pt>
+                <c:pt idx="98">
+                  <c:v>0.9</c:v>
+                </c:pt>
+                <c:pt idx="99">
+                  <c:v>0.9</c:v>
+                </c:pt>
+                <c:pt idx="100">
+                  <c:v>0.9</c:v>
+                </c:pt>
+                <c:pt idx="101">
+                  <c:v>0.9</c:v>
+                </c:pt>
+                <c:pt idx="102">
+                  <c:v>0.9</c:v>
+                </c:pt>
+                <c:pt idx="103">
+                  <c:v>0.9</c:v>
+                </c:pt>
+                <c:pt idx="104">
+                  <c:v>0.9</c:v>
+                </c:pt>
+                <c:pt idx="105">
+                  <c:v>0.9</c:v>
+                </c:pt>
+                <c:pt idx="106">
+                  <c:v>0.9</c:v>
+                </c:pt>
+                <c:pt idx="107">
+                  <c:v>0.9</c:v>
+                </c:pt>
+                <c:pt idx="108">
+                  <c:v>0.9</c:v>
+                </c:pt>
+                <c:pt idx="109">
+                  <c:v>0.9</c:v>
+                </c:pt>
+                <c:pt idx="110">
+                  <c:v>0.9</c:v>
+                </c:pt>
+                <c:pt idx="111">
+                  <c:v>0.9</c:v>
+                </c:pt>
+                <c:pt idx="112">
+                  <c:v>0.9</c:v>
+                </c:pt>
+                <c:pt idx="113">
+                  <c:v>0.9</c:v>
+                </c:pt>
+                <c:pt idx="114">
+                  <c:v>0.9</c:v>
+                </c:pt>
+                <c:pt idx="115">
+                  <c:v>0.9</c:v>
+                </c:pt>
+                <c:pt idx="116">
+                  <c:v>0.9</c:v>
+                </c:pt>
+                <c:pt idx="117">
+                  <c:v>0.9</c:v>
+                </c:pt>
+                <c:pt idx="118">
+                  <c:v>0.9</c:v>
+                </c:pt>
+                <c:pt idx="119">
+                  <c:v>0.9</c:v>
+                </c:pt>
+                <c:pt idx="120">
+                  <c:v>0.9</c:v>
+                </c:pt>
+                <c:pt idx="121">
+                  <c:v>0.9</c:v>
+                </c:pt>
+                <c:pt idx="122">
+                  <c:v>0.9</c:v>
+                </c:pt>
+                <c:pt idx="123">
+                  <c:v>0.9</c:v>
+                </c:pt>
+                <c:pt idx="124">
+                  <c:v>0.9</c:v>
+                </c:pt>
+                <c:pt idx="125">
+                  <c:v>0.9</c:v>
+                </c:pt>
+                <c:pt idx="126">
+                  <c:v>0.9</c:v>
+                </c:pt>
+                <c:pt idx="127">
+                  <c:v>0.9</c:v>
+                </c:pt>
+                <c:pt idx="128">
+                  <c:v>0.9</c:v>
+                </c:pt>
+                <c:pt idx="129">
+                  <c:v>0.9</c:v>
+                </c:pt>
+                <c:pt idx="130">
+                  <c:v>0.9</c:v>
+                </c:pt>
+                <c:pt idx="131">
+                  <c:v>0.9</c:v>
+                </c:pt>
+                <c:pt idx="132">
+                  <c:v>0.9</c:v>
+                </c:pt>
+                <c:pt idx="133">
+                  <c:v>0.9</c:v>
+                </c:pt>
+                <c:pt idx="134">
+                  <c:v>0.9</c:v>
+                </c:pt>
+                <c:pt idx="135">
+                  <c:v>0.9</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-2915-4B42-8543-ED26A42B7887}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -4788,6 +6026,46 @@
 </file>
 
 <file path=xl/charts/colors4.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors5.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
   <a:schemeClr val="accent2"/>
@@ -6827,6 +8105,506 @@
 </cs:chartStyle>
 </file>
 
+<file path=xl/charts/style5.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="235">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200" cap="all"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" b="0" kern="1200" cap="none" spc="0" normalizeH="0" baseline="0"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="38100" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="8"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:prstDash val="dash"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:prstDash val="dash"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="major">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="2000" b="0" kern="1200" cap="none" spc="0" normalizeH="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
@@ -6975,6 +8753,49 @@
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
               <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{6677EAB1-3090-4CC8-A23D-EB7582065BD0}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing5.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>561975</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>30</xdr:col>
+      <xdr:colOff>409575</xdr:colOff>
+      <xdr:row>37</xdr:row>
+      <xdr:rowOff>19050</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{1FB7CE0A-C722-4869-AEC9-CAB6F7648F41}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -11579,7 +13400,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{46279A08-E6DD-4519-895C-48ADC6AEC5C3}">
   <dimension ref="A1:D137"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
       <selection activeCell="B1" sqref="B1:B110"/>
     </sheetView>
   </sheetViews>
@@ -13129,4 +14950,1996 @@
   <pageSetup orientation="portrait" r:id="rId1"/>
   <drawing r:id="rId2"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0931CFBE-5882-45B2-BAF9-2F14C4CFFC9C}">
+  <dimension ref="A1:D178"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="B1" sqref="B1:B178"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="27.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="22.109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="8.88671875" style="2"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A2" s="1">
+        <v>0.9</v>
+      </c>
+      <c r="B2" s="1">
+        <v>466828517.77193397</v>
+      </c>
+      <c r="D2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A3" s="1">
+        <v>0.9</v>
+      </c>
+      <c r="B3" s="1">
+        <v>530838032.318699</v>
+      </c>
+      <c r="C3" s="2">
+        <f>(B3-B2)/B2</f>
+        <v>0.13711569047295533</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A4" s="1">
+        <v>0.9</v>
+      </c>
+      <c r="B4" s="1">
+        <v>370939279.01228499</v>
+      </c>
+      <c r="C4" s="2">
+        <f t="shared" ref="C4:C71" si="0">(B4-B3)/B3</f>
+        <v>-0.30121947481414757</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A5" s="1">
+        <v>0.9</v>
+      </c>
+      <c r="B5" s="1">
+        <v>287802144.25176901</v>
+      </c>
+      <c r="C5" s="2">
+        <f t="shared" si="0"/>
+        <v>-0.22412599437268707</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A6" s="1">
+        <v>0.9</v>
+      </c>
+      <c r="B6" s="1">
+        <v>248506795.35284099</v>
+      </c>
+      <c r="C6" s="2">
+        <f t="shared" si="0"/>
+        <v>-0.13653598377832962</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A7" s="1">
+        <v>0.9</v>
+      </c>
+      <c r="B7" s="1">
+        <v>219063937.33587301</v>
+      </c>
+      <c r="C7" s="2">
+        <f t="shared" si="0"/>
+        <v>-0.11847908615602927</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A8" s="1">
+        <v>0.9</v>
+      </c>
+      <c r="B8" s="1">
+        <v>138580850.40472999</v>
+      </c>
+      <c r="C8" s="2">
+        <f t="shared" si="0"/>
+        <v>-0.36739541847887458</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A9" s="1">
+        <v>0.9</v>
+      </c>
+      <c r="B9" s="1">
+        <v>143843237.58303201</v>
+      </c>
+      <c r="C9" s="2">
+        <f t="shared" si="0"/>
+        <v>3.7973408035331307E-2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A10" s="1">
+        <v>0.9</v>
+      </c>
+      <c r="B10" s="1">
+        <v>84740447.071308702</v>
+      </c>
+      <c r="C10" s="2">
+        <f t="shared" si="0"/>
+        <v>-0.41088334429073758</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A11" s="1">
+        <v>0.9</v>
+      </c>
+      <c r="B11" s="1">
+        <v>50829498.939668</v>
+      </c>
+      <c r="C11" s="2">
+        <f t="shared" si="0"/>
+        <v>-0.40017428870896554</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A12" s="1">
+        <v>0.9</v>
+      </c>
+      <c r="B12" s="1">
+        <v>45881076.786539502</v>
+      </c>
+      <c r="C12" s="2">
+        <f t="shared" si="0"/>
+        <v>-9.7353353000823789E-2</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A13" s="1">
+        <v>0.9</v>
+      </c>
+      <c r="B13" s="1">
+        <v>36884020.090438202</v>
+      </c>
+      <c r="C13" s="2">
+        <f t="shared" si="0"/>
+        <v>-0.19609515134005831</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A14" s="1">
+        <v>0.9</v>
+      </c>
+      <c r="B14" s="1">
+        <v>51961728.485883802</v>
+      </c>
+      <c r="C14" s="2">
+        <f t="shared" si="0"/>
+        <v>0.40878701287103841</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A15" s="1">
+        <v>0.9</v>
+      </c>
+      <c r="B15" s="1">
+        <v>23300455.492954198</v>
+      </c>
+      <c r="C15" s="2">
+        <f t="shared" si="0"/>
+        <v>-0.55158428766887302</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A16" s="1">
+        <v>0.9</v>
+      </c>
+      <c r="B16" s="1">
+        <v>18673919.715530898</v>
+      </c>
+      <c r="C16" s="2">
+        <f t="shared" si="0"/>
+        <v>-0.19855988561349427</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A17" s="1">
+        <v>0.9</v>
+      </c>
+      <c r="B17" s="1">
+        <v>22387443.221550301</v>
+      </c>
+      <c r="C17" s="2">
+        <f t="shared" si="0"/>
+        <v>0.19886149038816445</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A18" s="1">
+        <v>0.9</v>
+      </c>
+      <c r="B18" s="1">
+        <v>21727289.674221501</v>
+      </c>
+      <c r="C18" s="2">
+        <f t="shared" si="0"/>
+        <v>-2.9487670422915099E-2</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A19" s="1">
+        <v>0.9</v>
+      </c>
+      <c r="B19" s="1">
+        <v>25023973.804324102</v>
+      </c>
+      <c r="C19" s="2">
+        <f t="shared" si="0"/>
+        <v>0.15173011358218211</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A20" s="1">
+        <v>0.9</v>
+      </c>
+      <c r="B20" s="1">
+        <v>28457230.8928365</v>
+      </c>
+      <c r="C20" s="2">
+        <f t="shared" si="0"/>
+        <v>0.13719871653314858</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A21" s="1">
+        <v>0.9</v>
+      </c>
+      <c r="B21" s="1">
+        <v>20707684.776952799</v>
+      </c>
+      <c r="C21" s="2">
+        <f t="shared" si="0"/>
+        <v>-0.27232256522311465</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A22" s="1">
+        <v>0.9</v>
+      </c>
+      <c r="B22" s="1">
+        <v>14613419.506552</v>
+      </c>
+      <c r="C22" s="2">
+        <f t="shared" si="0"/>
+        <v>-0.29429969289389529</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A23" s="1">
+        <v>0.9</v>
+      </c>
+      <c r="B23" s="1">
+        <v>14221412.3280422</v>
+      </c>
+      <c r="C23" s="2">
+        <f t="shared" si="0"/>
+        <v>-2.6825150563428456E-2</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A24" s="1">
+        <v>0.9</v>
+      </c>
+      <c r="B24" s="1">
+        <v>13799211.4196239</v>
+      </c>
+      <c r="C24" s="2">
+        <f t="shared" si="0"/>
+        <v>-2.9687691959102504E-2</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A25" s="1">
+        <v>0.9</v>
+      </c>
+      <c r="B25" s="1">
+        <v>10991181.9397649</v>
+      </c>
+      <c r="C25" s="2">
+        <f t="shared" si="0"/>
+        <v>-0.20349202533890401</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A26" s="1">
+        <v>0.9</v>
+      </c>
+      <c r="B26" s="1">
+        <v>7827470.0282455198</v>
+      </c>
+      <c r="C26" s="2">
+        <f t="shared" si="0"/>
+        <v>-0.28784091909837423</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A27" s="1">
+        <v>0.9</v>
+      </c>
+      <c r="B27" s="1">
+        <v>11158393.262985799</v>
+      </c>
+      <c r="C27" s="2">
+        <f t="shared" si="0"/>
+        <v>0.42554276448464229</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A28" s="1">
+        <v>0.9</v>
+      </c>
+      <c r="B28" s="1">
+        <v>11228451.7032403</v>
+      </c>
+      <c r="C28" s="2">
+        <f t="shared" si="0"/>
+        <v>6.2785419552199642E-3</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A29" s="1">
+        <v>0.9</v>
+      </c>
+      <c r="B29" s="1">
+        <v>6580154.4599233698</v>
+      </c>
+      <c r="C29" s="2">
+        <f t="shared" si="0"/>
+        <v>-0.41397490644017526</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A30" s="1">
+        <v>0.9</v>
+      </c>
+      <c r="B30" s="1">
+        <v>5694237.1644831495</v>
+      </c>
+      <c r="C30" s="2">
+        <f t="shared" si="0"/>
+        <v>-0.13463472640892041</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A31" s="1">
+        <v>0.9</v>
+      </c>
+      <c r="B31" s="1">
+        <v>7602025.9353936203</v>
+      </c>
+      <c r="C31" s="2">
+        <f t="shared" si="0"/>
+        <v>0.33503851627571529</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A32" s="1">
+        <v>0.9</v>
+      </c>
+      <c r="B32" s="1">
+        <v>7774374.1914764</v>
+      </c>
+      <c r="C32" s="2">
+        <f>(B32-B30)/B30</f>
+        <v>0.36530565322564307</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A33" s="1">
+        <v>0.9</v>
+      </c>
+      <c r="B33" s="1">
+        <v>8887725.9137989692</v>
+      </c>
+      <c r="C33" s="2">
+        <f t="shared" si="0"/>
+        <v>0.14320788978014667</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A34" s="1">
+        <v>0.9</v>
+      </c>
+      <c r="B34" s="1">
+        <v>8256218.8607965596</v>
+      </c>
+      <c r="C34" s="2">
+        <f t="shared" si="0"/>
+        <v>-7.1053839770411895E-2</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A35" s="1">
+        <v>0.9</v>
+      </c>
+      <c r="B35" s="1">
+        <v>9346117.9973511808</v>
+      </c>
+      <c r="C35" s="2">
+        <f t="shared" si="0"/>
+        <v>0.13200947733227456</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A36" s="1">
+        <v>0.9</v>
+      </c>
+      <c r="B36" s="1">
+        <v>8787415.66559745</v>
+      </c>
+      <c r="C36" s="2">
+        <f t="shared" si="0"/>
+        <v>-5.9779079604181627E-2</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A37" s="1">
+        <v>0.9</v>
+      </c>
+      <c r="B37" s="1">
+        <v>6106326.5948853297</v>
+      </c>
+      <c r="C37" s="2">
+        <f t="shared" si="0"/>
+        <v>-0.30510552507587962</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A38" s="1">
+        <v>0.9</v>
+      </c>
+      <c r="B38" s="1">
+        <v>10212688.134928999</v>
+      </c>
+      <c r="C38" s="2">
+        <f t="shared" si="0"/>
+        <v>0.67247656610492557</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A39" s="1">
+        <v>0.9</v>
+      </c>
+      <c r="B39" s="1">
+        <v>12426570.6614541</v>
+      </c>
+      <c r="C39" s="2">
+        <f t="shared" si="0"/>
+        <v>0.21677764926094964</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A40" s="1">
+        <v>0.9</v>
+      </c>
+      <c r="B40" s="1">
+        <v>7555045.1385022402</v>
+      </c>
+      <c r="C40" s="2">
+        <f t="shared" si="0"/>
+        <v>-0.39202493235425068</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A41" s="1">
+        <v>0.9</v>
+      </c>
+      <c r="B41" s="1">
+        <v>5974048.4311196003</v>
+      </c>
+      <c r="C41" s="2">
+        <f t="shared" si="0"/>
+        <v>-0.20926370106321648</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A42" s="1">
+        <v>0.9</v>
+      </c>
+      <c r="B42" s="1">
+        <v>5586637.8612419497</v>
+      </c>
+      <c r="C42" s="2">
+        <f t="shared" si="0"/>
+        <v>-6.4848916834952031E-2</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A43" s="1">
+        <v>0.9</v>
+      </c>
+      <c r="B43" s="1">
+        <v>6283506.2962794499</v>
+      </c>
+      <c r="C43" s="2">
+        <f t="shared" si="0"/>
+        <v>0.12473842986532536</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A44" s="1">
+        <v>0.9</v>
+      </c>
+      <c r="B44" s="1">
+        <v>7465580.1919447798</v>
+      </c>
+      <c r="C44" s="2">
+        <f t="shared" si="0"/>
+        <v>0.18812329294000263</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A45" s="1">
+        <v>0.9</v>
+      </c>
+      <c r="B45" s="1">
+        <v>6318532.6921694595</v>
+      </c>
+      <c r="C45" s="2">
+        <f t="shared" si="0"/>
+        <v>-0.15364478986013208</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A46" s="1">
+        <v>0.9</v>
+      </c>
+      <c r="B46" s="1">
+        <v>7805773.7823088001</v>
+      </c>
+      <c r="C46" s="2">
+        <f t="shared" si="0"/>
+        <v>0.23537760467433752</v>
+      </c>
+    </row>
+    <row r="47" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A47" s="1">
+        <v>0.9</v>
+      </c>
+      <c r="B47" s="1">
+        <v>8864587.4604190998</v>
+      </c>
+      <c r="C47" s="2">
+        <f t="shared" si="0"/>
+        <v>0.13564493510047926</v>
+      </c>
+    </row>
+    <row r="48" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A48" s="1">
+        <v>0.9</v>
+      </c>
+      <c r="B48" s="1">
+        <v>6943692.4762246301</v>
+      </c>
+      <c r="C48" s="2">
+        <f t="shared" si="0"/>
+        <v>-0.21669310532175104</v>
+      </c>
+    </row>
+    <row r="49" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A49" s="1">
+        <v>0.9</v>
+      </c>
+      <c r="B49" s="1">
+        <v>5018393.19882455</v>
+      </c>
+      <c r="C49" s="2">
+        <f t="shared" si="0"/>
+        <v>-0.27727312002833521</v>
+      </c>
+    </row>
+    <row r="50" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A50" s="1">
+        <v>0.9</v>
+      </c>
+      <c r="B50" s="1">
+        <v>5936583.2975150002</v>
+      </c>
+      <c r="C50" s="2">
+        <f t="shared" si="0"/>
+        <v>0.18296495756958947</v>
+      </c>
+    </row>
+    <row r="51" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A51" s="1">
+        <v>0.9</v>
+      </c>
+      <c r="B51" s="1">
+        <v>8225772.5154284202</v>
+      </c>
+      <c r="C51" s="2">
+        <f t="shared" si="0"/>
+        <v>0.38560719241851688</v>
+      </c>
+    </row>
+    <row r="52" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A52" s="1">
+        <v>0.9</v>
+      </c>
+      <c r="B52" s="1">
+        <v>6907093.6067347797</v>
+      </c>
+      <c r="C52" s="2">
+        <f t="shared" si="0"/>
+        <v>-0.16031064635209646</v>
+      </c>
+    </row>
+    <row r="53" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A53" s="1">
+        <v>0.9</v>
+      </c>
+      <c r="B53" s="1">
+        <v>7761654.1245476799</v>
+      </c>
+      <c r="C53" s="2">
+        <f t="shared" si="0"/>
+        <v>0.12372215673748199</v>
+      </c>
+    </row>
+    <row r="54" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A54" s="1">
+        <v>0.9</v>
+      </c>
+      <c r="B54" s="1">
+        <v>8243263.69838861</v>
+      </c>
+      <c r="C54" s="2">
+        <f t="shared" si="0"/>
+        <v>6.2049862840157996E-2</v>
+      </c>
+    </row>
+    <row r="55" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A55" s="1">
+        <v>0.9</v>
+      </c>
+      <c r="B55" s="1">
+        <v>8773894.6373157408</v>
+      </c>
+      <c r="C55" s="2">
+        <f t="shared" si="0"/>
+        <v>6.4371462365186538E-2</v>
+      </c>
+    </row>
+    <row r="56" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A56" s="1">
+        <v>0.9</v>
+      </c>
+      <c r="B56" s="1">
+        <v>8716087.0516568795</v>
+      </c>
+      <c r="C56" s="2">
+        <f t="shared" si="0"/>
+        <v>-6.5885889959292699E-3</v>
+      </c>
+    </row>
+    <row r="57" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A57" s="1">
+        <v>0.9</v>
+      </c>
+      <c r="B57" s="1">
+        <v>9526198.3536674306</v>
+      </c>
+      <c r="C57" s="2">
+        <f t="shared" si="0"/>
+        <v>9.2944379422708209E-2</v>
+      </c>
+    </row>
+    <row r="58" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A58" s="1">
+        <v>0.9</v>
+      </c>
+      <c r="B58" s="1">
+        <v>11499360.383852899</v>
+      </c>
+      <c r="C58" s="2">
+        <f t="shared" si="0"/>
+        <v>0.20713005933010342</v>
+      </c>
+    </row>
+    <row r="59" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A59" s="1">
+        <v>0.9</v>
+      </c>
+      <c r="B59" s="1">
+        <v>11166373.0106229</v>
+      </c>
+      <c r="C59" s="2">
+        <f t="shared" si="0"/>
+        <v>-2.8957034314497289E-2</v>
+      </c>
+    </row>
+    <row r="60" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A60" s="1">
+        <v>0.9</v>
+      </c>
+      <c r="B60" s="1">
+        <v>9769672.7323780097</v>
+      </c>
+      <c r="C60" s="2">
+        <f t="shared" si="0"/>
+        <v>-0.12508092618043193</v>
+      </c>
+    </row>
+    <row r="61" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A61" s="1">
+        <v>0.9</v>
+      </c>
+      <c r="B61" s="1">
+        <v>9113302.0081548896</v>
+      </c>
+      <c r="C61" s="2">
+        <f t="shared" si="0"/>
+        <v>-6.7184514998933312E-2</v>
+      </c>
+    </row>
+    <row r="62" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A62" s="1">
+        <v>0.9</v>
+      </c>
+      <c r="B62" s="1">
+        <v>8908424.5873359703</v>
+      </c>
+      <c r="C62" s="2">
+        <f t="shared" si="0"/>
+        <v>-2.2481140275565113E-2</v>
+      </c>
+    </row>
+    <row r="63" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A63" s="1">
+        <v>0.9</v>
+      </c>
+      <c r="B63" s="1">
+        <v>6980347.5328304498</v>
+      </c>
+      <c r="C63" s="2">
+        <f t="shared" si="0"/>
+        <v>-0.21643299952793388</v>
+      </c>
+    </row>
+    <row r="64" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A64" s="1">
+        <v>0.9</v>
+      </c>
+      <c r="B64" s="1">
+        <v>10547658.4918481</v>
+      </c>
+      <c r="C64" s="2">
+        <f t="shared" si="0"/>
+        <v>0.51105062351689923</v>
+      </c>
+    </row>
+    <row r="65" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A65" s="1">
+        <v>0.9</v>
+      </c>
+      <c r="B65" s="1">
+        <v>7893663.9331381703</v>
+      </c>
+      <c r="C65" s="2">
+        <f t="shared" si="0"/>
+        <v>-0.251619310651848</v>
+      </c>
+    </row>
+    <row r="66" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A66" s="1">
+        <v>0.9</v>
+      </c>
+      <c r="B66" s="1">
+        <v>7872032.7382409796</v>
+      </c>
+      <c r="C66" s="2">
+        <f t="shared" si="0"/>
+        <v>-2.7403237685837312E-3</v>
+      </c>
+    </row>
+    <row r="67" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A67" s="1">
+        <v>0.9</v>
+      </c>
+      <c r="B67" s="1">
+        <v>9625715.7394120805</v>
+      </c>
+      <c r="C67" s="2">
+        <f t="shared" si="0"/>
+        <v>0.2227738450136279</v>
+      </c>
+    </row>
+    <row r="68" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A68" s="1">
+        <v>0.9</v>
+      </c>
+      <c r="B68" s="1">
+        <v>9473516.8728934303</v>
+      </c>
+      <c r="C68" s="2">
+        <f t="shared" si="0"/>
+        <v>-1.5811693451062394E-2</v>
+      </c>
+    </row>
+    <row r="69" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A69" s="1">
+        <v>0.9</v>
+      </c>
+      <c r="B69" s="1">
+        <v>6771778.9840001902</v>
+      </c>
+      <c r="C69" s="2">
+        <f t="shared" si="0"/>
+        <v>-0.28518848123063162</v>
+      </c>
+    </row>
+    <row r="70" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A70" s="1">
+        <v>0.9</v>
+      </c>
+      <c r="B70" s="1">
+        <v>9345339.9283929896</v>
+      </c>
+      <c r="C70" s="2">
+        <f t="shared" si="0"/>
+        <v>0.38004207616246782</v>
+      </c>
+    </row>
+    <row r="71" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A71" s="1">
+        <v>0.9</v>
+      </c>
+      <c r="B71" s="1">
+        <v>8749845.9247072209</v>
+      </c>
+      <c r="C71" s="2">
+        <f t="shared" si="0"/>
+        <v>-6.3720956995533165E-2</v>
+      </c>
+    </row>
+    <row r="72" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A72" s="1">
+        <v>0.9</v>
+      </c>
+      <c r="B72" s="1">
+        <v>9261091.2615985703</v>
+      </c>
+      <c r="C72" s="2">
+        <f t="shared" ref="C72:C135" si="1">(B72-B71)/B71</f>
+        <v>5.8429067356229616E-2</v>
+      </c>
+    </row>
+    <row r="73" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A73" s="1">
+        <v>0.9</v>
+      </c>
+      <c r="B73" s="1">
+        <v>7223886.9166597603</v>
+      </c>
+      <c r="C73" s="2">
+        <f t="shared" si="1"/>
+        <v>-0.21997454591405952</v>
+      </c>
+    </row>
+    <row r="74" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A74" s="1">
+        <v>0.9</v>
+      </c>
+      <c r="B74" s="1">
+        <v>9094109.5142613109</v>
+      </c>
+      <c r="C74" s="2">
+        <f t="shared" si="1"/>
+        <v>0.25889422400680651</v>
+      </c>
+    </row>
+    <row r="75" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A75" s="1">
+        <v>0.9</v>
+      </c>
+      <c r="B75" s="1">
+        <v>8086894.8526188498</v>
+      </c>
+      <c r="C75" s="2">
+        <f t="shared" si="1"/>
+        <v>-0.11075462199602445</v>
+      </c>
+    </row>
+    <row r="76" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A76" s="1">
+        <v>0.9</v>
+      </c>
+      <c r="B76" s="1">
+        <v>9608504.8194003105</v>
+      </c>
+      <c r="C76" s="2">
+        <f t="shared" si="1"/>
+        <v>0.18815750600351933</v>
+      </c>
+    </row>
+    <row r="77" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A77" s="1">
+        <v>0.9</v>
+      </c>
+      <c r="B77" s="1">
+        <v>8167561.5776757495</v>
+      </c>
+      <c r="C77" s="2">
+        <f t="shared" si="1"/>
+        <v>-0.14996539719844712</v>
+      </c>
+    </row>
+    <row r="78" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A78" s="1">
+        <v>0.9</v>
+      </c>
+      <c r="B78" s="1">
+        <v>9162142.1501978301</v>
+      </c>
+      <c r="C78" s="2">
+        <f t="shared" si="1"/>
+        <v>0.1217720323334384</v>
+      </c>
+    </row>
+    <row r="79" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A79" s="1">
+        <v>0.9</v>
+      </c>
+      <c r="B79" s="1">
+        <v>10179691.575688399</v>
+      </c>
+      <c r="C79" s="2">
+        <f t="shared" si="1"/>
+        <v>0.11106020937129842</v>
+      </c>
+    </row>
+    <row r="80" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A80" s="1">
+        <v>0.9</v>
+      </c>
+      <c r="B80" s="1">
+        <v>10752796.858561199</v>
+      </c>
+      <c r="C80" s="2">
+        <f t="shared" si="1"/>
+        <v>5.6298884756146812E-2</v>
+      </c>
+    </row>
+    <row r="81" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A81" s="1">
+        <v>0.9</v>
+      </c>
+      <c r="B81" s="1">
+        <v>9900381.7571215592</v>
+      </c>
+      <c r="C81" s="2">
+        <f t="shared" si="1"/>
+        <v>-7.9273803146477292E-2</v>
+      </c>
+    </row>
+    <row r="82" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A82" s="1">
+        <v>0.9</v>
+      </c>
+      <c r="B82" s="1">
+        <v>8339031.87166679</v>
+      </c>
+      <c r="C82" s="2">
+        <f t="shared" si="1"/>
+        <v>-0.15770602828841992</v>
+      </c>
+    </row>
+    <row r="83" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A83" s="1">
+        <v>0.9</v>
+      </c>
+      <c r="B83" s="1">
+        <v>7073649.2107376698</v>
+      </c>
+      <c r="C83" s="2">
+        <f t="shared" si="1"/>
+        <v>-0.15174215429352927</v>
+      </c>
+    </row>
+    <row r="84" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A84" s="1">
+        <v>0.9</v>
+      </c>
+      <c r="B84" s="1">
+        <v>7834860.1909906296</v>
+      </c>
+      <c r="C84" s="2">
+        <f t="shared" si="1"/>
+        <v>0.10761220376852382</v>
+      </c>
+    </row>
+    <row r="85" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A85" s="1">
+        <v>0.9</v>
+      </c>
+      <c r="B85" s="1">
+        <v>7875096.2232888797</v>
+      </c>
+      <c r="C85" s="2">
+        <f t="shared" si="1"/>
+        <v>5.1355137574143148E-3</v>
+      </c>
+    </row>
+    <row r="86" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A86" s="1">
+        <v>0.9</v>
+      </c>
+      <c r="B86" s="1">
+        <v>6798184.0071253702</v>
+      </c>
+      <c r="C86" s="2">
+        <f t="shared" si="1"/>
+        <v>-0.13674908669417607</v>
+      </c>
+    </row>
+    <row r="87" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A87" s="1">
+        <v>0.9</v>
+      </c>
+      <c r="B87" s="1">
+        <v>5947294.9817488296</v>
+      </c>
+      <c r="C87" s="2">
+        <f t="shared" si="1"/>
+        <v>-0.12516416508948561</v>
+      </c>
+    </row>
+    <row r="88" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A88" s="1">
+        <v>0.9</v>
+      </c>
+      <c r="B88" s="1">
+        <v>9243918.2330143806</v>
+      </c>
+      <c r="C88" s="2">
+        <f t="shared" si="1"/>
+        <v>0.55430632941232783</v>
+      </c>
+    </row>
+    <row r="89" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A89" s="1">
+        <v>0.9</v>
+      </c>
+      <c r="B89" s="1">
+        <v>10158971.5577267</v>
+      </c>
+      <c r="C89" s="2">
+        <f t="shared" si="1"/>
+        <v>9.898976836945976E-2</v>
+      </c>
+    </row>
+    <row r="90" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A90" s="1">
+        <v>0.9</v>
+      </c>
+      <c r="B90" s="1">
+        <v>9430798.9976223409</v>
+      </c>
+      <c r="C90" s="2">
+        <f t="shared" si="1"/>
+        <v>-7.1677783126632172E-2</v>
+      </c>
+    </row>
+    <row r="91" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A91" s="1">
+        <v>0.9</v>
+      </c>
+      <c r="B91" s="1">
+        <v>7920212.32179425</v>
+      </c>
+      <c r="C91" s="2">
+        <f t="shared" si="1"/>
+        <v>-0.16017589561700282</v>
+      </c>
+    </row>
+    <row r="92" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A92" s="1">
+        <v>0.9</v>
+      </c>
+      <c r="B92" s="1">
+        <v>7781097.7558316998</v>
+      </c>
+      <c r="C92" s="2">
+        <f t="shared" si="1"/>
+        <v>-1.7564499575313801E-2</v>
+      </c>
+    </row>
+    <row r="93" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A93" s="1">
+        <v>0.9</v>
+      </c>
+      <c r="B93" s="1">
+        <v>8909239.7825026009</v>
+      </c>
+      <c r="C93" s="2">
+        <f t="shared" si="1"/>
+        <v>0.14498494455045144</v>
+      </c>
+    </row>
+    <row r="94" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A94" s="1">
+        <v>0.9</v>
+      </c>
+      <c r="B94" s="1">
+        <v>8402575.5211147591</v>
+      </c>
+      <c r="C94" s="2">
+        <f t="shared" si="1"/>
+        <v>-5.6869528013255476E-2</v>
+      </c>
+    </row>
+    <row r="95" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A95" s="1">
+        <v>0.9</v>
+      </c>
+      <c r="B95" s="1">
+        <v>9763055.8355248403</v>
+      </c>
+      <c r="C95" s="2">
+        <f t="shared" si="1"/>
+        <v>0.16191229831750301</v>
+      </c>
+    </row>
+    <row r="96" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A96" s="1">
+        <v>0.9</v>
+      </c>
+      <c r="B96" s="1">
+        <v>8955216.1531386003</v>
+      </c>
+      <c r="C96" s="2">
+        <f t="shared" si="1"/>
+        <v>-8.2744552115204845E-2</v>
+      </c>
+    </row>
+    <row r="97" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A97" s="1">
+        <v>0.9</v>
+      </c>
+      <c r="B97" s="1">
+        <v>9327090.2172295991</v>
+      </c>
+      <c r="C97" s="2">
+        <f t="shared" si="1"/>
+        <v>4.1525972989570489E-2</v>
+      </c>
+    </row>
+    <row r="98" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A98" s="1">
+        <v>0.9</v>
+      </c>
+      <c r="B98" s="1">
+        <v>11922100.641083799</v>
+      </c>
+      <c r="C98" s="2">
+        <f t="shared" si="1"/>
+        <v>0.2782229359227737</v>
+      </c>
+    </row>
+    <row r="99" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A99" s="1">
+        <v>0.9</v>
+      </c>
+      <c r="B99" s="1">
+        <v>10177384.092680801</v>
+      </c>
+      <c r="C99" s="2">
+        <f t="shared" si="1"/>
+        <v>-0.1463430481697722</v>
+      </c>
+    </row>
+    <row r="100" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A100" s="1">
+        <v>0.9</v>
+      </c>
+      <c r="B100" s="1">
+        <v>10493422.551833799</v>
+      </c>
+      <c r="C100" s="2">
+        <f t="shared" si="1"/>
+        <v>3.1053014829250828E-2</v>
+      </c>
+    </row>
+    <row r="101" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A101" s="1">
+        <v>0.9</v>
+      </c>
+      <c r="B101" s="1">
+        <v>10571888.3616184</v>
+      </c>
+      <c r="C101" s="2">
+        <f t="shared" si="1"/>
+        <v>7.4776184221122463E-3</v>
+      </c>
+    </row>
+    <row r="102" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A102" s="1">
+        <v>0.9</v>
+      </c>
+      <c r="B102" s="1">
+        <v>11825761.163128899</v>
+      </c>
+      <c r="C102" s="2">
+        <f t="shared" si="1"/>
+        <v>0.11860443079050358</v>
+      </c>
+    </row>
+    <row r="103" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A103" s="1">
+        <v>0.9</v>
+      </c>
+      <c r="B103" s="1">
+        <v>11766830.277974</v>
+      </c>
+      <c r="C103" s="2">
+        <f t="shared" si="1"/>
+        <v>-4.983263600709071E-3</v>
+      </c>
+    </row>
+    <row r="104" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A104" s="1">
+        <v>0.9</v>
+      </c>
+      <c r="B104" s="1">
+        <v>11358980.4696874</v>
+      </c>
+      <c r="C104" s="2">
+        <f t="shared" si="1"/>
+        <v>-3.4660974846390233E-2</v>
+      </c>
+    </row>
+    <row r="105" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A105" s="1">
+        <v>0.9</v>
+      </c>
+      <c r="B105" s="1">
+        <v>10595959.5308841</v>
+      </c>
+      <c r="C105" s="2">
+        <f t="shared" si="1"/>
+        <v>-6.7173364796206808E-2</v>
+      </c>
+    </row>
+    <row r="106" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A106" s="1">
+        <v>0.9</v>
+      </c>
+      <c r="B106" s="1">
+        <v>10612407.833329</v>
+      </c>
+      <c r="C106" s="2">
+        <f t="shared" si="1"/>
+        <v>1.5523183527605497E-3</v>
+      </c>
+    </row>
+    <row r="107" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A107" s="1">
+        <v>0.9</v>
+      </c>
+      <c r="B107" s="1">
+        <v>11111308.095895801</v>
+      </c>
+      <c r="C107" s="2">
+        <f t="shared" si="1"/>
+        <v>4.7011033726009892E-2</v>
+      </c>
+    </row>
+    <row r="108" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A108" s="1">
+        <v>0.9</v>
+      </c>
+      <c r="B108" s="1">
+        <v>11482697.728402199</v>
+      </c>
+      <c r="C108" s="2">
+        <f t="shared" si="1"/>
+        <v>3.3424474355416282E-2</v>
+      </c>
+    </row>
+    <row r="109" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A109" s="1">
+        <v>0.9</v>
+      </c>
+      <c r="B109" s="1">
+        <v>12108463.663791399</v>
+      </c>
+      <c r="C109" s="2">
+        <f t="shared" si="1"/>
+        <v>5.4496421502186025E-2</v>
+      </c>
+    </row>
+    <row r="110" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A110" s="1">
+        <v>0.9</v>
+      </c>
+      <c r="B110" s="1">
+        <v>12703801.894834301</v>
+      </c>
+      <c r="C110" s="2">
+        <f t="shared" si="1"/>
+        <v>4.9167115463473167E-2</v>
+      </c>
+    </row>
+    <row r="111" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A111" s="1">
+        <v>0.9</v>
+      </c>
+      <c r="B111" s="1">
+        <v>13554301.475640699</v>
+      </c>
+      <c r="C111" s="2">
+        <f t="shared" si="1"/>
+        <v>6.6948429127522385E-2</v>
+      </c>
+    </row>
+    <row r="112" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A112" s="1">
+        <v>0.9</v>
+      </c>
+      <c r="B112" s="1">
+        <v>10685609.0402385</v>
+      </c>
+      <c r="C112" s="2">
+        <f t="shared" si="1"/>
+        <v>-0.21164443188442503</v>
+      </c>
+    </row>
+    <row r="113" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A113" s="1">
+        <v>0.9</v>
+      </c>
+      <c r="B113" s="1">
+        <v>10060266.226524999</v>
+      </c>
+      <c r="C113" s="2">
+        <f t="shared" si="1"/>
+        <v>-5.8521962703170623E-2</v>
+      </c>
+    </row>
+    <row r="114" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A114" s="1">
+        <v>0.9</v>
+      </c>
+      <c r="B114" s="1">
+        <v>13613881.8641649</v>
+      </c>
+      <c r="C114" s="2">
+        <f t="shared" si="1"/>
+        <v>0.35323276319173363</v>
+      </c>
+    </row>
+    <row r="115" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A115" s="1">
+        <v>0.9</v>
+      </c>
+      <c r="B115" s="1">
+        <v>9865531.9064659998</v>
+      </c>
+      <c r="C115" s="2">
+        <f t="shared" si="1"/>
+        <v>-0.27533292819041444</v>
+      </c>
+    </row>
+    <row r="116" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A116" s="1">
+        <v>0.9</v>
+      </c>
+      <c r="B116" s="1">
+        <v>10216602.912662201</v>
+      </c>
+      <c r="C116" s="2">
+        <f t="shared" si="1"/>
+        <v>3.5585613581169837E-2</v>
+      </c>
+    </row>
+    <row r="117" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A117" s="1">
+        <v>0.9</v>
+      </c>
+      <c r="B117" s="1">
+        <v>10655126.5385125</v>
+      </c>
+      <c r="C117" s="2">
+        <f t="shared" si="1"/>
+        <v>4.2922645579853577E-2</v>
+      </c>
+    </row>
+    <row r="118" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A118" s="1">
+        <v>0.9</v>
+      </c>
+      <c r="B118" s="1">
+        <v>12130281.546378801</v>
+      </c>
+      <c r="C118" s="2">
+        <f t="shared" si="1"/>
+        <v>0.13844556444584827</v>
+      </c>
+    </row>
+    <row r="119" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A119" s="1">
+        <v>0.9</v>
+      </c>
+      <c r="B119" s="1">
+        <v>13932043.1403326</v>
+      </c>
+      <c r="C119" s="2">
+        <f t="shared" si="1"/>
+        <v>0.14853419412113081</v>
+      </c>
+    </row>
+    <row r="120" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A120" s="1">
+        <v>0.9</v>
+      </c>
+      <c r="B120" s="1">
+        <v>9715604.4035289604</v>
+      </c>
+      <c r="C120" s="2">
+        <f t="shared" si="1"/>
+        <v>-0.30264324437793699</v>
+      </c>
+    </row>
+    <row r="121" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A121" s="1">
+        <v>0.9</v>
+      </c>
+      <c r="B121" s="1">
+        <v>14176028.9669978</v>
+      </c>
+      <c r="C121" s="2">
+        <f t="shared" si="1"/>
+        <v>0.45909903061189872</v>
+      </c>
+    </row>
+    <row r="122" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A122" s="1">
+        <v>0.9</v>
+      </c>
+      <c r="B122" s="1">
+        <v>11671773.8648635</v>
+      </c>
+      <c r="C122" s="2">
+        <f t="shared" si="1"/>
+        <v>-0.17665420323027539</v>
+      </c>
+    </row>
+    <row r="123" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A123" s="1">
+        <v>0.9</v>
+      </c>
+      <c r="B123" s="1">
+        <v>11033182.027128199</v>
+      </c>
+      <c r="C123" s="2">
+        <f t="shared" si="1"/>
+        <v>-5.471249230228032E-2</v>
+      </c>
+    </row>
+    <row r="124" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A124" s="1">
+        <v>0.9</v>
+      </c>
+      <c r="B124" s="1">
+        <v>11529359.8826105</v>
+      </c>
+      <c r="C124" s="2">
+        <f t="shared" si="1"/>
+        <v>4.4971419329646434E-2</v>
+      </c>
+    </row>
+    <row r="125" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A125" s="1">
+        <v>0.9</v>
+      </c>
+      <c r="B125" s="1">
+        <v>13431505.780205701</v>
+      </c>
+      <c r="C125" s="2">
+        <f t="shared" si="1"/>
+        <v>0.16498278455720417</v>
+      </c>
+    </row>
+    <row r="126" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A126" s="1">
+        <v>0.9</v>
+      </c>
+      <c r="B126" s="1">
+        <v>9501113.5666300207</v>
+      </c>
+      <c r="C126" s="2">
+        <f t="shared" si="1"/>
+        <v>-0.2926248387852376</v>
+      </c>
+    </row>
+    <row r="127" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A127" s="1">
+        <v>0.9</v>
+      </c>
+      <c r="B127" s="1">
+        <v>10408189.666232301</v>
+      </c>
+      <c r="C127" s="2">
+        <f t="shared" si="1"/>
+        <v>9.5470503877369592E-2</v>
+      </c>
+    </row>
+    <row r="128" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A128" s="1">
+        <v>0.9</v>
+      </c>
+      <c r="B128" s="1">
+        <v>9508783.8172435593</v>
+      </c>
+      <c r="C128" s="2">
+        <f t="shared" si="1"/>
+        <v>-8.6413283945691283E-2</v>
+      </c>
+    </row>
+    <row r="129" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A129" s="1">
+        <v>0.9</v>
+      </c>
+      <c r="B129" s="1">
+        <v>10907746.960920099</v>
+      </c>
+      <c r="C129" s="2">
+        <f t="shared" si="1"/>
+        <v>0.14712324631248966</v>
+      </c>
+    </row>
+    <row r="130" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A130" s="1">
+        <v>0.9</v>
+      </c>
+      <c r="B130" s="1">
+        <v>10917398.9459047</v>
+      </c>
+      <c r="C130" s="2">
+        <f t="shared" si="1"/>
+        <v>8.8487430256511414E-4</v>
+      </c>
+    </row>
+    <row r="131" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A131" s="1">
+        <v>0.9</v>
+      </c>
+      <c r="B131" s="1">
+        <v>14160304.8346682</v>
+      </c>
+      <c r="C131" s="2">
+        <f t="shared" si="1"/>
+        <v>0.29704015625259977</v>
+      </c>
+    </row>
+    <row r="132" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A132" s="1">
+        <v>0.9</v>
+      </c>
+      <c r="B132" s="1">
+        <v>13629440.0271507</v>
+      </c>
+      <c r="C132" s="2">
+        <f t="shared" si="1"/>
+        <v>-3.7489645436007989E-2</v>
+      </c>
+    </row>
+    <row r="133" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A133" s="1">
+        <v>0.9</v>
+      </c>
+      <c r="B133" s="1">
+        <v>11985011.9607371</v>
+      </c>
+      <c r="C133" s="2">
+        <f t="shared" si="1"/>
+        <v>-0.12065265066927153</v>
+      </c>
+    </row>
+    <row r="134" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A134" s="1">
+        <v>0.9</v>
+      </c>
+      <c r="B134" s="1">
+        <v>12182880.250477999</v>
+      </c>
+      <c r="C134" s="2">
+        <f t="shared" si="1"/>
+        <v>1.6509644745379987E-2</v>
+      </c>
+    </row>
+    <row r="135" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A135" s="1">
+        <v>0.9</v>
+      </c>
+      <c r="B135" s="1">
+        <v>14521517.5582019</v>
+      </c>
+      <c r="C135" s="2">
+        <f t="shared" si="1"/>
+        <v>0.19196095337407121</v>
+      </c>
+    </row>
+    <row r="136" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A136" s="1">
+        <v>0.9</v>
+      </c>
+      <c r="B136" s="1">
+        <v>13216335.4916855</v>
+      </c>
+      <c r="C136" s="2">
+        <f t="shared" ref="C136:C137" si="2">(B136-B135)/B135</f>
+        <v>-8.9879178349319244E-2</v>
+      </c>
+    </row>
+    <row r="137" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A137" s="1">
+        <v>0.9</v>
+      </c>
+      <c r="B137" s="1">
+        <v>11703223.0840302</v>
+      </c>
+      <c r="C137" s="2">
+        <f t="shared" si="2"/>
+        <v>-0.11448804463288718</v>
+      </c>
+    </row>
+    <row r="138" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A138">
+        <v>0.9</v>
+      </c>
+      <c r="B138">
+        <v>9462139.2012504209</v>
+      </c>
+    </row>
+    <row r="139" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A139">
+        <v>0.9</v>
+      </c>
+      <c r="B139">
+        <v>10140643.0278219</v>
+      </c>
+    </row>
+    <row r="140" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A140">
+        <v>0.9</v>
+      </c>
+      <c r="B140">
+        <v>11836601.603824399</v>
+      </c>
+    </row>
+    <row r="141" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A141">
+        <v>0.9</v>
+      </c>
+      <c r="B141">
+        <v>9422842.3194465693</v>
+      </c>
+    </row>
+    <row r="142" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A142">
+        <v>0.9</v>
+      </c>
+      <c r="B142">
+        <v>9956083.5383792706</v>
+      </c>
+    </row>
+    <row r="143" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A143">
+        <v>0.9</v>
+      </c>
+      <c r="B143">
+        <v>11052635.6461512</v>
+      </c>
+    </row>
+    <row r="144" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A144">
+        <v>0.9</v>
+      </c>
+      <c r="B144">
+        <v>9368232.5286609493</v>
+      </c>
+    </row>
+    <row r="145" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A145">
+        <v>0.9</v>
+      </c>
+      <c r="B145">
+        <v>8035129.1142357001</v>
+      </c>
+    </row>
+    <row r="146" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A146">
+        <v>0.9</v>
+      </c>
+      <c r="B146">
+        <v>8755057.3914310206</v>
+      </c>
+    </row>
+    <row r="147" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A147">
+        <v>0.9</v>
+      </c>
+      <c r="B147">
+        <v>10113663.9520045</v>
+      </c>
+    </row>
+    <row r="148" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A148">
+        <v>0.9</v>
+      </c>
+      <c r="B148">
+        <v>9256506.0298943408</v>
+      </c>
+    </row>
+    <row r="149" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A149">
+        <v>0.9</v>
+      </c>
+      <c r="B149">
+        <v>11622405.8031116</v>
+      </c>
+    </row>
+    <row r="150" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A150">
+        <v>0.9</v>
+      </c>
+      <c r="B150">
+        <v>10381440.1668764</v>
+      </c>
+    </row>
+    <row r="151" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A151">
+        <v>0.9</v>
+      </c>
+      <c r="B151">
+        <v>10352893.730533401</v>
+      </c>
+    </row>
+    <row r="152" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A152">
+        <v>0.9</v>
+      </c>
+      <c r="B152">
+        <v>10897656.658714101</v>
+      </c>
+    </row>
+    <row r="153" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A153">
+        <v>0.9</v>
+      </c>
+      <c r="B153">
+        <v>8460701.3957199994</v>
+      </c>
+    </row>
+    <row r="154" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A154">
+        <v>0.9</v>
+      </c>
+      <c r="B154">
+        <v>9565198.7669808399</v>
+      </c>
+    </row>
+    <row r="155" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A155">
+        <v>0.9</v>
+      </c>
+      <c r="B155">
+        <v>11325566.920112099</v>
+      </c>
+    </row>
+    <row r="156" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A156">
+        <v>0.9</v>
+      </c>
+      <c r="B156">
+        <v>10264873.1519859</v>
+      </c>
+    </row>
+    <row r="157" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A157">
+        <v>0.9</v>
+      </c>
+      <c r="B157">
+        <v>10160784.271545</v>
+      </c>
+    </row>
+    <row r="158" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A158">
+        <v>0.9</v>
+      </c>
+      <c r="B158">
+        <v>8983007.1700480301</v>
+      </c>
+    </row>
+    <row r="159" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A159">
+        <v>0.9</v>
+      </c>
+      <c r="B159">
+        <v>8835698.1042707209</v>
+      </c>
+    </row>
+    <row r="160" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A160">
+        <v>0.9</v>
+      </c>
+      <c r="B160">
+        <v>8014145.9304012703</v>
+      </c>
+    </row>
+    <row r="161" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A161">
+        <v>0.9</v>
+      </c>
+      <c r="B161">
+        <v>10459898.4393805</v>
+      </c>
+    </row>
+    <row r="162" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A162">
+        <v>0.9</v>
+      </c>
+      <c r="B162">
+        <v>11678967.5267171</v>
+      </c>
+    </row>
+    <row r="163" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A163">
+        <v>0.9</v>
+      </c>
+      <c r="B163">
+        <v>12915385.3178194</v>
+      </c>
+    </row>
+    <row r="164" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A164">
+        <v>0.9</v>
+      </c>
+      <c r="B164">
+        <v>10350550.3452453</v>
+      </c>
+    </row>
+    <row r="165" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A165">
+        <v>0.9</v>
+      </c>
+      <c r="B165">
+        <v>11530034.324007999</v>
+      </c>
+    </row>
+    <row r="166" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A166">
+        <v>0.9</v>
+      </c>
+      <c r="B166">
+        <v>10039595.308894601</v>
+      </c>
+    </row>
+    <row r="167" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A167">
+        <v>0.9</v>
+      </c>
+      <c r="B167">
+        <v>10531543.3634145</v>
+      </c>
+    </row>
+    <row r="168" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A168">
+        <v>0.9</v>
+      </c>
+      <c r="B168">
+        <v>11322046.236679001</v>
+      </c>
+    </row>
+    <row r="169" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A169">
+        <v>0.9</v>
+      </c>
+      <c r="B169">
+        <v>13919552.267551599</v>
+      </c>
+    </row>
+    <row r="170" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A170">
+        <v>0.9</v>
+      </c>
+      <c r="B170">
+        <v>12693246.7447527</v>
+      </c>
+    </row>
+    <row r="171" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A171">
+        <v>0.9</v>
+      </c>
+      <c r="B171">
+        <v>14816961.1335028</v>
+      </c>
+    </row>
+    <row r="172" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A172">
+        <v>0.9</v>
+      </c>
+      <c r="B172">
+        <v>11447928.8874959</v>
+      </c>
+    </row>
+    <row r="173" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A173">
+        <v>0.9</v>
+      </c>
+      <c r="B173">
+        <v>11783283.699706901</v>
+      </c>
+    </row>
+    <row r="174" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A174">
+        <v>0.9</v>
+      </c>
+      <c r="B174">
+        <v>13854411.550277401</v>
+      </c>
+    </row>
+    <row r="175" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A175">
+        <v>0.9</v>
+      </c>
+      <c r="B175">
+        <v>10337823.9272717</v>
+      </c>
+    </row>
+    <row r="176" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A176">
+        <v>0.9</v>
+      </c>
+      <c r="B176">
+        <v>10005847.592892099</v>
+      </c>
+    </row>
+    <row r="177" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A177">
+        <v>0.9</v>
+      </c>
+      <c r="B177">
+        <v>8981746.7223352008</v>
+      </c>
+    </row>
+    <row r="178" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A178">
+        <v>0.9</v>
+      </c>
+      <c r="B178">
+        <v>7440911.6710755304</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Merge Progress Report from Auto_Generated_Programs_from_Examples branch into Master Branch for continuity Code has bug with Multi-Thread. However, I am merging with the Master Branch so that the Progress Report maintains a single timeline of test results.
</commit_message>
<xml_diff>
--- a/Progress.xlsx
+++ b/Progress.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/c51537410c5afe56/Projects/Source/Repos/EdGarrity/SOS/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="237" documentId="114_{B2D123C0-10CD-4892-A2B1-0D4FB86B9D90}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{93029869-0C45-4CEC-94D3-406A34B69937}"/>
+  <xr:revisionPtr revIDLastSave="1" documentId="114_{5A039FB9-666C-4FDC-9FC6-FAFC9BEA3DF7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{57D00C6E-3558-4E3D-B9F8-F7262F485D2C}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="16896" activeTab="4" xr2:uid="{D7613C25-2959-4D88-A8C3-21B00E74DE47}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="16896" activeTab="5" xr2:uid="{D7613C25-2959-4D88-A8C3-21B00E74DE47}"/>
   </bookViews>
   <sheets>
     <sheet name="Run 1" sheetId="1" r:id="rId1"/>
@@ -18,6 +18,7 @@
     <sheet name="Run 3" sheetId="3" r:id="rId3"/>
     <sheet name="Run 4" sheetId="4" r:id="rId4"/>
     <sheet name="Run 5" sheetId="5" r:id="rId5"/>
+    <sheet name="Run 6" sheetId="6" r:id="rId6"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -37,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="9">
   <si>
     <t>BestIndividual_Training_Error</t>
   </si>
@@ -62,11 +63,17 @@
   <si>
     <t>BestIndividual_Training_Score</t>
   </si>
+  <si>
+    <t>Created_DTS</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="1">
+    <numFmt numFmtId="165" formatCode="[$-409]m/d/yy\ h:mm\ AM/PM;@"/>
+  </numFmts>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -96,10 +103,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="4" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -5073,6 +5081,1243 @@
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000001-212E-400E-9313-37DCD10EEC5E}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:marker val="1"/>
+        <c:smooth val="0"/>
+        <c:axId val="840836808"/>
+        <c:axId val="840833856"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="715829080"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" cap="none" spc="0" normalizeH="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="715823504"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="715823504"/>
+        <c:scaling>
+          <c:logBase val="10"/>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:minorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="5000"/>
+                  <a:lumOff val="95000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:minorGridlines>
+        <c:numFmt formatCode="#,##0.00" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="715829080"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="840833856"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="r"/>
+        <c:numFmt formatCode="#,##0.00" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="840836808"/>
+        <c:crosses val="max"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:catAx>
+        <c:axId val="840836808"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="1"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="840833856"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="t"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart6.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="2000" b="0" i="0" u="none" strike="noStrike" kern="1200" cap="none" spc="0" normalizeH="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mj-lt"/>
+              <a:ea typeface="+mj-ea"/>
+              <a:cs typeface="+mj-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Run 6'!$C$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Average_Training_Error</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="38100" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>'Run 6'!$C$2:$C$137</c:f>
+              <c:numCache>
+                <c:formatCode>#,##0.00</c:formatCode>
+                <c:ptCount val="136"/>
+                <c:pt idx="0">
+                  <c:v>466828517.77193397</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>530838032.318699</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>370939279.01228499</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>287802144.25176901</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>248506795.35284099</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>219063937.33587301</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>138580850.40472999</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>143843237.58303201</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>84740447.071308702</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>50829498.939668</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>45881076.786539502</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>36884020.090438202</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>51961728.485883802</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>23300455.492954198</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>18673919.715530898</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>22387443.221550301</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>21727289.674221501</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>25023973.804324102</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>28457230.8928365</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>20707684.776952799</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>14613419.506552</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>14221412.3280422</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>13799211.4196239</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>10991181.9397649</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>7827470.0282455198</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>11158393.262985799</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>11228451.7032403</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>6580154.4599233698</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>5694237.1644831495</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>7602025.9353936203</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>7774374.1914764</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>8887725.9137989692</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>8256218.8607965596</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>9346117.9973511808</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>8787415.66559745</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>6106326.5948853297</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>10212688.134928999</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>12426570.6614541</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>7555045.1385022402</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>5974048.4311196003</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>5586637.8612419497</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>6283506.2962794499</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>7465580.1919447798</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>6318532.6921694595</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>7805773.7823088001</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>8864587.4604190998</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>6943692.4762246301</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>5018393.19882455</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>5936583.2975150002</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>8225772.5154284202</c:v>
+                </c:pt>
+                <c:pt idx="50">
+                  <c:v>6907093.6067347797</c:v>
+                </c:pt>
+                <c:pt idx="51">
+                  <c:v>7761654.1245476799</c:v>
+                </c:pt>
+                <c:pt idx="52">
+                  <c:v>8243263.69838861</c:v>
+                </c:pt>
+                <c:pt idx="53">
+                  <c:v>8773894.6373157408</c:v>
+                </c:pt>
+                <c:pt idx="54">
+                  <c:v>8716087.0516568795</c:v>
+                </c:pt>
+                <c:pt idx="55">
+                  <c:v>9526198.3536674306</c:v>
+                </c:pt>
+                <c:pt idx="56">
+                  <c:v>11499360.383852899</c:v>
+                </c:pt>
+                <c:pt idx="57">
+                  <c:v>11166373.0106229</c:v>
+                </c:pt>
+                <c:pt idx="58">
+                  <c:v>9769672.7323780097</c:v>
+                </c:pt>
+                <c:pt idx="59">
+                  <c:v>9113302.0081548896</c:v>
+                </c:pt>
+                <c:pt idx="60">
+                  <c:v>8908424.5873359703</c:v>
+                </c:pt>
+                <c:pt idx="61">
+                  <c:v>6980347.5328304498</c:v>
+                </c:pt>
+                <c:pt idx="62">
+                  <c:v>10547658.4918481</c:v>
+                </c:pt>
+                <c:pt idx="63">
+                  <c:v>7893663.9331381703</c:v>
+                </c:pt>
+                <c:pt idx="64">
+                  <c:v>7872032.7382409796</c:v>
+                </c:pt>
+                <c:pt idx="65">
+                  <c:v>9625715.7394120805</c:v>
+                </c:pt>
+                <c:pt idx="66">
+                  <c:v>9473516.8728934303</c:v>
+                </c:pt>
+                <c:pt idx="67">
+                  <c:v>6771778.9840001902</c:v>
+                </c:pt>
+                <c:pt idx="68">
+                  <c:v>9345339.9283929896</c:v>
+                </c:pt>
+                <c:pt idx="69">
+                  <c:v>8749845.9247072209</c:v>
+                </c:pt>
+                <c:pt idx="70">
+                  <c:v>9261091.2615985703</c:v>
+                </c:pt>
+                <c:pt idx="71">
+                  <c:v>7223886.9166597603</c:v>
+                </c:pt>
+                <c:pt idx="72">
+                  <c:v>9094109.5142613109</c:v>
+                </c:pt>
+                <c:pt idx="73">
+                  <c:v>8086894.8526188498</c:v>
+                </c:pt>
+                <c:pt idx="74">
+                  <c:v>9608504.8194003105</c:v>
+                </c:pt>
+                <c:pt idx="75">
+                  <c:v>8167561.5776757495</c:v>
+                </c:pt>
+                <c:pt idx="76">
+                  <c:v>9162142.1501978301</c:v>
+                </c:pt>
+                <c:pt idx="77">
+                  <c:v>10179691.575688399</c:v>
+                </c:pt>
+                <c:pt idx="78">
+                  <c:v>10752796.858561199</c:v>
+                </c:pt>
+                <c:pt idx="79">
+                  <c:v>9900381.7571215592</c:v>
+                </c:pt>
+                <c:pt idx="80">
+                  <c:v>8339031.87166679</c:v>
+                </c:pt>
+                <c:pt idx="81">
+                  <c:v>7073649.2107376698</c:v>
+                </c:pt>
+                <c:pt idx="82">
+                  <c:v>7834860.1909906296</c:v>
+                </c:pt>
+                <c:pt idx="83">
+                  <c:v>7875096.2232888797</c:v>
+                </c:pt>
+                <c:pt idx="84">
+                  <c:v>6798184.0071253702</c:v>
+                </c:pt>
+                <c:pt idx="85">
+                  <c:v>5947294.9817488296</c:v>
+                </c:pt>
+                <c:pt idx="86">
+                  <c:v>9243918.2330143806</c:v>
+                </c:pt>
+                <c:pt idx="87">
+                  <c:v>10158971.5577267</c:v>
+                </c:pt>
+                <c:pt idx="88">
+                  <c:v>9430798.9976223409</c:v>
+                </c:pt>
+                <c:pt idx="89">
+                  <c:v>7920212.32179425</c:v>
+                </c:pt>
+                <c:pt idx="90">
+                  <c:v>7781097.7558316998</c:v>
+                </c:pt>
+                <c:pt idx="91">
+                  <c:v>8909239.7825026009</c:v>
+                </c:pt>
+                <c:pt idx="92">
+                  <c:v>8402575.5211147591</c:v>
+                </c:pt>
+                <c:pt idx="93">
+                  <c:v>9763055.8355248403</c:v>
+                </c:pt>
+                <c:pt idx="94">
+                  <c:v>8955216.1531386003</c:v>
+                </c:pt>
+                <c:pt idx="95">
+                  <c:v>9327090.2172295991</c:v>
+                </c:pt>
+                <c:pt idx="96">
+                  <c:v>11922100.641083799</c:v>
+                </c:pt>
+                <c:pt idx="97">
+                  <c:v>10177384.092680801</c:v>
+                </c:pt>
+                <c:pt idx="98">
+                  <c:v>10493422.551833799</c:v>
+                </c:pt>
+                <c:pt idx="99">
+                  <c:v>10571888.3616184</c:v>
+                </c:pt>
+                <c:pt idx="100">
+                  <c:v>11825761.163128899</c:v>
+                </c:pt>
+                <c:pt idx="101">
+                  <c:v>11766830.277974</c:v>
+                </c:pt>
+                <c:pt idx="102">
+                  <c:v>11358980.4696874</c:v>
+                </c:pt>
+                <c:pt idx="103">
+                  <c:v>10595959.5308841</c:v>
+                </c:pt>
+                <c:pt idx="104">
+                  <c:v>10612407.833329</c:v>
+                </c:pt>
+                <c:pt idx="105">
+                  <c:v>11111308.095895801</c:v>
+                </c:pt>
+                <c:pt idx="106">
+                  <c:v>11482697.728402199</c:v>
+                </c:pt>
+                <c:pt idx="107">
+                  <c:v>12108463.663791399</c:v>
+                </c:pt>
+                <c:pt idx="108">
+                  <c:v>12703801.894834301</c:v>
+                </c:pt>
+                <c:pt idx="109">
+                  <c:v>13554301.475640699</c:v>
+                </c:pt>
+                <c:pt idx="110">
+                  <c:v>10685609.0402385</c:v>
+                </c:pt>
+                <c:pt idx="111">
+                  <c:v>10060266.226524999</c:v>
+                </c:pt>
+                <c:pt idx="112">
+                  <c:v>13613881.8641649</c:v>
+                </c:pt>
+                <c:pt idx="113">
+                  <c:v>9865531.9064659998</c:v>
+                </c:pt>
+                <c:pt idx="114">
+                  <c:v>10216602.912662201</c:v>
+                </c:pt>
+                <c:pt idx="115">
+                  <c:v>10655126.5385125</c:v>
+                </c:pt>
+                <c:pt idx="116">
+                  <c:v>12130281.546378801</c:v>
+                </c:pt>
+                <c:pt idx="117">
+                  <c:v>13932043.1403326</c:v>
+                </c:pt>
+                <c:pt idx="118">
+                  <c:v>9715604.4035289604</c:v>
+                </c:pt>
+                <c:pt idx="119">
+                  <c:v>14176028.9669978</c:v>
+                </c:pt>
+                <c:pt idx="120">
+                  <c:v>11671773.8648635</c:v>
+                </c:pt>
+                <c:pt idx="121">
+                  <c:v>11033182.027128199</c:v>
+                </c:pt>
+                <c:pt idx="122">
+                  <c:v>11529359.8826105</c:v>
+                </c:pt>
+                <c:pt idx="123">
+                  <c:v>13431505.780205701</c:v>
+                </c:pt>
+                <c:pt idx="124">
+                  <c:v>9501113.5666300207</c:v>
+                </c:pt>
+                <c:pt idx="125">
+                  <c:v>10408189.666232301</c:v>
+                </c:pt>
+                <c:pt idx="126">
+                  <c:v>9508783.8172435593</c:v>
+                </c:pt>
+                <c:pt idx="127">
+                  <c:v>10907746.960920099</c:v>
+                </c:pt>
+                <c:pt idx="128">
+                  <c:v>10917398.9459047</c:v>
+                </c:pt>
+                <c:pt idx="129">
+                  <c:v>14160304.8346682</c:v>
+                </c:pt>
+                <c:pt idx="130">
+                  <c:v>13629440.0271507</c:v>
+                </c:pt>
+                <c:pt idx="131">
+                  <c:v>11985011.9607371</c:v>
+                </c:pt>
+                <c:pt idx="132">
+                  <c:v>12182880.250477999</c:v>
+                </c:pt>
+                <c:pt idx="133">
+                  <c:v>14521517.5582019</c:v>
+                </c:pt>
+                <c:pt idx="134">
+                  <c:v>13216335.4916855</c:v>
+                </c:pt>
+                <c:pt idx="135">
+                  <c:v>11703223.0840302</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-E105-455E-8DB8-9A6E08FF6146}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:marker val="1"/>
+        <c:smooth val="0"/>
+        <c:axId val="715829080"/>
+        <c:axId val="715823504"/>
+      </c:lineChart>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Run 6'!$B$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>BestIndividual_Training_Score</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="38100" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>'Run 6'!$B$2:$B$137</c:f>
+              <c:numCache>
+                <c:formatCode>#,##0.00</c:formatCode>
+                <c:ptCount val="136"/>
+                <c:pt idx="0">
+                  <c:v>0.9</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.9</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.9</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.9</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.9</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.9</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.9</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.9</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.9</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.9</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0.9</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0.9</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>0.9</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>0.9</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>0.9</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>0.9</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>0.9</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>0.9</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>0.9</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>0.9</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>0.9</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>0.9</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>0.9</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>0.9</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>0.9</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>0.9</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>0.9</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>0.9</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>0.9</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>0.9</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>0.9</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>0.9</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>0.9</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>0.9</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>0.9</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>0.9</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>0.9</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>0.9</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>0.9</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>0.9</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>0.9</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>0.9</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>0.9</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>0.9</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>0.9</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>0.9</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>0.9</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>0.9</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>0.9</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>0.9</c:v>
+                </c:pt>
+                <c:pt idx="50">
+                  <c:v>0.9</c:v>
+                </c:pt>
+                <c:pt idx="51">
+                  <c:v>0.9</c:v>
+                </c:pt>
+                <c:pt idx="52">
+                  <c:v>0.9</c:v>
+                </c:pt>
+                <c:pt idx="53">
+                  <c:v>0.9</c:v>
+                </c:pt>
+                <c:pt idx="54">
+                  <c:v>0.9</c:v>
+                </c:pt>
+                <c:pt idx="55">
+                  <c:v>0.9</c:v>
+                </c:pt>
+                <c:pt idx="56">
+                  <c:v>0.9</c:v>
+                </c:pt>
+                <c:pt idx="57">
+                  <c:v>0.9</c:v>
+                </c:pt>
+                <c:pt idx="58">
+                  <c:v>0.9</c:v>
+                </c:pt>
+                <c:pt idx="59">
+                  <c:v>0.9</c:v>
+                </c:pt>
+                <c:pt idx="60">
+                  <c:v>0.9</c:v>
+                </c:pt>
+                <c:pt idx="61">
+                  <c:v>0.9</c:v>
+                </c:pt>
+                <c:pt idx="62">
+                  <c:v>0.9</c:v>
+                </c:pt>
+                <c:pt idx="63">
+                  <c:v>0.9</c:v>
+                </c:pt>
+                <c:pt idx="64">
+                  <c:v>0.9</c:v>
+                </c:pt>
+                <c:pt idx="65">
+                  <c:v>0.9</c:v>
+                </c:pt>
+                <c:pt idx="66">
+                  <c:v>0.9</c:v>
+                </c:pt>
+                <c:pt idx="67">
+                  <c:v>0.9</c:v>
+                </c:pt>
+                <c:pt idx="68">
+                  <c:v>0.9</c:v>
+                </c:pt>
+                <c:pt idx="69">
+                  <c:v>0.9</c:v>
+                </c:pt>
+                <c:pt idx="70">
+                  <c:v>0.9</c:v>
+                </c:pt>
+                <c:pt idx="71">
+                  <c:v>0.9</c:v>
+                </c:pt>
+                <c:pt idx="72">
+                  <c:v>0.9</c:v>
+                </c:pt>
+                <c:pt idx="73">
+                  <c:v>0.9</c:v>
+                </c:pt>
+                <c:pt idx="74">
+                  <c:v>0.9</c:v>
+                </c:pt>
+                <c:pt idx="75">
+                  <c:v>0.9</c:v>
+                </c:pt>
+                <c:pt idx="76">
+                  <c:v>0.9</c:v>
+                </c:pt>
+                <c:pt idx="77">
+                  <c:v>0.9</c:v>
+                </c:pt>
+                <c:pt idx="78">
+                  <c:v>0.9</c:v>
+                </c:pt>
+                <c:pt idx="79">
+                  <c:v>0.9</c:v>
+                </c:pt>
+                <c:pt idx="80">
+                  <c:v>0.9</c:v>
+                </c:pt>
+                <c:pt idx="81">
+                  <c:v>0.9</c:v>
+                </c:pt>
+                <c:pt idx="82">
+                  <c:v>0.9</c:v>
+                </c:pt>
+                <c:pt idx="83">
+                  <c:v>0.9</c:v>
+                </c:pt>
+                <c:pt idx="84">
+                  <c:v>0.9</c:v>
+                </c:pt>
+                <c:pt idx="85">
+                  <c:v>0.9</c:v>
+                </c:pt>
+                <c:pt idx="86">
+                  <c:v>0.9</c:v>
+                </c:pt>
+                <c:pt idx="87">
+                  <c:v>0.9</c:v>
+                </c:pt>
+                <c:pt idx="88">
+                  <c:v>0.9</c:v>
+                </c:pt>
+                <c:pt idx="89">
+                  <c:v>0.9</c:v>
+                </c:pt>
+                <c:pt idx="90">
+                  <c:v>0.9</c:v>
+                </c:pt>
+                <c:pt idx="91">
+                  <c:v>0.9</c:v>
+                </c:pt>
+                <c:pt idx="92">
+                  <c:v>0.9</c:v>
+                </c:pt>
+                <c:pt idx="93">
+                  <c:v>0.9</c:v>
+                </c:pt>
+                <c:pt idx="94">
+                  <c:v>0.9</c:v>
+                </c:pt>
+                <c:pt idx="95">
+                  <c:v>0.9</c:v>
+                </c:pt>
+                <c:pt idx="96">
+                  <c:v>0.9</c:v>
+                </c:pt>
+                <c:pt idx="97">
+                  <c:v>0.9</c:v>
+                </c:pt>
+                <c:pt idx="98">
+                  <c:v>0.9</c:v>
+                </c:pt>
+                <c:pt idx="99">
+                  <c:v>0.9</c:v>
+                </c:pt>
+                <c:pt idx="100">
+                  <c:v>0.9</c:v>
+                </c:pt>
+                <c:pt idx="101">
+                  <c:v>0.9</c:v>
+                </c:pt>
+                <c:pt idx="102">
+                  <c:v>0.9</c:v>
+                </c:pt>
+                <c:pt idx="103">
+                  <c:v>0.9</c:v>
+                </c:pt>
+                <c:pt idx="104">
+                  <c:v>0.9</c:v>
+                </c:pt>
+                <c:pt idx="105">
+                  <c:v>0.9</c:v>
+                </c:pt>
+                <c:pt idx="106">
+                  <c:v>0.9</c:v>
+                </c:pt>
+                <c:pt idx="107">
+                  <c:v>0.9</c:v>
+                </c:pt>
+                <c:pt idx="108">
+                  <c:v>0.9</c:v>
+                </c:pt>
+                <c:pt idx="109">
+                  <c:v>0.9</c:v>
+                </c:pt>
+                <c:pt idx="110">
+                  <c:v>0.9</c:v>
+                </c:pt>
+                <c:pt idx="111">
+                  <c:v>0.9</c:v>
+                </c:pt>
+                <c:pt idx="112">
+                  <c:v>0.9</c:v>
+                </c:pt>
+                <c:pt idx="113">
+                  <c:v>0.9</c:v>
+                </c:pt>
+                <c:pt idx="114">
+                  <c:v>0.9</c:v>
+                </c:pt>
+                <c:pt idx="115">
+                  <c:v>0.9</c:v>
+                </c:pt>
+                <c:pt idx="116">
+                  <c:v>0.9</c:v>
+                </c:pt>
+                <c:pt idx="117">
+                  <c:v>0.9</c:v>
+                </c:pt>
+                <c:pt idx="118">
+                  <c:v>0.9</c:v>
+                </c:pt>
+                <c:pt idx="119">
+                  <c:v>0.9</c:v>
+                </c:pt>
+                <c:pt idx="120">
+                  <c:v>0.9</c:v>
+                </c:pt>
+                <c:pt idx="121">
+                  <c:v>0.9</c:v>
+                </c:pt>
+                <c:pt idx="122">
+                  <c:v>0.9</c:v>
+                </c:pt>
+                <c:pt idx="123">
+                  <c:v>0.9</c:v>
+                </c:pt>
+                <c:pt idx="124">
+                  <c:v>0.9</c:v>
+                </c:pt>
+                <c:pt idx="125">
+                  <c:v>0.9</c:v>
+                </c:pt>
+                <c:pt idx="126">
+                  <c:v>0.9</c:v>
+                </c:pt>
+                <c:pt idx="127">
+                  <c:v>0.9</c:v>
+                </c:pt>
+                <c:pt idx="128">
+                  <c:v>0.9</c:v>
+                </c:pt>
+                <c:pt idx="129">
+                  <c:v>0.9</c:v>
+                </c:pt>
+                <c:pt idx="130">
+                  <c:v>0.9</c:v>
+                </c:pt>
+                <c:pt idx="131">
+                  <c:v>0.9</c:v>
+                </c:pt>
+                <c:pt idx="132">
+                  <c:v>0.9</c:v>
+                </c:pt>
+                <c:pt idx="133">
+                  <c:v>0.9</c:v>
+                </c:pt>
+                <c:pt idx="134">
+                  <c:v>0.9</c:v>
+                </c:pt>
+                <c:pt idx="135">
+                  <c:v>0.9</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-E105-455E-8DB8-9A6E08FF6146}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -5508,6 +6753,46 @@
 </file>
 
 <file path=xl/charts/colors5.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors6.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
   <a:schemeClr val="accent2"/>
@@ -8047,6 +9332,506 @@
 </cs:chartStyle>
 </file>
 
+<file path=xl/charts/style6.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="235">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200" cap="all"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" b="0" kern="1200" cap="none" spc="0" normalizeH="0" baseline="0"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="38100" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="8"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:prstDash val="dash"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:prstDash val="dash"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="major">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="2000" b="0" kern="1200" cap="none" spc="0" normalizeH="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
@@ -8238,6 +10023,49 @@
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
               <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{7DFC844A-CA4D-4416-AB8A-185B200BC67E}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing6.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>561975</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>31</xdr:col>
+      <xdr:colOff>409575</xdr:colOff>
+      <xdr:row>37</xdr:row>
+      <xdr:rowOff>19050</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F21C3A37-B741-4E6F-B275-A30D51DA0DD2}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -14398,9 +16226,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0FE1FBB3-2F2A-4BF3-AA47-B20CE8C7B019}">
   <dimension ref="A1:D137"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1:B44"/>
-    </sheetView>
+    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -15684,4 +17510,2531 @@
   <pageSetup orientation="portrait" r:id="rId1"/>
   <drawing r:id="rId2"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E95F638A-2EEB-4C6A-9BCC-C221B0F3EBAC}">
+  <dimension ref="A1:E178"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection sqref="A1:A1048576"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="15.88671875" style="3" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="27.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="22.109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="8.88671875" style="2"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A1" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A2" s="3">
+        <v>43730.805581516201</v>
+      </c>
+      <c r="B2" s="1">
+        <v>0.9</v>
+      </c>
+      <c r="C2" s="1">
+        <v>466828517.77193397</v>
+      </c>
+      <c r="E2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A3" s="3">
+        <v>43730.836399074076</v>
+      </c>
+      <c r="B3" s="1">
+        <v>0.9</v>
+      </c>
+      <c r="C3" s="1">
+        <v>530838032.318699</v>
+      </c>
+      <c r="D3" s="2">
+        <f>(C3-C2)/C2</f>
+        <v>0.13711569047295533</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A4" s="3">
+        <v>43730.863731018515</v>
+      </c>
+      <c r="B4" s="1">
+        <v>0.9</v>
+      </c>
+      <c r="C4" s="1">
+        <v>370939279.01228499</v>
+      </c>
+      <c r="D4" s="2">
+        <f>(C4-C3)/C3</f>
+        <v>-0.30121947481414757</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A5" s="3">
+        <v>43730.887981678243</v>
+      </c>
+      <c r="B5" s="1">
+        <v>0.9</v>
+      </c>
+      <c r="C5" s="1">
+        <v>287802144.25176901</v>
+      </c>
+      <c r="D5" s="2">
+        <f>(C5-C4)/C4</f>
+        <v>-0.22412599437268707</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A6" s="3">
+        <v>43730.911335567129</v>
+      </c>
+      <c r="B6" s="1">
+        <v>0.9</v>
+      </c>
+      <c r="C6" s="1">
+        <v>248506795.35284099</v>
+      </c>
+      <c r="D6" s="2">
+        <f>(C6-C5)/C5</f>
+        <v>-0.13653598377832962</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A7" s="3">
+        <v>43730.933723692127</v>
+      </c>
+      <c r="B7" s="1">
+        <v>0.9</v>
+      </c>
+      <c r="C7" s="1">
+        <v>219063937.33587301</v>
+      </c>
+      <c r="D7" s="2">
+        <f>(C7-C6)/C6</f>
+        <v>-0.11847908615602927</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A8" s="3">
+        <v>43730.955216550923</v>
+      </c>
+      <c r="B8" s="1">
+        <v>0.9</v>
+      </c>
+      <c r="C8" s="1">
+        <v>138580850.40472999</v>
+      </c>
+      <c r="D8" s="2">
+        <f>(C8-C7)/C7</f>
+        <v>-0.36739541847887458</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A9" s="3">
+        <v>43730.978247303239</v>
+      </c>
+      <c r="B9" s="1">
+        <v>0.9</v>
+      </c>
+      <c r="C9" s="1">
+        <v>143843237.58303201</v>
+      </c>
+      <c r="D9" s="2">
+        <f>(C9-C8)/C8</f>
+        <v>3.7973408035331307E-2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A10" s="3">
+        <v>43730.999832372683</v>
+      </c>
+      <c r="B10" s="1">
+        <v>0.9</v>
+      </c>
+      <c r="C10" s="1">
+        <v>84740447.071308702</v>
+      </c>
+      <c r="D10" s="2">
+        <f>(C10-C9)/C9</f>
+        <v>-0.41088334429073758</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A11" s="3">
+        <v>43731.022561342594</v>
+      </c>
+      <c r="B11" s="1">
+        <v>0.9</v>
+      </c>
+      <c r="C11" s="1">
+        <v>50829498.939668</v>
+      </c>
+      <c r="D11" s="2">
+        <f>(C11-C10)/C10</f>
+        <v>-0.40017428870896554</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A12" s="3">
+        <v>43731.046191898145</v>
+      </c>
+      <c r="B12" s="1">
+        <v>0.9</v>
+      </c>
+      <c r="C12" s="1">
+        <v>45881076.786539502</v>
+      </c>
+      <c r="D12" s="2">
+        <f>(C12-C11)/C11</f>
+        <v>-9.7353353000823789E-2</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A13" s="3">
+        <v>43731.069916354165</v>
+      </c>
+      <c r="B13" s="1">
+        <v>0.9</v>
+      </c>
+      <c r="C13" s="1">
+        <v>36884020.090438202</v>
+      </c>
+      <c r="D13" s="2">
+        <f>(C13-C12)/C12</f>
+        <v>-0.19609515134005831</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A14" s="3">
+        <v>43731.093321793982</v>
+      </c>
+      <c r="B14" s="1">
+        <v>0.9</v>
+      </c>
+      <c r="C14" s="1">
+        <v>51961728.485883802</v>
+      </c>
+      <c r="D14" s="2">
+        <f>(C14-C13)/C13</f>
+        <v>0.40878701287103841</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A15" s="3">
+        <v>43731.116856678243</v>
+      </c>
+      <c r="B15" s="1">
+        <v>0.9</v>
+      </c>
+      <c r="C15" s="1">
+        <v>23300455.492954198</v>
+      </c>
+      <c r="D15" s="2">
+        <f>(C15-C14)/C14</f>
+        <v>-0.55158428766887302</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A16" s="3">
+        <v>43731.139706944443</v>
+      </c>
+      <c r="B16" s="1">
+        <v>0.9</v>
+      </c>
+      <c r="C16" s="1">
+        <v>18673919.715530898</v>
+      </c>
+      <c r="D16" s="2">
+        <f>(C16-C15)/C15</f>
+        <v>-0.19855988561349427</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A17" s="3">
+        <v>43731.163294016202</v>
+      </c>
+      <c r="B17" s="1">
+        <v>0.9</v>
+      </c>
+      <c r="C17" s="1">
+        <v>22387443.221550301</v>
+      </c>
+      <c r="D17" s="2">
+        <f>(C17-C16)/C16</f>
+        <v>0.19886149038816445</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A18" s="3">
+        <v>43731.186685729168</v>
+      </c>
+      <c r="B18" s="1">
+        <v>0.9</v>
+      </c>
+      <c r="C18" s="1">
+        <v>21727289.674221501</v>
+      </c>
+      <c r="D18" s="2">
+        <f>(C18-C17)/C17</f>
+        <v>-2.9487670422915099E-2</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A19" s="3">
+        <v>43731.210210381942</v>
+      </c>
+      <c r="B19" s="1">
+        <v>0.9</v>
+      </c>
+      <c r="C19" s="1">
+        <v>25023973.804324102</v>
+      </c>
+      <c r="D19" s="2">
+        <f>(C19-C18)/C18</f>
+        <v>0.15173011358218211</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A20" s="3">
+        <v>43731.233252627317</v>
+      </c>
+      <c r="B20" s="1">
+        <v>0.9</v>
+      </c>
+      <c r="C20" s="1">
+        <v>28457230.8928365</v>
+      </c>
+      <c r="D20" s="2">
+        <f>(C20-C19)/C19</f>
+        <v>0.13719871653314858</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A21" s="3">
+        <v>43731.257403553238</v>
+      </c>
+      <c r="B21" s="1">
+        <v>0.9</v>
+      </c>
+      <c r="C21" s="1">
+        <v>20707684.776952799</v>
+      </c>
+      <c r="D21" s="2">
+        <f>(C21-C20)/C20</f>
+        <v>-0.27232256522311465</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A22" s="3">
+        <v>43731.282719212963</v>
+      </c>
+      <c r="B22" s="1">
+        <v>0.9</v>
+      </c>
+      <c r="C22" s="1">
+        <v>14613419.506552</v>
+      </c>
+      <c r="D22" s="2">
+        <f>(C22-C21)/C21</f>
+        <v>-0.29429969289389529</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A23" s="3">
+        <v>43731.307794131943</v>
+      </c>
+      <c r="B23" s="1">
+        <v>0.9</v>
+      </c>
+      <c r="C23" s="1">
+        <v>14221412.3280422</v>
+      </c>
+      <c r="D23" s="2">
+        <f>(C23-C22)/C22</f>
+        <v>-2.6825150563428456E-2</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A24" s="3">
+        <v>43731.332913043982</v>
+      </c>
+      <c r="B24" s="1">
+        <v>0.9</v>
+      </c>
+      <c r="C24" s="1">
+        <v>13799211.4196239</v>
+      </c>
+      <c r="D24" s="2">
+        <f>(C24-C23)/C23</f>
+        <v>-2.9687691959102504E-2</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A25" s="3">
+        <v>43731.356953784722</v>
+      </c>
+      <c r="B25" s="1">
+        <v>0.9</v>
+      </c>
+      <c r="C25" s="1">
+        <v>10991181.9397649</v>
+      </c>
+      <c r="D25" s="2">
+        <f>(C25-C24)/C24</f>
+        <v>-0.20349202533890401</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A26" s="3">
+        <v>43731.381473530091</v>
+      </c>
+      <c r="B26" s="1">
+        <v>0.9</v>
+      </c>
+      <c r="C26" s="1">
+        <v>7827470.0282455198</v>
+      </c>
+      <c r="D26" s="2">
+        <f>(C26-C25)/C25</f>
+        <v>-0.28784091909837423</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A27" s="3">
+        <v>43731.411144097219</v>
+      </c>
+      <c r="B27" s="1">
+        <v>0.9</v>
+      </c>
+      <c r="C27" s="1">
+        <v>11158393.262985799</v>
+      </c>
+      <c r="D27" s="2">
+        <f>(C27-C26)/C26</f>
+        <v>0.42554276448464229</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A28" s="3">
+        <v>43731.43582017361</v>
+      </c>
+      <c r="B28" s="1">
+        <v>0.9</v>
+      </c>
+      <c r="C28" s="1">
+        <v>11228451.7032403</v>
+      </c>
+      <c r="D28" s="2">
+        <f>(C28-C27)/C27</f>
+        <v>6.2785419552199642E-3</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A29" s="3">
+        <v>43731.460327280096</v>
+      </c>
+      <c r="B29" s="1">
+        <v>0.9</v>
+      </c>
+      <c r="C29" s="1">
+        <v>6580154.4599233698</v>
+      </c>
+      <c r="D29" s="2">
+        <f>(C29-C28)/C28</f>
+        <v>-0.41397490644017526</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A30" s="3">
+        <v>43731.484351354164</v>
+      </c>
+      <c r="B30" s="1">
+        <v>0.9</v>
+      </c>
+      <c r="C30" s="1">
+        <v>5694237.1644831495</v>
+      </c>
+      <c r="D30" s="2">
+        <f>(C30-C29)/C29</f>
+        <v>-0.13463472640892041</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A31" s="3">
+        <v>43731.508697951387</v>
+      </c>
+      <c r="B31" s="1">
+        <v>0.9</v>
+      </c>
+      <c r="C31" s="1">
+        <v>7602025.9353936203</v>
+      </c>
+      <c r="D31" s="2">
+        <f>(C31-C30)/C30</f>
+        <v>0.33503851627571529</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A32" s="3">
+        <v>43731.533164085646</v>
+      </c>
+      <c r="B32" s="1">
+        <v>0.9</v>
+      </c>
+      <c r="C32" s="1">
+        <v>7774374.1914764</v>
+      </c>
+      <c r="D32" s="2">
+        <f>(C32-C30)/C30</f>
+        <v>0.36530565322564307</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A33" s="3">
+        <v>43731.558252314811</v>
+      </c>
+      <c r="B33" s="1">
+        <v>0.9</v>
+      </c>
+      <c r="C33" s="1">
+        <v>8887725.9137989692</v>
+      </c>
+      <c r="D33" s="2">
+        <f>(C33-C32)/C32</f>
+        <v>0.14320788978014667</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A34" s="3">
+        <v>43731.581540358799</v>
+      </c>
+      <c r="B34" s="1">
+        <v>0.9</v>
+      </c>
+      <c r="C34" s="1">
+        <v>8256218.8607965596</v>
+      </c>
+      <c r="D34" s="2">
+        <f>(C34-C33)/C33</f>
+        <v>-7.1053839770411895E-2</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A35" s="3">
+        <v>43731.605839085649</v>
+      </c>
+      <c r="B35" s="1">
+        <v>0.9</v>
+      </c>
+      <c r="C35" s="1">
+        <v>9346117.9973511808</v>
+      </c>
+      <c r="D35" s="2">
+        <f>(C35-C34)/C34</f>
+        <v>0.13200947733227456</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A36" s="3">
+        <v>43731.629231712963</v>
+      </c>
+      <c r="B36" s="1">
+        <v>0.9</v>
+      </c>
+      <c r="C36" s="1">
+        <v>8787415.66559745</v>
+      </c>
+      <c r="D36" s="2">
+        <f>(C36-C35)/C35</f>
+        <v>-5.9779079604181627E-2</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A37" s="3">
+        <v>43731.652940740743</v>
+      </c>
+      <c r="B37" s="1">
+        <v>0.9</v>
+      </c>
+      <c r="C37" s="1">
+        <v>6106326.5948853297</v>
+      </c>
+      <c r="D37" s="2">
+        <f>(C37-C36)/C36</f>
+        <v>-0.30510552507587962</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A38" s="3">
+        <v>43731.676352164352</v>
+      </c>
+      <c r="B38" s="1">
+        <v>0.9</v>
+      </c>
+      <c r="C38" s="1">
+        <v>10212688.134928999</v>
+      </c>
+      <c r="D38" s="2">
+        <f>(C38-C37)/C37</f>
+        <v>0.67247656610492557</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A39" s="3">
+        <v>43731.69932334491</v>
+      </c>
+      <c r="B39" s="1">
+        <v>0.9</v>
+      </c>
+      <c r="C39" s="1">
+        <v>12426570.6614541</v>
+      </c>
+      <c r="D39" s="2">
+        <f>(C39-C38)/C38</f>
+        <v>0.21677764926094964</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A40" s="3">
+        <v>43731.722271296298</v>
+      </c>
+      <c r="B40" s="1">
+        <v>0.9</v>
+      </c>
+      <c r="C40" s="1">
+        <v>7555045.1385022402</v>
+      </c>
+      <c r="D40" s="2">
+        <f>(C40-C39)/C39</f>
+        <v>-0.39202493235425068</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A41" s="3">
+        <v>43731.745768553243</v>
+      </c>
+      <c r="B41" s="1">
+        <v>0.9</v>
+      </c>
+      <c r="C41" s="1">
+        <v>5974048.4311196003</v>
+      </c>
+      <c r="D41" s="2">
+        <f>(C41-C40)/C40</f>
+        <v>-0.20926370106321648</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A42" s="3">
+        <v>43731.769044594905</v>
+      </c>
+      <c r="B42" s="1">
+        <v>0.9</v>
+      </c>
+      <c r="C42" s="1">
+        <v>5586637.8612419497</v>
+      </c>
+      <c r="D42" s="2">
+        <f>(C42-C41)/C41</f>
+        <v>-6.4848916834952031E-2</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A43" s="3">
+        <v>43731.791736493054</v>
+      </c>
+      <c r="B43" s="1">
+        <v>0.9</v>
+      </c>
+      <c r="C43" s="1">
+        <v>6283506.2962794499</v>
+      </c>
+      <c r="D43" s="2">
+        <f>(C43-C42)/C42</f>
+        <v>0.12473842986532536</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A44" s="3">
+        <v>43731.815108414354</v>
+      </c>
+      <c r="B44" s="1">
+        <v>0.9</v>
+      </c>
+      <c r="C44" s="1">
+        <v>7465580.1919447798</v>
+      </c>
+      <c r="D44" s="2">
+        <f>(C44-C43)/C43</f>
+        <v>0.18812329294000263</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A45" s="3">
+        <v>43731.836908645833</v>
+      </c>
+      <c r="B45" s="1">
+        <v>0.9</v>
+      </c>
+      <c r="C45" s="1">
+        <v>6318532.6921694595</v>
+      </c>
+      <c r="D45" s="2">
+        <f>(C45-C44)/C44</f>
+        <v>-0.15364478986013208</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A46" s="3">
+        <v>43731.862660300925</v>
+      </c>
+      <c r="B46" s="1">
+        <v>0.9</v>
+      </c>
+      <c r="C46" s="1">
+        <v>7805773.7823088001</v>
+      </c>
+      <c r="D46" s="2">
+        <f>(C46-C45)/C45</f>
+        <v>0.23537760467433752</v>
+      </c>
+    </row>
+    <row r="47" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A47" s="3">
+        <v>43731.884564618056</v>
+      </c>
+      <c r="B47" s="1">
+        <v>0.9</v>
+      </c>
+      <c r="C47" s="1">
+        <v>8864587.4604190998</v>
+      </c>
+      <c r="D47" s="2">
+        <f>(C47-C46)/C46</f>
+        <v>0.13564493510047926</v>
+      </c>
+    </row>
+    <row r="48" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A48" s="3">
+        <v>43731.907564201392</v>
+      </c>
+      <c r="B48" s="1">
+        <v>0.9</v>
+      </c>
+      <c r="C48" s="1">
+        <v>6943692.4762246301</v>
+      </c>
+      <c r="D48" s="2">
+        <f>(C48-C47)/C47</f>
+        <v>-0.21669310532175104</v>
+      </c>
+    </row>
+    <row r="49" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A49" s="3">
+        <v>43731.929784571759</v>
+      </c>
+      <c r="B49" s="1">
+        <v>0.9</v>
+      </c>
+      <c r="C49" s="1">
+        <v>5018393.19882455</v>
+      </c>
+      <c r="D49" s="2">
+        <f>(C49-C48)/C48</f>
+        <v>-0.27727312002833521</v>
+      </c>
+    </row>
+    <row r="50" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A50" s="3">
+        <v>43731.950563738428</v>
+      </c>
+      <c r="B50" s="1">
+        <v>0.9</v>
+      </c>
+      <c r="C50" s="1">
+        <v>5936583.2975150002</v>
+      </c>
+      <c r="D50" s="2">
+        <f>(C50-C49)/C49</f>
+        <v>0.18296495756958947</v>
+      </c>
+    </row>
+    <row r="51" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A51" s="3">
+        <v>43731.972943020832</v>
+      </c>
+      <c r="B51" s="1">
+        <v>0.9</v>
+      </c>
+      <c r="C51" s="1">
+        <v>8225772.5154284202</v>
+      </c>
+      <c r="D51" s="2">
+        <f>(C51-C50)/C50</f>
+        <v>0.38560719241851688</v>
+      </c>
+    </row>
+    <row r="52" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A52" s="3">
+        <v>43731.994411377316</v>
+      </c>
+      <c r="B52" s="1">
+        <v>0.9</v>
+      </c>
+      <c r="C52" s="1">
+        <v>6907093.6067347797</v>
+      </c>
+      <c r="D52" s="2">
+        <f>(C52-C51)/C51</f>
+        <v>-0.16031064635209646</v>
+      </c>
+    </row>
+    <row r="53" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A53" s="3">
+        <v>43732.017248645832</v>
+      </c>
+      <c r="B53" s="1">
+        <v>0.9</v>
+      </c>
+      <c r="C53" s="1">
+        <v>7761654.1245476799</v>
+      </c>
+      <c r="D53" s="2">
+        <f>(C53-C52)/C52</f>
+        <v>0.12372215673748199</v>
+      </c>
+    </row>
+    <row r="54" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A54" s="3">
+        <v>43732.038523229166</v>
+      </c>
+      <c r="B54" s="1">
+        <v>0.9</v>
+      </c>
+      <c r="C54" s="1">
+        <v>8243263.69838861</v>
+      </c>
+      <c r="D54" s="2">
+        <f>(C54-C53)/C53</f>
+        <v>6.2049862840157996E-2</v>
+      </c>
+    </row>
+    <row r="55" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A55" s="3">
+        <v>43732.06148773148</v>
+      </c>
+      <c r="B55" s="1">
+        <v>0.9</v>
+      </c>
+      <c r="C55" s="1">
+        <v>8773894.6373157408</v>
+      </c>
+      <c r="D55" s="2">
+        <f>(C55-C54)/C54</f>
+        <v>6.4371462365186538E-2</v>
+      </c>
+    </row>
+    <row r="56" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A56" s="3">
+        <v>43732.083573495373</v>
+      </c>
+      <c r="B56" s="1">
+        <v>0.9</v>
+      </c>
+      <c r="C56" s="1">
+        <v>8716087.0516568795</v>
+      </c>
+      <c r="D56" s="2">
+        <f>(C56-C55)/C55</f>
+        <v>-6.5885889959292699E-3</v>
+      </c>
+    </row>
+    <row r="57" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A57" s="3">
+        <v>43732.103231631947</v>
+      </c>
+      <c r="B57" s="1">
+        <v>0.9</v>
+      </c>
+      <c r="C57" s="1">
+        <v>9526198.3536674306</v>
+      </c>
+      <c r="D57" s="2">
+        <f>(C57-C56)/C56</f>
+        <v>9.2944379422708209E-2</v>
+      </c>
+    </row>
+    <row r="58" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A58" s="3">
+        <v>43732.124374340281</v>
+      </c>
+      <c r="B58" s="1">
+        <v>0.9</v>
+      </c>
+      <c r="C58" s="1">
+        <v>11499360.383852899</v>
+      </c>
+      <c r="D58" s="2">
+        <f>(C58-C57)/C57</f>
+        <v>0.20713005933010342</v>
+      </c>
+    </row>
+    <row r="59" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A59" s="3">
+        <v>43732.144245370371</v>
+      </c>
+      <c r="B59" s="1">
+        <v>0.9</v>
+      </c>
+      <c r="C59" s="1">
+        <v>11166373.0106229</v>
+      </c>
+      <c r="D59" s="2">
+        <f>(C59-C58)/C58</f>
+        <v>-2.8957034314497289E-2</v>
+      </c>
+    </row>
+    <row r="60" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A60" s="3">
+        <v>43732.164338344905</v>
+      </c>
+      <c r="B60" s="1">
+        <v>0.9</v>
+      </c>
+      <c r="C60" s="1">
+        <v>9769672.7323780097</v>
+      </c>
+      <c r="D60" s="2">
+        <f>(C60-C59)/C59</f>
+        <v>-0.12508092618043193</v>
+      </c>
+    </row>
+    <row r="61" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A61" s="3">
+        <v>43732.184289236109</v>
+      </c>
+      <c r="B61" s="1">
+        <v>0.9</v>
+      </c>
+      <c r="C61" s="1">
+        <v>9113302.0081548896</v>
+      </c>
+      <c r="D61" s="2">
+        <f>(C61-C60)/C60</f>
+        <v>-6.7184514998933312E-2</v>
+      </c>
+    </row>
+    <row r="62" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A62" s="3">
+        <v>43732.204511574077</v>
+      </c>
+      <c r="B62" s="1">
+        <v>0.9</v>
+      </c>
+      <c r="C62" s="1">
+        <v>8908424.5873359703</v>
+      </c>
+      <c r="D62" s="2">
+        <f>(C62-C61)/C61</f>
+        <v>-2.2481140275565113E-2</v>
+      </c>
+    </row>
+    <row r="63" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A63" s="3">
+        <v>43732.224398576385</v>
+      </c>
+      <c r="B63" s="1">
+        <v>0.9</v>
+      </c>
+      <c r="C63" s="1">
+        <v>6980347.5328304498</v>
+      </c>
+      <c r="D63" s="2">
+        <f>(C63-C62)/C62</f>
+        <v>-0.21643299952793388</v>
+      </c>
+    </row>
+    <row r="64" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A64" s="3">
+        <v>43732.244451238425</v>
+      </c>
+      <c r="B64" s="1">
+        <v>0.9</v>
+      </c>
+      <c r="C64" s="1">
+        <v>10547658.4918481</v>
+      </c>
+      <c r="D64" s="2">
+        <f>(C64-C63)/C63</f>
+        <v>0.51105062351689923</v>
+      </c>
+    </row>
+    <row r="65" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A65" s="3">
+        <v>43732.264649849538</v>
+      </c>
+      <c r="B65" s="1">
+        <v>0.9</v>
+      </c>
+      <c r="C65" s="1">
+        <v>7893663.9331381703</v>
+      </c>
+      <c r="D65" s="2">
+        <f>(C65-C64)/C64</f>
+        <v>-0.251619310651848</v>
+      </c>
+    </row>
+    <row r="66" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A66" s="3">
+        <v>43732.284828900461</v>
+      </c>
+      <c r="B66" s="1">
+        <v>0.9</v>
+      </c>
+      <c r="C66" s="1">
+        <v>7872032.7382409796</v>
+      </c>
+      <c r="D66" s="2">
+        <f>(C66-C65)/C65</f>
+        <v>-2.7403237685837312E-3</v>
+      </c>
+    </row>
+    <row r="67" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A67" s="3">
+        <v>43732.30446605324</v>
+      </c>
+      <c r="B67" s="1">
+        <v>0.9</v>
+      </c>
+      <c r="C67" s="1">
+        <v>9625715.7394120805</v>
+      </c>
+      <c r="D67" s="2">
+        <f>(C67-C66)/C66</f>
+        <v>0.2227738450136279</v>
+      </c>
+    </row>
+    <row r="68" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A68" s="3">
+        <v>43732.325286030093</v>
+      </c>
+      <c r="B68" s="1">
+        <v>0.9</v>
+      </c>
+      <c r="C68" s="1">
+        <v>9473516.8728934303</v>
+      </c>
+      <c r="D68" s="2">
+        <f>(C68-C67)/C67</f>
+        <v>-1.5811693451062394E-2</v>
+      </c>
+    </row>
+    <row r="69" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A69" s="3">
+        <v>43732.345893715275</v>
+      </c>
+      <c r="B69" s="1">
+        <v>0.9</v>
+      </c>
+      <c r="C69" s="1">
+        <v>6771778.9840001902</v>
+      </c>
+      <c r="D69" s="2">
+        <f>(C69-C68)/C68</f>
+        <v>-0.28518848123063162</v>
+      </c>
+    </row>
+    <row r="70" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A70" s="3">
+        <v>43732.365969641207</v>
+      </c>
+      <c r="B70" s="1">
+        <v>0.9</v>
+      </c>
+      <c r="C70" s="1">
+        <v>9345339.9283929896</v>
+      </c>
+      <c r="D70" s="2">
+        <f>(C70-C69)/C69</f>
+        <v>0.38004207616246782</v>
+      </c>
+    </row>
+    <row r="71" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A71" s="3">
+        <v>43732.386019212965</v>
+      </c>
+      <c r="B71" s="1">
+        <v>0.9</v>
+      </c>
+      <c r="C71" s="1">
+        <v>8749845.9247072209</v>
+      </c>
+      <c r="D71" s="2">
+        <f>(C71-C70)/C70</f>
+        <v>-6.3720956995533165E-2</v>
+      </c>
+    </row>
+    <row r="72" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A72" s="3">
+        <v>43732.405909374997</v>
+      </c>
+      <c r="B72" s="1">
+        <v>0.9</v>
+      </c>
+      <c r="C72" s="1">
+        <v>9261091.2615985703</v>
+      </c>
+      <c r="D72" s="2">
+        <f>(C72-C71)/C71</f>
+        <v>5.8429067356229616E-2</v>
+      </c>
+    </row>
+    <row r="73" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A73" s="3">
+        <v>43732.426122766206</v>
+      </c>
+      <c r="B73" s="1">
+        <v>0.9</v>
+      </c>
+      <c r="C73" s="1">
+        <v>7223886.9166597603</v>
+      </c>
+      <c r="D73" s="2">
+        <f>(C73-C72)/C72</f>
+        <v>-0.21997454591405952</v>
+      </c>
+    </row>
+    <row r="74" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A74" s="3">
+        <v>43732.446152118056</v>
+      </c>
+      <c r="B74" s="1">
+        <v>0.9</v>
+      </c>
+      <c r="C74" s="1">
+        <v>9094109.5142613109</v>
+      </c>
+      <c r="D74" s="2">
+        <f>(C74-C73)/C73</f>
+        <v>0.25889422400680651</v>
+      </c>
+    </row>
+    <row r="75" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A75" s="3">
+        <v>43732.466284409726</v>
+      </c>
+      <c r="B75" s="1">
+        <v>0.9</v>
+      </c>
+      <c r="C75" s="1">
+        <v>8086894.8526188498</v>
+      </c>
+      <c r="D75" s="2">
+        <f>(C75-C74)/C74</f>
+        <v>-0.11075462199602445</v>
+      </c>
+    </row>
+    <row r="76" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A76" s="3">
+        <v>43732.486670219907</v>
+      </c>
+      <c r="B76" s="1">
+        <v>0.9</v>
+      </c>
+      <c r="C76" s="1">
+        <v>9608504.8194003105</v>
+      </c>
+      <c r="D76" s="2">
+        <f>(C76-C75)/C75</f>
+        <v>0.18815750600351933</v>
+      </c>
+    </row>
+    <row r="77" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A77" s="3">
+        <v>43732.506780821757</v>
+      </c>
+      <c r="B77" s="1">
+        <v>0.9</v>
+      </c>
+      <c r="C77" s="1">
+        <v>8167561.5776757495</v>
+      </c>
+      <c r="D77" s="2">
+        <f>(C77-C76)/C76</f>
+        <v>-0.14996539719844712</v>
+      </c>
+    </row>
+    <row r="78" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A78" s="3">
+        <v>43732.527575231485</v>
+      </c>
+      <c r="B78" s="1">
+        <v>0.9</v>
+      </c>
+      <c r="C78" s="1">
+        <v>9162142.1501978301</v>
+      </c>
+      <c r="D78" s="2">
+        <f>(C78-C77)/C77</f>
+        <v>0.1217720323334384</v>
+      </c>
+    </row>
+    <row r="79" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A79" s="3">
+        <v>43732.548066469906</v>
+      </c>
+      <c r="B79" s="1">
+        <v>0.9</v>
+      </c>
+      <c r="C79" s="1">
+        <v>10179691.575688399</v>
+      </c>
+      <c r="D79" s="2">
+        <f>(C79-C78)/C78</f>
+        <v>0.11106020937129842</v>
+      </c>
+    </row>
+    <row r="80" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A80" s="3">
+        <v>43732.568241053239</v>
+      </c>
+      <c r="B80" s="1">
+        <v>0.9</v>
+      </c>
+      <c r="C80" s="1">
+        <v>10752796.858561199</v>
+      </c>
+      <c r="D80" s="2">
+        <f>(C80-C79)/C79</f>
+        <v>5.6298884756146812E-2</v>
+      </c>
+    </row>
+    <row r="81" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A81" s="3">
+        <v>43732.588273958332</v>
+      </c>
+      <c r="B81" s="1">
+        <v>0.9</v>
+      </c>
+      <c r="C81" s="1">
+        <v>9900381.7571215592</v>
+      </c>
+      <c r="D81" s="2">
+        <f>(C81-C80)/C80</f>
+        <v>-7.9273803146477292E-2</v>
+      </c>
+    </row>
+    <row r="82" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A82" s="3">
+        <v>43732.608516863424</v>
+      </c>
+      <c r="B82" s="1">
+        <v>0.9</v>
+      </c>
+      <c r="C82" s="1">
+        <v>8339031.87166679</v>
+      </c>
+      <c r="D82" s="2">
+        <f>(C82-C81)/C81</f>
+        <v>-0.15770602828841992</v>
+      </c>
+    </row>
+    <row r="83" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A83" s="3">
+        <v>43732.628855787036</v>
+      </c>
+      <c r="B83" s="1">
+        <v>0.9</v>
+      </c>
+      <c r="C83" s="1">
+        <v>7073649.2107376698</v>
+      </c>
+      <c r="D83" s="2">
+        <f>(C83-C82)/C82</f>
+        <v>-0.15174215429352927</v>
+      </c>
+    </row>
+    <row r="84" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A84" s="3">
+        <v>43732.649320868055</v>
+      </c>
+      <c r="B84" s="1">
+        <v>0.9</v>
+      </c>
+      <c r="C84" s="1">
+        <v>7834860.1909906296</v>
+      </c>
+      <c r="D84" s="2">
+        <f>(C84-C83)/C83</f>
+        <v>0.10761220376852382</v>
+      </c>
+    </row>
+    <row r="85" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A85" s="3">
+        <v>43732.669473993054</v>
+      </c>
+      <c r="B85" s="1">
+        <v>0.9</v>
+      </c>
+      <c r="C85" s="1">
+        <v>7875096.2232888797</v>
+      </c>
+      <c r="D85" s="2">
+        <f>(C85-C84)/C84</f>
+        <v>5.1355137574143148E-3</v>
+      </c>
+    </row>
+    <row r="86" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A86" s="3">
+        <v>43732.690235729169</v>
+      </c>
+      <c r="B86" s="1">
+        <v>0.9</v>
+      </c>
+      <c r="C86" s="1">
+        <v>6798184.0071253702</v>
+      </c>
+      <c r="D86" s="2">
+        <f>(C86-C85)/C85</f>
+        <v>-0.13674908669417607</v>
+      </c>
+    </row>
+    <row r="87" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A87" s="3">
+        <v>43732.710538310188</v>
+      </c>
+      <c r="B87" s="1">
+        <v>0.9</v>
+      </c>
+      <c r="C87" s="1">
+        <v>5947294.9817488296</v>
+      </c>
+      <c r="D87" s="2">
+        <f>(C87-C86)/C86</f>
+        <v>-0.12516416508948561</v>
+      </c>
+    </row>
+    <row r="88" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A88" s="3">
+        <v>43732.731065081018</v>
+      </c>
+      <c r="B88" s="1">
+        <v>0.9</v>
+      </c>
+      <c r="C88" s="1">
+        <v>9243918.2330143806</v>
+      </c>
+      <c r="D88" s="2">
+        <f>(C88-C87)/C87</f>
+        <v>0.55430632941232783</v>
+      </c>
+    </row>
+    <row r="89" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A89" s="3">
+        <v>43732.751798530095</v>
+      </c>
+      <c r="B89" s="1">
+        <v>0.9</v>
+      </c>
+      <c r="C89" s="1">
+        <v>10158971.5577267</v>
+      </c>
+      <c r="D89" s="2">
+        <f>(C89-C88)/C88</f>
+        <v>9.898976836945976E-2</v>
+      </c>
+    </row>
+    <row r="90" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A90" s="3">
+        <v>43732.772150578705</v>
+      </c>
+      <c r="B90" s="1">
+        <v>0.9</v>
+      </c>
+      <c r="C90" s="1">
+        <v>9430798.9976223409</v>
+      </c>
+      <c r="D90" s="2">
+        <f>(C90-C89)/C89</f>
+        <v>-7.1677783126632172E-2</v>
+      </c>
+    </row>
+    <row r="91" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A91" s="3">
+        <v>43732.792863888892</v>
+      </c>
+      <c r="B91" s="1">
+        <v>0.9</v>
+      </c>
+      <c r="C91" s="1">
+        <v>7920212.32179425</v>
+      </c>
+      <c r="D91" s="2">
+        <f>(C91-C90)/C90</f>
+        <v>-0.16017589561700282</v>
+      </c>
+    </row>
+    <row r="92" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A92" s="3">
+        <v>43732.813123460648</v>
+      </c>
+      <c r="B92" s="1">
+        <v>0.9</v>
+      </c>
+      <c r="C92" s="1">
+        <v>7781097.7558316998</v>
+      </c>
+      <c r="D92" s="2">
+        <f>(C92-C91)/C91</f>
+        <v>-1.7564499575313801E-2</v>
+      </c>
+    </row>
+    <row r="93" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A93" s="3">
+        <v>43732.833722835647</v>
+      </c>
+      <c r="B93" s="1">
+        <v>0.9</v>
+      </c>
+      <c r="C93" s="1">
+        <v>8909239.7825026009</v>
+      </c>
+      <c r="D93" s="2">
+        <f>(C93-C92)/C92</f>
+        <v>0.14498494455045144</v>
+      </c>
+    </row>
+    <row r="94" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A94" s="3">
+        <v>43732.853825497688</v>
+      </c>
+      <c r="B94" s="1">
+        <v>0.9</v>
+      </c>
+      <c r="C94" s="1">
+        <v>8402575.5211147591</v>
+      </c>
+      <c r="D94" s="2">
+        <f>(C94-C93)/C93</f>
+        <v>-5.6869528013255476E-2</v>
+      </c>
+    </row>
+    <row r="95" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A95" s="3">
+        <v>43732.873943287035</v>
+      </c>
+      <c r="B95" s="1">
+        <v>0.9</v>
+      </c>
+      <c r="C95" s="1">
+        <v>9763055.8355248403</v>
+      </c>
+      <c r="D95" s="2">
+        <f>(C95-C94)/C94</f>
+        <v>0.16191229831750301</v>
+      </c>
+    </row>
+    <row r="96" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A96" s="3">
+        <v>43732.894267326388</v>
+      </c>
+      <c r="B96" s="1">
+        <v>0.9</v>
+      </c>
+      <c r="C96" s="1">
+        <v>8955216.1531386003</v>
+      </c>
+      <c r="D96" s="2">
+        <f>(C96-C95)/C95</f>
+        <v>-8.2744552115204845E-2</v>
+      </c>
+    </row>
+    <row r="97" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A97" s="3">
+        <v>43732.914320138887</v>
+      </c>
+      <c r="B97" s="1">
+        <v>0.9</v>
+      </c>
+      <c r="C97" s="1">
+        <v>9327090.2172295991</v>
+      </c>
+      <c r="D97" s="2">
+        <f>(C97-C96)/C96</f>
+        <v>4.1525972989570489E-2</v>
+      </c>
+    </row>
+    <row r="98" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A98" s="3">
+        <v>43732.934666898145</v>
+      </c>
+      <c r="B98" s="1">
+        <v>0.9</v>
+      </c>
+      <c r="C98" s="1">
+        <v>11922100.641083799</v>
+      </c>
+      <c r="D98" s="2">
+        <f>(C98-C97)/C97</f>
+        <v>0.2782229359227737</v>
+      </c>
+    </row>
+    <row r="99" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A99" s="3">
+        <v>43732.954982870368</v>
+      </c>
+      <c r="B99" s="1">
+        <v>0.9</v>
+      </c>
+      <c r="C99" s="1">
+        <v>10177384.092680801</v>
+      </c>
+      <c r="D99" s="2">
+        <f>(C99-C98)/C98</f>
+        <v>-0.1463430481697722</v>
+      </c>
+    </row>
+    <row r="100" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A100" s="3">
+        <v>43732.975228206022</v>
+      </c>
+      <c r="B100" s="1">
+        <v>0.9</v>
+      </c>
+      <c r="C100" s="1">
+        <v>10493422.551833799</v>
+      </c>
+      <c r="D100" s="2">
+        <f>(C100-C99)/C99</f>
+        <v>3.1053014829250828E-2</v>
+      </c>
+    </row>
+    <row r="101" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A101" s="3">
+        <v>43732.995505208331</v>
+      </c>
+      <c r="B101" s="1">
+        <v>0.9</v>
+      </c>
+      <c r="C101" s="1">
+        <v>10571888.3616184</v>
+      </c>
+      <c r="D101" s="2">
+        <f>(C101-C100)/C100</f>
+        <v>7.4776184221122463E-3</v>
+      </c>
+    </row>
+    <row r="102" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A102" s="3">
+        <v>43733.015987465275</v>
+      </c>
+      <c r="B102" s="1">
+        <v>0.9</v>
+      </c>
+      <c r="C102" s="1">
+        <v>11825761.163128899</v>
+      </c>
+      <c r="D102" s="2">
+        <f>(C102-C101)/C101</f>
+        <v>0.11860443079050358</v>
+      </c>
+    </row>
+    <row r="103" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A103" s="3">
+        <v>43733.036045949077</v>
+      </c>
+      <c r="B103" s="1">
+        <v>0.9</v>
+      </c>
+      <c r="C103" s="1">
+        <v>11766830.277974</v>
+      </c>
+      <c r="D103" s="2">
+        <f>(C103-C102)/C102</f>
+        <v>-4.983263600709071E-3</v>
+      </c>
+    </row>
+    <row r="104" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A104" s="3">
+        <v>43733.056632951389</v>
+      </c>
+      <c r="B104" s="1">
+        <v>0.9</v>
+      </c>
+      <c r="C104" s="1">
+        <v>11358980.4696874</v>
+      </c>
+      <c r="D104" s="2">
+        <f>(C104-C103)/C103</f>
+        <v>-3.4660974846390233E-2</v>
+      </c>
+    </row>
+    <row r="105" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A105" s="3">
+        <v>43733.076948530092</v>
+      </c>
+      <c r="B105" s="1">
+        <v>0.9</v>
+      </c>
+      <c r="C105" s="1">
+        <v>10595959.5308841</v>
+      </c>
+      <c r="D105" s="2">
+        <f>(C105-C104)/C104</f>
+        <v>-6.7173364796206808E-2</v>
+      </c>
+    </row>
+    <row r="106" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A106" s="3">
+        <v>43733.097139814818</v>
+      </c>
+      <c r="B106" s="1">
+        <v>0.9</v>
+      </c>
+      <c r="C106" s="1">
+        <v>10612407.833329</v>
+      </c>
+      <c r="D106" s="2">
+        <f>(C106-C105)/C105</f>
+        <v>1.5523183527605497E-3</v>
+      </c>
+    </row>
+    <row r="107" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A107" s="3">
+        <v>43733.117048611108</v>
+      </c>
+      <c r="B107" s="1">
+        <v>0.9</v>
+      </c>
+      <c r="C107" s="1">
+        <v>11111308.095895801</v>
+      </c>
+      <c r="D107" s="2">
+        <f>(C107-C106)/C106</f>
+        <v>4.7011033726009892E-2</v>
+      </c>
+    </row>
+    <row r="108" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A108" s="3">
+        <v>43733.136765740739</v>
+      </c>
+      <c r="B108" s="1">
+        <v>0.9</v>
+      </c>
+      <c r="C108" s="1">
+        <v>11482697.728402199</v>
+      </c>
+      <c r="D108" s="2">
+        <f>(C108-C107)/C107</f>
+        <v>3.3424474355416282E-2</v>
+      </c>
+    </row>
+    <row r="109" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A109" s="3">
+        <v>43733.156851388892</v>
+      </c>
+      <c r="B109" s="1">
+        <v>0.9</v>
+      </c>
+      <c r="C109" s="1">
+        <v>12108463.663791399</v>
+      </c>
+      <c r="D109" s="2">
+        <f>(C109-C108)/C108</f>
+        <v>5.4496421502186025E-2</v>
+      </c>
+    </row>
+    <row r="110" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A110" s="3">
+        <v>43733.176932754628</v>
+      </c>
+      <c r="B110" s="1">
+        <v>0.9</v>
+      </c>
+      <c r="C110" s="1">
+        <v>12703801.894834301</v>
+      </c>
+      <c r="D110" s="2">
+        <f>(C110-C109)/C109</f>
+        <v>4.9167115463473167E-2</v>
+      </c>
+    </row>
+    <row r="111" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A111" s="3">
+        <v>43733.196987418982</v>
+      </c>
+      <c r="B111" s="1">
+        <v>0.9</v>
+      </c>
+      <c r="C111" s="1">
+        <v>13554301.475640699</v>
+      </c>
+      <c r="D111" s="2">
+        <f>(C111-C110)/C110</f>
+        <v>6.6948429127522385E-2</v>
+      </c>
+    </row>
+    <row r="112" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A112" s="3">
+        <v>43733.216769560182</v>
+      </c>
+      <c r="B112" s="1">
+        <v>0.9</v>
+      </c>
+      <c r="C112" s="1">
+        <v>10685609.0402385</v>
+      </c>
+      <c r="D112" s="2">
+        <f>(C112-C111)/C111</f>
+        <v>-0.21164443188442503</v>
+      </c>
+    </row>
+    <row r="113" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A113" s="3">
+        <v>43733.236735219907</v>
+      </c>
+      <c r="B113" s="1">
+        <v>0.9</v>
+      </c>
+      <c r="C113" s="1">
+        <v>10060266.226524999</v>
+      </c>
+      <c r="D113" s="2">
+        <f>(C113-C112)/C112</f>
+        <v>-5.8521962703170623E-2</v>
+      </c>
+    </row>
+    <row r="114" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A114" s="3">
+        <v>43733.256904131944</v>
+      </c>
+      <c r="B114" s="1">
+        <v>0.9</v>
+      </c>
+      <c r="C114" s="1">
+        <v>13613881.8641649</v>
+      </c>
+      <c r="D114" s="2">
+        <f>(C114-C113)/C113</f>
+        <v>0.35323276319173363</v>
+      </c>
+    </row>
+    <row r="115" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A115" s="3">
+        <v>43733.27718892361</v>
+      </c>
+      <c r="B115" s="1">
+        <v>0.9</v>
+      </c>
+      <c r="C115" s="1">
+        <v>9865531.9064659998</v>
+      </c>
+      <c r="D115" s="2">
+        <f>(C115-C114)/C114</f>
+        <v>-0.27533292819041444</v>
+      </c>
+    </row>
+    <row r="116" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A116" s="3">
+        <v>43733.297144675926</v>
+      </c>
+      <c r="B116" s="1">
+        <v>0.9</v>
+      </c>
+      <c r="C116" s="1">
+        <v>10216602.912662201</v>
+      </c>
+      <c r="D116" s="2">
+        <f>(C116-C115)/C115</f>
+        <v>3.5585613581169837E-2</v>
+      </c>
+    </row>
+    <row r="117" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A117" s="3">
+        <v>43733.317124074078</v>
+      </c>
+      <c r="B117" s="1">
+        <v>0.9</v>
+      </c>
+      <c r="C117" s="1">
+        <v>10655126.5385125</v>
+      </c>
+      <c r="D117" s="2">
+        <f>(C117-C116)/C116</f>
+        <v>4.2922645579853577E-2</v>
+      </c>
+    </row>
+    <row r="118" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A118" s="3">
+        <v>43733.336891701387</v>
+      </c>
+      <c r="B118" s="1">
+        <v>0.9</v>
+      </c>
+      <c r="C118" s="1">
+        <v>12130281.546378801</v>
+      </c>
+      <c r="D118" s="2">
+        <f>(C118-C117)/C117</f>
+        <v>0.13844556444584827</v>
+      </c>
+    </row>
+    <row r="119" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A119" s="3">
+        <v>43733.356873414348</v>
+      </c>
+      <c r="B119" s="1">
+        <v>0.9</v>
+      </c>
+      <c r="C119" s="1">
+        <v>13932043.1403326</v>
+      </c>
+      <c r="D119" s="2">
+        <f>(C119-C118)/C118</f>
+        <v>0.14853419412113081</v>
+      </c>
+    </row>
+    <row r="120" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A120" s="3">
+        <v>43733.376863275465</v>
+      </c>
+      <c r="B120" s="1">
+        <v>0.9</v>
+      </c>
+      <c r="C120" s="1">
+        <v>9715604.4035289604</v>
+      </c>
+      <c r="D120" s="2">
+        <f>(C120-C119)/C119</f>
+        <v>-0.30264324437793699</v>
+      </c>
+    </row>
+    <row r="121" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A121" s="3">
+        <v>43733.396708564818</v>
+      </c>
+      <c r="B121" s="1">
+        <v>0.9</v>
+      </c>
+      <c r="C121" s="1">
+        <v>14176028.9669978</v>
+      </c>
+      <c r="D121" s="2">
+        <f>(C121-C120)/C120</f>
+        <v>0.45909903061189872</v>
+      </c>
+    </row>
+    <row r="122" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A122" s="3">
+        <v>43733.416619178242</v>
+      </c>
+      <c r="B122" s="1">
+        <v>0.9</v>
+      </c>
+      <c r="C122" s="1">
+        <v>11671773.8648635</v>
+      </c>
+      <c r="D122" s="2">
+        <f>(C122-C121)/C121</f>
+        <v>-0.17665420323027539</v>
+      </c>
+    </row>
+    <row r="123" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A123" s="3">
+        <v>43733.43666068287</v>
+      </c>
+      <c r="B123" s="1">
+        <v>0.9</v>
+      </c>
+      <c r="C123" s="1">
+        <v>11033182.027128199</v>
+      </c>
+      <c r="D123" s="2">
+        <f>(C123-C122)/C122</f>
+        <v>-5.471249230228032E-2</v>
+      </c>
+    </row>
+    <row r="124" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A124" s="3">
+        <v>43733.456342395832</v>
+      </c>
+      <c r="B124" s="1">
+        <v>0.9</v>
+      </c>
+      <c r="C124" s="1">
+        <v>11529359.8826105</v>
+      </c>
+      <c r="D124" s="2">
+        <f>(C124-C123)/C123</f>
+        <v>4.4971419329646434E-2</v>
+      </c>
+    </row>
+    <row r="125" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A125" s="3">
+        <v>43733.476366863426</v>
+      </c>
+      <c r="B125" s="1">
+        <v>0.9</v>
+      </c>
+      <c r="C125" s="1">
+        <v>13431505.780205701</v>
+      </c>
+      <c r="D125" s="2">
+        <f>(C125-C124)/C124</f>
+        <v>0.16498278455720417</v>
+      </c>
+    </row>
+    <row r="126" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A126" s="3">
+        <v>43733.496078206015</v>
+      </c>
+      <c r="B126" s="1">
+        <v>0.9</v>
+      </c>
+      <c r="C126" s="1">
+        <v>9501113.5666300207</v>
+      </c>
+      <c r="D126" s="2">
+        <f>(C126-C125)/C125</f>
+        <v>-0.2926248387852376</v>
+      </c>
+    </row>
+    <row r="127" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A127" s="3">
+        <v>43733.515961770834</v>
+      </c>
+      <c r="B127" s="1">
+        <v>0.9</v>
+      </c>
+      <c r="C127" s="1">
+        <v>10408189.666232301</v>
+      </c>
+      <c r="D127" s="2">
+        <f>(C127-C126)/C126</f>
+        <v>9.5470503877369592E-2</v>
+      </c>
+    </row>
+    <row r="128" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A128" s="3">
+        <v>43733.535490590279</v>
+      </c>
+      <c r="B128" s="1">
+        <v>0.9</v>
+      </c>
+      <c r="C128" s="1">
+        <v>9508783.8172435593</v>
+      </c>
+      <c r="D128" s="2">
+        <f>(C128-C127)/C127</f>
+        <v>-8.6413283945691283E-2</v>
+      </c>
+    </row>
+    <row r="129" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A129" s="3">
+        <v>43733.554867164348</v>
+      </c>
+      <c r="B129" s="1">
+        <v>0.9</v>
+      </c>
+      <c r="C129" s="1">
+        <v>10907746.960920099</v>
+      </c>
+      <c r="D129" s="2">
+        <f>(C129-C128)/C128</f>
+        <v>0.14712324631248966</v>
+      </c>
+    </row>
+    <row r="130" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A130" s="3">
+        <v>43733.574338969906</v>
+      </c>
+      <c r="B130" s="1">
+        <v>0.9</v>
+      </c>
+      <c r="C130" s="1">
+        <v>10917398.9459047</v>
+      </c>
+      <c r="D130" s="2">
+        <f>(C130-C129)/C129</f>
+        <v>8.8487430256511414E-4</v>
+      </c>
+    </row>
+    <row r="131" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A131" s="3">
+        <v>43733.593819178241</v>
+      </c>
+      <c r="B131" s="1">
+        <v>0.9</v>
+      </c>
+      <c r="C131" s="1">
+        <v>14160304.8346682</v>
+      </c>
+      <c r="D131" s="2">
+        <f>(C131-C130)/C130</f>
+        <v>0.29704015625259977</v>
+      </c>
+    </row>
+    <row r="132" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A132" s="3">
+        <v>43733.613480636574</v>
+      </c>
+      <c r="B132" s="1">
+        <v>0.9</v>
+      </c>
+      <c r="C132" s="1">
+        <v>13629440.0271507</v>
+      </c>
+      <c r="D132" s="2">
+        <f>(C132-C131)/C131</f>
+        <v>-3.7489645436007989E-2</v>
+      </c>
+    </row>
+    <row r="133" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A133" s="3">
+        <v>43733.632949108796</v>
+      </c>
+      <c r="B133" s="1">
+        <v>0.9</v>
+      </c>
+      <c r="C133" s="1">
+        <v>11985011.9607371</v>
+      </c>
+      <c r="D133" s="2">
+        <f>(C133-C132)/C132</f>
+        <v>-0.12065265066927153</v>
+      </c>
+    </row>
+    <row r="134" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A134" s="3">
+        <v>43733.65242071759</v>
+      </c>
+      <c r="B134" s="1">
+        <v>0.9</v>
+      </c>
+      <c r="C134" s="1">
+        <v>12182880.250477999</v>
+      </c>
+      <c r="D134" s="2">
+        <f>(C134-C133)/C133</f>
+        <v>1.6509644745379987E-2</v>
+      </c>
+    </row>
+    <row r="135" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A135" s="3">
+        <v>43733.671911805555</v>
+      </c>
+      <c r="B135" s="1">
+        <v>0.9</v>
+      </c>
+      <c r="C135" s="1">
+        <v>14521517.5582019</v>
+      </c>
+      <c r="D135" s="2">
+        <f>(C135-C134)/C134</f>
+        <v>0.19196095337407121</v>
+      </c>
+    </row>
+    <row r="136" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A136" s="3">
+        <v>43733.691627546294</v>
+      </c>
+      <c r="B136" s="1">
+        <v>0.9</v>
+      </c>
+      <c r="C136" s="1">
+        <v>13216335.4916855</v>
+      </c>
+      <c r="D136" s="2">
+        <f>(C136-C135)/C135</f>
+        <v>-8.9879178349319244E-2</v>
+      </c>
+    </row>
+    <row r="137" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A137" s="3">
+        <v>43733.711316203706</v>
+      </c>
+      <c r="B137" s="1">
+        <v>0.9</v>
+      </c>
+      <c r="C137" s="1">
+        <v>11703223.0840302</v>
+      </c>
+      <c r="D137" s="2">
+        <f>(C137-C136)/C136</f>
+        <v>-0.11448804463288718</v>
+      </c>
+    </row>
+    <row r="138" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A138" s="3">
+        <v>43733.730873692133</v>
+      </c>
+      <c r="B138">
+        <v>0.9</v>
+      </c>
+      <c r="C138">
+        <v>9462139.2012504209</v>
+      </c>
+    </row>
+    <row r="139" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A139" s="3">
+        <v>43733.750414895832</v>
+      </c>
+      <c r="B139">
+        <v>0.9</v>
+      </c>
+      <c r="C139">
+        <v>10140643.0278219</v>
+      </c>
+    </row>
+    <row r="140" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A140" s="3">
+        <v>43733.769744942132</v>
+      </c>
+      <c r="B140">
+        <v>0.9</v>
+      </c>
+      <c r="C140">
+        <v>11836601.603824399</v>
+      </c>
+    </row>
+    <row r="141" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A141" s="3">
+        <v>43733.789209259259</v>
+      </c>
+      <c r="B141">
+        <v>0.9</v>
+      </c>
+      <c r="C141">
+        <v>9422842.3194465693</v>
+      </c>
+    </row>
+    <row r="142" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A142" s="3">
+        <v>43733.808580011573</v>
+      </c>
+      <c r="B142">
+        <v>0.9</v>
+      </c>
+      <c r="C142">
+        <v>9956083.5383792706</v>
+      </c>
+    </row>
+    <row r="143" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A143" s="3">
+        <v>43733.827945567129</v>
+      </c>
+      <c r="B143">
+        <v>0.9</v>
+      </c>
+      <c r="C143">
+        <v>11052635.6461512</v>
+      </c>
+    </row>
+    <row r="144" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A144" s="3">
+        <v>43733.847169328707</v>
+      </c>
+      <c r="B144">
+        <v>0.9</v>
+      </c>
+      <c r="C144">
+        <v>9368232.5286609493</v>
+      </c>
+    </row>
+    <row r="145" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A145" s="3">
+        <v>43733.866648611111</v>
+      </c>
+      <c r="B145">
+        <v>0.9</v>
+      </c>
+      <c r="C145">
+        <v>8035129.1142357001</v>
+      </c>
+    </row>
+    <row r="146" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A146" s="3">
+        <v>43733.88601952546</v>
+      </c>
+      <c r="B146">
+        <v>0.9</v>
+      </c>
+      <c r="C146">
+        <v>8755057.3914310206</v>
+      </c>
+    </row>
+    <row r="147" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A147" s="3">
+        <v>43733.905326423614</v>
+      </c>
+      <c r="B147">
+        <v>0.9</v>
+      </c>
+      <c r="C147">
+        <v>10113663.9520045</v>
+      </c>
+    </row>
+    <row r="148" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A148" s="3">
+        <v>43733.924996099537</v>
+      </c>
+      <c r="B148">
+        <v>0.9</v>
+      </c>
+      <c r="C148">
+        <v>9256506.0298943408</v>
+      </c>
+    </row>
+    <row r="149" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A149" s="3">
+        <v>43733.944277743052</v>
+      </c>
+      <c r="B149">
+        <v>0.9</v>
+      </c>
+      <c r="C149">
+        <v>11622405.8031116</v>
+      </c>
+    </row>
+    <row r="150" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A150" s="3">
+        <v>43733.963666122683</v>
+      </c>
+      <c r="B150">
+        <v>0.9</v>
+      </c>
+      <c r="C150">
+        <v>10381440.1668764</v>
+      </c>
+    </row>
+    <row r="151" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A151" s="3">
+        <v>43733.982845983795</v>
+      </c>
+      <c r="B151">
+        <v>0.9</v>
+      </c>
+      <c r="C151">
+        <v>10352893.730533401</v>
+      </c>
+    </row>
+    <row r="152" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A152" s="3">
+        <v>43734.002202430558</v>
+      </c>
+      <c r="B152">
+        <v>0.9</v>
+      </c>
+      <c r="C152">
+        <v>10897656.658714101</v>
+      </c>
+    </row>
+    <row r="153" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A153" s="3">
+        <v>43734.021421331017</v>
+      </c>
+      <c r="B153">
+        <v>0.9</v>
+      </c>
+      <c r="C153">
+        <v>8460701.3957199994</v>
+      </c>
+    </row>
+    <row r="154" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A154" s="3">
+        <v>43734.040835532411</v>
+      </c>
+      <c r="B154">
+        <v>0.9</v>
+      </c>
+      <c r="C154">
+        <v>9565198.7669808399</v>
+      </c>
+    </row>
+    <row r="155" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A155" s="3">
+        <v>43734.060293206021</v>
+      </c>
+      <c r="B155">
+        <v>0.9</v>
+      </c>
+      <c r="C155">
+        <v>11325566.920112099</v>
+      </c>
+    </row>
+    <row r="156" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A156" s="3">
+        <v>43734.079940821757</v>
+      </c>
+      <c r="B156">
+        <v>0.9</v>
+      </c>
+      <c r="C156">
+        <v>10264873.1519859</v>
+      </c>
+    </row>
+    <row r="157" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A157" s="3">
+        <v>43734.099278969908</v>
+      </c>
+      <c r="B157">
+        <v>0.9</v>
+      </c>
+      <c r="C157">
+        <v>10160784.271545</v>
+      </c>
+    </row>
+    <row r="158" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A158" s="3">
+        <v>43734.118626620373</v>
+      </c>
+      <c r="B158">
+        <v>0.9</v>
+      </c>
+      <c r="C158">
+        <v>8983007.1700480301</v>
+      </c>
+    </row>
+    <row r="159" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A159" s="3">
+        <v>43734.13796068287</v>
+      </c>
+      <c r="B159">
+        <v>0.9</v>
+      </c>
+      <c r="C159">
+        <v>8835698.1042707209</v>
+      </c>
+    </row>
+    <row r="160" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A160" s="3">
+        <v>43734.15766646991</v>
+      </c>
+      <c r="B160">
+        <v>0.9</v>
+      </c>
+      <c r="C160">
+        <v>8014145.9304012703</v>
+      </c>
+    </row>
+    <row r="161" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A161" s="3">
+        <v>43734.177351388891</v>
+      </c>
+      <c r="B161">
+        <v>0.9</v>
+      </c>
+      <c r="C161">
+        <v>10459898.4393805</v>
+      </c>
+    </row>
+    <row r="162" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A162" s="3">
+        <v>43734.196645717595</v>
+      </c>
+      <c r="B162">
+        <v>0.9</v>
+      </c>
+      <c r="C162">
+        <v>11678967.5267171</v>
+      </c>
+    </row>
+    <row r="163" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A163" s="3">
+        <v>43734.21634684028</v>
+      </c>
+      <c r="B163">
+        <v>0.9</v>
+      </c>
+      <c r="C163">
+        <v>12915385.3178194</v>
+      </c>
+    </row>
+    <row r="164" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A164" s="3">
+        <v>43734.235757986113</v>
+      </c>
+      <c r="B164">
+        <v>0.9</v>
+      </c>
+      <c r="C164">
+        <v>10350550.3452453</v>
+      </c>
+    </row>
+    <row r="165" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A165" s="3">
+        <v>43734.255516666664</v>
+      </c>
+      <c r="B165">
+        <v>0.9</v>
+      </c>
+      <c r="C165">
+        <v>11530034.324007999</v>
+      </c>
+    </row>
+    <row r="166" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A166" s="3">
+        <v>43734.274753206017</v>
+      </c>
+      <c r="B166">
+        <v>0.9</v>
+      </c>
+      <c r="C166">
+        <v>10039595.308894601</v>
+      </c>
+    </row>
+    <row r="167" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A167" s="3">
+        <v>43734.294012349535</v>
+      </c>
+      <c r="B167">
+        <v>0.9</v>
+      </c>
+      <c r="C167">
+        <v>10531543.3634145</v>
+      </c>
+    </row>
+    <row r="168" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A168" s="3">
+        <v>43734.313276006942</v>
+      </c>
+      <c r="B168">
+        <v>0.9</v>
+      </c>
+      <c r="C168">
+        <v>11322046.236679001</v>
+      </c>
+    </row>
+    <row r="169" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A169" s="3">
+        <v>43734.332780902776</v>
+      </c>
+      <c r="B169">
+        <v>0.9</v>
+      </c>
+      <c r="C169">
+        <v>13919552.267551599</v>
+      </c>
+    </row>
+    <row r="170" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A170" s="3">
+        <v>43734.35224375</v>
+      </c>
+      <c r="B170">
+        <v>0.9</v>
+      </c>
+      <c r="C170">
+        <v>12693246.7447527</v>
+      </c>
+    </row>
+    <row r="171" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A171" s="3">
+        <v>43734.371597106481</v>
+      </c>
+      <c r="B171">
+        <v>0.9</v>
+      </c>
+      <c r="C171">
+        <v>14816961.1335028</v>
+      </c>
+    </row>
+    <row r="172" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A172" s="3">
+        <v>43734.390951076392</v>
+      </c>
+      <c r="B172">
+        <v>0.9</v>
+      </c>
+      <c r="C172">
+        <v>11447928.8874959</v>
+      </c>
+    </row>
+    <row r="173" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A173" s="3">
+        <v>43734.410385844909</v>
+      </c>
+      <c r="B173">
+        <v>0.9</v>
+      </c>
+      <c r="C173">
+        <v>11783283.699706901</v>
+      </c>
+    </row>
+    <row r="174" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A174" s="3">
+        <v>43734.429855358794</v>
+      </c>
+      <c r="B174">
+        <v>0.9</v>
+      </c>
+      <c r="C174">
+        <v>13854411.550277401</v>
+      </c>
+    </row>
+    <row r="175" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A175" s="3">
+        <v>43734.449173032408</v>
+      </c>
+      <c r="B175">
+        <v>0.9</v>
+      </c>
+      <c r="C175">
+        <v>10337823.9272717</v>
+      </c>
+    </row>
+    <row r="176" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A176" s="3">
+        <v>43734.468393287039</v>
+      </c>
+      <c r="B176">
+        <v>0.9</v>
+      </c>
+      <c r="C176">
+        <v>10005847.592892099</v>
+      </c>
+    </row>
+    <row r="177" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A177" s="3">
+        <v>43734.487661458334</v>
+      </c>
+      <c r="B177">
+        <v>0.9</v>
+      </c>
+      <c r="C177">
+        <v>8981746.7223352008</v>
+      </c>
+    </row>
+    <row r="178" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A178" s="3">
+        <v>43734.507771412034</v>
+      </c>
+      <c r="B178">
+        <v>0.9</v>
+      </c>
+      <c r="C178">
+        <v>7440911.6710755304</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Test: Feed Through. Example Input: One Integer Expected Output: One Integer equle to input Results: Found solution with initial generation Population size: 50,000 Observations: Started to converge on a solution early on in the run (at about generation 5). Then, it quickly lost momentum.
</commit_message>
<xml_diff>
--- a/Progress.xlsx
+++ b/Progress.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/c51537410c5afe56/Projects/Source/Repos/EdGarrity/SOS/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1" documentId="114_{5A039FB9-666C-4FDC-9FC6-FAFC9BEA3DF7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{57D00C6E-3558-4E3D-B9F8-F7262F485D2C}"/>
+  <xr:revisionPtr revIDLastSave="7" documentId="114_{5A039FB9-666C-4FDC-9FC6-FAFC9BEA3DF7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{756919E3-2431-4072-A686-9C96D6390330}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="16896" activeTab="5" xr2:uid="{D7613C25-2959-4D88-A8C3-21B00E74DE47}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="16896" activeTab="6" xr2:uid="{D7613C25-2959-4D88-A8C3-21B00E74DE47}"/>
   </bookViews>
   <sheets>
     <sheet name="Run 1" sheetId="1" r:id="rId1"/>
@@ -19,6 +19,7 @@
     <sheet name="Run 4" sheetId="4" r:id="rId4"/>
     <sheet name="Run 5" sheetId="5" r:id="rId5"/>
     <sheet name="Run 6" sheetId="6" r:id="rId6"/>
+    <sheet name="Run 7" sheetId="7" r:id="rId7"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -38,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="9">
   <si>
     <t>BestIndividual_Training_Error</t>
   </si>
@@ -72,7 +73,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="165" formatCode="[$-409]m/d/yy\ h:mm\ AM/PM;@"/>
+    <numFmt numFmtId="164" formatCode="[$-409]m/d/yy\ h:mm\ AM/PM;@"/>
   </numFmts>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
@@ -107,7 +108,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="4" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -6318,6 +6319,520 @@
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000001-E105-455E-8DB8-9A6E08FF6146}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:marker val="1"/>
+        <c:smooth val="0"/>
+        <c:axId val="840836808"/>
+        <c:axId val="840833856"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="715829080"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" cap="none" spc="0" normalizeH="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="715823504"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="715823504"/>
+        <c:scaling>
+          <c:logBase val="10"/>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:minorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="5000"/>
+                  <a:lumOff val="95000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:minorGridlines>
+        <c:numFmt formatCode="#,##0.00" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="715829080"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="840833856"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="r"/>
+        <c:numFmt formatCode="#,##0.00" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="840836808"/>
+        <c:crosses val="max"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:catAx>
+        <c:axId val="840836808"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="1"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="840833856"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="t"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart7.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="2000" b="0" i="0" u="none" strike="noStrike" kern="1200" cap="none" spc="0" normalizeH="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mj-lt"/>
+              <a:ea typeface="+mj-ea"/>
+              <a:cs typeface="+mj-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Run 7'!$C$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>55.51</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="38100" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>'Run 7'!$C$2:$C$137</c:f>
+              <c:numCache>
+                <c:formatCode>#,##0.00</c:formatCode>
+                <c:ptCount val="136"/>
+                <c:pt idx="0">
+                  <c:v>30.584943021058798</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>17.746874526241601</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>10.0181005540574</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>7.2290272178458803</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>6.6771103803667904</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>7.5015055072453602</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>8.38253016746682</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>8.9607441725513404</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>9.6961129784558899</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>9.6409287893557902</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>10.0660067822889</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>10.692740662699</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>10.7597631534928</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>10.642569513773401</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>10.161364431125</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-BBC5-4B07-989B-8D5ABC85EACB}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:marker val="1"/>
+        <c:smooth val="0"/>
+        <c:axId val="715829080"/>
+        <c:axId val="715823504"/>
+      </c:lineChart>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Run 7'!$B$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>BestIndividual_Training_Error</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="38100" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>'Run 7'!$B$2:$B$137</c:f>
+              <c:numCache>
+                <c:formatCode>#,##0.00</c:formatCode>
+                <c:ptCount val="136"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-BBC5-4B07-989B-8D5ABC85EACB}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -6793,6 +7308,46 @@
 </file>
 
 <file path=xl/charts/colors6.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors7.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
   <a:schemeClr val="accent2"/>
@@ -9832,6 +10387,506 @@
 </cs:chartStyle>
 </file>
 
+<file path=xl/charts/style7.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="235">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200" cap="all"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" b="0" kern="1200" cap="none" spc="0" normalizeH="0" baseline="0"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="38100" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="8"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:prstDash val="dash"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:prstDash val="dash"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="major">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="2000" b="0" kern="1200" cap="none" spc="0" normalizeH="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
@@ -10066,6 +11121,49 @@
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
               <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F21C3A37-B741-4E6F-B275-A30D51DA0DD2}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing7.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>561975</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>31</xdr:col>
+      <xdr:colOff>409575</xdr:colOff>
+      <xdr:row>37</xdr:row>
+      <xdr:rowOff>19050</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{595E29DF-3832-45BA-B68A-8E1AFCF37295}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -17516,7 +18614,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E95F638A-2EEB-4C6A-9BCC-C221B0F3EBAC}">
   <dimension ref="A1:E178"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
       <selection sqref="A1:A1048576"/>
     </sheetView>
   </sheetViews>
@@ -17567,7 +18665,7 @@
         <v>530838032.318699</v>
       </c>
       <c r="D3" s="2">
-        <f>(C3-C2)/C2</f>
+        <f t="shared" ref="D3:D31" si="0">(C3-C2)/C2</f>
         <v>0.13711569047295533</v>
       </c>
     </row>
@@ -17582,7 +18680,7 @@
         <v>370939279.01228499</v>
       </c>
       <c r="D4" s="2">
-        <f>(C4-C3)/C3</f>
+        <f t="shared" si="0"/>
         <v>-0.30121947481414757</v>
       </c>
     </row>
@@ -17597,7 +18695,7 @@
         <v>287802144.25176901</v>
       </c>
       <c r="D5" s="2">
-        <f>(C5-C4)/C4</f>
+        <f t="shared" si="0"/>
         <v>-0.22412599437268707</v>
       </c>
     </row>
@@ -17612,7 +18710,7 @@
         <v>248506795.35284099</v>
       </c>
       <c r="D6" s="2">
-        <f>(C6-C5)/C5</f>
+        <f t="shared" si="0"/>
         <v>-0.13653598377832962</v>
       </c>
     </row>
@@ -17627,7 +18725,7 @@
         <v>219063937.33587301</v>
       </c>
       <c r="D7" s="2">
-        <f>(C7-C6)/C6</f>
+        <f t="shared" si="0"/>
         <v>-0.11847908615602927</v>
       </c>
     </row>
@@ -17642,7 +18740,7 @@
         <v>138580850.40472999</v>
       </c>
       <c r="D8" s="2">
-        <f>(C8-C7)/C7</f>
+        <f t="shared" si="0"/>
         <v>-0.36739541847887458</v>
       </c>
     </row>
@@ -17657,7 +18755,7 @@
         <v>143843237.58303201</v>
       </c>
       <c r="D9" s="2">
-        <f>(C9-C8)/C8</f>
+        <f t="shared" si="0"/>
         <v>3.7973408035331307E-2</v>
       </c>
     </row>
@@ -17672,7 +18770,7 @@
         <v>84740447.071308702</v>
       </c>
       <c r="D10" s="2">
-        <f>(C10-C9)/C9</f>
+        <f t="shared" si="0"/>
         <v>-0.41088334429073758</v>
       </c>
     </row>
@@ -17687,7 +18785,7 @@
         <v>50829498.939668</v>
       </c>
       <c r="D11" s="2">
-        <f>(C11-C10)/C10</f>
+        <f t="shared" si="0"/>
         <v>-0.40017428870896554</v>
       </c>
     </row>
@@ -17702,7 +18800,7 @@
         <v>45881076.786539502</v>
       </c>
       <c r="D12" s="2">
-        <f>(C12-C11)/C11</f>
+        <f t="shared" si="0"/>
         <v>-9.7353353000823789E-2</v>
       </c>
     </row>
@@ -17717,7 +18815,7 @@
         <v>36884020.090438202</v>
       </c>
       <c r="D13" s="2">
-        <f>(C13-C12)/C12</f>
+        <f t="shared" si="0"/>
         <v>-0.19609515134005831</v>
       </c>
     </row>
@@ -17732,7 +18830,7 @@
         <v>51961728.485883802</v>
       </c>
       <c r="D14" s="2">
-        <f>(C14-C13)/C13</f>
+        <f t="shared" si="0"/>
         <v>0.40878701287103841</v>
       </c>
     </row>
@@ -17747,7 +18845,7 @@
         <v>23300455.492954198</v>
       </c>
       <c r="D15" s="2">
-        <f>(C15-C14)/C14</f>
+        <f t="shared" si="0"/>
         <v>-0.55158428766887302</v>
       </c>
     </row>
@@ -17762,7 +18860,7 @@
         <v>18673919.715530898</v>
       </c>
       <c r="D16" s="2">
-        <f>(C16-C15)/C15</f>
+        <f t="shared" si="0"/>
         <v>-0.19855988561349427</v>
       </c>
     </row>
@@ -17777,7 +18875,7 @@
         <v>22387443.221550301</v>
       </c>
       <c r="D17" s="2">
-        <f>(C17-C16)/C16</f>
+        <f t="shared" si="0"/>
         <v>0.19886149038816445</v>
       </c>
     </row>
@@ -17792,7 +18890,7 @@
         <v>21727289.674221501</v>
       </c>
       <c r="D18" s="2">
-        <f>(C18-C17)/C17</f>
+        <f t="shared" si="0"/>
         <v>-2.9487670422915099E-2</v>
       </c>
     </row>
@@ -17807,7 +18905,7 @@
         <v>25023973.804324102</v>
       </c>
       <c r="D19" s="2">
-        <f>(C19-C18)/C18</f>
+        <f t="shared" si="0"/>
         <v>0.15173011358218211</v>
       </c>
     </row>
@@ -17822,7 +18920,7 @@
         <v>28457230.8928365</v>
       </c>
       <c r="D20" s="2">
-        <f>(C20-C19)/C19</f>
+        <f t="shared" si="0"/>
         <v>0.13719871653314858</v>
       </c>
     </row>
@@ -17837,7 +18935,7 @@
         <v>20707684.776952799</v>
       </c>
       <c r="D21" s="2">
-        <f>(C21-C20)/C20</f>
+        <f t="shared" si="0"/>
         <v>-0.27232256522311465</v>
       </c>
     </row>
@@ -17852,7 +18950,7 @@
         <v>14613419.506552</v>
       </c>
       <c r="D22" s="2">
-        <f>(C22-C21)/C21</f>
+        <f t="shared" si="0"/>
         <v>-0.29429969289389529</v>
       </c>
     </row>
@@ -17867,7 +18965,7 @@
         <v>14221412.3280422</v>
       </c>
       <c r="D23" s="2">
-        <f>(C23-C22)/C22</f>
+        <f t="shared" si="0"/>
         <v>-2.6825150563428456E-2</v>
       </c>
     </row>
@@ -17882,7 +18980,7 @@
         <v>13799211.4196239</v>
       </c>
       <c r="D24" s="2">
-        <f>(C24-C23)/C23</f>
+        <f t="shared" si="0"/>
         <v>-2.9687691959102504E-2</v>
       </c>
     </row>
@@ -17897,7 +18995,7 @@
         <v>10991181.9397649</v>
       </c>
       <c r="D25" s="2">
-        <f>(C25-C24)/C24</f>
+        <f t="shared" si="0"/>
         <v>-0.20349202533890401</v>
       </c>
     </row>
@@ -17912,7 +19010,7 @@
         <v>7827470.0282455198</v>
       </c>
       <c r="D26" s="2">
-        <f>(C26-C25)/C25</f>
+        <f t="shared" si="0"/>
         <v>-0.28784091909837423</v>
       </c>
     </row>
@@ -17927,7 +19025,7 @@
         <v>11158393.262985799</v>
       </c>
       <c r="D27" s="2">
-        <f>(C27-C26)/C26</f>
+        <f t="shared" si="0"/>
         <v>0.42554276448464229</v>
       </c>
     </row>
@@ -17942,7 +19040,7 @@
         <v>11228451.7032403</v>
       </c>
       <c r="D28" s="2">
-        <f>(C28-C27)/C27</f>
+        <f t="shared" si="0"/>
         <v>6.2785419552199642E-3</v>
       </c>
     </row>
@@ -17957,7 +19055,7 @@
         <v>6580154.4599233698</v>
       </c>
       <c r="D29" s="2">
-        <f>(C29-C28)/C28</f>
+        <f t="shared" si="0"/>
         <v>-0.41397490644017526</v>
       </c>
     </row>
@@ -17972,7 +19070,7 @@
         <v>5694237.1644831495</v>
       </c>
       <c r="D30" s="2">
-        <f>(C30-C29)/C29</f>
+        <f t="shared" si="0"/>
         <v>-0.13463472640892041</v>
       </c>
     </row>
@@ -17987,7 +19085,7 @@
         <v>7602025.9353936203</v>
       </c>
       <c r="D31" s="2">
-        <f>(C31-C30)/C30</f>
+        <f t="shared" si="0"/>
         <v>0.33503851627571529</v>
       </c>
     </row>
@@ -18017,7 +19115,7 @@
         <v>8887725.9137989692</v>
       </c>
       <c r="D33" s="2">
-        <f>(C33-C32)/C32</f>
+        <f t="shared" ref="D33:D64" si="1">(C33-C32)/C32</f>
         <v>0.14320788978014667</v>
       </c>
     </row>
@@ -18032,7 +19130,7 @@
         <v>8256218.8607965596</v>
       </c>
       <c r="D34" s="2">
-        <f>(C34-C33)/C33</f>
+        <f t="shared" si="1"/>
         <v>-7.1053839770411895E-2</v>
       </c>
     </row>
@@ -18047,7 +19145,7 @@
         <v>9346117.9973511808</v>
       </c>
       <c r="D35" s="2">
-        <f>(C35-C34)/C34</f>
+        <f t="shared" si="1"/>
         <v>0.13200947733227456</v>
       </c>
     </row>
@@ -18062,7 +19160,7 @@
         <v>8787415.66559745</v>
       </c>
       <c r="D36" s="2">
-        <f>(C36-C35)/C35</f>
+        <f t="shared" si="1"/>
         <v>-5.9779079604181627E-2</v>
       </c>
     </row>
@@ -18077,7 +19175,7 @@
         <v>6106326.5948853297</v>
       </c>
       <c r="D37" s="2">
-        <f>(C37-C36)/C36</f>
+        <f t="shared" si="1"/>
         <v>-0.30510552507587962</v>
       </c>
     </row>
@@ -18092,7 +19190,7 @@
         <v>10212688.134928999</v>
       </c>
       <c r="D38" s="2">
-        <f>(C38-C37)/C37</f>
+        <f t="shared" si="1"/>
         <v>0.67247656610492557</v>
       </c>
     </row>
@@ -18107,7 +19205,7 @@
         <v>12426570.6614541</v>
       </c>
       <c r="D39" s="2">
-        <f>(C39-C38)/C38</f>
+        <f t="shared" si="1"/>
         <v>0.21677764926094964</v>
       </c>
     </row>
@@ -18122,7 +19220,7 @@
         <v>7555045.1385022402</v>
       </c>
       <c r="D40" s="2">
-        <f>(C40-C39)/C39</f>
+        <f t="shared" si="1"/>
         <v>-0.39202493235425068</v>
       </c>
     </row>
@@ -18137,7 +19235,7 @@
         <v>5974048.4311196003</v>
       </c>
       <c r="D41" s="2">
-        <f>(C41-C40)/C40</f>
+        <f t="shared" si="1"/>
         <v>-0.20926370106321648</v>
       </c>
     </row>
@@ -18152,7 +19250,7 @@
         <v>5586637.8612419497</v>
       </c>
       <c r="D42" s="2">
-        <f>(C42-C41)/C41</f>
+        <f t="shared" si="1"/>
         <v>-6.4848916834952031E-2</v>
       </c>
     </row>
@@ -18167,7 +19265,7 @@
         <v>6283506.2962794499</v>
       </c>
       <c r="D43" s="2">
-        <f>(C43-C42)/C42</f>
+        <f t="shared" si="1"/>
         <v>0.12473842986532536</v>
       </c>
     </row>
@@ -18182,7 +19280,7 @@
         <v>7465580.1919447798</v>
       </c>
       <c r="D44" s="2">
-        <f>(C44-C43)/C43</f>
+        <f t="shared" si="1"/>
         <v>0.18812329294000263</v>
       </c>
     </row>
@@ -18197,7 +19295,7 @@
         <v>6318532.6921694595</v>
       </c>
       <c r="D45" s="2">
-        <f>(C45-C44)/C44</f>
+        <f t="shared" si="1"/>
         <v>-0.15364478986013208</v>
       </c>
     </row>
@@ -18212,7 +19310,7 @@
         <v>7805773.7823088001</v>
       </c>
       <c r="D46" s="2">
-        <f>(C46-C45)/C45</f>
+        <f t="shared" si="1"/>
         <v>0.23537760467433752</v>
       </c>
     </row>
@@ -18227,7 +19325,7 @@
         <v>8864587.4604190998</v>
       </c>
       <c r="D47" s="2">
-        <f>(C47-C46)/C46</f>
+        <f t="shared" si="1"/>
         <v>0.13564493510047926</v>
       </c>
     </row>
@@ -18242,7 +19340,7 @@
         <v>6943692.4762246301</v>
       </c>
       <c r="D48" s="2">
-        <f>(C48-C47)/C47</f>
+        <f t="shared" si="1"/>
         <v>-0.21669310532175104</v>
       </c>
     </row>
@@ -18257,7 +19355,7 @@
         <v>5018393.19882455</v>
       </c>
       <c r="D49" s="2">
-        <f>(C49-C48)/C48</f>
+        <f t="shared" si="1"/>
         <v>-0.27727312002833521</v>
       </c>
     </row>
@@ -18272,7 +19370,7 @@
         <v>5936583.2975150002</v>
       </c>
       <c r="D50" s="2">
-        <f>(C50-C49)/C49</f>
+        <f t="shared" si="1"/>
         <v>0.18296495756958947</v>
       </c>
     </row>
@@ -18287,7 +19385,7 @@
         <v>8225772.5154284202</v>
       </c>
       <c r="D51" s="2">
-        <f>(C51-C50)/C50</f>
+        <f t="shared" si="1"/>
         <v>0.38560719241851688</v>
       </c>
     </row>
@@ -18302,7 +19400,7 @@
         <v>6907093.6067347797</v>
       </c>
       <c r="D52" s="2">
-        <f>(C52-C51)/C51</f>
+        <f t="shared" si="1"/>
         <v>-0.16031064635209646</v>
       </c>
     </row>
@@ -18317,7 +19415,7 @@
         <v>7761654.1245476799</v>
       </c>
       <c r="D53" s="2">
-        <f>(C53-C52)/C52</f>
+        <f t="shared" si="1"/>
         <v>0.12372215673748199</v>
       </c>
     </row>
@@ -18332,7 +19430,7 @@
         <v>8243263.69838861</v>
       </c>
       <c r="D54" s="2">
-        <f>(C54-C53)/C53</f>
+        <f t="shared" si="1"/>
         <v>6.2049862840157996E-2</v>
       </c>
     </row>
@@ -18347,7 +19445,7 @@
         <v>8773894.6373157408</v>
       </c>
       <c r="D55" s="2">
-        <f>(C55-C54)/C54</f>
+        <f t="shared" si="1"/>
         <v>6.4371462365186538E-2</v>
       </c>
     </row>
@@ -18362,7 +19460,7 @@
         <v>8716087.0516568795</v>
       </c>
       <c r="D56" s="2">
-        <f>(C56-C55)/C55</f>
+        <f t="shared" si="1"/>
         <v>-6.5885889959292699E-3</v>
       </c>
     </row>
@@ -18377,7 +19475,7 @@
         <v>9526198.3536674306</v>
       </c>
       <c r="D57" s="2">
-        <f>(C57-C56)/C56</f>
+        <f t="shared" si="1"/>
         <v>9.2944379422708209E-2</v>
       </c>
     </row>
@@ -18392,7 +19490,7 @@
         <v>11499360.383852899</v>
       </c>
       <c r="D58" s="2">
-        <f>(C58-C57)/C57</f>
+        <f t="shared" si="1"/>
         <v>0.20713005933010342</v>
       </c>
     </row>
@@ -18407,7 +19505,7 @@
         <v>11166373.0106229</v>
       </c>
       <c r="D59" s="2">
-        <f>(C59-C58)/C58</f>
+        <f t="shared" si="1"/>
         <v>-2.8957034314497289E-2</v>
       </c>
     </row>
@@ -18422,7 +19520,7 @@
         <v>9769672.7323780097</v>
       </c>
       <c r="D60" s="2">
-        <f>(C60-C59)/C59</f>
+        <f t="shared" si="1"/>
         <v>-0.12508092618043193</v>
       </c>
     </row>
@@ -18437,7 +19535,7 @@
         <v>9113302.0081548896</v>
       </c>
       <c r="D61" s="2">
-        <f>(C61-C60)/C60</f>
+        <f t="shared" si="1"/>
         <v>-6.7184514998933312E-2</v>
       </c>
     </row>
@@ -18452,7 +19550,7 @@
         <v>8908424.5873359703</v>
       </c>
       <c r="D62" s="2">
-        <f>(C62-C61)/C61</f>
+        <f t="shared" si="1"/>
         <v>-2.2481140275565113E-2</v>
       </c>
     </row>
@@ -18467,7 +19565,7 @@
         <v>6980347.5328304498</v>
       </c>
       <c r="D63" s="2">
-        <f>(C63-C62)/C62</f>
+        <f t="shared" si="1"/>
         <v>-0.21643299952793388</v>
       </c>
     </row>
@@ -18482,7 +19580,7 @@
         <v>10547658.4918481</v>
       </c>
       <c r="D64" s="2">
-        <f>(C64-C63)/C63</f>
+        <f t="shared" si="1"/>
         <v>0.51105062351689923</v>
       </c>
     </row>
@@ -18497,7 +19595,7 @@
         <v>7893663.9331381703</v>
       </c>
       <c r="D65" s="2">
-        <f>(C65-C64)/C64</f>
+        <f t="shared" ref="D65:D96" si="2">(C65-C64)/C64</f>
         <v>-0.251619310651848</v>
       </c>
     </row>
@@ -18512,7 +19610,7 @@
         <v>7872032.7382409796</v>
       </c>
       <c r="D66" s="2">
-        <f>(C66-C65)/C65</f>
+        <f t="shared" si="2"/>
         <v>-2.7403237685837312E-3</v>
       </c>
     </row>
@@ -18527,7 +19625,7 @@
         <v>9625715.7394120805</v>
       </c>
       <c r="D67" s="2">
-        <f>(C67-C66)/C66</f>
+        <f t="shared" si="2"/>
         <v>0.2227738450136279</v>
       </c>
     </row>
@@ -18542,7 +19640,7 @@
         <v>9473516.8728934303</v>
       </c>
       <c r="D68" s="2">
-        <f>(C68-C67)/C67</f>
+        <f t="shared" si="2"/>
         <v>-1.5811693451062394E-2</v>
       </c>
     </row>
@@ -18557,7 +19655,7 @@
         <v>6771778.9840001902</v>
       </c>
       <c r="D69" s="2">
-        <f>(C69-C68)/C68</f>
+        <f t="shared" si="2"/>
         <v>-0.28518848123063162</v>
       </c>
     </row>
@@ -18572,7 +19670,7 @@
         <v>9345339.9283929896</v>
       </c>
       <c r="D70" s="2">
-        <f>(C70-C69)/C69</f>
+        <f t="shared" si="2"/>
         <v>0.38004207616246782</v>
       </c>
     </row>
@@ -18587,7 +19685,7 @@
         <v>8749845.9247072209</v>
       </c>
       <c r="D71" s="2">
-        <f>(C71-C70)/C70</f>
+        <f t="shared" si="2"/>
         <v>-6.3720956995533165E-2</v>
       </c>
     </row>
@@ -18602,7 +19700,7 @@
         <v>9261091.2615985703</v>
       </c>
       <c r="D72" s="2">
-        <f>(C72-C71)/C71</f>
+        <f t="shared" si="2"/>
         <v>5.8429067356229616E-2</v>
       </c>
     </row>
@@ -18617,7 +19715,7 @@
         <v>7223886.9166597603</v>
       </c>
       <c r="D73" s="2">
-        <f>(C73-C72)/C72</f>
+        <f t="shared" si="2"/>
         <v>-0.21997454591405952</v>
       </c>
     </row>
@@ -18632,7 +19730,7 @@
         <v>9094109.5142613109</v>
       </c>
       <c r="D74" s="2">
-        <f>(C74-C73)/C73</f>
+        <f t="shared" si="2"/>
         <v>0.25889422400680651</v>
       </c>
     </row>
@@ -18647,7 +19745,7 @@
         <v>8086894.8526188498</v>
       </c>
       <c r="D75" s="2">
-        <f>(C75-C74)/C74</f>
+        <f t="shared" si="2"/>
         <v>-0.11075462199602445</v>
       </c>
     </row>
@@ -18662,7 +19760,7 @@
         <v>9608504.8194003105</v>
       </c>
       <c r="D76" s="2">
-        <f>(C76-C75)/C75</f>
+        <f t="shared" si="2"/>
         <v>0.18815750600351933</v>
       </c>
     </row>
@@ -18677,7 +19775,7 @@
         <v>8167561.5776757495</v>
       </c>
       <c r="D77" s="2">
-        <f>(C77-C76)/C76</f>
+        <f t="shared" si="2"/>
         <v>-0.14996539719844712</v>
       </c>
     </row>
@@ -18692,7 +19790,7 @@
         <v>9162142.1501978301</v>
       </c>
       <c r="D78" s="2">
-        <f>(C78-C77)/C77</f>
+        <f t="shared" si="2"/>
         <v>0.1217720323334384</v>
       </c>
     </row>
@@ -18707,7 +19805,7 @@
         <v>10179691.575688399</v>
       </c>
       <c r="D79" s="2">
-        <f>(C79-C78)/C78</f>
+        <f t="shared" si="2"/>
         <v>0.11106020937129842</v>
       </c>
     </row>
@@ -18722,7 +19820,7 @@
         <v>10752796.858561199</v>
       </c>
       <c r="D80" s="2">
-        <f>(C80-C79)/C79</f>
+        <f t="shared" si="2"/>
         <v>5.6298884756146812E-2</v>
       </c>
     </row>
@@ -18737,7 +19835,7 @@
         <v>9900381.7571215592</v>
       </c>
       <c r="D81" s="2">
-        <f>(C81-C80)/C80</f>
+        <f t="shared" si="2"/>
         <v>-7.9273803146477292E-2</v>
       </c>
     </row>
@@ -18752,7 +19850,7 @@
         <v>8339031.87166679</v>
       </c>
       <c r="D82" s="2">
-        <f>(C82-C81)/C81</f>
+        <f t="shared" si="2"/>
         <v>-0.15770602828841992</v>
       </c>
     </row>
@@ -18767,7 +19865,7 @@
         <v>7073649.2107376698</v>
       </c>
       <c r="D83" s="2">
-        <f>(C83-C82)/C82</f>
+        <f t="shared" si="2"/>
         <v>-0.15174215429352927</v>
       </c>
     </row>
@@ -18782,7 +19880,7 @@
         <v>7834860.1909906296</v>
       </c>
       <c r="D84" s="2">
-        <f>(C84-C83)/C83</f>
+        <f t="shared" si="2"/>
         <v>0.10761220376852382</v>
       </c>
     </row>
@@ -18797,7 +19895,7 @@
         <v>7875096.2232888797</v>
       </c>
       <c r="D85" s="2">
-        <f>(C85-C84)/C84</f>
+        <f t="shared" si="2"/>
         <v>5.1355137574143148E-3</v>
       </c>
     </row>
@@ -18812,7 +19910,7 @@
         <v>6798184.0071253702</v>
       </c>
       <c r="D86" s="2">
-        <f>(C86-C85)/C85</f>
+        <f t="shared" si="2"/>
         <v>-0.13674908669417607</v>
       </c>
     </row>
@@ -18827,7 +19925,7 @@
         <v>5947294.9817488296</v>
       </c>
       <c r="D87" s="2">
-        <f>(C87-C86)/C86</f>
+        <f t="shared" si="2"/>
         <v>-0.12516416508948561</v>
       </c>
     </row>
@@ -18842,7 +19940,7 @@
         <v>9243918.2330143806</v>
       </c>
       <c r="D88" s="2">
-        <f>(C88-C87)/C87</f>
+        <f t="shared" si="2"/>
         <v>0.55430632941232783</v>
       </c>
     </row>
@@ -18857,7 +19955,7 @@
         <v>10158971.5577267</v>
       </c>
       <c r="D89" s="2">
-        <f>(C89-C88)/C88</f>
+        <f t="shared" si="2"/>
         <v>9.898976836945976E-2</v>
       </c>
     </row>
@@ -18872,7 +19970,7 @@
         <v>9430798.9976223409</v>
       </c>
       <c r="D90" s="2">
-        <f>(C90-C89)/C89</f>
+        <f t="shared" si="2"/>
         <v>-7.1677783126632172E-2</v>
       </c>
     </row>
@@ -18887,7 +19985,7 @@
         <v>7920212.32179425</v>
       </c>
       <c r="D91" s="2">
-        <f>(C91-C90)/C90</f>
+        <f t="shared" si="2"/>
         <v>-0.16017589561700282</v>
       </c>
     </row>
@@ -18902,7 +20000,7 @@
         <v>7781097.7558316998</v>
       </c>
       <c r="D92" s="2">
-        <f>(C92-C91)/C91</f>
+        <f t="shared" si="2"/>
         <v>-1.7564499575313801E-2</v>
       </c>
     </row>
@@ -18917,7 +20015,7 @@
         <v>8909239.7825026009</v>
       </c>
       <c r="D93" s="2">
-        <f>(C93-C92)/C92</f>
+        <f t="shared" si="2"/>
         <v>0.14498494455045144</v>
       </c>
     </row>
@@ -18932,7 +20030,7 @@
         <v>8402575.5211147591</v>
       </c>
       <c r="D94" s="2">
-        <f>(C94-C93)/C93</f>
+        <f t="shared" si="2"/>
         <v>-5.6869528013255476E-2</v>
       </c>
     </row>
@@ -18947,7 +20045,7 @@
         <v>9763055.8355248403</v>
       </c>
       <c r="D95" s="2">
-        <f>(C95-C94)/C94</f>
+        <f t="shared" si="2"/>
         <v>0.16191229831750301</v>
       </c>
     </row>
@@ -18962,7 +20060,7 @@
         <v>8955216.1531386003</v>
       </c>
       <c r="D96" s="2">
-        <f>(C96-C95)/C95</f>
+        <f t="shared" si="2"/>
         <v>-8.2744552115204845E-2</v>
       </c>
     </row>
@@ -18977,7 +20075,7 @@
         <v>9327090.2172295991</v>
       </c>
       <c r="D97" s="2">
-        <f>(C97-C96)/C96</f>
+        <f t="shared" ref="D97:D128" si="3">(C97-C96)/C96</f>
         <v>4.1525972989570489E-2</v>
       </c>
     </row>
@@ -18992,7 +20090,7 @@
         <v>11922100.641083799</v>
       </c>
       <c r="D98" s="2">
-        <f>(C98-C97)/C97</f>
+        <f t="shared" si="3"/>
         <v>0.2782229359227737</v>
       </c>
     </row>
@@ -19007,7 +20105,7 @@
         <v>10177384.092680801</v>
       </c>
       <c r="D99" s="2">
-        <f>(C99-C98)/C98</f>
+        <f t="shared" si="3"/>
         <v>-0.1463430481697722</v>
       </c>
     </row>
@@ -19022,7 +20120,7 @@
         <v>10493422.551833799</v>
       </c>
       <c r="D100" s="2">
-        <f>(C100-C99)/C99</f>
+        <f t="shared" si="3"/>
         <v>3.1053014829250828E-2</v>
       </c>
     </row>
@@ -19037,7 +20135,7 @@
         <v>10571888.3616184</v>
       </c>
       <c r="D101" s="2">
-        <f>(C101-C100)/C100</f>
+        <f t="shared" si="3"/>
         <v>7.4776184221122463E-3</v>
       </c>
     </row>
@@ -19052,7 +20150,7 @@
         <v>11825761.163128899</v>
       </c>
       <c r="D102" s="2">
-        <f>(C102-C101)/C101</f>
+        <f t="shared" si="3"/>
         <v>0.11860443079050358</v>
       </c>
     </row>
@@ -19067,7 +20165,7 @@
         <v>11766830.277974</v>
       </c>
       <c r="D103" s="2">
-        <f>(C103-C102)/C102</f>
+        <f t="shared" si="3"/>
         <v>-4.983263600709071E-3</v>
       </c>
     </row>
@@ -19082,7 +20180,7 @@
         <v>11358980.4696874</v>
       </c>
       <c r="D104" s="2">
-        <f>(C104-C103)/C103</f>
+        <f t="shared" si="3"/>
         <v>-3.4660974846390233E-2</v>
       </c>
     </row>
@@ -19097,7 +20195,7 @@
         <v>10595959.5308841</v>
       </c>
       <c r="D105" s="2">
-        <f>(C105-C104)/C104</f>
+        <f t="shared" si="3"/>
         <v>-6.7173364796206808E-2</v>
       </c>
     </row>
@@ -19112,7 +20210,7 @@
         <v>10612407.833329</v>
       </c>
       <c r="D106" s="2">
-        <f>(C106-C105)/C105</f>
+        <f t="shared" si="3"/>
         <v>1.5523183527605497E-3</v>
       </c>
     </row>
@@ -19127,7 +20225,7 @@
         <v>11111308.095895801</v>
       </c>
       <c r="D107" s="2">
-        <f>(C107-C106)/C106</f>
+        <f t="shared" si="3"/>
         <v>4.7011033726009892E-2</v>
       </c>
     </row>
@@ -19142,7 +20240,7 @@
         <v>11482697.728402199</v>
       </c>
       <c r="D108" s="2">
-        <f>(C108-C107)/C107</f>
+        <f t="shared" si="3"/>
         <v>3.3424474355416282E-2</v>
       </c>
     </row>
@@ -19157,7 +20255,7 @@
         <v>12108463.663791399</v>
       </c>
       <c r="D109" s="2">
-        <f>(C109-C108)/C108</f>
+        <f t="shared" si="3"/>
         <v>5.4496421502186025E-2</v>
       </c>
     </row>
@@ -19172,7 +20270,7 @@
         <v>12703801.894834301</v>
       </c>
       <c r="D110" s="2">
-        <f>(C110-C109)/C109</f>
+        <f t="shared" si="3"/>
         <v>4.9167115463473167E-2</v>
       </c>
     </row>
@@ -19187,7 +20285,7 @@
         <v>13554301.475640699</v>
       </c>
       <c r="D111" s="2">
-        <f>(C111-C110)/C110</f>
+        <f t="shared" si="3"/>
         <v>6.6948429127522385E-2</v>
       </c>
     </row>
@@ -19202,7 +20300,7 @@
         <v>10685609.0402385</v>
       </c>
       <c r="D112" s="2">
-        <f>(C112-C111)/C111</f>
+        <f t="shared" si="3"/>
         <v>-0.21164443188442503</v>
       </c>
     </row>
@@ -19217,7 +20315,7 @@
         <v>10060266.226524999</v>
       </c>
       <c r="D113" s="2">
-        <f>(C113-C112)/C112</f>
+        <f t="shared" si="3"/>
         <v>-5.8521962703170623E-2</v>
       </c>
     </row>
@@ -19232,7 +20330,7 @@
         <v>13613881.8641649</v>
       </c>
       <c r="D114" s="2">
-        <f>(C114-C113)/C113</f>
+        <f t="shared" si="3"/>
         <v>0.35323276319173363</v>
       </c>
     </row>
@@ -19247,7 +20345,7 @@
         <v>9865531.9064659998</v>
       </c>
       <c r="D115" s="2">
-        <f>(C115-C114)/C114</f>
+        <f t="shared" si="3"/>
         <v>-0.27533292819041444</v>
       </c>
     </row>
@@ -19262,7 +20360,7 @@
         <v>10216602.912662201</v>
       </c>
       <c r="D116" s="2">
-        <f>(C116-C115)/C115</f>
+        <f t="shared" si="3"/>
         <v>3.5585613581169837E-2</v>
       </c>
     </row>
@@ -19277,7 +20375,7 @@
         <v>10655126.5385125</v>
       </c>
       <c r="D117" s="2">
-        <f>(C117-C116)/C116</f>
+        <f t="shared" si="3"/>
         <v>4.2922645579853577E-2</v>
       </c>
     </row>
@@ -19292,7 +20390,7 @@
         <v>12130281.546378801</v>
       </c>
       <c r="D118" s="2">
-        <f>(C118-C117)/C117</f>
+        <f t="shared" si="3"/>
         <v>0.13844556444584827</v>
       </c>
     </row>
@@ -19307,7 +20405,7 @@
         <v>13932043.1403326</v>
       </c>
       <c r="D119" s="2">
-        <f>(C119-C118)/C118</f>
+        <f t="shared" si="3"/>
         <v>0.14853419412113081</v>
       </c>
     </row>
@@ -19322,7 +20420,7 @@
         <v>9715604.4035289604</v>
       </c>
       <c r="D120" s="2">
-        <f>(C120-C119)/C119</f>
+        <f t="shared" si="3"/>
         <v>-0.30264324437793699</v>
       </c>
     </row>
@@ -19337,7 +20435,7 @@
         <v>14176028.9669978</v>
       </c>
       <c r="D121" s="2">
-        <f>(C121-C120)/C120</f>
+        <f t="shared" si="3"/>
         <v>0.45909903061189872</v>
       </c>
     </row>
@@ -19352,7 +20450,7 @@
         <v>11671773.8648635</v>
       </c>
       <c r="D122" s="2">
-        <f>(C122-C121)/C121</f>
+        <f t="shared" si="3"/>
         <v>-0.17665420323027539</v>
       </c>
     </row>
@@ -19367,7 +20465,7 @@
         <v>11033182.027128199</v>
       </c>
       <c r="D123" s="2">
-        <f>(C123-C122)/C122</f>
+        <f t="shared" si="3"/>
         <v>-5.471249230228032E-2</v>
       </c>
     </row>
@@ -19382,7 +20480,7 @@
         <v>11529359.8826105</v>
       </c>
       <c r="D124" s="2">
-        <f>(C124-C123)/C123</f>
+        <f t="shared" si="3"/>
         <v>4.4971419329646434E-2</v>
       </c>
     </row>
@@ -19397,7 +20495,7 @@
         <v>13431505.780205701</v>
       </c>
       <c r="D125" s="2">
-        <f>(C125-C124)/C124</f>
+        <f t="shared" si="3"/>
         <v>0.16498278455720417</v>
       </c>
     </row>
@@ -19412,7 +20510,7 @@
         <v>9501113.5666300207</v>
       </c>
       <c r="D126" s="2">
-        <f>(C126-C125)/C125</f>
+        <f t="shared" si="3"/>
         <v>-0.2926248387852376</v>
       </c>
     </row>
@@ -19427,7 +20525,7 @@
         <v>10408189.666232301</v>
       </c>
       <c r="D127" s="2">
-        <f>(C127-C126)/C126</f>
+        <f t="shared" si="3"/>
         <v>9.5470503877369592E-2</v>
       </c>
     </row>
@@ -19442,7 +20540,7 @@
         <v>9508783.8172435593</v>
       </c>
       <c r="D128" s="2">
-        <f>(C128-C127)/C127</f>
+        <f t="shared" si="3"/>
         <v>-8.6413283945691283E-2</v>
       </c>
     </row>
@@ -19457,7 +20555,7 @@
         <v>10907746.960920099</v>
       </c>
       <c r="D129" s="2">
-        <f>(C129-C128)/C128</f>
+        <f t="shared" ref="D129:D160" si="4">(C129-C128)/C128</f>
         <v>0.14712324631248966</v>
       </c>
     </row>
@@ -19472,7 +20570,7 @@
         <v>10917398.9459047</v>
       </c>
       <c r="D130" s="2">
-        <f>(C130-C129)/C129</f>
+        <f t="shared" si="4"/>
         <v>8.8487430256511414E-4</v>
       </c>
     </row>
@@ -19487,7 +20585,7 @@
         <v>14160304.8346682</v>
       </c>
       <c r="D131" s="2">
-        <f>(C131-C130)/C130</f>
+        <f t="shared" si="4"/>
         <v>0.29704015625259977</v>
       </c>
     </row>
@@ -19502,7 +20600,7 @@
         <v>13629440.0271507</v>
       </c>
       <c r="D132" s="2">
-        <f>(C132-C131)/C131</f>
+        <f t="shared" si="4"/>
         <v>-3.7489645436007989E-2</v>
       </c>
     </row>
@@ -19517,7 +20615,7 @@
         <v>11985011.9607371</v>
       </c>
       <c r="D133" s="2">
-        <f>(C133-C132)/C132</f>
+        <f t="shared" si="4"/>
         <v>-0.12065265066927153</v>
       </c>
     </row>
@@ -19532,7 +20630,7 @@
         <v>12182880.250477999</v>
       </c>
       <c r="D134" s="2">
-        <f>(C134-C133)/C133</f>
+        <f t="shared" si="4"/>
         <v>1.6509644745379987E-2</v>
       </c>
     </row>
@@ -19547,7 +20645,7 @@
         <v>14521517.5582019</v>
       </c>
       <c r="D135" s="2">
-        <f>(C135-C134)/C134</f>
+        <f t="shared" si="4"/>
         <v>0.19196095337407121</v>
       </c>
     </row>
@@ -19562,7 +20660,7 @@
         <v>13216335.4916855</v>
       </c>
       <c r="D136" s="2">
-        <f>(C136-C135)/C135</f>
+        <f t="shared" si="4"/>
         <v>-8.9879178349319244E-2</v>
       </c>
     </row>
@@ -19577,7 +20675,7 @@
         <v>11703223.0840302</v>
       </c>
       <c r="D137" s="2">
-        <f>(C137-C136)/C136</f>
+        <f t="shared" si="4"/>
         <v>-0.11448804463288718</v>
       </c>
     </row>
@@ -20030,6 +21128,1240 @@
       </c>
       <c r="C178">
         <v>7440911.6710755304</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F8C63BBB-BF09-40A1-9217-0C56FAFFC066}">
+  <dimension ref="A1:E137"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="C2" sqref="C2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="15.88671875" style="3" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="27.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="22.109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="8.88671875" style="2"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A1" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="1">
+        <v>55.5092148861143</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A2" s="3">
+        <v>43735.968249884259</v>
+      </c>
+      <c r="B2" s="1">
+        <v>0</v>
+      </c>
+      <c r="C2" s="1">
+        <v>30.584943021058798</v>
+      </c>
+      <c r="E2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A3" s="3">
+        <v>43735.998179548609</v>
+      </c>
+      <c r="B3" s="1">
+        <v>0</v>
+      </c>
+      <c r="C3" s="1">
+        <v>17.746874526241601</v>
+      </c>
+      <c r="D3" s="2">
+        <f t="shared" ref="D3:D31" si="0">(C3-C2)/C2</f>
+        <v>-0.41975126407715518</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A4" s="3">
+        <v>43736.031291550928</v>
+      </c>
+      <c r="B4" s="1">
+        <v>0</v>
+      </c>
+      <c r="C4" s="1">
+        <v>10.0181005540574</v>
+      </c>
+      <c r="D4" s="2">
+        <f t="shared" si="0"/>
+        <v>-0.43550057001620029</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A5" s="3">
+        <v>43736.068190081016</v>
+      </c>
+      <c r="B5" s="1">
+        <v>0</v>
+      </c>
+      <c r="C5" s="1">
+        <v>7.2290272178458803</v>
+      </c>
+      <c r="D5" s="2">
+        <f t="shared" si="0"/>
+        <v>-0.27840340802747537</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A6" s="3">
+        <v>43736.105619675924</v>
+      </c>
+      <c r="B6" s="1">
+        <v>0</v>
+      </c>
+      <c r="C6" s="1">
+        <v>6.6771103803667904</v>
+      </c>
+      <c r="D6" s="2">
+        <f t="shared" si="0"/>
+        <v>-7.6347317674583498E-2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A7" s="3">
+        <v>43736.144425196762</v>
+      </c>
+      <c r="B7" s="1">
+        <v>0</v>
+      </c>
+      <c r="C7" s="1">
+        <v>7.5015055072453602</v>
+      </c>
+      <c r="D7" s="2">
+        <f t="shared" si="0"/>
+        <v>0.12346585272913876</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A8" s="3">
+        <v>43736.183644791665</v>
+      </c>
+      <c r="B8" s="1">
+        <v>0</v>
+      </c>
+      <c r="C8" s="1">
+        <v>8.38253016746682</v>
+      </c>
+      <c r="D8" s="2">
+        <f t="shared" si="0"/>
+        <v>0.11744637917955515</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A9" s="3">
+        <v>43736.223712233797</v>
+      </c>
+      <c r="B9" s="1">
+        <v>0</v>
+      </c>
+      <c r="C9" s="1">
+        <v>8.9607441725513404</v>
+      </c>
+      <c r="D9" s="2">
+        <f t="shared" si="0"/>
+        <v>6.8978457999305381E-2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A10" s="3">
+        <v>43736.26462253472</v>
+      </c>
+      <c r="B10" s="1">
+        <v>0</v>
+      </c>
+      <c r="C10" s="1">
+        <v>9.6961129784558899</v>
+      </c>
+      <c r="D10" s="2">
+        <f t="shared" si="0"/>
+        <v>8.2065595417525714E-2</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A11" s="3">
+        <v>43736.305625081019</v>
+      </c>
+      <c r="B11" s="1">
+        <v>0</v>
+      </c>
+      <c r="C11" s="1">
+        <v>9.6409287893557902</v>
+      </c>
+      <c r="D11" s="2">
+        <f t="shared" si="0"/>
+        <v>-5.6913723285521994E-3</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A12" s="3">
+        <v>43736.346949305553</v>
+      </c>
+      <c r="B12" s="1">
+        <v>0</v>
+      </c>
+      <c r="C12" s="1">
+        <v>10.0660067822889</v>
+      </c>
+      <c r="D12" s="2">
+        <f t="shared" si="0"/>
+        <v>4.4090979429536242E-2</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A13" s="3">
+        <v>43736.388075000003</v>
+      </c>
+      <c r="B13" s="1">
+        <v>0</v>
+      </c>
+      <c r="C13" s="1">
+        <v>10.692740662699</v>
+      </c>
+      <c r="D13" s="2">
+        <f t="shared" si="0"/>
+        <v>6.2262413881226067E-2</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A14" s="3">
+        <v>43736.429416354164</v>
+      </c>
+      <c r="B14" s="1">
+        <v>0</v>
+      </c>
+      <c r="C14" s="1">
+        <v>10.7597631534928</v>
+      </c>
+      <c r="D14" s="2">
+        <f t="shared" si="0"/>
+        <v>6.268036690313083E-3</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A15" s="3">
+        <v>43736.471038425923</v>
+      </c>
+      <c r="B15" s="1">
+        <v>0</v>
+      </c>
+      <c r="C15" s="1">
+        <v>10.642569513773401</v>
+      </c>
+      <c r="D15" s="2">
+        <f t="shared" si="0"/>
+        <v>-1.0891841952985417E-2</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A16" s="3">
+        <v>43736.512736770834</v>
+      </c>
+      <c r="B16" s="1">
+        <v>0</v>
+      </c>
+      <c r="C16" s="1">
+        <v>10.161364431125</v>
+      </c>
+      <c r="D16" s="2">
+        <f t="shared" si="0"/>
+        <v>-4.5215122346688466E-2</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A17" s="3">
+        <v>43736.55419545139</v>
+      </c>
+      <c r="B17" s="1">
+        <v>0</v>
+      </c>
+      <c r="C17" s="1"/>
+      <c r="D17" s="2">
+        <f t="shared" si="0"/>
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B18" s="1"/>
+      <c r="C18" s="1"/>
+      <c r="D18" s="2" t="e">
+        <f t="shared" si="0"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B19" s="1"/>
+      <c r="C19" s="1"/>
+      <c r="D19" s="2" t="e">
+        <f t="shared" si="0"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B20" s="1"/>
+      <c r="C20" s="1"/>
+      <c r="D20" s="2" t="e">
+        <f t="shared" si="0"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B21" s="1"/>
+      <c r="C21" s="1"/>
+      <c r="D21" s="2" t="e">
+        <f t="shared" si="0"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B22" s="1"/>
+      <c r="C22" s="1"/>
+      <c r="D22" s="2" t="e">
+        <f t="shared" si="0"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B23" s="1"/>
+      <c r="C23" s="1"/>
+      <c r="D23" s="2" t="e">
+        <f t="shared" si="0"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B24" s="1"/>
+      <c r="C24" s="1"/>
+      <c r="D24" s="2" t="e">
+        <f t="shared" si="0"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B25" s="1"/>
+      <c r="C25" s="1"/>
+      <c r="D25" s="2" t="e">
+        <f t="shared" si="0"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B26" s="1"/>
+      <c r="C26" s="1"/>
+      <c r="D26" s="2" t="e">
+        <f t="shared" si="0"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B27" s="1"/>
+      <c r="C27" s="1"/>
+      <c r="D27" s="2" t="e">
+        <f t="shared" si="0"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B28" s="1"/>
+      <c r="C28" s="1"/>
+      <c r="D28" s="2" t="e">
+        <f t="shared" si="0"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B29" s="1"/>
+      <c r="C29" s="1"/>
+      <c r="D29" s="2" t="e">
+        <f t="shared" si="0"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B30" s="1"/>
+      <c r="C30" s="1"/>
+      <c r="D30" s="2" t="e">
+        <f t="shared" si="0"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B31" s="1"/>
+      <c r="C31" s="1"/>
+      <c r="D31" s="2" t="e">
+        <f t="shared" si="0"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B32" s="1"/>
+      <c r="C32" s="1"/>
+      <c r="D32" s="2" t="e">
+        <f>(C32-C30)/C30</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="33" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B33" s="1"/>
+      <c r="C33" s="1"/>
+      <c r="D33" s="2" t="e">
+        <f t="shared" ref="D33:D96" si="1">(C33-C32)/C32</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="34" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B34" s="1"/>
+      <c r="C34" s="1"/>
+      <c r="D34" s="2" t="e">
+        <f t="shared" si="1"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="35" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B35" s="1"/>
+      <c r="C35" s="1"/>
+      <c r="D35" s="2" t="e">
+        <f t="shared" si="1"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="36" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B36" s="1"/>
+      <c r="C36" s="1"/>
+      <c r="D36" s="2" t="e">
+        <f t="shared" si="1"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="37" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B37" s="1"/>
+      <c r="C37" s="1"/>
+      <c r="D37" s="2" t="e">
+        <f t="shared" si="1"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="38" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B38" s="1"/>
+      <c r="C38" s="1"/>
+      <c r="D38" s="2" t="e">
+        <f t="shared" si="1"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="39" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B39" s="1"/>
+      <c r="C39" s="1"/>
+      <c r="D39" s="2" t="e">
+        <f t="shared" si="1"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="40" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B40" s="1"/>
+      <c r="C40" s="1"/>
+      <c r="D40" s="2" t="e">
+        <f t="shared" si="1"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="41" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B41" s="1"/>
+      <c r="C41" s="1"/>
+      <c r="D41" s="2" t="e">
+        <f t="shared" si="1"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="42" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B42" s="1"/>
+      <c r="C42" s="1"/>
+      <c r="D42" s="2" t="e">
+        <f t="shared" si="1"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="43" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B43" s="1"/>
+      <c r="C43" s="1"/>
+      <c r="D43" s="2" t="e">
+        <f t="shared" si="1"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="44" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B44" s="1"/>
+      <c r="C44" s="1"/>
+      <c r="D44" s="2" t="e">
+        <f t="shared" si="1"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="45" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B45" s="1"/>
+      <c r="C45" s="1"/>
+      <c r="D45" s="2" t="e">
+        <f t="shared" si="1"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="46" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B46" s="1"/>
+      <c r="C46" s="1"/>
+      <c r="D46" s="2" t="e">
+        <f t="shared" si="1"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="47" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B47" s="1"/>
+      <c r="C47" s="1"/>
+      <c r="D47" s="2" t="e">
+        <f t="shared" si="1"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="48" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B48" s="1"/>
+      <c r="C48" s="1"/>
+      <c r="D48" s="2" t="e">
+        <f t="shared" si="1"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="49" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B49" s="1"/>
+      <c r="C49" s="1"/>
+      <c r="D49" s="2" t="e">
+        <f t="shared" si="1"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="50" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B50" s="1"/>
+      <c r="C50" s="1"/>
+      <c r="D50" s="2" t="e">
+        <f t="shared" si="1"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="51" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B51" s="1"/>
+      <c r="C51" s="1"/>
+      <c r="D51" s="2" t="e">
+        <f t="shared" si="1"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="52" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B52" s="1"/>
+      <c r="C52" s="1"/>
+      <c r="D52" s="2" t="e">
+        <f t="shared" si="1"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="53" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B53" s="1"/>
+      <c r="C53" s="1"/>
+      <c r="D53" s="2" t="e">
+        <f t="shared" si="1"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="54" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B54" s="1"/>
+      <c r="C54" s="1"/>
+      <c r="D54" s="2" t="e">
+        <f t="shared" si="1"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="55" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B55" s="1"/>
+      <c r="C55" s="1"/>
+      <c r="D55" s="2" t="e">
+        <f t="shared" si="1"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="56" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B56" s="1"/>
+      <c r="C56" s="1"/>
+      <c r="D56" s="2" t="e">
+        <f t="shared" si="1"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="57" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B57" s="1"/>
+      <c r="C57" s="1"/>
+      <c r="D57" s="2" t="e">
+        <f t="shared" si="1"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="58" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B58" s="1"/>
+      <c r="C58" s="1"/>
+      <c r="D58" s="2" t="e">
+        <f t="shared" si="1"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="59" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B59" s="1"/>
+      <c r="C59" s="1"/>
+      <c r="D59" s="2" t="e">
+        <f t="shared" si="1"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="60" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B60" s="1"/>
+      <c r="C60" s="1"/>
+      <c r="D60" s="2" t="e">
+        <f t="shared" si="1"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="61" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B61" s="1"/>
+      <c r="C61" s="1"/>
+      <c r="D61" s="2" t="e">
+        <f t="shared" si="1"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="62" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B62" s="1"/>
+      <c r="C62" s="1"/>
+      <c r="D62" s="2" t="e">
+        <f t="shared" si="1"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="63" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B63" s="1"/>
+      <c r="C63" s="1"/>
+      <c r="D63" s="2" t="e">
+        <f t="shared" si="1"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="64" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B64" s="1"/>
+      <c r="C64" s="1"/>
+      <c r="D64" s="2" t="e">
+        <f t="shared" si="1"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="65" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B65" s="1"/>
+      <c r="C65" s="1"/>
+      <c r="D65" s="2" t="e">
+        <f t="shared" si="1"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="66" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B66" s="1"/>
+      <c r="C66" s="1"/>
+      <c r="D66" s="2" t="e">
+        <f t="shared" si="1"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="67" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B67" s="1"/>
+      <c r="C67" s="1"/>
+      <c r="D67" s="2" t="e">
+        <f t="shared" si="1"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="68" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B68" s="1"/>
+      <c r="C68" s="1"/>
+      <c r="D68" s="2" t="e">
+        <f t="shared" si="1"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="69" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B69" s="1"/>
+      <c r="C69" s="1"/>
+      <c r="D69" s="2" t="e">
+        <f t="shared" si="1"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="70" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B70" s="1"/>
+      <c r="C70" s="1"/>
+      <c r="D70" s="2" t="e">
+        <f t="shared" si="1"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="71" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B71" s="1"/>
+      <c r="C71" s="1"/>
+      <c r="D71" s="2" t="e">
+        <f t="shared" si="1"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="72" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B72" s="1"/>
+      <c r="C72" s="1"/>
+      <c r="D72" s="2" t="e">
+        <f t="shared" si="1"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="73" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B73" s="1"/>
+      <c r="C73" s="1"/>
+      <c r="D73" s="2" t="e">
+        <f t="shared" si="1"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="74" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B74" s="1"/>
+      <c r="C74" s="1"/>
+      <c r="D74" s="2" t="e">
+        <f t="shared" si="1"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="75" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B75" s="1"/>
+      <c r="C75" s="1"/>
+      <c r="D75" s="2" t="e">
+        <f t="shared" si="1"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="76" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B76" s="1"/>
+      <c r="C76" s="1"/>
+      <c r="D76" s="2" t="e">
+        <f t="shared" si="1"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="77" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B77" s="1"/>
+      <c r="C77" s="1"/>
+      <c r="D77" s="2" t="e">
+        <f t="shared" si="1"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="78" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B78" s="1"/>
+      <c r="C78" s="1"/>
+      <c r="D78" s="2" t="e">
+        <f t="shared" si="1"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="79" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B79" s="1"/>
+      <c r="C79" s="1"/>
+      <c r="D79" s="2" t="e">
+        <f t="shared" si="1"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="80" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B80" s="1"/>
+      <c r="C80" s="1"/>
+      <c r="D80" s="2" t="e">
+        <f t="shared" si="1"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="81" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B81" s="1"/>
+      <c r="C81" s="1"/>
+      <c r="D81" s="2" t="e">
+        <f t="shared" si="1"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="82" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B82" s="1"/>
+      <c r="C82" s="1"/>
+      <c r="D82" s="2" t="e">
+        <f t="shared" si="1"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="83" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B83" s="1"/>
+      <c r="C83" s="1"/>
+      <c r="D83" s="2" t="e">
+        <f t="shared" si="1"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="84" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B84" s="1"/>
+      <c r="C84" s="1"/>
+      <c r="D84" s="2" t="e">
+        <f t="shared" si="1"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="85" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B85" s="1"/>
+      <c r="C85" s="1"/>
+      <c r="D85" s="2" t="e">
+        <f t="shared" si="1"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="86" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B86" s="1"/>
+      <c r="C86" s="1"/>
+      <c r="D86" s="2" t="e">
+        <f t="shared" si="1"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="87" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B87" s="1"/>
+      <c r="C87" s="1"/>
+      <c r="D87" s="2" t="e">
+        <f t="shared" si="1"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="88" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B88" s="1"/>
+      <c r="C88" s="1"/>
+      <c r="D88" s="2" t="e">
+        <f t="shared" si="1"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="89" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B89" s="1"/>
+      <c r="C89" s="1"/>
+      <c r="D89" s="2" t="e">
+        <f t="shared" si="1"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="90" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B90" s="1"/>
+      <c r="C90" s="1"/>
+      <c r="D90" s="2" t="e">
+        <f t="shared" si="1"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="91" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B91" s="1"/>
+      <c r="C91" s="1"/>
+      <c r="D91" s="2" t="e">
+        <f t="shared" si="1"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="92" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B92" s="1"/>
+      <c r="C92" s="1"/>
+      <c r="D92" s="2" t="e">
+        <f t="shared" si="1"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="93" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B93" s="1"/>
+      <c r="C93" s="1"/>
+      <c r="D93" s="2" t="e">
+        <f t="shared" si="1"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="94" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B94" s="1"/>
+      <c r="C94" s="1"/>
+      <c r="D94" s="2" t="e">
+        <f t="shared" si="1"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="95" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B95" s="1"/>
+      <c r="C95" s="1"/>
+      <c r="D95" s="2" t="e">
+        <f t="shared" si="1"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="96" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B96" s="1"/>
+      <c r="C96" s="1"/>
+      <c r="D96" s="2" t="e">
+        <f t="shared" si="1"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="97" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B97" s="1"/>
+      <c r="C97" s="1"/>
+      <c r="D97" s="2" t="e">
+        <f t="shared" ref="D97:D137" si="2">(C97-C96)/C96</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="98" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B98" s="1"/>
+      <c r="C98" s="1"/>
+      <c r="D98" s="2" t="e">
+        <f t="shared" si="2"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="99" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B99" s="1"/>
+      <c r="C99" s="1"/>
+      <c r="D99" s="2" t="e">
+        <f t="shared" si="2"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="100" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B100" s="1"/>
+      <c r="C100" s="1"/>
+      <c r="D100" s="2" t="e">
+        <f t="shared" si="2"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="101" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B101" s="1"/>
+      <c r="C101" s="1"/>
+      <c r="D101" s="2" t="e">
+        <f t="shared" si="2"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="102" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B102" s="1"/>
+      <c r="C102" s="1"/>
+      <c r="D102" s="2" t="e">
+        <f t="shared" si="2"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="103" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B103" s="1"/>
+      <c r="C103" s="1"/>
+      <c r="D103" s="2" t="e">
+        <f t="shared" si="2"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="104" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B104" s="1"/>
+      <c r="C104" s="1"/>
+      <c r="D104" s="2" t="e">
+        <f t="shared" si="2"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="105" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B105" s="1"/>
+      <c r="C105" s="1"/>
+      <c r="D105" s="2" t="e">
+        <f t="shared" si="2"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="106" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B106" s="1"/>
+      <c r="C106" s="1"/>
+      <c r="D106" s="2" t="e">
+        <f t="shared" si="2"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="107" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B107" s="1"/>
+      <c r="C107" s="1"/>
+      <c r="D107" s="2" t="e">
+        <f t="shared" si="2"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="108" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B108" s="1"/>
+      <c r="C108" s="1"/>
+      <c r="D108" s="2" t="e">
+        <f t="shared" si="2"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="109" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B109" s="1"/>
+      <c r="C109" s="1"/>
+      <c r="D109" s="2" t="e">
+        <f t="shared" si="2"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="110" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B110" s="1"/>
+      <c r="C110" s="1"/>
+      <c r="D110" s="2" t="e">
+        <f t="shared" si="2"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="111" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B111" s="1"/>
+      <c r="C111" s="1"/>
+      <c r="D111" s="2" t="e">
+        <f t="shared" si="2"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="112" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B112" s="1"/>
+      <c r="C112" s="1"/>
+      <c r="D112" s="2" t="e">
+        <f t="shared" si="2"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="113" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B113" s="1"/>
+      <c r="C113" s="1"/>
+      <c r="D113" s="2" t="e">
+        <f t="shared" si="2"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="114" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B114" s="1"/>
+      <c r="C114" s="1"/>
+      <c r="D114" s="2" t="e">
+        <f t="shared" si="2"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="115" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B115" s="1"/>
+      <c r="C115" s="1"/>
+      <c r="D115" s="2" t="e">
+        <f t="shared" si="2"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="116" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B116" s="1"/>
+      <c r="C116" s="1"/>
+      <c r="D116" s="2" t="e">
+        <f t="shared" si="2"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="117" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B117" s="1"/>
+      <c r="C117" s="1"/>
+      <c r="D117" s="2" t="e">
+        <f t="shared" si="2"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="118" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B118" s="1"/>
+      <c r="C118" s="1"/>
+      <c r="D118" s="2" t="e">
+        <f t="shared" si="2"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="119" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B119" s="1"/>
+      <c r="C119" s="1"/>
+      <c r="D119" s="2" t="e">
+        <f t="shared" si="2"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="120" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B120" s="1"/>
+      <c r="C120" s="1"/>
+      <c r="D120" s="2" t="e">
+        <f t="shared" si="2"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="121" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B121" s="1"/>
+      <c r="C121" s="1"/>
+      <c r="D121" s="2" t="e">
+        <f t="shared" si="2"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="122" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B122" s="1"/>
+      <c r="C122" s="1"/>
+      <c r="D122" s="2" t="e">
+        <f t="shared" si="2"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="123" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B123" s="1"/>
+      <c r="C123" s="1"/>
+      <c r="D123" s="2" t="e">
+        <f t="shared" si="2"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="124" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B124" s="1"/>
+      <c r="C124" s="1"/>
+      <c r="D124" s="2" t="e">
+        <f t="shared" si="2"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="125" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B125" s="1"/>
+      <c r="C125" s="1"/>
+      <c r="D125" s="2" t="e">
+        <f t="shared" si="2"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="126" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B126" s="1"/>
+      <c r="C126" s="1"/>
+      <c r="D126" s="2" t="e">
+        <f t="shared" si="2"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="127" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B127" s="1"/>
+      <c r="C127" s="1"/>
+      <c r="D127" s="2" t="e">
+        <f t="shared" si="2"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="128" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B128" s="1"/>
+      <c r="C128" s="1"/>
+      <c r="D128" s="2" t="e">
+        <f t="shared" si="2"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="129" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B129" s="1"/>
+      <c r="C129" s="1"/>
+      <c r="D129" s="2" t="e">
+        <f t="shared" si="2"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="130" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B130" s="1"/>
+      <c r="C130" s="1"/>
+      <c r="D130" s="2" t="e">
+        <f t="shared" si="2"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="131" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B131" s="1"/>
+      <c r="C131" s="1"/>
+      <c r="D131" s="2" t="e">
+        <f t="shared" si="2"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="132" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B132" s="1"/>
+      <c r="C132" s="1"/>
+      <c r="D132" s="2" t="e">
+        <f t="shared" si="2"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="133" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B133" s="1"/>
+      <c r="C133" s="1"/>
+      <c r="D133" s="2" t="e">
+        <f t="shared" si="2"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="134" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B134" s="1"/>
+      <c r="C134" s="1"/>
+      <c r="D134" s="2" t="e">
+        <f t="shared" si="2"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="135" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B135" s="1"/>
+      <c r="C135" s="1"/>
+      <c r="D135" s="2" t="e">
+        <f t="shared" si="2"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="136" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B136" s="1"/>
+      <c r="C136" s="1"/>
+      <c r="D136" s="2" t="e">
+        <f t="shared" si="2"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="137" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B137" s="1"/>
+      <c r="C137" s="1"/>
+      <c r="D137" s="2" t="e">
+        <f t="shared" si="2"/>
+        <v>#DIV/0!</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Test: Feed Through Example Input: Two Integers Expected Output: Two Integers equal to input Results: Found solution within 120 generations Population size: 500 Example Cases: 10 Training, 10 Test Observations: Error stayed constant from generation 11 to generation 120 where it dropped to zero.  Error may not be a good measurement of velocity to convergence.  Standard Deviation of population error may be a better metric.
</commit_message>
<xml_diff>
--- a/Progress.xlsx
+++ b/Progress.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/c51537410c5afe56/Projects/Source/Repos/EdGarrity/SOS/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="14" documentId="114_{5A039FB9-666C-4FDC-9FC6-FAFC9BEA3DF7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{27C81BE5-1061-451C-8480-FBBDE2194214}"/>
+  <xr:revisionPtr revIDLastSave="20" documentId="114_{5A039FB9-666C-4FDC-9FC6-FAFC9BEA3DF7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{F1FE90D5-B715-4962-8188-AC3836FC4A45}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="16896" activeTab="7" xr2:uid="{D7613C25-2959-4D88-A8C3-21B00E74DE47}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="8" xr2:uid="{D7613C25-2959-4D88-A8C3-21B00E74DE47}"/>
   </bookViews>
   <sheets>
     <sheet name="Run 1" sheetId="1" r:id="rId1"/>
@@ -21,6 +21,7 @@
     <sheet name="Run 6" sheetId="6" r:id="rId6"/>
     <sheet name="Run 7" sheetId="7" r:id="rId7"/>
     <sheet name="Run 8" sheetId="8" r:id="rId8"/>
+    <sheet name="Run 9" sheetId="9" r:id="rId9"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -40,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="9">
   <si>
     <t>BestIndividual_Training_Error</t>
   </si>
@@ -8071,6 +8072,1177 @@
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000001-0EA6-4623-BD95-7C62E426508A}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:marker val="1"/>
+        <c:smooth val="0"/>
+        <c:axId val="840836808"/>
+        <c:axId val="840833856"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="715829080"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" cap="none" spc="0" normalizeH="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="715823504"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="715823504"/>
+        <c:scaling>
+          <c:logBase val="10"/>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:minorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="5000"/>
+                  <a:lumOff val="95000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:minorGridlines>
+        <c:numFmt formatCode="#,##0.00" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="715829080"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="840833856"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="r"/>
+        <c:numFmt formatCode="#,##0.00" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="840836808"/>
+        <c:crosses val="max"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:catAx>
+        <c:axId val="840836808"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="1"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="840833856"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="t"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart9.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="2000" b="0" i="0" u="none" strike="noStrike" kern="1200" cap="none" spc="0" normalizeH="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mj-lt"/>
+              <a:ea typeface="+mj-ea"/>
+              <a:cs typeface="+mj-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Run 9'!$C$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Average_Training_Error</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="38100" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>'Run 9'!$C$2:$C$137</c:f>
+              <c:numCache>
+                <c:formatCode>#,##0.00</c:formatCode>
+                <c:ptCount val="136"/>
+                <c:pt idx="0">
+                  <c:v>13.0499078979577</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>14.464019060265199</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>14.532736067509299</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>15.535724420429</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>12.640800395544099</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>16.2265803014248</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>13.003967127045099</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>20.0617768318156</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>13.302949538077799</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>14.3226043066167</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>22.6820680946728</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>18.273667707861001</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>35.446128012302999</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>13.969985612233801</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>13.042461821872299</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>26.901175347880098</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>27.172790939276201</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>15.380265699865101</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>19.685752659757199</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>16.037818693792001</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>7.8527135253693299</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>13.5377143010395</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>5.7204083906842103</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>13.829005008951899</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>18.657386454085</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>10.580133530833701</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>5.8767219752196498</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>5.8767219752196498</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>11.9798459765098</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>4.2414932095446796</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>14.647511806765699</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>9.0868230803968597</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>8.1307110920489301</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>5.7149269953681801</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>7.0103874399711099</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>5.9764477475904698</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>4.8234195015361196</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>3.70828725255069</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>14.861556435048501</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>5.46884557026533</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>8.9450580285821992</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>20.778980594238998</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>9.8334403231426606</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>2.0502093590878299</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>6.79748149949463</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>10.3323090896818</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>2.93630386468574</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>4.7891940598410603</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>8.1652471987670996</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>8.7557100940955408</c:v>
+                </c:pt>
+                <c:pt idx="50">
+                  <c:v>7.7658970518980297</c:v>
+                </c:pt>
+                <c:pt idx="51">
+                  <c:v>3.2589824211929899</c:v>
+                </c:pt>
+                <c:pt idx="52">
+                  <c:v>6.3207939401770803</c:v>
+                </c:pt>
+                <c:pt idx="53">
+                  <c:v>5.7895195067772098</c:v>
+                </c:pt>
+                <c:pt idx="54">
+                  <c:v>10.6388842852389</c:v>
+                </c:pt>
+                <c:pt idx="55">
+                  <c:v>6.1795799716499999</c:v>
+                </c:pt>
+                <c:pt idx="56">
+                  <c:v>3.0112406984858402</c:v>
+                </c:pt>
+                <c:pt idx="57">
+                  <c:v>5.1871294098564702</c:v>
+                </c:pt>
+                <c:pt idx="58">
+                  <c:v>6.1505851217096401</c:v>
+                </c:pt>
+                <c:pt idx="59">
+                  <c:v>3.7343628498103798</c:v>
+                </c:pt>
+                <c:pt idx="60">
+                  <c:v>5.8252693243340001</c:v>
+                </c:pt>
+                <c:pt idx="61">
+                  <c:v>5.23096655072003</c:v>
+                </c:pt>
+                <c:pt idx="62">
+                  <c:v>8.2483258880272405</c:v>
+                </c:pt>
+                <c:pt idx="63">
+                  <c:v>8.2004391966152603</c:v>
+                </c:pt>
+                <c:pt idx="64">
+                  <c:v>5.9544052790168296</c:v>
+                </c:pt>
+                <c:pt idx="65">
+                  <c:v>4.56506804735917</c:v>
+                </c:pt>
+                <c:pt idx="66">
+                  <c:v>8.9145437654091904</c:v>
+                </c:pt>
+                <c:pt idx="67">
+                  <c:v>12.5490244679438</c:v>
+                </c:pt>
+                <c:pt idx="68">
+                  <c:v>10.2846375412668</c:v>
+                </c:pt>
+                <c:pt idx="69">
+                  <c:v>2.7602194110505498</c:v>
+                </c:pt>
+                <c:pt idx="70">
+                  <c:v>12.6515683545335</c:v>
+                </c:pt>
+                <c:pt idx="71">
+                  <c:v>6.9335909111350604</c:v>
+                </c:pt>
+                <c:pt idx="72">
+                  <c:v>5.2499778135006103</c:v>
+                </c:pt>
+                <c:pt idx="73">
+                  <c:v>6.6309613105116698</c:v>
+                </c:pt>
+                <c:pt idx="74">
+                  <c:v>11.5594535511351</c:v>
+                </c:pt>
+                <c:pt idx="75">
+                  <c:v>11.960306334626701</c:v>
+                </c:pt>
+                <c:pt idx="76">
+                  <c:v>5.3638978139560001</c:v>
+                </c:pt>
+                <c:pt idx="77">
+                  <c:v>7.6216335923932501</c:v>
+                </c:pt>
+                <c:pt idx="78">
+                  <c:v>6.8516991415573099</c:v>
+                </c:pt>
+                <c:pt idx="79">
+                  <c:v>8.0231200566894696</c:v>
+                </c:pt>
+                <c:pt idx="80">
+                  <c:v>8.7053989311749103</c:v>
+                </c:pt>
+                <c:pt idx="81">
+                  <c:v>6.8530055325879804</c:v>
+                </c:pt>
+                <c:pt idx="82">
+                  <c:v>7.4742017652380204</c:v>
+                </c:pt>
+                <c:pt idx="83">
+                  <c:v>6.1049410540921203</c:v>
+                </c:pt>
+                <c:pt idx="84">
+                  <c:v>5.6634270850888901</c:v>
+                </c:pt>
+                <c:pt idx="85">
+                  <c:v>8.8415351222308605</c:v>
+                </c:pt>
+                <c:pt idx="86">
+                  <c:v>6.6417824018626304</c:v>
+                </c:pt>
+                <c:pt idx="87">
+                  <c:v>9.2305143458888494</c:v>
+                </c:pt>
+                <c:pt idx="88">
+                  <c:v>5.7787042184060899</c:v>
+                </c:pt>
+                <c:pt idx="89">
+                  <c:v>3.7266015614128598</c:v>
+                </c:pt>
+                <c:pt idx="90">
+                  <c:v>6.8275727590079898</c:v>
+                </c:pt>
+                <c:pt idx="91">
+                  <c:v>3.84302600118657</c:v>
+                </c:pt>
+                <c:pt idx="92">
+                  <c:v>5.2522813292056796</c:v>
+                </c:pt>
+                <c:pt idx="93">
+                  <c:v>5.5985585661172896</c:v>
+                </c:pt>
+                <c:pt idx="94">
+                  <c:v>4.1937641931389802</c:v>
+                </c:pt>
+                <c:pt idx="95">
+                  <c:v>7.5729032797595197</c:v>
+                </c:pt>
+                <c:pt idx="96">
+                  <c:v>13.166490998260899</c:v>
+                </c:pt>
+                <c:pt idx="97">
+                  <c:v>9.9209748360553007</c:v>
+                </c:pt>
+                <c:pt idx="98">
+                  <c:v>10.075451036583599</c:v>
+                </c:pt>
+                <c:pt idx="99">
+                  <c:v>6.1252177353729103</c:v>
+                </c:pt>
+                <c:pt idx="100">
+                  <c:v>14.990699514277701</c:v>
+                </c:pt>
+                <c:pt idx="101">
+                  <c:v>6.3439485060649696</c:v>
+                </c:pt>
+                <c:pt idx="102">
+                  <c:v>8.7959508614286701</c:v>
+                </c:pt>
+                <c:pt idx="103">
+                  <c:v>6.2362819709260604</c:v>
+                </c:pt>
+                <c:pt idx="104">
+                  <c:v>5.28673054076177</c:v>
+                </c:pt>
+                <c:pt idx="105">
+                  <c:v>4.6162763397507902</c:v>
+                </c:pt>
+                <c:pt idx="106">
+                  <c:v>3.3347612414102299</c:v>
+                </c:pt>
+                <c:pt idx="107">
+                  <c:v>7.4416327177573498</c:v>
+                </c:pt>
+                <c:pt idx="108">
+                  <c:v>4.5889122917307601</c:v>
+                </c:pt>
+                <c:pt idx="109">
+                  <c:v>6.3552143572670499</c:v>
+                </c:pt>
+                <c:pt idx="110">
+                  <c:v>6.4044349134591601</c:v>
+                </c:pt>
+                <c:pt idx="111">
+                  <c:v>3.8620445837867301</c:v>
+                </c:pt>
+                <c:pt idx="112">
+                  <c:v>8.1793302310839593</c:v>
+                </c:pt>
+                <c:pt idx="113">
+                  <c:v>13.723497759026399</c:v>
+                </c:pt>
+                <c:pt idx="114">
+                  <c:v>2.6227058014242099</c:v>
+                </c:pt>
+                <c:pt idx="115">
+                  <c:v>4.0964623634805397</c:v>
+                </c:pt>
+                <c:pt idx="116">
+                  <c:v>3.7738483007313399</c:v>
+                </c:pt>
+                <c:pt idx="117">
+                  <c:v>4.7637230874232701</c:v>
+                </c:pt>
+                <c:pt idx="118">
+                  <c:v>3.6882892580561699</c:v>
+                </c:pt>
+                <c:pt idx="119">
+                  <c:v>3.8830020078476899</c:v>
+                </c:pt>
+                <c:pt idx="120">
+                  <c:v>11.5972761144219</c:v>
+                </c:pt>
+                <c:pt idx="121">
+                  <c:v>21.455149123122101</c:v>
+                </c:pt>
+                <c:pt idx="122">
+                  <c:v>21.835631909000099</c:v>
+                </c:pt>
+                <c:pt idx="123">
+                  <c:v>24.590362788530602</c:v>
+                </c:pt>
+                <c:pt idx="124">
+                  <c:v>29.974044881506</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-432D-48D6-B4AD-7B5C9F5DA845}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:marker val="1"/>
+        <c:smooth val="0"/>
+        <c:axId val="715829080"/>
+        <c:axId val="715823504"/>
+      </c:lineChart>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Run 9'!$B$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>BestIndividual_Training_Error</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="38100" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>'Run 9'!$B$2:$B$137</c:f>
+              <c:numCache>
+                <c:formatCode>#,##0.00</c:formatCode>
+                <c:ptCount val="136"/>
+                <c:pt idx="0">
+                  <c:v>0.182012749487487</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.182012749487487</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.182012749487487</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.182012749487487</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.182012749487487</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.182012749487487</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.182012749487487</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.182012749487487</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.182012749487487</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.182012749487487</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0.16628741099722999</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0.16628741099722999</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>0.16628741099722999</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>0.16628741099722999</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>0.16628741099722999</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>0.16628741099722999</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>0.16628741099722999</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>0.16628741099722999</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>0.16628741099722999</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>0.16628741099722999</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>0.16628741099722999</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>0.16628741099722999</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>0.16628741099722999</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>0.16628741099722999</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>0.16628741099722999</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>0.16628741099722999</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>0.16628741099722999</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>0.16628741099722999</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>0.16628741099722999</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>0.16628741099722999</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>0.16628741099722999</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>0.16628741099722999</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>0.16628741099722999</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>0.16628741099722999</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>0.16628741099722999</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>0.16628741099722999</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>0.16628741099722999</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>0.16628741099722999</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>0.16628741099722999</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>0.16628741099722999</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>0.16628741099722999</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>0.16628741099722999</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>0.16628741099722999</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>0.16628741099722999</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>0.16628741099722999</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>0.16628741099722999</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>0.16628741099722999</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>0.16628741099722999</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>0.16628741099722999</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>0.16628741099722999</c:v>
+                </c:pt>
+                <c:pt idx="50">
+                  <c:v>0.16628741099722999</c:v>
+                </c:pt>
+                <c:pt idx="51">
+                  <c:v>0.16628741099722999</c:v>
+                </c:pt>
+                <c:pt idx="52">
+                  <c:v>0.16628741099722999</c:v>
+                </c:pt>
+                <c:pt idx="53">
+                  <c:v>0.16628741099722999</c:v>
+                </c:pt>
+                <c:pt idx="54">
+                  <c:v>0.16628741099722999</c:v>
+                </c:pt>
+                <c:pt idx="55">
+                  <c:v>0.16628741099722999</c:v>
+                </c:pt>
+                <c:pt idx="56">
+                  <c:v>0.16628741099722999</c:v>
+                </c:pt>
+                <c:pt idx="57">
+                  <c:v>0.16628741099722999</c:v>
+                </c:pt>
+                <c:pt idx="58">
+                  <c:v>0.16628741099722999</c:v>
+                </c:pt>
+                <c:pt idx="59">
+                  <c:v>0.16628741099722999</c:v>
+                </c:pt>
+                <c:pt idx="60">
+                  <c:v>0.16628741099722999</c:v>
+                </c:pt>
+                <c:pt idx="61">
+                  <c:v>0.16628741099722999</c:v>
+                </c:pt>
+                <c:pt idx="62">
+                  <c:v>0.16628741099722999</c:v>
+                </c:pt>
+                <c:pt idx="63">
+                  <c:v>0.16628741099722999</c:v>
+                </c:pt>
+                <c:pt idx="64">
+                  <c:v>0.16628741099722999</c:v>
+                </c:pt>
+                <c:pt idx="65">
+                  <c:v>0.16628741099722999</c:v>
+                </c:pt>
+                <c:pt idx="66">
+                  <c:v>0.16628741099722999</c:v>
+                </c:pt>
+                <c:pt idx="67">
+                  <c:v>0.16628741099722999</c:v>
+                </c:pt>
+                <c:pt idx="68">
+                  <c:v>0.16628741099722999</c:v>
+                </c:pt>
+                <c:pt idx="69">
+                  <c:v>0.16628741099722999</c:v>
+                </c:pt>
+                <c:pt idx="70">
+                  <c:v>0.16628741099722999</c:v>
+                </c:pt>
+                <c:pt idx="71">
+                  <c:v>0.16628741099722999</c:v>
+                </c:pt>
+                <c:pt idx="72">
+                  <c:v>0.16628741099722999</c:v>
+                </c:pt>
+                <c:pt idx="73">
+                  <c:v>0.16628741099722999</c:v>
+                </c:pt>
+                <c:pt idx="74">
+                  <c:v>0.16628741099722999</c:v>
+                </c:pt>
+                <c:pt idx="75">
+                  <c:v>0.16628741099722999</c:v>
+                </c:pt>
+                <c:pt idx="76">
+                  <c:v>0.16628741099722999</c:v>
+                </c:pt>
+                <c:pt idx="77">
+                  <c:v>0.16628741099722999</c:v>
+                </c:pt>
+                <c:pt idx="78">
+                  <c:v>0.16628741099722999</c:v>
+                </c:pt>
+                <c:pt idx="79">
+                  <c:v>0.16628741099722999</c:v>
+                </c:pt>
+                <c:pt idx="80">
+                  <c:v>0.16628741099722999</c:v>
+                </c:pt>
+                <c:pt idx="81">
+                  <c:v>0.16628741099722999</c:v>
+                </c:pt>
+                <c:pt idx="82">
+                  <c:v>0.16628741099722999</c:v>
+                </c:pt>
+                <c:pt idx="83">
+                  <c:v>0.16628741099722999</c:v>
+                </c:pt>
+                <c:pt idx="84">
+                  <c:v>0.16628741099722999</c:v>
+                </c:pt>
+                <c:pt idx="85">
+                  <c:v>0.16628741099722999</c:v>
+                </c:pt>
+                <c:pt idx="86">
+                  <c:v>0.16628741099722999</c:v>
+                </c:pt>
+                <c:pt idx="87">
+                  <c:v>0.16628741099722999</c:v>
+                </c:pt>
+                <c:pt idx="88">
+                  <c:v>0.16628741099722999</c:v>
+                </c:pt>
+                <c:pt idx="89">
+                  <c:v>0.16628741099722999</c:v>
+                </c:pt>
+                <c:pt idx="90">
+                  <c:v>0.16628741099722999</c:v>
+                </c:pt>
+                <c:pt idx="91">
+                  <c:v>0.16628741099722999</c:v>
+                </c:pt>
+                <c:pt idx="92">
+                  <c:v>0.16628741099722999</c:v>
+                </c:pt>
+                <c:pt idx="93">
+                  <c:v>0.16628741099722999</c:v>
+                </c:pt>
+                <c:pt idx="94">
+                  <c:v>0.16628741099722999</c:v>
+                </c:pt>
+                <c:pt idx="95">
+                  <c:v>0.16628741099722999</c:v>
+                </c:pt>
+                <c:pt idx="96">
+                  <c:v>0.16628741099722999</c:v>
+                </c:pt>
+                <c:pt idx="97">
+                  <c:v>0.16628741099722999</c:v>
+                </c:pt>
+                <c:pt idx="98">
+                  <c:v>0.16628741099722999</c:v>
+                </c:pt>
+                <c:pt idx="99">
+                  <c:v>0.16628741099722999</c:v>
+                </c:pt>
+                <c:pt idx="100">
+                  <c:v>0.16628741099722999</c:v>
+                </c:pt>
+                <c:pt idx="101">
+                  <c:v>0.16628741099722999</c:v>
+                </c:pt>
+                <c:pt idx="102">
+                  <c:v>0.16628741099722999</c:v>
+                </c:pt>
+                <c:pt idx="103">
+                  <c:v>0.16628741099722999</c:v>
+                </c:pt>
+                <c:pt idx="104">
+                  <c:v>0.16628741099722999</c:v>
+                </c:pt>
+                <c:pt idx="105">
+                  <c:v>0.16628741099722999</c:v>
+                </c:pt>
+                <c:pt idx="106">
+                  <c:v>0.16628741099722999</c:v>
+                </c:pt>
+                <c:pt idx="107">
+                  <c:v>0.16628741099722999</c:v>
+                </c:pt>
+                <c:pt idx="108">
+                  <c:v>0.16628741099722999</c:v>
+                </c:pt>
+                <c:pt idx="109">
+                  <c:v>0.16628741099722999</c:v>
+                </c:pt>
+                <c:pt idx="110">
+                  <c:v>0.16628741099722999</c:v>
+                </c:pt>
+                <c:pt idx="111">
+                  <c:v>0.16628741099722999</c:v>
+                </c:pt>
+                <c:pt idx="112">
+                  <c:v>0.16628741099722999</c:v>
+                </c:pt>
+                <c:pt idx="113">
+                  <c:v>0.16628741099722999</c:v>
+                </c:pt>
+                <c:pt idx="114">
+                  <c:v>0.16628741099722999</c:v>
+                </c:pt>
+                <c:pt idx="115">
+                  <c:v>0.16628741099722999</c:v>
+                </c:pt>
+                <c:pt idx="116">
+                  <c:v>0.16628741099722999</c:v>
+                </c:pt>
+                <c:pt idx="117">
+                  <c:v>0.16628741099722999</c:v>
+                </c:pt>
+                <c:pt idx="118">
+                  <c:v>0.16628741099722999</c:v>
+                </c:pt>
+                <c:pt idx="119">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="120">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="121">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="122">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="123">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="124">
+                  <c:v>0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-432D-48D6-B4AD-7B5C9F5DA845}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -8626,6 +9798,46 @@
 </file>
 
 <file path=xl/charts/colors8.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors9.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
   <a:schemeClr val="accent2"/>
@@ -12665,6 +13877,506 @@
 </cs:chartStyle>
 </file>
 
+<file path=xl/charts/style9.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="235">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200" cap="all"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" b="0" kern="1200" cap="none" spc="0" normalizeH="0" baseline="0"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="38100" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="8"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:prstDash val="dash"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:prstDash val="dash"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="major">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="2000" b="0" kern="1200" cap="none" spc="0" normalizeH="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
@@ -13007,6 +14719,49 @@
 </xdr:wsDr>
 </file>
 
+<file path=xl/drawings/drawing9.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>561975</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>31</xdr:col>
+      <xdr:colOff>409575</xdr:colOff>
+      <xdr:row>37</xdr:row>
+      <xdr:rowOff>19050</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{575D20B7-02E4-452B-B18E-B75766D6AD7F}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
@@ -24196,7 +25951,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{67DC838C-5D4A-4A72-B767-13EF7D35EBCD}">
   <dimension ref="A1:E171"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
       <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
@@ -26640,4 +28395,2003 @@
   <pageSetup orientation="portrait" r:id="rId1"/>
   <drawing r:id="rId2"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EA93F0B8-4E7F-4AC8-819E-3E2AF7FA35C1}">
+  <dimension ref="A1:E137"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="E1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="C2" sqref="C2:C126"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="15.88671875" style="3" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="27.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="22.109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="8.88671875" style="2"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A1" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A2" s="3">
+        <v>43737.614945914349</v>
+      </c>
+      <c r="B2" s="1">
+        <v>0.182012749487487</v>
+      </c>
+      <c r="C2" s="1">
+        <v>13.0499078979577</v>
+      </c>
+      <c r="E2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A3" s="3">
+        <v>43737.614991354167</v>
+      </c>
+      <c r="B3" s="1">
+        <v>0.182012749487487</v>
+      </c>
+      <c r="C3" s="1">
+        <v>14.464019060265199</v>
+      </c>
+      <c r="D3" s="2">
+        <f t="shared" ref="D3:D31" si="0">(C3-C2)/C2</f>
+        <v>0.10836177338299885</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A4" s="3">
+        <v>43737.615045520834</v>
+      </c>
+      <c r="B4" s="1">
+        <v>0.182012749487487</v>
+      </c>
+      <c r="C4" s="1">
+        <v>14.532736067509299</v>
+      </c>
+      <c r="D4" s="2">
+        <f t="shared" si="0"/>
+        <v>4.7508930234249824E-3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A5" s="3">
+        <v>43737.61508880787</v>
+      </c>
+      <c r="B5" s="1">
+        <v>0.182012749487487</v>
+      </c>
+      <c r="C5" s="1">
+        <v>15.535724420429</v>
+      </c>
+      <c r="D5" s="2">
+        <f t="shared" si="0"/>
+        <v>6.9015796355241896E-2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A6" s="3">
+        <v>43737.615114930559</v>
+      </c>
+      <c r="B6" s="1">
+        <v>0.182012749487487</v>
+      </c>
+      <c r="C6" s="1">
+        <v>12.640800395544099</v>
+      </c>
+      <c r="D6" s="2">
+        <f t="shared" si="0"/>
+        <v>-0.18633981567529381</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A7" s="3">
+        <v>43737.615152696759</v>
+      </c>
+      <c r="B7" s="1">
+        <v>0.182012749487487</v>
+      </c>
+      <c r="C7" s="1">
+        <v>16.2265803014248</v>
+      </c>
+      <c r="D7" s="2">
+        <f t="shared" si="0"/>
+        <v>0.28366715664181308</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A8" s="3">
+        <v>43737.615181909721</v>
+      </c>
+      <c r="B8" s="1">
+        <v>0.182012749487487</v>
+      </c>
+      <c r="C8" s="1">
+        <v>13.003967127045099</v>
+      </c>
+      <c r="D8" s="2">
+        <f t="shared" si="0"/>
+        <v>-0.19860088290425151</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A9" s="3">
+        <v>43737.615225347225</v>
+      </c>
+      <c r="B9" s="1">
+        <v>0.182012749487487</v>
+      </c>
+      <c r="C9" s="1">
+        <v>20.0617768318156</v>
+      </c>
+      <c r="D9" s="2">
+        <f t="shared" si="0"/>
+        <v>0.54274281346743547</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A10" s="3">
+        <v>43737.615257025464</v>
+      </c>
+      <c r="B10" s="1">
+        <v>0.182012749487487</v>
+      </c>
+      <c r="C10" s="1">
+        <v>13.302949538077799</v>
+      </c>
+      <c r="D10" s="2">
+        <f t="shared" si="0"/>
+        <v>-0.33690073169486673</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A11" s="3">
+        <v>43737.615287233799</v>
+      </c>
+      <c r="B11" s="1">
+        <v>0.182012749487487</v>
+      </c>
+      <c r="C11" s="1">
+        <v>14.3226043066167</v>
+      </c>
+      <c r="D11" s="2">
+        <f t="shared" si="0"/>
+        <v>7.6648773688893918E-2</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A12" s="3">
+        <v>43737.615333761576</v>
+      </c>
+      <c r="B12" s="1">
+        <v>0.16628741099722999</v>
+      </c>
+      <c r="C12" s="1">
+        <v>22.6820680946728</v>
+      </c>
+      <c r="D12" s="2">
+        <f t="shared" si="0"/>
+        <v>0.5836552912513423</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A13" s="3">
+        <v>43737.61537832176</v>
+      </c>
+      <c r="B13" s="1">
+        <v>0.16628741099722999</v>
+      </c>
+      <c r="C13" s="1">
+        <v>18.273667707861001</v>
+      </c>
+      <c r="D13" s="2">
+        <f t="shared" si="0"/>
+        <v>-0.19435619223130599</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A14" s="3">
+        <v>43737.615426655095</v>
+      </c>
+      <c r="B14" s="1">
+        <v>0.16628741099722999</v>
+      </c>
+      <c r="C14" s="1">
+        <v>35.446128012302999</v>
+      </c>
+      <c r="D14" s="2">
+        <f t="shared" si="0"/>
+        <v>0.93973801970004722</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A15" s="3">
+        <v>43737.615474189814</v>
+      </c>
+      <c r="B15" s="1">
+        <v>0.16628741099722999</v>
+      </c>
+      <c r="C15" s="1">
+        <v>13.969985612233801</v>
+      </c>
+      <c r="D15" s="2">
+        <f t="shared" si="0"/>
+        <v>-0.60588119505225069</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A16" s="3">
+        <v>43737.61551103009</v>
+      </c>
+      <c r="B16" s="1">
+        <v>0.16628741099722999</v>
+      </c>
+      <c r="C16" s="1">
+        <v>13.042461821872299</v>
+      </c>
+      <c r="D16" s="2">
+        <f t="shared" si="0"/>
+        <v>-6.6394040488434725E-2</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A17" s="3">
+        <v>43737.615561261577</v>
+      </c>
+      <c r="B17" s="1">
+        <v>0.16628741099722999</v>
+      </c>
+      <c r="C17" s="1">
+        <v>26.901175347880098</v>
+      </c>
+      <c r="D17" s="2">
+        <f t="shared" si="0"/>
+        <v>1.0625841743133677</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A18" s="3">
+        <v>43737.615608912034</v>
+      </c>
+      <c r="B18" s="1">
+        <v>0.16628741099722999</v>
+      </c>
+      <c r="C18" s="1">
+        <v>27.172790939276201</v>
+      </c>
+      <c r="D18" s="2">
+        <f t="shared" si="0"/>
+        <v>1.0096792719412042E-2</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A19" s="3">
+        <v>43737.615645486112</v>
+      </c>
+      <c r="B19" s="1">
+        <v>0.16628741099722999</v>
+      </c>
+      <c r="C19" s="1">
+        <v>15.380265699865101</v>
+      </c>
+      <c r="D19" s="2">
+        <f t="shared" si="0"/>
+        <v>-0.43398284945275545</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A20" s="3">
+        <v>43737.615673807872</v>
+      </c>
+      <c r="B20" s="1">
+        <v>0.16628741099722999</v>
+      </c>
+      <c r="C20" s="1">
+        <v>19.685752659757199</v>
+      </c>
+      <c r="D20" s="2">
+        <f t="shared" si="0"/>
+        <v>0.27993579850378408</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A21" s="3">
+        <v>43737.615698298614</v>
+      </c>
+      <c r="B21" s="1">
+        <v>0.16628741099722999</v>
+      </c>
+      <c r="C21" s="1">
+        <v>16.037818693792001</v>
+      </c>
+      <c r="D21" s="2">
+        <f t="shared" si="0"/>
+        <v>-0.18530833080223161</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A22" s="3">
+        <v>43737.615728703706</v>
+      </c>
+      <c r="B22" s="1">
+        <v>0.16628741099722999</v>
+      </c>
+      <c r="C22" s="1">
+        <v>7.8527135253693299</v>
+      </c>
+      <c r="D22" s="2">
+        <f t="shared" si="0"/>
+        <v>-0.51036274475349963</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A23" s="3">
+        <v>43737.615756562504</v>
+      </c>
+      <c r="B23" s="1">
+        <v>0.16628741099722999</v>
+      </c>
+      <c r="C23" s="1">
+        <v>13.5377143010395</v>
+      </c>
+      <c r="D23" s="2">
+        <f t="shared" si="0"/>
+        <v>0.72395366993892629</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A24" s="3">
+        <v>43737.615787465278</v>
+      </c>
+      <c r="B24" s="1">
+        <v>0.16628741099722999</v>
+      </c>
+      <c r="C24" s="1">
+        <v>5.7204083906842103</v>
+      </c>
+      <c r="D24" s="2">
+        <f t="shared" si="0"/>
+        <v>-0.57744651249990064</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A25" s="3">
+        <v>43737.615811226853</v>
+      </c>
+      <c r="B25" s="1">
+        <v>0.16628741099722999</v>
+      </c>
+      <c r="C25" s="1">
+        <v>13.829005008951899</v>
+      </c>
+      <c r="D25" s="2">
+        <f t="shared" si="0"/>
+        <v>1.417485617193466</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A26" s="3">
+        <v>43737.61584082176</v>
+      </c>
+      <c r="B26" s="1">
+        <v>0.16628741099722999</v>
+      </c>
+      <c r="C26" s="1">
+        <v>18.657386454085</v>
+      </c>
+      <c r="D26" s="2">
+        <f t="shared" si="0"/>
+        <v>0.34914886804998296</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A27" s="3">
+        <v>43737.615859756945</v>
+      </c>
+      <c r="B27" s="1">
+        <v>0.16628741099722999</v>
+      </c>
+      <c r="C27" s="1">
+        <v>10.580133530833701</v>
+      </c>
+      <c r="D27" s="2">
+        <f t="shared" si="0"/>
+        <v>-0.43292520863675416</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A28" s="3">
+        <v>43737.615877893521</v>
+      </c>
+      <c r="B28" s="1">
+        <v>0.16628741099722999</v>
+      </c>
+      <c r="C28" s="1">
+        <v>5.8767219752196498</v>
+      </c>
+      <c r="D28" s="2">
+        <f t="shared" si="0"/>
+        <v>-0.44455124709975452</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A29" s="3">
+        <v>43737.631487465274</v>
+      </c>
+      <c r="B29" s="1">
+        <v>0.16628741099722999</v>
+      </c>
+      <c r="C29" s="1">
+        <v>5.8767219752196498</v>
+      </c>
+      <c r="D29" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A30" s="3">
+        <v>43737.631504050929</v>
+      </c>
+      <c r="B30" s="1">
+        <v>0.16628741099722999</v>
+      </c>
+      <c r="C30" s="1">
+        <v>11.9798459765098</v>
+      </c>
+      <c r="D30" s="2">
+        <f t="shared" si="0"/>
+        <v>1.0385252232494866</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A31" s="3">
+        <v>43737.631530636572</v>
+      </c>
+      <c r="B31" s="1">
+        <v>0.16628741099722999</v>
+      </c>
+      <c r="C31" s="1">
+        <v>4.2414932095446796</v>
+      </c>
+      <c r="D31" s="2">
+        <f t="shared" si="0"/>
+        <v>-0.64594760084049152</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A32" s="3">
+        <v>43737.631550196762</v>
+      </c>
+      <c r="B32" s="1">
+        <v>0.16628741099722999</v>
+      </c>
+      <c r="C32" s="1">
+        <v>14.647511806765699</v>
+      </c>
+      <c r="D32" s="2">
+        <f>(C32-C30)/C30</f>
+        <v>0.22267947647129058</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A33" s="3">
+        <v>43737.631571180558</v>
+      </c>
+      <c r="B33" s="1">
+        <v>0.16628741099722999</v>
+      </c>
+      <c r="C33" s="1">
+        <v>9.0868230803968597</v>
+      </c>
+      <c r="D33" s="2">
+        <f t="shared" ref="D33:D96" si="1">(C33-C32)/C32</f>
+        <v>-0.37963367428728423</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A34" s="3">
+        <v>43737.631591203703</v>
+      </c>
+      <c r="B34" s="1">
+        <v>0.16628741099722999</v>
+      </c>
+      <c r="C34" s="1">
+        <v>8.1307110920489301</v>
+      </c>
+      <c r="D34" s="2">
+        <f t="shared" si="1"/>
+        <v>-0.10521961084623342</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A35" s="3">
+        <v>43737.631605787035</v>
+      </c>
+      <c r="B35" s="1">
+        <v>0.16628741099722999</v>
+      </c>
+      <c r="C35" s="1">
+        <v>5.7149269953681801</v>
+      </c>
+      <c r="D35" s="2">
+        <f t="shared" si="1"/>
+        <v>-0.29711842781416248</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A36" s="3">
+        <v>43737.631622881941</v>
+      </c>
+      <c r="B36" s="1">
+        <v>0.16628741099722999</v>
+      </c>
+      <c r="C36" s="1">
+        <v>7.0103874399711099</v>
+      </c>
+      <c r="D36" s="2">
+        <f t="shared" si="1"/>
+        <v>0.22668013881067448</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A37" s="3">
+        <v>43737.631636770835</v>
+      </c>
+      <c r="B37" s="1">
+        <v>0.16628741099722999</v>
+      </c>
+      <c r="C37" s="1">
+        <v>5.9764477475904698</v>
+      </c>
+      <c r="D37" s="2">
+        <f t="shared" si="1"/>
+        <v>-0.14748681171106587</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A38" s="3">
+        <v>43737.631656481484</v>
+      </c>
+      <c r="B38" s="1">
+        <v>0.16628741099722999</v>
+      </c>
+      <c r="C38" s="1">
+        <v>4.8234195015361196</v>
+      </c>
+      <c r="D38" s="2">
+        <f t="shared" si="1"/>
+        <v>-0.19292869188377287</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A39" s="3">
+        <v>43737.631672025462</v>
+      </c>
+      <c r="B39" s="1">
+        <v>0.16628741099722999</v>
+      </c>
+      <c r="C39" s="1">
+        <v>3.70828725255069</v>
+      </c>
+      <c r="D39" s="2">
+        <f t="shared" si="1"/>
+        <v>-0.23119122204284578</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A40" s="3">
+        <v>43737.631689317132</v>
+      </c>
+      <c r="B40" s="1">
+        <v>0.16628741099722999</v>
+      </c>
+      <c r="C40" s="1">
+        <v>14.861556435048501</v>
+      </c>
+      <c r="D40" s="2">
+        <f t="shared" si="1"/>
+        <v>3.0076605243636938</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A41" s="3">
+        <v>43737.631708912035</v>
+      </c>
+      <c r="B41" s="1">
+        <v>0.16628741099722999</v>
+      </c>
+      <c r="C41" s="1">
+        <v>5.46884557026533</v>
+      </c>
+      <c r="D41" s="2">
+        <f t="shared" si="1"/>
+        <v>-0.63201394186627924</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A42" s="3">
+        <v>43737.63172503472</v>
+      </c>
+      <c r="B42" s="1">
+        <v>0.16628741099722999</v>
+      </c>
+      <c r="C42" s="1">
+        <v>8.9450580285821992</v>
+      </c>
+      <c r="D42" s="2">
+        <f t="shared" si="1"/>
+        <v>0.635639169849189</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A43" s="3">
+        <v>43737.631742245372</v>
+      </c>
+      <c r="B43" s="1">
+        <v>0.16628741099722999</v>
+      </c>
+      <c r="C43" s="1">
+        <v>20.778980594238998</v>
+      </c>
+      <c r="D43" s="2">
+        <f t="shared" si="1"/>
+        <v>1.3229564892529253</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A44" s="3">
+        <v>43737.631762233796</v>
+      </c>
+      <c r="B44" s="1">
+        <v>0.16628741099722999</v>
+      </c>
+      <c r="C44" s="1">
+        <v>9.8334403231426606</v>
+      </c>
+      <c r="D44" s="2">
+        <f t="shared" si="1"/>
+        <v>-0.52676021431633679</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A45" s="3">
+        <v>43737.631776770831</v>
+      </c>
+      <c r="B45" s="1">
+        <v>0.16628741099722999</v>
+      </c>
+      <c r="C45" s="1">
+        <v>2.0502093590878299</v>
+      </c>
+      <c r="D45" s="2">
+        <f t="shared" si="1"/>
+        <v>-0.79150640145110418</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A46" s="3">
+        <v>43737.631793020832</v>
+      </c>
+      <c r="B46" s="1">
+        <v>0.16628741099722999</v>
+      </c>
+      <c r="C46" s="1">
+        <v>6.79748149949463</v>
+      </c>
+      <c r="D46" s="2">
+        <f t="shared" si="1"/>
+        <v>2.3155060332564941</v>
+      </c>
+    </row>
+    <row r="47" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A47" s="3">
+        <v>43737.631814085646</v>
+      </c>
+      <c r="B47" s="1">
+        <v>0.16628741099722999</v>
+      </c>
+      <c r="C47" s="1">
+        <v>10.3323090896818</v>
+      </c>
+      <c r="D47" s="2">
+        <f t="shared" si="1"/>
+        <v>0.5200201854833989</v>
+      </c>
+    </row>
+    <row r="48" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A48" s="3">
+        <v>43737.631826655095</v>
+      </c>
+      <c r="B48" s="1">
+        <v>0.16628741099722999</v>
+      </c>
+      <c r="C48" s="1">
+        <v>2.93630386468574</v>
+      </c>
+      <c r="D48" s="2">
+        <f t="shared" si="1"/>
+        <v>-0.71581339280509571</v>
+      </c>
+    </row>
+    <row r="49" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A49" s="3">
+        <v>43737.631843518517</v>
+      </c>
+      <c r="B49" s="1">
+        <v>0.16628741099722999</v>
+      </c>
+      <c r="C49" s="1">
+        <v>4.7891940598410603</v>
+      </c>
+      <c r="D49" s="2">
+        <f t="shared" si="1"/>
+        <v>0.63102808174576552</v>
+      </c>
+    </row>
+    <row r="50" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A50" s="3">
+        <v>43737.631859606481</v>
+      </c>
+      <c r="B50" s="1">
+        <v>0.16628741099722999</v>
+      </c>
+      <c r="C50" s="1">
+        <v>8.1652471987670996</v>
+      </c>
+      <c r="D50" s="2">
+        <f t="shared" si="1"/>
+        <v>0.70493137190562727</v>
+      </c>
+    </row>
+    <row r="51" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A51" s="3">
+        <v>43737.631876736108</v>
+      </c>
+      <c r="B51" s="1">
+        <v>0.16628741099722999</v>
+      </c>
+      <c r="C51" s="1">
+        <v>8.7557100940955408</v>
+      </c>
+      <c r="D51" s="2">
+        <f t="shared" si="1"/>
+        <v>7.2314148115147983E-2</v>
+      </c>
+    </row>
+    <row r="52" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A52" s="3">
+        <v>43737.631889004631</v>
+      </c>
+      <c r="B52" s="1">
+        <v>0.16628741099722999</v>
+      </c>
+      <c r="C52" s="1">
+        <v>7.7658970518980297</v>
+      </c>
+      <c r="D52" s="2">
+        <f t="shared" si="1"/>
+        <v>-0.11304771761059068</v>
+      </c>
+    </row>
+    <row r="53" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A53" s="3">
+        <v>43737.63190497685</v>
+      </c>
+      <c r="B53" s="1">
+        <v>0.16628741099722999</v>
+      </c>
+      <c r="C53" s="1">
+        <v>3.2589824211929899</v>
+      </c>
+      <c r="D53" s="2">
+        <f t="shared" si="1"/>
+        <v>-0.58034694518690855</v>
+      </c>
+    </row>
+    <row r="54" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A54" s="3">
+        <v>43737.631923032408</v>
+      </c>
+      <c r="B54" s="1">
+        <v>0.16628741099722999</v>
+      </c>
+      <c r="C54" s="1">
+        <v>6.3207939401770803</v>
+      </c>
+      <c r="D54" s="2">
+        <f t="shared" si="1"/>
+        <v>0.93949924340594548</v>
+      </c>
+    </row>
+    <row r="55" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A55" s="3">
+        <v>43737.631941747684</v>
+      </c>
+      <c r="B55" s="1">
+        <v>0.16628741099722999</v>
+      </c>
+      <c r="C55" s="1">
+        <v>5.7895195067772098</v>
+      </c>
+      <c r="D55" s="2">
+        <f t="shared" si="1"/>
+        <v>-8.4051851464878882E-2</v>
+      </c>
+    </row>
+    <row r="56" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A56" s="3">
+        <v>43737.631957754631</v>
+      </c>
+      <c r="B56" s="1">
+        <v>0.16628741099722999</v>
+      </c>
+      <c r="C56" s="1">
+        <v>10.6388842852389</v>
+      </c>
+      <c r="D56" s="2">
+        <f t="shared" si="1"/>
+        <v>0.83761092311460827</v>
+      </c>
+    </row>
+    <row r="57" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A57" s="3">
+        <v>43737.631976701392</v>
+      </c>
+      <c r="B57" s="1">
+        <v>0.16628741099722999</v>
+      </c>
+      <c r="C57" s="1">
+        <v>6.1795799716499999</v>
+      </c>
+      <c r="D57" s="2">
+        <f t="shared" si="1"/>
+        <v>-0.41915150066779439</v>
+      </c>
+    </row>
+    <row r="58" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A58" s="3">
+        <v>43737.631995104166</v>
+      </c>
+      <c r="B58" s="1">
+        <v>0.16628741099722999</v>
+      </c>
+      <c r="C58" s="1">
+        <v>3.0112406984858402</v>
+      </c>
+      <c r="D58" s="2">
+        <f t="shared" si="1"/>
+        <v>-0.5127111045895546</v>
+      </c>
+    </row>
+    <row r="59" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A59" s="3">
+        <v>43737.632005590276</v>
+      </c>
+      <c r="B59" s="1">
+        <v>0.16628741099722999</v>
+      </c>
+      <c r="C59" s="1">
+        <v>5.1871294098564702</v>
+      </c>
+      <c r="D59" s="2">
+        <f t="shared" si="1"/>
+        <v>0.72258876962733165</v>
+      </c>
+    </row>
+    <row r="60" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A60" s="3">
+        <v>43737.632021377314</v>
+      </c>
+      <c r="B60" s="1">
+        <v>0.16628741099722999</v>
+      </c>
+      <c r="C60" s="1">
+        <v>6.1505851217096401</v>
+      </c>
+      <c r="D60" s="2">
+        <f t="shared" si="1"/>
+        <v>0.18573967135318281</v>
+      </c>
+    </row>
+    <row r="61" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A61" s="3">
+        <v>43737.632035844908</v>
+      </c>
+      <c r="B61" s="1">
+        <v>0.16628741099722999</v>
+      </c>
+      <c r="C61" s="1">
+        <v>3.7343628498103798</v>
+      </c>
+      <c r="D61" s="2">
+        <f t="shared" si="1"/>
+        <v>-0.39284429433725776</v>
+      </c>
+    </row>
+    <row r="62" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A62" s="3">
+        <v>43737.63205158565</v>
+      </c>
+      <c r="B62" s="1">
+        <v>0.16628741099722999</v>
+      </c>
+      <c r="C62" s="1">
+        <v>5.8252693243340001</v>
+      </c>
+      <c r="D62" s="2">
+        <f t="shared" si="1"/>
+        <v>0.55990983164096941</v>
+      </c>
+    </row>
+    <row r="63" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A63" s="3">
+        <v>43737.632063159719</v>
+      </c>
+      <c r="B63" s="1">
+        <v>0.16628741099722999</v>
+      </c>
+      <c r="C63" s="1">
+        <v>5.23096655072003</v>
+      </c>
+      <c r="D63" s="2">
+        <f t="shared" si="1"/>
+        <v>-0.10202151016973218</v>
+      </c>
+    </row>
+    <row r="64" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A64" s="3">
+        <v>43737.632074652778</v>
+      </c>
+      <c r="B64" s="1">
+        <v>0.16628741099722999</v>
+      </c>
+      <c r="C64" s="1">
+        <v>8.2483258880272405</v>
+      </c>
+      <c r="D64" s="2">
+        <f t="shared" si="1"/>
+        <v>0.57682634902184149</v>
+      </c>
+    </row>
+    <row r="65" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A65" s="3">
+        <v>43737.632089814811</v>
+      </c>
+      <c r="B65" s="1">
+        <v>0.16628741099722999</v>
+      </c>
+      <c r="C65" s="1">
+        <v>8.2004391966152603</v>
+      </c>
+      <c r="D65" s="2">
+        <f t="shared" si="1"/>
+        <v>-5.8056255368728301E-3</v>
+      </c>
+    </row>
+    <row r="66" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A66" s="3">
+        <v>43737.632107835649</v>
+      </c>
+      <c r="B66" s="1">
+        <v>0.16628741099722999</v>
+      </c>
+      <c r="C66" s="1">
+        <v>5.9544052790168296</v>
+      </c>
+      <c r="D66" s="2">
+        <f t="shared" si="1"/>
+        <v>-0.27389190551226616</v>
+      </c>
+    </row>
+    <row r="67" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A67" s="3">
+        <v>43737.632119756941</v>
+      </c>
+      <c r="B67" s="1">
+        <v>0.16628741099722999</v>
+      </c>
+      <c r="C67" s="1">
+        <v>4.56506804735917</v>
+      </c>
+      <c r="D67" s="2">
+        <f t="shared" si="1"/>
+        <v>-0.23332930268513097</v>
+      </c>
+    </row>
+    <row r="68" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A68" s="3">
+        <v>43737.63213607639</v>
+      </c>
+      <c r="B68" s="1">
+        <v>0.16628741099722999</v>
+      </c>
+      <c r="C68" s="1">
+        <v>8.9145437654091904</v>
+      </c>
+      <c r="D68" s="2">
+        <f t="shared" si="1"/>
+        <v>0.95277346863780776</v>
+      </c>
+    </row>
+    <row r="69" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A69" s="3">
+        <v>43737.632162037036</v>
+      </c>
+      <c r="B69" s="1">
+        <v>0.16628741099722999</v>
+      </c>
+      <c r="C69" s="1">
+        <v>12.5490244679438</v>
+      </c>
+      <c r="D69" s="2">
+        <f t="shared" si="1"/>
+        <v>0.40770237918819419</v>
+      </c>
+    </row>
+    <row r="70" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A70" s="3">
+        <v>43737.632183877315</v>
+      </c>
+      <c r="B70" s="1">
+        <v>0.16628741099722999</v>
+      </c>
+      <c r="C70" s="1">
+        <v>10.2846375412668</v>
+      </c>
+      <c r="D70" s="2">
+        <f t="shared" si="1"/>
+        <v>-0.18044326333583341</v>
+      </c>
+    </row>
+    <row r="71" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A71" s="3">
+        <v>43737.632214780089</v>
+      </c>
+      <c r="B71" s="1">
+        <v>0.16628741099722999</v>
+      </c>
+      <c r="C71" s="1">
+        <v>2.7602194110505498</v>
+      </c>
+      <c r="D71" s="2">
+        <f t="shared" si="1"/>
+        <v>-0.73161723979330806</v>
+      </c>
+    </row>
+    <row r="72" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A72" s="3">
+        <v>43737.632241666666</v>
+      </c>
+      <c r="B72" s="1">
+        <v>0.16628741099722999</v>
+      </c>
+      <c r="C72" s="1">
+        <v>12.6515683545335</v>
+      </c>
+      <c r="D72" s="2">
+        <f t="shared" si="1"/>
+        <v>3.583537201384388</v>
+      </c>
+    </row>
+    <row r="73" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A73" s="3">
+        <v>43737.632263622683</v>
+      </c>
+      <c r="B73" s="1">
+        <v>0.16628741099722999</v>
+      </c>
+      <c r="C73" s="1">
+        <v>6.9335909111350604</v>
+      </c>
+      <c r="D73" s="2">
+        <f t="shared" si="1"/>
+        <v>-0.45195799312497792</v>
+      </c>
+    </row>
+    <row r="74" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A74" s="3">
+        <v>43737.632279745369</v>
+      </c>
+      <c r="B74" s="1">
+        <v>0.16628741099722999</v>
+      </c>
+      <c r="C74" s="1">
+        <v>5.2499778135006103</v>
+      </c>
+      <c r="D74" s="2">
+        <f t="shared" si="1"/>
+        <v>-0.24281979124707762</v>
+      </c>
+    </row>
+    <row r="75" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A75" s="3">
+        <v>43737.632296377313</v>
+      </c>
+      <c r="B75" s="1">
+        <v>0.16628741099722999</v>
+      </c>
+      <c r="C75" s="1">
+        <v>6.6309613105116698</v>
+      </c>
+      <c r="D75" s="2">
+        <f t="shared" si="1"/>
+        <v>0.26304558725177535</v>
+      </c>
+    </row>
+    <row r="76" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A76" s="3">
+        <v>43737.632308368055</v>
+      </c>
+      <c r="B76" s="1">
+        <v>0.16628741099722999</v>
+      </c>
+      <c r="C76" s="1">
+        <v>11.5594535511351</v>
+      </c>
+      <c r="D76" s="2">
+        <f t="shared" si="1"/>
+        <v>0.74325456141790236</v>
+      </c>
+    </row>
+    <row r="77" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A77" s="3">
+        <v>43737.632324849539</v>
+      </c>
+      <c r="B77" s="1">
+        <v>0.16628741099722999</v>
+      </c>
+      <c r="C77" s="1">
+        <v>11.960306334626701</v>
+      </c>
+      <c r="D77" s="2">
+        <f t="shared" si="1"/>
+        <v>3.4677485550537852E-2</v>
+      </c>
+    </row>
+    <row r="78" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A78" s="3">
+        <v>43737.632344872683</v>
+      </c>
+      <c r="B78" s="1">
+        <v>0.16628741099722999</v>
+      </c>
+      <c r="C78" s="1">
+        <v>5.3638978139560001</v>
+      </c>
+      <c r="D78" s="2">
+        <f t="shared" si="1"/>
+        <v>-0.55152504761297028</v>
+      </c>
+    </row>
+    <row r="79" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A79" s="3">
+        <v>43737.632358680552</v>
+      </c>
+      <c r="B79" s="1">
+        <v>0.16628741099722999</v>
+      </c>
+      <c r="C79" s="1">
+        <v>7.6216335923932501</v>
+      </c>
+      <c r="D79" s="2">
+        <f t="shared" si="1"/>
+        <v>0.42091327179331872</v>
+      </c>
+    </row>
+    <row r="80" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A80" s="3">
+        <v>43737.632379317132</v>
+      </c>
+      <c r="B80" s="1">
+        <v>0.16628741099722999</v>
+      </c>
+      <c r="C80" s="1">
+        <v>6.8516991415573099</v>
+      </c>
+      <c r="D80" s="2">
+        <f t="shared" si="1"/>
+        <v>-0.10101960970734294</v>
+      </c>
+    </row>
+    <row r="81" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A81" s="3">
+        <v>43737.632405324075</v>
+      </c>
+      <c r="B81" s="1">
+        <v>0.16628741099722999</v>
+      </c>
+      <c r="C81" s="1">
+        <v>8.0231200566894696</v>
+      </c>
+      <c r="D81" s="2">
+        <f t="shared" si="1"/>
+        <v>0.17096794399905738</v>
+      </c>
+    </row>
+    <row r="82" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A82" s="3">
+        <v>43737.632423229166</v>
+      </c>
+      <c r="B82" s="1">
+        <v>0.16628741099722999</v>
+      </c>
+      <c r="C82" s="1">
+        <v>8.7053989311749103</v>
+      </c>
+      <c r="D82" s="2">
+        <f t="shared" si="1"/>
+        <v>8.5039095721442456E-2</v>
+      </c>
+    </row>
+    <row r="83" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A83" s="3">
+        <v>43737.632444479168</v>
+      </c>
+      <c r="B83" s="1">
+        <v>0.16628741099722999</v>
+      </c>
+      <c r="C83" s="1">
+        <v>6.8530055325879804</v>
+      </c>
+      <c r="D83" s="2">
+        <f t="shared" si="1"/>
+        <v>-0.21278673306438864</v>
+      </c>
+    </row>
+    <row r="84" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A84" s="3">
+        <v>43737.632465393515</v>
+      </c>
+      <c r="B84" s="1">
+        <v>0.16628741099722999</v>
+      </c>
+      <c r="C84" s="1">
+        <v>7.4742017652380204</v>
+      </c>
+      <c r="D84" s="2">
+        <f t="shared" si="1"/>
+        <v>9.0645809301637958E-2</v>
+      </c>
+    </row>
+    <row r="85" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A85" s="3">
+        <v>43737.632479548614</v>
+      </c>
+      <c r="B85" s="1">
+        <v>0.16628741099722999</v>
+      </c>
+      <c r="C85" s="1">
+        <v>6.1049410540921203</v>
+      </c>
+      <c r="D85" s="2">
+        <f t="shared" si="1"/>
+        <v>-0.18319825369368994</v>
+      </c>
+    </row>
+    <row r="86" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A86" s="3">
+        <v>43737.632496261576</v>
+      </c>
+      <c r="B86" s="1">
+        <v>0.16628741099722999</v>
+      </c>
+      <c r="C86" s="1">
+        <v>5.6634270850888901</v>
+      </c>
+      <c r="D86" s="2">
+        <f t="shared" si="1"/>
+        <v>-7.2320758724981449E-2</v>
+      </c>
+    </row>
+    <row r="87" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A87" s="3">
+        <v>43737.632520023151</v>
+      </c>
+      <c r="B87" s="1">
+        <v>0.16628741099722999</v>
+      </c>
+      <c r="C87" s="1">
+        <v>8.8415351222308605</v>
+      </c>
+      <c r="D87" s="2">
+        <f t="shared" si="1"/>
+        <v>0.56116340678412535</v>
+      </c>
+    </row>
+    <row r="88" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A88" s="3">
+        <v>43737.632535335651</v>
+      </c>
+      <c r="B88" s="1">
+        <v>0.16628741099722999</v>
+      </c>
+      <c r="C88" s="1">
+        <v>6.6417824018626304</v>
+      </c>
+      <c r="D88" s="2">
+        <f t="shared" si="1"/>
+        <v>-0.24879760018565614</v>
+      </c>
+    </row>
+    <row r="89" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A89" s="3">
+        <v>43737.632555439814</v>
+      </c>
+      <c r="B89" s="1">
+        <v>0.16628741099722999</v>
+      </c>
+      <c r="C89" s="1">
+        <v>9.2305143458888494</v>
+      </c>
+      <c r="D89" s="2">
+        <f t="shared" si="1"/>
+        <v>0.38976464259055393</v>
+      </c>
+    </row>
+    <row r="90" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A90" s="3">
+        <v>43737.63257696759</v>
+      </c>
+      <c r="B90" s="1">
+        <v>0.16628741099722999</v>
+      </c>
+      <c r="C90" s="1">
+        <v>5.7787042184060899</v>
+      </c>
+      <c r="D90" s="2">
+        <f t="shared" si="1"/>
+        <v>-0.37395642302643195</v>
+      </c>
+    </row>
+    <row r="91" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A91" s="3">
+        <v>43737.632594363429</v>
+      </c>
+      <c r="B91" s="1">
+        <v>0.16628741099722999</v>
+      </c>
+      <c r="C91" s="1">
+        <v>3.7266015614128598</v>
+      </c>
+      <c r="D91" s="2">
+        <f t="shared" si="1"/>
+        <v>-0.35511467267297703</v>
+      </c>
+    </row>
+    <row r="92" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A92" s="3">
+        <v>43737.632612152775</v>
+      </c>
+      <c r="B92" s="1">
+        <v>0.16628741099722999</v>
+      </c>
+      <c r="C92" s="1">
+        <v>6.8275727590079898</v>
+      </c>
+      <c r="D92" s="2">
+        <f t="shared" si="1"/>
+        <v>0.83211772079531476</v>
+      </c>
+    </row>
+    <row r="93" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A93" s="3">
+        <v>43737.632629398147</v>
+      </c>
+      <c r="B93" s="1">
+        <v>0.16628741099722999</v>
+      </c>
+      <c r="C93" s="1">
+        <v>3.84302600118657</v>
+      </c>
+      <c r="D93" s="2">
+        <f t="shared" si="1"/>
+        <v>-0.43713144673321047</v>
+      </c>
+    </row>
+    <row r="94" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A94" s="3">
+        <v>43737.632645601851</v>
+      </c>
+      <c r="B94" s="1">
+        <v>0.16628741099722999</v>
+      </c>
+      <c r="C94" s="1">
+        <v>5.2522813292056796</v>
+      </c>
+      <c r="D94" s="2">
+        <f t="shared" si="1"/>
+        <v>0.36670460402401361</v>
+      </c>
+    </row>
+    <row r="95" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A95" s="3">
+        <v>43737.632661539355</v>
+      </c>
+      <c r="B95" s="1">
+        <v>0.16628741099722999</v>
+      </c>
+      <c r="C95" s="1">
+        <v>5.5985585661172896</v>
+      </c>
+      <c r="D95" s="2">
+        <f t="shared" si="1"/>
+        <v>6.5928920255301462E-2</v>
+      </c>
+    </row>
+    <row r="96" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A96" s="3">
+        <v>43737.632677777779</v>
+      </c>
+      <c r="B96" s="1">
+        <v>0.16628741099722999</v>
+      </c>
+      <c r="C96" s="1">
+        <v>4.1937641931389802</v>
+      </c>
+      <c r="D96" s="2">
+        <f t="shared" si="1"/>
+        <v>-0.25092072475229316</v>
+      </c>
+    </row>
+    <row r="97" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A97" s="3">
+        <v>43737.63269525463</v>
+      </c>
+      <c r="B97" s="1">
+        <v>0.16628741099722999</v>
+      </c>
+      <c r="C97" s="1">
+        <v>7.5729032797595197</v>
+      </c>
+      <c r="D97" s="2">
+        <f t="shared" ref="D97:D137" si="2">(C97-C96)/C96</f>
+        <v>0.80575324004836235</v>
+      </c>
+    </row>
+    <row r="98" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A98" s="3">
+        <v>43737.632712500003</v>
+      </c>
+      <c r="B98" s="1">
+        <v>0.16628741099722999</v>
+      </c>
+      <c r="C98" s="1">
+        <v>13.166490998260899</v>
+      </c>
+      <c r="D98" s="2">
+        <f t="shared" si="2"/>
+        <v>0.7386318710093186</v>
+      </c>
+    </row>
+    <row r="99" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A99" s="3">
+        <v>43737.632729201388</v>
+      </c>
+      <c r="B99" s="1">
+        <v>0.16628741099722999</v>
+      </c>
+      <c r="C99" s="1">
+        <v>9.9209748360553007</v>
+      </c>
+      <c r="D99" s="2">
+        <f t="shared" si="2"/>
+        <v>-0.24649818715056909</v>
+      </c>
+    </row>
+    <row r="100" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A100" s="3">
+        <v>43737.632752280093</v>
+      </c>
+      <c r="B100" s="1">
+        <v>0.16628741099722999</v>
+      </c>
+      <c r="C100" s="1">
+        <v>10.075451036583599</v>
+      </c>
+      <c r="D100" s="2">
+        <f t="shared" si="2"/>
+        <v>1.5570667508085353E-2</v>
+      </c>
+    </row>
+    <row r="101" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A101" s="3">
+        <v>43737.632770717595</v>
+      </c>
+      <c r="B101" s="1">
+        <v>0.16628741099722999</v>
+      </c>
+      <c r="C101" s="1">
+        <v>6.1252177353729103</v>
+      </c>
+      <c r="D101" s="2">
+        <f t="shared" si="2"/>
+        <v>-0.39206515786415264</v>
+      </c>
+    </row>
+    <row r="102" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A102" s="3">
+        <v>43737.632789965275</v>
+      </c>
+      <c r="B102" s="1">
+        <v>0.16628741099722999</v>
+      </c>
+      <c r="C102" s="1">
+        <v>14.990699514277701</v>
+      </c>
+      <c r="D102" s="2">
+        <f t="shared" si="2"/>
+        <v>1.4473741443846078</v>
+      </c>
+    </row>
+    <row r="103" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A103" s="3">
+        <v>43737.632808993054</v>
+      </c>
+      <c r="B103" s="1">
+        <v>0.16628741099722999</v>
+      </c>
+      <c r="C103" s="1">
+        <v>6.3439485060649696</v>
+      </c>
+      <c r="D103" s="2">
+        <f t="shared" si="2"/>
+        <v>-0.57680770667020864</v>
+      </c>
+    </row>
+    <row r="104" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A104" s="3">
+        <v>43737.632824537039</v>
+      </c>
+      <c r="B104" s="1">
+        <v>0.16628741099722999</v>
+      </c>
+      <c r="C104" s="1">
+        <v>8.7959508614286701</v>
+      </c>
+      <c r="D104" s="2">
+        <f t="shared" si="2"/>
+        <v>0.38651044424769943</v>
+      </c>
+    </row>
+    <row r="105" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A105" s="3">
+        <v>43737.632844409723</v>
+      </c>
+      <c r="B105" s="1">
+        <v>0.16628741099722999</v>
+      </c>
+      <c r="C105" s="1">
+        <v>6.2362819709260604</v>
+      </c>
+      <c r="D105" s="2">
+        <f t="shared" si="2"/>
+        <v>-0.29100536494889639</v>
+      </c>
+    </row>
+    <row r="106" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A106" s="3">
+        <v>43737.632867442131</v>
+      </c>
+      <c r="B106" s="1">
+        <v>0.16628741099722999</v>
+      </c>
+      <c r="C106" s="1">
+        <v>5.28673054076177</v>
+      </c>
+      <c r="D106" s="2">
+        <f t="shared" si="2"/>
+        <v>-0.15226242729099793</v>
+      </c>
+    </row>
+    <row r="107" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A107" s="3">
+        <v>43737.632889004628</v>
+      </c>
+      <c r="B107" s="1">
+        <v>0.16628741099722999</v>
+      </c>
+      <c r="C107" s="1">
+        <v>4.6162763397507902</v>
+      </c>
+      <c r="D107" s="2">
+        <f t="shared" si="2"/>
+        <v>-0.12681830402394093</v>
+      </c>
+    </row>
+    <row r="108" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A108" s="3">
+        <v>43737.632913657406</v>
+      </c>
+      <c r="B108" s="1">
+        <v>0.16628741099722999</v>
+      </c>
+      <c r="C108" s="1">
+        <v>3.3347612414102299</v>
+      </c>
+      <c r="D108" s="2">
+        <f t="shared" si="2"/>
+        <v>-0.27760796885260619</v>
+      </c>
+    </row>
+    <row r="109" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A109" s="3">
+        <v>43737.632932673609</v>
+      </c>
+      <c r="B109" s="1">
+        <v>0.16628741099722999</v>
+      </c>
+      <c r="C109" s="1">
+        <v>7.4416327177573498</v>
+      </c>
+      <c r="D109" s="2">
+        <f t="shared" si="2"/>
+        <v>1.2315338877485495</v>
+      </c>
+    </row>
+    <row r="110" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A110" s="3">
+        <v>43737.632949733794</v>
+      </c>
+      <c r="B110" s="1">
+        <v>0.16628741099722999</v>
+      </c>
+      <c r="C110" s="1">
+        <v>4.5889122917307601</v>
+      </c>
+      <c r="D110" s="2">
+        <f t="shared" si="2"/>
+        <v>-0.38334603899751463</v>
+      </c>
+    </row>
+    <row r="111" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A111" s="3">
+        <v>43737.632967361111</v>
+      </c>
+      <c r="B111" s="1">
+        <v>0.16628741099722999</v>
+      </c>
+      <c r="C111" s="1">
+        <v>6.3552143572670499</v>
+      </c>
+      <c r="D111" s="2">
+        <f t="shared" si="2"/>
+        <v>0.38490647744982481</v>
+      </c>
+    </row>
+    <row r="112" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A112" s="3">
+        <v>43737.632995254629</v>
+      </c>
+      <c r="B112" s="1">
+        <v>0.16628741099722999</v>
+      </c>
+      <c r="C112" s="1">
+        <v>6.4044349134591601</v>
+      </c>
+      <c r="D112" s="2">
+        <f t="shared" si="2"/>
+        <v>7.7449088929356959E-3</v>
+      </c>
+    </row>
+    <row r="113" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A113" s="3">
+        <v>43737.633016087966</v>
+      </c>
+      <c r="B113" s="1">
+        <v>0.16628741099722999</v>
+      </c>
+      <c r="C113" s="1">
+        <v>3.8620445837867301</v>
+      </c>
+      <c r="D113" s="2">
+        <f t="shared" si="2"/>
+        <v>-0.3969734042154916</v>
+      </c>
+    </row>
+    <row r="114" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A114" s="3">
+        <v>43737.633034687497</v>
+      </c>
+      <c r="B114" s="1">
+        <v>0.16628741099722999</v>
+      </c>
+      <c r="C114" s="1">
+        <v>8.1793302310839593</v>
+      </c>
+      <c r="D114" s="2">
+        <f t="shared" si="2"/>
+        <v>1.1178756623943829</v>
+      </c>
+    </row>
+    <row r="115" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A115" s="3">
+        <v>43737.633051122684</v>
+      </c>
+      <c r="B115" s="1">
+        <v>0.16628741099722999</v>
+      </c>
+      <c r="C115" s="1">
+        <v>13.723497759026399</v>
+      </c>
+      <c r="D115" s="2">
+        <f t="shared" si="2"/>
+        <v>0.67782659109090693</v>
+      </c>
+    </row>
+    <row r="116" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A116" s="3">
+        <v>43737.633075196762</v>
+      </c>
+      <c r="B116" s="1">
+        <v>0.16628741099722999</v>
+      </c>
+      <c r="C116" s="1">
+        <v>2.6227058014242099</v>
+      </c>
+      <c r="D116" s="2">
+        <f t="shared" si="2"/>
+        <v>-0.80888940651451846</v>
+      </c>
+    </row>
+    <row r="117" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A117" s="3">
+        <v>43737.633108136572</v>
+      </c>
+      <c r="B117" s="1">
+        <v>0.16628741099722999</v>
+      </c>
+      <c r="C117" s="1">
+        <v>4.0964623634805397</v>
+      </c>
+      <c r="D117" s="2">
+        <f t="shared" si="2"/>
+        <v>0.5619221802369273</v>
+      </c>
+    </row>
+    <row r="118" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A118" s="3">
+        <v>43737.633134837961</v>
+      </c>
+      <c r="B118" s="1">
+        <v>0.16628741099722999</v>
+      </c>
+      <c r="C118" s="1">
+        <v>3.7738483007313399</v>
+      </c>
+      <c r="D118" s="2">
+        <f t="shared" si="2"/>
+        <v>-7.8754308992379535E-2</v>
+      </c>
+    </row>
+    <row r="119" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A119" s="3">
+        <v>43737.633162731479</v>
+      </c>
+      <c r="B119" s="1">
+        <v>0.16628741099722999</v>
+      </c>
+      <c r="C119" s="1">
+        <v>4.7637230874232701</v>
+      </c>
+      <c r="D119" s="2">
+        <f t="shared" si="2"/>
+        <v>0.26229851011766975</v>
+      </c>
+    </row>
+    <row r="120" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A120" s="3">
+        <v>43737.633183796293</v>
+      </c>
+      <c r="B120" s="1">
+        <v>0.16628741099722999</v>
+      </c>
+      <c r="C120" s="1">
+        <v>3.6882892580561699</v>
+      </c>
+      <c r="D120" s="2">
+        <f t="shared" si="2"/>
+        <v>-0.22575490002900434</v>
+      </c>
+    </row>
+    <row r="121" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A121" s="3">
+        <v>43737.633197951393</v>
+      </c>
+      <c r="B121" s="1">
+        <v>0</v>
+      </c>
+      <c r="C121" s="1">
+        <v>3.8830020078476899</v>
+      </c>
+      <c r="D121" s="2">
+        <f t="shared" si="2"/>
+        <v>5.2792158143837926E-2</v>
+      </c>
+    </row>
+    <row r="122" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A122" s="3">
+        <v>43737.633225347221</v>
+      </c>
+      <c r="B122" s="1">
+        <v>0</v>
+      </c>
+      <c r="C122" s="1">
+        <v>11.5972761144219</v>
+      </c>
+      <c r="D122" s="2">
+        <f t="shared" si="2"/>
+        <v>1.9866778567158552</v>
+      </c>
+    </row>
+    <row r="123" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A123" s="3">
+        <v>43737.633281284725</v>
+      </c>
+      <c r="B123" s="1">
+        <v>0</v>
+      </c>
+      <c r="C123" s="1">
+        <v>21.455149123122101</v>
+      </c>
+      <c r="D123" s="2">
+        <f t="shared" si="2"/>
+        <v>0.85001623755783062</v>
+      </c>
+    </row>
+    <row r="124" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A124" s="3">
+        <v>43737.633333796293</v>
+      </c>
+      <c r="B124" s="1">
+        <v>0</v>
+      </c>
+      <c r="C124" s="1">
+        <v>21.835631909000099</v>
+      </c>
+      <c r="D124" s="2">
+        <f t="shared" si="2"/>
+        <v>1.7733868158853937E-2</v>
+      </c>
+    </row>
+    <row r="125" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A125" s="3">
+        <v>43737.633387581016</v>
+      </c>
+      <c r="B125" s="1">
+        <v>0</v>
+      </c>
+      <c r="C125" s="1">
+        <v>24.590362788530602</v>
+      </c>
+      <c r="D125" s="2">
+        <f t="shared" si="2"/>
+        <v>0.12615759832419007</v>
+      </c>
+    </row>
+    <row r="126" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A126" s="3">
+        <v>43737.633443715276</v>
+      </c>
+      <c r="B126" s="1">
+        <v>0</v>
+      </c>
+      <c r="C126" s="1">
+        <v>29.974044881506</v>
+      </c>
+      <c r="D126" s="2">
+        <f t="shared" si="2"/>
+        <v>0.21893463464827151</v>
+      </c>
+    </row>
+    <row r="127" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B127" s="1"/>
+      <c r="C127" s="1"/>
+      <c r="D127" s="2">
+        <f t="shared" si="2"/>
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="128" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B128" s="1"/>
+      <c r="C128" s="1"/>
+      <c r="D128" s="2" t="e">
+        <f t="shared" si="2"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="129" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B129" s="1"/>
+      <c r="C129" s="1"/>
+      <c r="D129" s="2" t="e">
+        <f t="shared" si="2"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="130" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B130" s="1"/>
+      <c r="C130" s="1"/>
+      <c r="D130" s="2" t="e">
+        <f t="shared" si="2"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="131" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B131" s="1"/>
+      <c r="C131" s="1"/>
+      <c r="D131" s="2" t="e">
+        <f t="shared" si="2"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="132" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B132" s="1"/>
+      <c r="C132" s="1"/>
+      <c r="D132" s="2" t="e">
+        <f t="shared" si="2"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="133" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B133" s="1"/>
+      <c r="C133" s="1"/>
+      <c r="D133" s="2" t="e">
+        <f t="shared" si="2"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="134" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B134" s="1"/>
+      <c r="C134" s="1"/>
+      <c r="D134" s="2" t="e">
+        <f t="shared" si="2"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="135" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B135" s="1"/>
+      <c r="C135" s="1"/>
+      <c r="D135" s="2" t="e">
+        <f t="shared" si="2"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="136" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B136" s="1"/>
+      <c r="C136" s="1"/>
+      <c r="D136" s="2" t="e">
+        <f t="shared" si="2"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="137" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B137" s="1"/>
+      <c r="C137" s="1"/>
+      <c r="D137" s="2" t="e">
+        <f t="shared" si="2"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
+</worksheet>
 </file>
</xml_diff>